<commit_message>
edit text and hyperlink comparison calc
</commit_message>
<xml_diff>
--- a/examples/ExamplesComparisonTest.xlsx
+++ b/examples/ExamplesComparisonTest.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\cygwin64\home\Joh\git\ReinsuranceTestTool\examples\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{515644D1-F509-4279-B624-BFC69D9585B5}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{2471A560-E43D-4354-A940-35CF0DD22AC9}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="30720" windowHeight="9072" firstSheet="1" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="456" uniqueCount="162">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="476" uniqueCount="163">
   <si>
     <t>Limit</t>
   </si>
@@ -508,6 +508,9 @@
   </si>
   <si>
     <t>Input files same as loc_SS. Adding a second ReinsuranceNumber doesn’t work.</t>
+  </si>
+  <si>
+    <t>Treaty 1 on each account: 10% ceded. Treaty 2 on each account at same inuring level 20% ceded</t>
   </si>
 </sst>
 </file>
@@ -808,7 +811,7 @@
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="96">
+  <cellXfs count="98">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
@@ -1031,10 +1034,16 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="1" fontId="13" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1042,6 +1051,15 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -1070,20 +1088,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="1" fontId="13" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="6">
@@ -1495,10 +1504,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:U335"/>
+  <dimension ref="A1:U351"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A308" zoomScale="84" zoomScaleNormal="84" workbookViewId="0">
-      <selection activeCell="I337" sqref="I337"/>
+    <sheetView showGridLines="0" topLeftCell="A175" zoomScale="84" zoomScaleNormal="84" workbookViewId="0">
+      <selection activeCell="A175" sqref="A175"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1884,26 +1893,26 @@
       <c r="B25" s="25" t="s">
         <v>48</v>
       </c>
-      <c r="C25" s="86">
+      <c r="C25" s="91">
         <v>100</v>
       </c>
-      <c r="D25" s="86"/>
-      <c r="E25" s="87"/>
-      <c r="F25" s="86">
+      <c r="D25" s="91"/>
+      <c r="E25" s="92"/>
+      <c r="F25" s="91">
         <v>100</v>
       </c>
-      <c r="G25" s="86"/>
-      <c r="H25" s="87"/>
-      <c r="I25" s="88">
+      <c r="G25" s="91"/>
+      <c r="H25" s="92"/>
+      <c r="I25" s="93">
         <v>100</v>
       </c>
-      <c r="J25" s="86"/>
-      <c r="K25" s="87"/>
-      <c r="L25" s="86">
+      <c r="J25" s="91"/>
+      <c r="K25" s="92"/>
+      <c r="L25" s="91">
         <v>100</v>
       </c>
-      <c r="M25" s="86"/>
-      <c r="N25" s="87"/>
+      <c r="M25" s="91"/>
+      <c r="N25" s="92"/>
       <c r="O25" s="8"/>
       <c r="P25" s="8"/>
       <c r="Q25" s="11"/>
@@ -2144,30 +2153,30 @@
       <c r="B34" s="8" t="s">
         <v>50</v>
       </c>
-      <c r="C34" s="89">
+      <c r="C34" s="94">
         <f>SUMIF($C$21:$N$21,C21,$C$31:$N$31)</f>
         <v>2000</v>
       </c>
-      <c r="D34" s="89"/>
-      <c r="E34" s="90"/>
-      <c r="F34" s="89">
+      <c r="D34" s="94"/>
+      <c r="E34" s="95"/>
+      <c r="F34" s="94">
         <f>SUMIF($C$21:$N$21,F21,$C$31:$N$31)</f>
         <v>2000</v>
       </c>
-      <c r="G34" s="89"/>
-      <c r="H34" s="90"/>
-      <c r="I34" s="89">
+      <c r="G34" s="94"/>
+      <c r="H34" s="95"/>
+      <c r="I34" s="94">
         <f>SUMIF($C$21:$N$21,I21,$C$31:$N$31)</f>
         <v>2000</v>
       </c>
-      <c r="J34" s="89"/>
-      <c r="K34" s="90"/>
-      <c r="L34" s="89">
+      <c r="J34" s="94"/>
+      <c r="K34" s="95"/>
+      <c r="L34" s="94">
         <f>SUMIF($C$21:$N$21,L21,$C$31:$N$31)</f>
         <v>2000</v>
       </c>
-      <c r="M34" s="89"/>
-      <c r="N34" s="90"/>
+      <c r="M34" s="94"/>
+      <c r="N34" s="95"/>
       <c r="O34" s="8"/>
       <c r="P34" s="23"/>
       <c r="Q34" s="11"/>
@@ -2179,30 +2188,30 @@
       <c r="B35" s="36" t="s">
         <v>52</v>
       </c>
-      <c r="C35" s="82">
+      <c r="C35" s="87">
         <f>MIN(C34, C25)</f>
         <v>100</v>
       </c>
-      <c r="D35" s="83"/>
-      <c r="E35" s="84"/>
-      <c r="F35" s="82">
+      <c r="D35" s="88"/>
+      <c r="E35" s="89"/>
+      <c r="F35" s="87">
         <f>MIN(F34, F25)</f>
         <v>100</v>
       </c>
-      <c r="G35" s="83"/>
-      <c r="H35" s="84"/>
-      <c r="I35" s="82">
+      <c r="G35" s="88"/>
+      <c r="H35" s="89"/>
+      <c r="I35" s="87">
         <f>MIN(I34, I25)</f>
         <v>100</v>
       </c>
-      <c r="J35" s="83"/>
-      <c r="K35" s="84"/>
-      <c r="L35" s="85">
+      <c r="J35" s="88"/>
+      <c r="K35" s="89"/>
+      <c r="L35" s="90">
         <f>MIN(L34, L25)</f>
         <v>100</v>
       </c>
-      <c r="M35" s="83"/>
-      <c r="N35" s="84"/>
+      <c r="M35" s="88"/>
+      <c r="N35" s="89"/>
       <c r="O35" s="12">
         <f>SUM(C35:N35)</f>
         <v>400</v>
@@ -2535,11 +2544,11 @@
       <c r="A53" s="43" t="s">
         <v>61</v>
       </c>
-      <c r="C53" s="80">
-        <v>1</v>
-      </c>
-      <c r="D53" s="80"/>
-      <c r="E53" s="81"/>
+      <c r="C53" s="82">
+        <v>1</v>
+      </c>
+      <c r="D53" s="82"/>
+      <c r="E53" s="83"/>
       <c r="H53" s="40"/>
       <c r="N53" s="40"/>
     </row>
@@ -2547,11 +2556,11 @@
       <c r="A54" s="43" t="s">
         <v>62</v>
       </c>
-      <c r="C54" s="80" t="s">
+      <c r="C54" s="82" t="s">
         <v>70</v>
       </c>
-      <c r="D54" s="80"/>
-      <c r="E54" s="81"/>
+      <c r="D54" s="82"/>
+      <c r="E54" s="83"/>
       <c r="H54" s="40"/>
       <c r="N54" s="40"/>
     </row>
@@ -2559,11 +2568,11 @@
       <c r="A55" s="43" t="s">
         <v>63</v>
       </c>
-      <c r="C55" s="80">
-        <v>1</v>
-      </c>
-      <c r="D55" s="80"/>
-      <c r="E55" s="81"/>
+      <c r="C55" s="82">
+        <v>1</v>
+      </c>
+      <c r="D55" s="82"/>
+      <c r="E55" s="83"/>
       <c r="H55" s="40"/>
       <c r="N55" s="40"/>
     </row>
@@ -2571,11 +2580,11 @@
       <c r="A56" s="43" t="s">
         <v>64</v>
       </c>
-      <c r="C56" s="78">
+      <c r="C56" s="81">
         <v>0</v>
       </c>
-      <c r="D56" s="78"/>
-      <c r="E56" s="81"/>
+      <c r="D56" s="81"/>
+      <c r="E56" s="83"/>
       <c r="H56" s="40"/>
       <c r="N56" s="40"/>
     </row>
@@ -2583,12 +2592,12 @@
       <c r="A57" s="44" t="s">
         <v>65</v>
       </c>
-      <c r="C57" s="78">
+      <c r="C57" s="81">
         <f>MAX(0, SUM(C$50:E$50)-C56)</f>
         <v>100</v>
       </c>
-      <c r="D57" s="78"/>
-      <c r="E57" s="81"/>
+      <c r="D57" s="81"/>
+      <c r="E57" s="83"/>
       <c r="H57" s="40"/>
       <c r="N57" s="40"/>
     </row>
@@ -2596,11 +2605,11 @@
       <c r="A58" s="43" t="s">
         <v>0</v>
       </c>
-      <c r="C58" s="78">
+      <c r="C58" s="81">
         <v>10</v>
       </c>
-      <c r="D58" s="78"/>
-      <c r="E58" s="81"/>
+      <c r="D58" s="81"/>
+      <c r="E58" s="83"/>
       <c r="H58" s="40"/>
       <c r="N58" s="40"/>
     </row>
@@ -2608,12 +2617,12 @@
       <c r="A59" s="44" t="s">
         <v>66</v>
       </c>
-      <c r="C59" s="78">
+      <c r="C59" s="81">
         <f>IF(C58="Unlimited", C57, MIN(C57, C58))</f>
         <v>10</v>
       </c>
-      <c r="D59" s="78"/>
-      <c r="E59" s="81"/>
+      <c r="D59" s="81"/>
+      <c r="E59" s="83"/>
       <c r="H59" s="40"/>
       <c r="N59" s="40"/>
     </row>
@@ -2621,11 +2630,11 @@
       <c r="A60" s="43" t="s">
         <v>71</v>
       </c>
-      <c r="C60" s="79">
-        <v>1</v>
-      </c>
-      <c r="D60" s="79"/>
-      <c r="E60" s="93"/>
+      <c r="C60" s="80">
+        <v>1</v>
+      </c>
+      <c r="D60" s="80"/>
+      <c r="E60" s="84"/>
       <c r="H60" s="40"/>
       <c r="N60" s="40"/>
     </row>
@@ -2633,12 +2642,12 @@
       <c r="A61" s="44" t="s">
         <v>72</v>
       </c>
-      <c r="C61" s="78">
+      <c r="C61" s="81">
         <f>C60*C59</f>
         <v>10</v>
       </c>
-      <c r="D61" s="78"/>
-      <c r="E61" s="81"/>
+      <c r="D61" s="81"/>
+      <c r="E61" s="83"/>
       <c r="H61" s="40"/>
       <c r="N61" s="40"/>
     </row>
@@ -2646,9 +2655,9 @@
       <c r="A62" s="43" t="s">
         <v>3</v>
       </c>
-      <c r="C62" s="91"/>
-      <c r="D62" s="91"/>
-      <c r="E62" s="92"/>
+      <c r="C62" s="85"/>
+      <c r="D62" s="85"/>
+      <c r="E62" s="86"/>
       <c r="H62" s="40"/>
       <c r="N62" s="40"/>
     </row>
@@ -2656,9 +2665,9 @@
       <c r="A63" s="43" t="s">
         <v>67</v>
       </c>
-      <c r="C63" s="91"/>
-      <c r="D63" s="91"/>
-      <c r="E63" s="92"/>
+      <c r="C63" s="85"/>
+      <c r="D63" s="85"/>
+      <c r="E63" s="86"/>
       <c r="H63" s="40"/>
       <c r="N63" s="40"/>
     </row>
@@ -2666,12 +2675,12 @@
       <c r="A64" s="45" t="s">
         <v>68</v>
       </c>
-      <c r="C64" s="78">
+      <c r="C64" s="81">
         <f>MIN(C61,IF(OR(C63="Unlimited",C63=""),10^18,C63))</f>
         <v>10</v>
       </c>
-      <c r="D64" s="78"/>
-      <c r="E64" s="81"/>
+      <c r="D64" s="81"/>
+      <c r="E64" s="83"/>
       <c r="H64" s="40"/>
       <c r="N64" s="40"/>
     </row>
@@ -2752,11 +2761,11 @@
       <c r="A68" s="43" t="s">
         <v>61</v>
       </c>
-      <c r="C68" s="80">
-        <v>1</v>
-      </c>
-      <c r="D68" s="80"/>
-      <c r="E68" s="78"/>
+      <c r="C68" s="82">
+        <v>1</v>
+      </c>
+      <c r="D68" s="82"/>
+      <c r="E68" s="81"/>
       <c r="F68" s="13"/>
       <c r="H68" s="40"/>
       <c r="N68" s="40"/>
@@ -2765,11 +2774,11 @@
       <c r="A69" s="43" t="s">
         <v>62</v>
       </c>
-      <c r="C69" s="80" t="s">
+      <c r="C69" s="82" t="s">
         <v>83</v>
       </c>
-      <c r="D69" s="80"/>
-      <c r="E69" s="78"/>
+      <c r="D69" s="82"/>
+      <c r="E69" s="81"/>
       <c r="F69" s="13"/>
       <c r="H69" s="40"/>
       <c r="N69" s="40"/>
@@ -2778,11 +2787,11 @@
       <c r="A70" s="43" t="s">
         <v>63</v>
       </c>
-      <c r="C70" s="80">
-        <v>1</v>
-      </c>
-      <c r="D70" s="80"/>
-      <c r="E70" s="78"/>
+      <c r="C70" s="82">
+        <v>1</v>
+      </c>
+      <c r="D70" s="82"/>
+      <c r="E70" s="81"/>
       <c r="F70" s="13"/>
       <c r="H70" s="40"/>
       <c r="N70" s="40"/>
@@ -2791,11 +2800,11 @@
       <c r="A71" s="43" t="s">
         <v>64</v>
       </c>
-      <c r="C71" s="78">
+      <c r="C71" s="81">
         <v>0</v>
       </c>
-      <c r="D71" s="78"/>
-      <c r="E71" s="78"/>
+      <c r="D71" s="81"/>
+      <c r="E71" s="81"/>
       <c r="F71" s="13"/>
       <c r="H71" s="40"/>
       <c r="N71" s="40"/>
@@ -2804,12 +2813,12 @@
       <c r="A72" s="44" t="s">
         <v>65</v>
       </c>
-      <c r="C72" s="78">
+      <c r="C72" s="81">
         <f>MAX(0, SUM(C$50:H$50)-C71)</f>
         <v>200</v>
       </c>
-      <c r="D72" s="78"/>
-      <c r="E72" s="78"/>
+      <c r="D72" s="81"/>
+      <c r="E72" s="81"/>
       <c r="F72" s="13"/>
       <c r="H72" s="40"/>
       <c r="N72" s="40"/>
@@ -2818,11 +2827,11 @@
       <c r="A73" s="43" t="s">
         <v>0</v>
       </c>
-      <c r="C73" s="78">
+      <c r="C73" s="81">
         <v>10</v>
       </c>
-      <c r="D73" s="78"/>
-      <c r="E73" s="78"/>
+      <c r="D73" s="81"/>
+      <c r="E73" s="81"/>
       <c r="F73" s="13"/>
       <c r="H73" s="40"/>
       <c r="N73" s="40"/>
@@ -2831,12 +2840,12 @@
       <c r="A74" s="44" t="s">
         <v>66</v>
       </c>
-      <c r="C74" s="78">
+      <c r="C74" s="81">
         <f>IF(C73="Unlimited", C72, MIN(C72, C73))</f>
         <v>10</v>
       </c>
-      <c r="D74" s="78"/>
-      <c r="E74" s="78"/>
+      <c r="D74" s="81"/>
+      <c r="E74" s="81"/>
       <c r="F74" s="13"/>
       <c r="H74" s="40"/>
       <c r="N74" s="40"/>
@@ -2845,11 +2854,11 @@
       <c r="A75" s="43" t="s">
         <v>71</v>
       </c>
-      <c r="C75" s="79">
-        <v>1</v>
-      </c>
-      <c r="D75" s="79"/>
-      <c r="E75" s="79"/>
+      <c r="C75" s="80">
+        <v>1</v>
+      </c>
+      <c r="D75" s="80"/>
+      <c r="E75" s="80"/>
       <c r="F75" s="13"/>
       <c r="H75" s="40"/>
       <c r="N75" s="40"/>
@@ -2858,12 +2867,12 @@
       <c r="A76" s="44" t="s">
         <v>72</v>
       </c>
-      <c r="C76" s="78">
+      <c r="C76" s="81">
         <f>C75*C74</f>
         <v>10</v>
       </c>
-      <c r="D76" s="78"/>
-      <c r="E76" s="78"/>
+      <c r="D76" s="81"/>
+      <c r="E76" s="81"/>
       <c r="F76" s="13"/>
       <c r="H76" s="40"/>
       <c r="N76" s="40"/>
@@ -2872,9 +2881,9 @@
       <c r="A77" s="43" t="s">
         <v>3</v>
       </c>
-      <c r="C77" s="91"/>
-      <c r="D77" s="91"/>
-      <c r="E77" s="91"/>
+      <c r="C77" s="85"/>
+      <c r="D77" s="85"/>
+      <c r="E77" s="85"/>
       <c r="F77" s="13"/>
       <c r="H77" s="40"/>
       <c r="N77" s="40"/>
@@ -2883,9 +2892,9 @@
       <c r="A78" s="43" t="s">
         <v>67</v>
       </c>
-      <c r="C78" s="91"/>
-      <c r="D78" s="91"/>
-      <c r="E78" s="91"/>
+      <c r="C78" s="85"/>
+      <c r="D78" s="85"/>
+      <c r="E78" s="85"/>
       <c r="F78" s="13"/>
       <c r="H78" s="40"/>
       <c r="N78" s="40"/>
@@ -2894,12 +2903,12 @@
       <c r="A79" s="45" t="s">
         <v>68</v>
       </c>
-      <c r="C79" s="78">
+      <c r="C79" s="81">
         <f>MIN(C76,IF(OR(C78="Unlimited",C78=""),10^18,C78))</f>
         <v>10</v>
       </c>
-      <c r="D79" s="78"/>
-      <c r="E79" s="78"/>
+      <c r="D79" s="81"/>
+      <c r="E79" s="81"/>
       <c r="F79" s="13"/>
       <c r="H79" s="40"/>
       <c r="N79" s="40"/>
@@ -2982,11 +2991,11 @@
       <c r="A83" s="43" t="s">
         <v>61</v>
       </c>
-      <c r="C83" s="80">
-        <v>1</v>
-      </c>
-      <c r="D83" s="80"/>
-      <c r="E83" s="78"/>
+      <c r="C83" s="82">
+        <v>1</v>
+      </c>
+      <c r="D83" s="82"/>
+      <c r="E83" s="81"/>
       <c r="F83" s="13"/>
       <c r="H83" s="40"/>
       <c r="N83" s="40"/>
@@ -2995,11 +3004,11 @@
       <c r="A84" s="43" t="s">
         <v>62</v>
       </c>
-      <c r="C84" s="80" t="s">
+      <c r="C84" s="82" t="s">
         <v>85</v>
       </c>
-      <c r="D84" s="80"/>
-      <c r="E84" s="78"/>
+      <c r="D84" s="82"/>
+      <c r="E84" s="81"/>
       <c r="F84" s="13"/>
       <c r="H84" s="40"/>
       <c r="N84" s="40"/>
@@ -3008,11 +3017,11 @@
       <c r="A85" s="43" t="s">
         <v>63</v>
       </c>
-      <c r="C85" s="80">
-        <v>1</v>
-      </c>
-      <c r="D85" s="80"/>
-      <c r="E85" s="78"/>
+      <c r="C85" s="82">
+        <v>1</v>
+      </c>
+      <c r="D85" s="82"/>
+      <c r="E85" s="81"/>
       <c r="F85" s="13"/>
       <c r="H85" s="40"/>
       <c r="N85" s="40"/>
@@ -3021,11 +3030,11 @@
       <c r="A86" s="43" t="s">
         <v>64</v>
       </c>
-      <c r="C86" s="78">
+      <c r="C86" s="81">
         <v>0</v>
       </c>
-      <c r="D86" s="78"/>
-      <c r="E86" s="78"/>
+      <c r="D86" s="81"/>
+      <c r="E86" s="81"/>
       <c r="F86" s="13"/>
       <c r="H86" s="40"/>
       <c r="N86" s="40"/>
@@ -3034,12 +3043,12 @@
       <c r="A87" s="44" t="s">
         <v>65</v>
       </c>
-      <c r="C87" s="78">
+      <c r="C87" s="81">
         <f>MAX(0, SUM(C$50:H$50)-C86)</f>
         <v>200</v>
       </c>
-      <c r="D87" s="78"/>
-      <c r="E87" s="78"/>
+      <c r="D87" s="81"/>
+      <c r="E87" s="81"/>
       <c r="F87" s="13"/>
       <c r="H87" s="40"/>
       <c r="N87" s="40"/>
@@ -3048,11 +3057,11 @@
       <c r="A88" s="43" t="s">
         <v>0</v>
       </c>
-      <c r="C88" s="78">
+      <c r="C88" s="81">
         <v>10</v>
       </c>
-      <c r="D88" s="78"/>
-      <c r="E88" s="78"/>
+      <c r="D88" s="81"/>
+      <c r="E88" s="81"/>
       <c r="F88" s="13"/>
       <c r="H88" s="40"/>
       <c r="N88" s="40"/>
@@ -3061,12 +3070,12 @@
       <c r="A89" s="44" t="s">
         <v>66</v>
       </c>
-      <c r="C89" s="78">
+      <c r="C89" s="81">
         <f>IF(C88="Unlimited", C87, MIN(C87, C88))</f>
         <v>10</v>
       </c>
-      <c r="D89" s="78"/>
-      <c r="E89" s="78"/>
+      <c r="D89" s="81"/>
+      <c r="E89" s="81"/>
       <c r="F89" s="13"/>
       <c r="H89" s="40"/>
       <c r="N89" s="40"/>
@@ -3075,11 +3084,11 @@
       <c r="A90" s="43" t="s">
         <v>71</v>
       </c>
-      <c r="C90" s="79">
-        <v>1</v>
-      </c>
-      <c r="D90" s="79"/>
-      <c r="E90" s="79"/>
+      <c r="C90" s="80">
+        <v>1</v>
+      </c>
+      <c r="D90" s="80"/>
+      <c r="E90" s="80"/>
       <c r="F90" s="13"/>
       <c r="H90" s="40"/>
       <c r="N90" s="40"/>
@@ -3088,12 +3097,12 @@
       <c r="A91" s="44" t="s">
         <v>72</v>
       </c>
-      <c r="C91" s="78">
+      <c r="C91" s="81">
         <f>C90*C89</f>
         <v>10</v>
       </c>
-      <c r="D91" s="78"/>
-      <c r="E91" s="78"/>
+      <c r="D91" s="81"/>
+      <c r="E91" s="81"/>
       <c r="F91" s="13"/>
       <c r="H91" s="40"/>
       <c r="N91" s="40"/>
@@ -3102,9 +3111,9 @@
       <c r="A92" s="43" t="s">
         <v>3</v>
       </c>
-      <c r="C92" s="91"/>
-      <c r="D92" s="91"/>
-      <c r="E92" s="91"/>
+      <c r="C92" s="85"/>
+      <c r="D92" s="85"/>
+      <c r="E92" s="85"/>
       <c r="F92" s="13"/>
       <c r="H92" s="40"/>
       <c r="N92" s="40"/>
@@ -3113,9 +3122,9 @@
       <c r="A93" s="43" t="s">
         <v>67</v>
       </c>
-      <c r="C93" s="91"/>
-      <c r="D93" s="91"/>
-      <c r="E93" s="91"/>
+      <c r="C93" s="85"/>
+      <c r="D93" s="85"/>
+      <c r="E93" s="85"/>
       <c r="F93" s="13"/>
       <c r="H93" s="40"/>
       <c r="N93" s="40"/>
@@ -3124,12 +3133,12 @@
       <c r="A94" s="45" t="s">
         <v>68</v>
       </c>
-      <c r="C94" s="78">
+      <c r="C94" s="81">
         <f>MIN(C91,IF(OR(C93="Unlimited",C93=""),10^18,C93))</f>
         <v>10</v>
       </c>
-      <c r="D94" s="78"/>
-      <c r="E94" s="78"/>
+      <c r="D94" s="81"/>
+      <c r="E94" s="81"/>
       <c r="F94" s="13"/>
       <c r="H94" s="40"/>
       <c r="N94" s="40"/>
@@ -3215,192 +3224,192 @@
       <c r="A98" s="43" t="s">
         <v>61</v>
       </c>
-      <c r="C98" s="80">
-        <v>1</v>
-      </c>
-      <c r="D98" s="80"/>
-      <c r="E98" s="78"/>
-      <c r="F98" s="80">
-        <v>1</v>
-      </c>
-      <c r="G98" s="80"/>
-      <c r="H98" s="78"/>
+      <c r="C98" s="82">
+        <v>1</v>
+      </c>
+      <c r="D98" s="82"/>
+      <c r="E98" s="81"/>
+      <c r="F98" s="82">
+        <v>1</v>
+      </c>
+      <c r="G98" s="82"/>
+      <c r="H98" s="81"/>
       <c r="N98" s="40"/>
     </row>
     <row r="99" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A99" s="43" t="s">
         <v>62</v>
       </c>
-      <c r="C99" s="80" t="s">
+      <c r="C99" s="82" t="s">
         <v>70</v>
       </c>
-      <c r="D99" s="80"/>
-      <c r="E99" s="78"/>
-      <c r="F99" s="80" t="s">
+      <c r="D99" s="82"/>
+      <c r="E99" s="81"/>
+      <c r="F99" s="82" t="s">
         <v>70</v>
       </c>
-      <c r="G99" s="80"/>
-      <c r="H99" s="78"/>
+      <c r="G99" s="82"/>
+      <c r="H99" s="81"/>
       <c r="N99" s="40"/>
     </row>
     <row r="100" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A100" s="43" t="s">
         <v>63</v>
       </c>
-      <c r="C100" s="80">
-        <v>1</v>
-      </c>
-      <c r="D100" s="80"/>
-      <c r="E100" s="78"/>
-      <c r="F100" s="80">
-        <v>1</v>
-      </c>
-      <c r="G100" s="80"/>
-      <c r="H100" s="78"/>
+      <c r="C100" s="82">
+        <v>1</v>
+      </c>
+      <c r="D100" s="82"/>
+      <c r="E100" s="81"/>
+      <c r="F100" s="82">
+        <v>1</v>
+      </c>
+      <c r="G100" s="82"/>
+      <c r="H100" s="81"/>
       <c r="N100" s="40"/>
     </row>
     <row r="101" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A101" s="43" t="s">
         <v>64</v>
       </c>
-      <c r="C101" s="78">
+      <c r="C101" s="81">
         <v>0</v>
       </c>
-      <c r="D101" s="78"/>
-      <c r="E101" s="78"/>
-      <c r="F101" s="78">
+      <c r="D101" s="81"/>
+      <c r="E101" s="81"/>
+      <c r="F101" s="81">
         <v>0</v>
       </c>
-      <c r="G101" s="78"/>
-      <c r="H101" s="78"/>
+      <c r="G101" s="81"/>
+      <c r="H101" s="81"/>
       <c r="N101" s="40"/>
     </row>
     <row r="102" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A102" s="44" t="s">
         <v>65</v>
       </c>
-      <c r="C102" s="78">
+      <c r="C102" s="81">
         <f>MAX(0, SUM(C$50:E$50)-C101)</f>
         <v>100</v>
       </c>
-      <c r="D102" s="78"/>
-      <c r="E102" s="78"/>
-      <c r="F102" s="78">
+      <c r="D102" s="81"/>
+      <c r="E102" s="81"/>
+      <c r="F102" s="81">
         <f>MAX(0, SUM(F$50:H$50)-F101)</f>
         <v>100</v>
       </c>
-      <c r="G102" s="78"/>
-      <c r="H102" s="78"/>
+      <c r="G102" s="81"/>
+      <c r="H102" s="81"/>
       <c r="N102" s="40"/>
     </row>
     <row r="103" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A103" s="43" t="s">
         <v>0</v>
       </c>
-      <c r="C103" s="78">
+      <c r="C103" s="81">
         <v>10</v>
       </c>
-      <c r="D103" s="78"/>
-      <c r="E103" s="78"/>
-      <c r="F103" s="78">
+      <c r="D103" s="81"/>
+      <c r="E103" s="81"/>
+      <c r="F103" s="81">
         <v>10</v>
       </c>
-      <c r="G103" s="78"/>
-      <c r="H103" s="78"/>
+      <c r="G103" s="81"/>
+      <c r="H103" s="81"/>
       <c r="N103" s="40"/>
     </row>
     <row r="104" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A104" s="44" t="s">
         <v>66</v>
       </c>
-      <c r="C104" s="78">
+      <c r="C104" s="81">
         <f>IF(C103="Unlimited", C102, MIN(C102, C103))</f>
         <v>10</v>
       </c>
-      <c r="D104" s="78"/>
-      <c r="E104" s="78"/>
-      <c r="F104" s="78">
+      <c r="D104" s="81"/>
+      <c r="E104" s="81"/>
+      <c r="F104" s="81">
         <f>IF(F103="Unlimited", F102, MIN(F102, F103))</f>
         <v>10</v>
       </c>
-      <c r="G104" s="78"/>
-      <c r="H104" s="78"/>
+      <c r="G104" s="81"/>
+      <c r="H104" s="81"/>
       <c r="N104" s="40"/>
     </row>
     <row r="105" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A105" s="43" t="s">
         <v>71</v>
       </c>
-      <c r="C105" s="79">
-        <v>1</v>
-      </c>
-      <c r="D105" s="79"/>
-      <c r="E105" s="79"/>
-      <c r="F105" s="79">
-        <v>1</v>
-      </c>
-      <c r="G105" s="79"/>
-      <c r="H105" s="79"/>
+      <c r="C105" s="80">
+        <v>1</v>
+      </c>
+      <c r="D105" s="80"/>
+      <c r="E105" s="80"/>
+      <c r="F105" s="80">
+        <v>1</v>
+      </c>
+      <c r="G105" s="80"/>
+      <c r="H105" s="80"/>
       <c r="N105" s="40"/>
     </row>
     <row r="106" spans="1:15" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A106" s="44" t="s">
         <v>72</v>
       </c>
-      <c r="C106" s="78">
+      <c r="C106" s="81">
         <f>C105*C104</f>
         <v>10</v>
       </c>
-      <c r="D106" s="78"/>
-      <c r="E106" s="78"/>
-      <c r="F106" s="78">
+      <c r="D106" s="81"/>
+      <c r="E106" s="81"/>
+      <c r="F106" s="81">
         <f>F105*F104</f>
         <v>10</v>
       </c>
-      <c r="G106" s="78"/>
-      <c r="H106" s="78"/>
+      <c r="G106" s="81"/>
+      <c r="H106" s="81"/>
       <c r="N106" s="40"/>
     </row>
     <row r="107" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A107" s="43" t="s">
         <v>3</v>
       </c>
-      <c r="C107" s="91"/>
-      <c r="D107" s="91"/>
-      <c r="E107" s="91"/>
-      <c r="F107" s="91"/>
-      <c r="G107" s="91"/>
-      <c r="H107" s="91"/>
+      <c r="C107" s="85"/>
+      <c r="D107" s="85"/>
+      <c r="E107" s="85"/>
+      <c r="F107" s="85"/>
+      <c r="G107" s="85"/>
+      <c r="H107" s="85"/>
       <c r="N107" s="40"/>
     </row>
     <row r="108" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A108" s="43" t="s">
         <v>67</v>
       </c>
-      <c r="C108" s="91"/>
-      <c r="D108" s="91"/>
-      <c r="E108" s="91"/>
-      <c r="F108" s="91"/>
-      <c r="G108" s="91"/>
-      <c r="H108" s="91"/>
+      <c r="C108" s="85"/>
+      <c r="D108" s="85"/>
+      <c r="E108" s="85"/>
+      <c r="F108" s="85"/>
+      <c r="G108" s="85"/>
+      <c r="H108" s="85"/>
       <c r="N108" s="40"/>
     </row>
     <row r="109" spans="1:15" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A109" s="45" t="s">
         <v>68</v>
       </c>
-      <c r="C109" s="78">
+      <c r="C109" s="81">
         <f>MIN(C106,IF(OR(C108="Unlimited",C108=""),10^18,C108))</f>
         <v>10</v>
       </c>
-      <c r="D109" s="78"/>
-      <c r="E109" s="78"/>
-      <c r="F109" s="78">
+      <c r="D109" s="81"/>
+      <c r="E109" s="81"/>
+      <c r="F109" s="81">
         <f>MIN(F106,IF(OR(F108="Unlimited",F108=""),10^18,F108))</f>
         <v>10</v>
       </c>
-      <c r="G109" s="78"/>
-      <c r="H109" s="78"/>
+      <c r="G109" s="81"/>
+      <c r="H109" s="81"/>
       <c r="N109" s="40"/>
     </row>
     <row r="110" spans="1:15" x14ac:dyDescent="0.3">
@@ -3478,228 +3487,228 @@
       <c r="A112" s="43" t="s">
         <v>61</v>
       </c>
-      <c r="C112" s="80">
-        <v>1</v>
-      </c>
-      <c r="D112" s="80"/>
-      <c r="E112" s="78"/>
-      <c r="F112" s="80"/>
-      <c r="G112" s="80"/>
-      <c r="H112" s="78"/>
-      <c r="I112" s="80">
-        <v>1</v>
-      </c>
-      <c r="J112" s="80"/>
-      <c r="K112" s="78"/>
+      <c r="C112" s="82">
+        <v>1</v>
+      </c>
+      <c r="D112" s="82"/>
+      <c r="E112" s="81"/>
+      <c r="F112" s="82"/>
+      <c r="G112" s="82"/>
+      <c r="H112" s="81"/>
+      <c r="I112" s="82">
+        <v>1</v>
+      </c>
+      <c r="J112" s="82"/>
+      <c r="K112" s="81"/>
       <c r="N112" s="40"/>
     </row>
     <row r="113" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A113" s="43" t="s">
         <v>62</v>
       </c>
-      <c r="C113" s="80" t="s">
+      <c r="C113" s="82" t="s">
         <v>85</v>
       </c>
-      <c r="D113" s="80"/>
-      <c r="E113" s="78"/>
-      <c r="F113" s="80"/>
-      <c r="G113" s="80"/>
-      <c r="H113" s="78"/>
-      <c r="I113" s="80" t="s">
+      <c r="D113" s="82"/>
+      <c r="E113" s="81"/>
+      <c r="F113" s="82"/>
+      <c r="G113" s="82"/>
+      <c r="H113" s="81"/>
+      <c r="I113" s="82" t="s">
         <v>83</v>
       </c>
-      <c r="J113" s="80"/>
-      <c r="K113" s="78"/>
+      <c r="J113" s="82"/>
+      <c r="K113" s="81"/>
       <c r="N113" s="40"/>
     </row>
     <row r="114" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A114" s="43" t="s">
         <v>63</v>
       </c>
-      <c r="C114" s="80">
-        <v>1</v>
-      </c>
-      <c r="D114" s="80"/>
-      <c r="E114" s="78"/>
-      <c r="F114" s="80"/>
-      <c r="G114" s="80"/>
-      <c r="H114" s="78"/>
-      <c r="I114" s="80">
-        <v>1</v>
-      </c>
-      <c r="J114" s="80"/>
-      <c r="K114" s="78"/>
+      <c r="C114" s="82">
+        <v>1</v>
+      </c>
+      <c r="D114" s="82"/>
+      <c r="E114" s="81"/>
+      <c r="F114" s="82"/>
+      <c r="G114" s="82"/>
+      <c r="H114" s="81"/>
+      <c r="I114" s="82">
+        <v>1</v>
+      </c>
+      <c r="J114" s="82"/>
+      <c r="K114" s="81"/>
       <c r="N114" s="40"/>
     </row>
     <row r="115" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A115" s="43" t="s">
         <v>64</v>
       </c>
-      <c r="C115" s="78">
+      <c r="C115" s="81">
         <v>0</v>
       </c>
-      <c r="D115" s="78"/>
-      <c r="E115" s="78"/>
-      <c r="F115" s="78"/>
-      <c r="G115" s="78"/>
-      <c r="H115" s="78"/>
-      <c r="I115" s="78">
+      <c r="D115" s="81"/>
+      <c r="E115" s="81"/>
+      <c r="F115" s="81"/>
+      <c r="G115" s="81"/>
+      <c r="H115" s="81"/>
+      <c r="I115" s="81">
         <v>0</v>
       </c>
-      <c r="J115" s="78"/>
-      <c r="K115" s="78"/>
+      <c r="J115" s="81"/>
+      <c r="K115" s="81"/>
       <c r="N115" s="40"/>
     </row>
     <row r="116" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A116" s="44" t="s">
         <v>65</v>
       </c>
-      <c r="C116" s="78">
+      <c r="C116" s="81">
         <f>MAX(0, SUM(C$110:H$110)-C115)</f>
         <v>180</v>
       </c>
-      <c r="D116" s="78"/>
-      <c r="E116" s="78"/>
-      <c r="F116" s="78"/>
-      <c r="G116" s="78"/>
-      <c r="H116" s="78"/>
-      <c r="I116" s="78">
+      <c r="D116" s="81"/>
+      <c r="E116" s="81"/>
+      <c r="F116" s="81"/>
+      <c r="G116" s="81"/>
+      <c r="H116" s="81"/>
+      <c r="I116" s="81">
         <f>MAX(0, SUM(I$110:N$110)-I115)</f>
         <v>200</v>
       </c>
-      <c r="J116" s="78"/>
-      <c r="K116" s="78"/>
+      <c r="J116" s="81"/>
+      <c r="K116" s="81"/>
       <c r="N116" s="40"/>
     </row>
     <row r="117" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A117" s="43" t="s">
         <v>0</v>
       </c>
-      <c r="C117" s="78">
+      <c r="C117" s="81">
         <v>10</v>
       </c>
-      <c r="D117" s="78"/>
-      <c r="E117" s="78"/>
-      <c r="F117" s="78"/>
-      <c r="G117" s="78"/>
-      <c r="H117" s="78"/>
-      <c r="I117" s="78">
+      <c r="D117" s="81"/>
+      <c r="E117" s="81"/>
+      <c r="F117" s="81"/>
+      <c r="G117" s="81"/>
+      <c r="H117" s="81"/>
+      <c r="I117" s="81">
         <v>10</v>
       </c>
-      <c r="J117" s="78"/>
-      <c r="K117" s="78"/>
+      <c r="J117" s="81"/>
+      <c r="K117" s="81"/>
       <c r="N117" s="40"/>
     </row>
     <row r="118" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A118" s="44" t="s">
         <v>66</v>
       </c>
-      <c r="C118" s="78">
+      <c r="C118" s="81">
         <f>IF(C117="Unlimited", C116, MIN(C116, C117))</f>
         <v>10</v>
       </c>
-      <c r="D118" s="78"/>
-      <c r="E118" s="78"/>
-      <c r="F118" s="78"/>
-      <c r="G118" s="78"/>
-      <c r="H118" s="78"/>
-      <c r="I118" s="78">
+      <c r="D118" s="81"/>
+      <c r="E118" s="81"/>
+      <c r="F118" s="81"/>
+      <c r="G118" s="81"/>
+      <c r="H118" s="81"/>
+      <c r="I118" s="81">
         <f>IF(I117="Unlimited", I116, MIN(I116, I117))</f>
         <v>10</v>
       </c>
-      <c r="J118" s="78"/>
-      <c r="K118" s="78"/>
+      <c r="J118" s="81"/>
+      <c r="K118" s="81"/>
       <c r="N118" s="40"/>
     </row>
     <row r="119" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A119" s="43" t="s">
         <v>71</v>
       </c>
-      <c r="C119" s="79">
-        <v>1</v>
-      </c>
-      <c r="D119" s="79"/>
-      <c r="E119" s="79"/>
-      <c r="F119" s="79"/>
-      <c r="G119" s="79"/>
-      <c r="H119" s="79"/>
-      <c r="I119" s="79">
-        <v>1</v>
-      </c>
-      <c r="J119" s="79"/>
-      <c r="K119" s="79"/>
+      <c r="C119" s="80">
+        <v>1</v>
+      </c>
+      <c r="D119" s="80"/>
+      <c r="E119" s="80"/>
+      <c r="F119" s="80"/>
+      <c r="G119" s="80"/>
+      <c r="H119" s="80"/>
+      <c r="I119" s="80">
+        <v>1</v>
+      </c>
+      <c r="J119" s="80"/>
+      <c r="K119" s="80"/>
       <c r="N119" s="40"/>
     </row>
     <row r="120" spans="1:15" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A120" s="44" t="s">
         <v>72</v>
       </c>
-      <c r="C120" s="78">
+      <c r="C120" s="81">
         <f>C119*C118</f>
         <v>10</v>
       </c>
-      <c r="D120" s="78"/>
-      <c r="E120" s="78"/>
-      <c r="F120" s="78"/>
-      <c r="G120" s="78"/>
-      <c r="H120" s="78"/>
-      <c r="I120" s="78">
+      <c r="D120" s="81"/>
+      <c r="E120" s="81"/>
+      <c r="F120" s="81"/>
+      <c r="G120" s="81"/>
+      <c r="H120" s="81"/>
+      <c r="I120" s="81">
         <f>I119*I118</f>
         <v>10</v>
       </c>
-      <c r="J120" s="78"/>
-      <c r="K120" s="78"/>
+      <c r="J120" s="81"/>
+      <c r="K120" s="81"/>
       <c r="N120" s="40"/>
     </row>
     <row r="121" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A121" s="43" t="s">
         <v>3</v>
       </c>
-      <c r="C121" s="91"/>
-      <c r="D121" s="91"/>
-      <c r="E121" s="91"/>
-      <c r="F121" s="91"/>
-      <c r="G121" s="91"/>
-      <c r="H121" s="91"/>
-      <c r="I121" s="91"/>
-      <c r="J121" s="91"/>
-      <c r="K121" s="91"/>
+      <c r="C121" s="85"/>
+      <c r="D121" s="85"/>
+      <c r="E121" s="85"/>
+      <c r="F121" s="85"/>
+      <c r="G121" s="85"/>
+      <c r="H121" s="85"/>
+      <c r="I121" s="85"/>
+      <c r="J121" s="85"/>
+      <c r="K121" s="85"/>
       <c r="N121" s="40"/>
     </row>
     <row r="122" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A122" s="43" t="s">
         <v>67</v>
       </c>
-      <c r="C122" s="91"/>
-      <c r="D122" s="91"/>
-      <c r="E122" s="91"/>
-      <c r="F122" s="91"/>
-      <c r="G122" s="91"/>
-      <c r="H122" s="91"/>
-      <c r="I122" s="91"/>
-      <c r="J122" s="91"/>
-      <c r="K122" s="91"/>
+      <c r="C122" s="85"/>
+      <c r="D122" s="85"/>
+      <c r="E122" s="85"/>
+      <c r="F122" s="85"/>
+      <c r="G122" s="85"/>
+      <c r="H122" s="85"/>
+      <c r="I122" s="85"/>
+      <c r="J122" s="85"/>
+      <c r="K122" s="85"/>
       <c r="N122" s="40"/>
     </row>
     <row r="123" spans="1:15" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A123" s="45" t="s">
         <v>68</v>
       </c>
-      <c r="C123" s="78">
+      <c r="C123" s="81">
         <f>MIN(C120,IF(OR(C122="Unlimited",C122=""),10^18,C122))</f>
         <v>10</v>
       </c>
-      <c r="D123" s="78"/>
-      <c r="E123" s="78"/>
-      <c r="F123" s="78"/>
-      <c r="G123" s="78"/>
-      <c r="H123" s="78"/>
-      <c r="I123" s="78">
+      <c r="D123" s="81"/>
+      <c r="E123" s="81"/>
+      <c r="F123" s="81"/>
+      <c r="G123" s="81"/>
+      <c r="H123" s="81"/>
+      <c r="I123" s="81">
         <f>MIN(I120,IF(OR(I122="Unlimited",I122=""),10^18,I122))</f>
         <v>10</v>
       </c>
-      <c r="J123" s="78"/>
-      <c r="K123" s="78"/>
+      <c r="J123" s="81"/>
+      <c r="K123" s="81"/>
       <c r="N123" s="40"/>
     </row>
     <row r="124" spans="1:15" x14ac:dyDescent="0.3">
@@ -4840,134 +4849,134 @@
       <c r="A192" s="43" t="s">
         <v>61</v>
       </c>
-      <c r="C192" s="80">
-        <v>1</v>
-      </c>
-      <c r="D192" s="80"/>
-      <c r="E192" s="78"/>
-      <c r="F192" s="80">
-        <v>1</v>
-      </c>
-      <c r="G192" s="80"/>
-      <c r="H192" s="78"/>
-      <c r="I192" s="80">
-        <v>1</v>
-      </c>
-      <c r="J192" s="80"/>
-      <c r="K192" s="78"/>
-      <c r="L192" s="80">
-        <v>1</v>
-      </c>
-      <c r="M192" s="80"/>
-      <c r="N192" s="78"/>
+      <c r="C192" s="82">
+        <v>1</v>
+      </c>
+      <c r="D192" s="82"/>
+      <c r="E192" s="81"/>
+      <c r="F192" s="82">
+        <v>1</v>
+      </c>
+      <c r="G192" s="82"/>
+      <c r="H192" s="81"/>
+      <c r="I192" s="82">
+        <v>1</v>
+      </c>
+      <c r="J192" s="82"/>
+      <c r="K192" s="81"/>
+      <c r="L192" s="82">
+        <v>1</v>
+      </c>
+      <c r="M192" s="82"/>
+      <c r="N192" s="81"/>
       <c r="O192" s="73"/>
     </row>
     <row r="193" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A193" s="43" t="s">
         <v>62</v>
       </c>
-      <c r="C193" s="80" t="s">
+      <c r="C193" s="82" t="s">
         <v>141</v>
       </c>
-      <c r="D193" s="80"/>
-      <c r="E193" s="78"/>
-      <c r="F193" s="80" t="s">
+      <c r="D193" s="82"/>
+      <c r="E193" s="81"/>
+      <c r="F193" s="82" t="s">
         <v>142</v>
       </c>
-      <c r="G193" s="80"/>
-      <c r="H193" s="78"/>
-      <c r="I193" s="80" t="s">
+      <c r="G193" s="82"/>
+      <c r="H193" s="81"/>
+      <c r="I193" s="82" t="s">
         <v>143</v>
       </c>
-      <c r="J193" s="80"/>
-      <c r="K193" s="78"/>
-      <c r="L193" s="80" t="s">
+      <c r="J193" s="82"/>
+      <c r="K193" s="81"/>
+      <c r="L193" s="82" t="s">
         <v>144</v>
       </c>
-      <c r="M193" s="80"/>
-      <c r="N193" s="78"/>
+      <c r="M193" s="82"/>
+      <c r="N193" s="81"/>
       <c r="O193" s="74"/>
     </row>
     <row r="194" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A194" s="43" t="s">
         <v>63</v>
       </c>
-      <c r="C194" s="80">
-        <v>1</v>
-      </c>
-      <c r="D194" s="80"/>
-      <c r="E194" s="78"/>
-      <c r="F194" s="80">
-        <v>1</v>
-      </c>
-      <c r="G194" s="80"/>
-      <c r="H194" s="78"/>
-      <c r="I194" s="80">
-        <v>1</v>
-      </c>
-      <c r="J194" s="80"/>
-      <c r="K194" s="78"/>
-      <c r="L194" s="80">
-        <v>1</v>
-      </c>
-      <c r="M194" s="80"/>
-      <c r="N194" s="78"/>
+      <c r="C194" s="82">
+        <v>1</v>
+      </c>
+      <c r="D194" s="82"/>
+      <c r="E194" s="81"/>
+      <c r="F194" s="82">
+        <v>1</v>
+      </c>
+      <c r="G194" s="82"/>
+      <c r="H194" s="81"/>
+      <c r="I194" s="82">
+        <v>1</v>
+      </c>
+      <c r="J194" s="82"/>
+      <c r="K194" s="81"/>
+      <c r="L194" s="82">
+        <v>1</v>
+      </c>
+      <c r="M194" s="82"/>
+      <c r="N194" s="81"/>
       <c r="O194" s="73"/>
     </row>
     <row r="195" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A195" s="43" t="s">
         <v>64</v>
       </c>
-      <c r="C195" s="78">
+      <c r="C195" s="81">
         <v>0</v>
       </c>
-      <c r="D195" s="78"/>
-      <c r="E195" s="78"/>
-      <c r="F195" s="78">
+      <c r="D195" s="81"/>
+      <c r="E195" s="81"/>
+      <c r="F195" s="81">
         <v>0</v>
       </c>
-      <c r="G195" s="78"/>
-      <c r="H195" s="78"/>
-      <c r="I195" s="78">
+      <c r="G195" s="81"/>
+      <c r="H195" s="81"/>
+      <c r="I195" s="81">
         <v>0</v>
       </c>
-      <c r="J195" s="78"/>
-      <c r="K195" s="78"/>
-      <c r="L195" s="78">
+      <c r="J195" s="81"/>
+      <c r="K195" s="81"/>
+      <c r="L195" s="81">
         <v>0</v>
       </c>
-      <c r="M195" s="78"/>
-      <c r="N195" s="78"/>
+      <c r="M195" s="81"/>
+      <c r="N195" s="81"/>
       <c r="O195" s="73"/>
     </row>
     <row r="196" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A196" s="44" t="s">
         <v>65</v>
       </c>
-      <c r="C196" s="78">
+      <c r="C196" s="81">
         <f>MAX(0, SUM(C$50:E$50)*C199-C195)</f>
         <v>50</v>
       </c>
-      <c r="D196" s="78"/>
-      <c r="E196" s="78"/>
-      <c r="F196" s="78">
+      <c r="D196" s="81"/>
+      <c r="E196" s="81"/>
+      <c r="F196" s="81">
         <f>MAX(0, SUM(F$50:H$50)-F195)</f>
         <v>100</v>
       </c>
-      <c r="G196" s="78"/>
-      <c r="H196" s="78"/>
-      <c r="I196" s="78">
+      <c r="G196" s="81"/>
+      <c r="H196" s="81"/>
+      <c r="I196" s="81">
         <f>MAX(0, SUM(I$50:K$50)-I195)</f>
         <v>100</v>
       </c>
-      <c r="J196" s="78"/>
-      <c r="K196" s="78"/>
-      <c r="L196" s="78">
+      <c r="J196" s="81"/>
+      <c r="K196" s="81"/>
+      <c r="L196" s="81">
         <f>MAX(0, SUM(L$50:N$50)-L195)</f>
         <v>100</v>
       </c>
-      <c r="M196" s="78"/>
-      <c r="N196" s="78"/>
+      <c r="M196" s="81"/>
+      <c r="N196" s="81"/>
       <c r="O196" s="73"/>
       <c r="P196" s="6"/>
       <c r="Q196" s="6"/>
@@ -4976,26 +4985,26 @@
       <c r="A197" s="43" t="s">
         <v>0</v>
       </c>
-      <c r="C197" s="78">
+      <c r="C197" s="81">
         <v>10</v>
       </c>
-      <c r="D197" s="78"/>
-      <c r="E197" s="78"/>
-      <c r="F197" s="78">
+      <c r="D197" s="81"/>
+      <c r="E197" s="81"/>
+      <c r="F197" s="81">
         <v>10</v>
       </c>
-      <c r="G197" s="78"/>
-      <c r="H197" s="78"/>
-      <c r="I197" s="78">
+      <c r="G197" s="81"/>
+      <c r="H197" s="81"/>
+      <c r="I197" s="81">
         <v>10</v>
       </c>
-      <c r="J197" s="78"/>
-      <c r="K197" s="78"/>
-      <c r="L197" s="78">
+      <c r="J197" s="81"/>
+      <c r="K197" s="81"/>
+      <c r="L197" s="81">
         <v>10</v>
       </c>
-      <c r="M197" s="78"/>
-      <c r="N197" s="78"/>
+      <c r="M197" s="81"/>
+      <c r="N197" s="81"/>
       <c r="O197" s="73"/>
       <c r="Q197" s="6"/>
     </row>
@@ -5003,30 +5012,30 @@
       <c r="A198" s="44" t="s">
         <v>66</v>
       </c>
-      <c r="C198" s="78">
+      <c r="C198" s="81">
         <f>IF(C197="Unlimited", C196, MIN(C196, C197))</f>
         <v>10</v>
       </c>
-      <c r="D198" s="78"/>
-      <c r="E198" s="78"/>
-      <c r="F198" s="78">
+      <c r="D198" s="81"/>
+      <c r="E198" s="81"/>
+      <c r="F198" s="81">
         <f>IF(F197="Unlimited", F196, MIN(F196, F197))</f>
         <v>10</v>
       </c>
-      <c r="G198" s="78"/>
-      <c r="H198" s="78"/>
-      <c r="I198" s="78">
+      <c r="G198" s="81"/>
+      <c r="H198" s="81"/>
+      <c r="I198" s="81">
         <f>IF(I197="Unlimited", I196, MIN(I196, I197))</f>
         <v>10</v>
       </c>
-      <c r="J198" s="78"/>
-      <c r="K198" s="78"/>
-      <c r="L198" s="78">
+      <c r="J198" s="81"/>
+      <c r="K198" s="81"/>
+      <c r="L198" s="81">
         <f>IF(L197="Unlimited", L196, MIN(L196, L197))</f>
         <v>10</v>
       </c>
-      <c r="M198" s="78"/>
-      <c r="N198" s="78"/>
+      <c r="M198" s="81"/>
+      <c r="N198" s="81"/>
       <c r="O198" s="73"/>
       <c r="P198" s="6"/>
       <c r="Q198" s="6"/>
@@ -5035,26 +5044,26 @@
       <c r="A199" s="43" t="s">
         <v>71</v>
       </c>
-      <c r="C199" s="79">
+      <c r="C199" s="80">
         <v>0.5</v>
       </c>
-      <c r="D199" s="79"/>
-      <c r="E199" s="79"/>
-      <c r="F199" s="79">
+      <c r="D199" s="80"/>
+      <c r="E199" s="80"/>
+      <c r="F199" s="80">
         <v>0.5</v>
       </c>
-      <c r="G199" s="79"/>
-      <c r="H199" s="79"/>
-      <c r="I199" s="79">
+      <c r="G199" s="80"/>
+      <c r="H199" s="80"/>
+      <c r="I199" s="80">
         <v>0.5</v>
       </c>
-      <c r="J199" s="79"/>
-      <c r="K199" s="79"/>
-      <c r="L199" s="79">
+      <c r="J199" s="80"/>
+      <c r="K199" s="80"/>
+      <c r="L199" s="80">
         <v>0.5</v>
       </c>
-      <c r="M199" s="79"/>
-      <c r="N199" s="79"/>
+      <c r="M199" s="80"/>
+      <c r="N199" s="80"/>
       <c r="O199" s="75"/>
       <c r="Q199" s="6"/>
     </row>
@@ -5062,30 +5071,30 @@
       <c r="A200" s="44" t="s">
         <v>72</v>
       </c>
-      <c r="C200" s="78">
+      <c r="C200" s="81">
         <f>C198</f>
         <v>10</v>
       </c>
-      <c r="D200" s="78"/>
-      <c r="E200" s="78"/>
-      <c r="F200" s="78">
+      <c r="D200" s="81"/>
+      <c r="E200" s="81"/>
+      <c r="F200" s="81">
         <f t="shared" ref="F200" si="28">F198</f>
         <v>10</v>
       </c>
-      <c r="G200" s="78"/>
-      <c r="H200" s="78"/>
-      <c r="I200" s="78">
+      <c r="G200" s="81"/>
+      <c r="H200" s="81"/>
+      <c r="I200" s="81">
         <f t="shared" ref="I200" si="29">I198</f>
         <v>10</v>
       </c>
-      <c r="J200" s="78"/>
-      <c r="K200" s="78"/>
-      <c r="L200" s="78">
+      <c r="J200" s="81"/>
+      <c r="K200" s="81"/>
+      <c r="L200" s="81">
         <f t="shared" ref="L200" si="30">L198</f>
         <v>10</v>
       </c>
-      <c r="M200" s="78"/>
-      <c r="N200" s="81"/>
+      <c r="M200" s="81"/>
+      <c r="N200" s="83"/>
       <c r="O200" s="73"/>
     </row>
     <row r="201" spans="1:17" x14ac:dyDescent="0.3">
@@ -5244,112 +5253,112 @@
       <c r="A208" s="43" t="s">
         <v>61</v>
       </c>
-      <c r="C208" s="80">
-        <v>1</v>
-      </c>
-      <c r="D208" s="80"/>
-      <c r="E208" s="80"/>
-      <c r="F208" s="80"/>
-      <c r="G208" s="80"/>
-      <c r="H208" s="80"/>
-      <c r="I208" s="80">
-        <v>1</v>
-      </c>
-      <c r="J208" s="80"/>
-      <c r="K208" s="80"/>
-      <c r="L208" s="80"/>
-      <c r="M208" s="80"/>
-      <c r="N208" s="81"/>
+      <c r="C208" s="82">
+        <v>1</v>
+      </c>
+      <c r="D208" s="82"/>
+      <c r="E208" s="82"/>
+      <c r="F208" s="82"/>
+      <c r="G208" s="82"/>
+      <c r="H208" s="82"/>
+      <c r="I208" s="82">
+        <v>1</v>
+      </c>
+      <c r="J208" s="82"/>
+      <c r="K208" s="82"/>
+      <c r="L208" s="82"/>
+      <c r="M208" s="82"/>
+      <c r="N208" s="83"/>
       <c r="O208" s="73"/>
     </row>
     <row r="209" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A209" s="43" t="s">
         <v>62</v>
       </c>
-      <c r="C209" s="80" t="s">
+      <c r="C209" s="82" t="s">
         <v>140</v>
       </c>
-      <c r="D209" s="80"/>
-      <c r="E209" s="80"/>
-      <c r="F209" s="80"/>
-      <c r="G209" s="80"/>
-      <c r="H209" s="80"/>
-      <c r="I209" s="80" t="s">
+      <c r="D209" s="82"/>
+      <c r="E209" s="82"/>
+      <c r="F209" s="82"/>
+      <c r="G209" s="82"/>
+      <c r="H209" s="82"/>
+      <c r="I209" s="82" t="s">
         <v>145</v>
       </c>
-      <c r="J209" s="80"/>
-      <c r="K209" s="80"/>
-      <c r="L209" s="80"/>
-      <c r="M209" s="80"/>
-      <c r="N209" s="81"/>
+      <c r="J209" s="82"/>
+      <c r="K209" s="82"/>
+      <c r="L209" s="82"/>
+      <c r="M209" s="82"/>
+      <c r="N209" s="83"/>
       <c r="O209" s="74"/>
     </row>
     <row r="210" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A210" s="43" t="s">
         <v>63</v>
       </c>
-      <c r="C210" s="80">
-        <v>1</v>
-      </c>
-      <c r="D210" s="80"/>
-      <c r="E210" s="80"/>
-      <c r="F210" s="80"/>
-      <c r="G210" s="80"/>
-      <c r="H210" s="80"/>
-      <c r="I210" s="80">
-        <v>1</v>
-      </c>
-      <c r="J210" s="80"/>
-      <c r="K210" s="80"/>
-      <c r="L210" s="80"/>
-      <c r="M210" s="80"/>
-      <c r="N210" s="80"/>
+      <c r="C210" s="82">
+        <v>1</v>
+      </c>
+      <c r="D210" s="82"/>
+      <c r="E210" s="82"/>
+      <c r="F210" s="82"/>
+      <c r="G210" s="82"/>
+      <c r="H210" s="82"/>
+      <c r="I210" s="82">
+        <v>1</v>
+      </c>
+      <c r="J210" s="82"/>
+      <c r="K210" s="82"/>
+      <c r="L210" s="82"/>
+      <c r="M210" s="82"/>
+      <c r="N210" s="82"/>
       <c r="O210" s="73"/>
     </row>
     <row r="211" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A211" s="43" t="s">
         <v>64</v>
       </c>
-      <c r="C211" s="78">
+      <c r="C211" s="81">
         <v>0</v>
       </c>
-      <c r="D211" s="78"/>
-      <c r="E211" s="78"/>
-      <c r="F211" s="78"/>
-      <c r="G211" s="78"/>
-      <c r="H211" s="78"/>
-      <c r="I211" s="78">
+      <c r="D211" s="81"/>
+      <c r="E211" s="81"/>
+      <c r="F211" s="81"/>
+      <c r="G211" s="81"/>
+      <c r="H211" s="81"/>
+      <c r="I211" s="81">
         <v>0</v>
       </c>
-      <c r="J211" s="78"/>
-      <c r="K211" s="78"/>
-      <c r="L211" s="78"/>
-      <c r="M211" s="78"/>
-      <c r="N211" s="78"/>
+      <c r="J211" s="81"/>
+      <c r="K211" s="81"/>
+      <c r="L211" s="81"/>
+      <c r="M211" s="81"/>
+      <c r="N211" s="81"/>
       <c r="O211" s="73"/>
     </row>
     <row r="212" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A212" s="44" t="s">
         <v>65</v>
       </c>
-      <c r="C212" s="78">
+      <c r="C212" s="81">
         <f>MAX(0, SUM(C$50:H$50)*C215-C211)</f>
         <v>100</v>
       </c>
-      <c r="D212" s="78"/>
-      <c r="E212" s="78"/>
-      <c r="F212" s="78"/>
-      <c r="G212" s="78"/>
-      <c r="H212" s="78"/>
-      <c r="I212" s="78">
+      <c r="D212" s="81"/>
+      <c r="E212" s="81"/>
+      <c r="F212" s="81"/>
+      <c r="G212" s="81"/>
+      <c r="H212" s="81"/>
+      <c r="I212" s="81">
         <f>MAX(0, SUM(I$50:K$50)*I215-I211)</f>
         <v>50</v>
       </c>
-      <c r="J212" s="78"/>
-      <c r="K212" s="78"/>
-      <c r="L212" s="78"/>
-      <c r="M212" s="78"/>
-      <c r="N212" s="78"/>
+      <c r="J212" s="81"/>
+      <c r="K212" s="81"/>
+      <c r="L212" s="81"/>
+      <c r="M212" s="81"/>
+      <c r="N212" s="81"/>
       <c r="O212" s="73"/>
       <c r="P212" s="6"/>
       <c r="Q212" s="6"/>
@@ -5358,22 +5367,22 @@
       <c r="A213" s="43" t="s">
         <v>0</v>
       </c>
-      <c r="C213" s="78">
+      <c r="C213" s="81">
         <v>10</v>
       </c>
-      <c r="D213" s="78"/>
-      <c r="E213" s="78"/>
-      <c r="F213" s="78"/>
-      <c r="G213" s="78"/>
-      <c r="H213" s="78"/>
-      <c r="I213" s="78">
+      <c r="D213" s="81"/>
+      <c r="E213" s="81"/>
+      <c r="F213" s="81"/>
+      <c r="G213" s="81"/>
+      <c r="H213" s="81"/>
+      <c r="I213" s="81">
         <v>10</v>
       </c>
-      <c r="J213" s="78"/>
-      <c r="K213" s="78"/>
-      <c r="L213" s="78"/>
-      <c r="M213" s="78"/>
-      <c r="N213" s="78"/>
+      <c r="J213" s="81"/>
+      <c r="K213" s="81"/>
+      <c r="L213" s="81"/>
+      <c r="M213" s="81"/>
+      <c r="N213" s="81"/>
       <c r="O213" s="73"/>
       <c r="Q213" s="6"/>
     </row>
@@ -5381,24 +5390,24 @@
       <c r="A214" s="44" t="s">
         <v>66</v>
       </c>
-      <c r="C214" s="78">
+      <c r="C214" s="81">
         <f>IF(C213="Unlimited", C212, MIN(C212, C213))</f>
         <v>10</v>
       </c>
-      <c r="D214" s="78"/>
-      <c r="E214" s="78"/>
-      <c r="F214" s="78"/>
-      <c r="G214" s="78"/>
-      <c r="H214" s="78"/>
-      <c r="I214" s="78">
+      <c r="D214" s="81"/>
+      <c r="E214" s="81"/>
+      <c r="F214" s="81"/>
+      <c r="G214" s="81"/>
+      <c r="H214" s="81"/>
+      <c r="I214" s="81">
         <f>IF(I213="Unlimited", I212, MIN(I212, I213))</f>
         <v>10</v>
       </c>
-      <c r="J214" s="78"/>
-      <c r="K214" s="78"/>
-      <c r="L214" s="78"/>
-      <c r="M214" s="78"/>
-      <c r="N214" s="78"/>
+      <c r="J214" s="81"/>
+      <c r="K214" s="81"/>
+      <c r="L214" s="81"/>
+      <c r="M214" s="81"/>
+      <c r="N214" s="81"/>
       <c r="O214" s="73"/>
       <c r="P214" s="6"/>
       <c r="Q214" s="6"/>
@@ -5407,22 +5416,22 @@
       <c r="A215" s="43" t="s">
         <v>71</v>
       </c>
-      <c r="C215" s="79">
+      <c r="C215" s="80">
         <v>0.5</v>
       </c>
-      <c r="D215" s="79"/>
-      <c r="E215" s="79"/>
-      <c r="F215" s="79"/>
-      <c r="G215" s="79"/>
-      <c r="H215" s="79"/>
-      <c r="I215" s="79">
+      <c r="D215" s="80"/>
+      <c r="E215" s="80"/>
+      <c r="F215" s="80"/>
+      <c r="G215" s="80"/>
+      <c r="H215" s="80"/>
+      <c r="I215" s="80">
         <v>0.5</v>
       </c>
-      <c r="J215" s="79"/>
-      <c r="K215" s="79"/>
-      <c r="L215" s="79"/>
-      <c r="M215" s="79"/>
-      <c r="N215" s="79"/>
+      <c r="J215" s="80"/>
+      <c r="K215" s="80"/>
+      <c r="L215" s="80"/>
+      <c r="M215" s="80"/>
+      <c r="N215" s="80"/>
       <c r="O215" s="75"/>
       <c r="Q215" s="6"/>
     </row>
@@ -5430,24 +5439,24 @@
       <c r="A216" s="44" t="s">
         <v>72</v>
       </c>
-      <c r="C216" s="78">
+      <c r="C216" s="81">
         <f>C214</f>
         <v>10</v>
       </c>
-      <c r="D216" s="78"/>
-      <c r="E216" s="78"/>
-      <c r="F216" s="78"/>
-      <c r="G216" s="78"/>
-      <c r="H216" s="78"/>
-      <c r="I216" s="78">
+      <c r="D216" s="81"/>
+      <c r="E216" s="81"/>
+      <c r="F216" s="81"/>
+      <c r="G216" s="81"/>
+      <c r="H216" s="81"/>
+      <c r="I216" s="81">
         <f>I214</f>
         <v>10</v>
       </c>
-      <c r="J216" s="78"/>
-      <c r="K216" s="78"/>
-      <c r="L216" s="78"/>
-      <c r="M216" s="78"/>
-      <c r="N216" s="78"/>
+      <c r="J216" s="81"/>
+      <c r="K216" s="81"/>
+      <c r="L216" s="81"/>
+      <c r="M216" s="81"/>
+      <c r="N216" s="81"/>
       <c r="O216" s="73"/>
     </row>
     <row r="217" spans="1:17" x14ac:dyDescent="0.3">
@@ -5606,112 +5615,112 @@
       <c r="A224" s="43" t="s">
         <v>61</v>
       </c>
-      <c r="C224" s="80">
-        <v>1</v>
-      </c>
-      <c r="D224" s="80"/>
-      <c r="E224" s="80"/>
-      <c r="F224" s="80"/>
-      <c r="G224" s="80"/>
-      <c r="H224" s="80"/>
-      <c r="I224" s="80">
-        <v>1</v>
-      </c>
-      <c r="J224" s="80"/>
-      <c r="K224" s="80"/>
-      <c r="L224" s="80"/>
-      <c r="M224" s="80"/>
-      <c r="N224" s="81"/>
+      <c r="C224" s="82">
+        <v>1</v>
+      </c>
+      <c r="D224" s="82"/>
+      <c r="E224" s="82"/>
+      <c r="F224" s="82"/>
+      <c r="G224" s="82"/>
+      <c r="H224" s="82"/>
+      <c r="I224" s="82">
+        <v>1</v>
+      </c>
+      <c r="J224" s="82"/>
+      <c r="K224" s="82"/>
+      <c r="L224" s="82"/>
+      <c r="M224" s="82"/>
+      <c r="N224" s="83"/>
       <c r="O224" s="73"/>
     </row>
     <row r="225" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A225" s="43" t="s">
         <v>62</v>
       </c>
-      <c r="C225" s="80" t="s">
+      <c r="C225" s="82" t="s">
         <v>148</v>
       </c>
-      <c r="D225" s="80"/>
-      <c r="E225" s="80"/>
-      <c r="F225" s="80"/>
-      <c r="G225" s="80"/>
-      <c r="H225" s="80"/>
-      <c r="I225" s="80" t="s">
+      <c r="D225" s="82"/>
+      <c r="E225" s="82"/>
+      <c r="F225" s="82"/>
+      <c r="G225" s="82"/>
+      <c r="H225" s="82"/>
+      <c r="I225" s="82" t="s">
         <v>149</v>
       </c>
-      <c r="J225" s="80"/>
-      <c r="K225" s="80"/>
-      <c r="L225" s="80"/>
-      <c r="M225" s="80"/>
-      <c r="N225" s="81"/>
+      <c r="J225" s="82"/>
+      <c r="K225" s="82"/>
+      <c r="L225" s="82"/>
+      <c r="M225" s="82"/>
+      <c r="N225" s="83"/>
       <c r="O225" s="74"/>
     </row>
     <row r="226" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A226" s="43" t="s">
         <v>63</v>
       </c>
-      <c r="C226" s="80">
-        <v>1</v>
-      </c>
-      <c r="D226" s="80"/>
-      <c r="E226" s="80"/>
-      <c r="F226" s="80"/>
-      <c r="G226" s="80"/>
-      <c r="H226" s="80"/>
-      <c r="I226" s="80">
-        <v>1</v>
-      </c>
-      <c r="J226" s="80"/>
-      <c r="K226" s="80"/>
-      <c r="L226" s="80"/>
-      <c r="M226" s="80"/>
-      <c r="N226" s="80"/>
+      <c r="C226" s="82">
+        <v>1</v>
+      </c>
+      <c r="D226" s="82"/>
+      <c r="E226" s="82"/>
+      <c r="F226" s="82"/>
+      <c r="G226" s="82"/>
+      <c r="H226" s="82"/>
+      <c r="I226" s="82">
+        <v>1</v>
+      </c>
+      <c r="J226" s="82"/>
+      <c r="K226" s="82"/>
+      <c r="L226" s="82"/>
+      <c r="M226" s="82"/>
+      <c r="N226" s="82"/>
       <c r="O226" s="73"/>
     </row>
     <row r="227" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A227" s="43" t="s">
         <v>64</v>
       </c>
-      <c r="C227" s="78">
+      <c r="C227" s="81">
         <v>0</v>
       </c>
-      <c r="D227" s="78"/>
-      <c r="E227" s="78"/>
-      <c r="F227" s="78"/>
-      <c r="G227" s="78"/>
-      <c r="H227" s="78"/>
-      <c r="I227" s="78">
+      <c r="D227" s="81"/>
+      <c r="E227" s="81"/>
+      <c r="F227" s="81"/>
+      <c r="G227" s="81"/>
+      <c r="H227" s="81"/>
+      <c r="I227" s="81">
         <v>0</v>
       </c>
-      <c r="J227" s="78"/>
-      <c r="K227" s="78"/>
-      <c r="L227" s="78"/>
-      <c r="M227" s="78"/>
-      <c r="N227" s="78"/>
+      <c r="J227" s="81"/>
+      <c r="K227" s="81"/>
+      <c r="L227" s="81"/>
+      <c r="M227" s="81"/>
+      <c r="N227" s="81"/>
       <c r="O227" s="73"/>
     </row>
     <row r="228" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A228" s="44" t="s">
         <v>65</v>
       </c>
-      <c r="C228" s="78">
+      <c r="C228" s="81">
         <f>MAX(0, SUM(C$50:H$50)*C231-C227)</f>
         <v>100</v>
       </c>
-      <c r="D228" s="78"/>
-      <c r="E228" s="78"/>
-      <c r="F228" s="78"/>
-      <c r="G228" s="78"/>
-      <c r="H228" s="78"/>
-      <c r="I228" s="78">
+      <c r="D228" s="81"/>
+      <c r="E228" s="81"/>
+      <c r="F228" s="81"/>
+      <c r="G228" s="81"/>
+      <c r="H228" s="81"/>
+      <c r="I228" s="81">
         <f>MAX(0, SUM(I$50:K$50)*I231-I227)</f>
         <v>50</v>
       </c>
-      <c r="J228" s="78"/>
-      <c r="K228" s="78"/>
-      <c r="L228" s="78"/>
-      <c r="M228" s="78"/>
-      <c r="N228" s="78"/>
+      <c r="J228" s="81"/>
+      <c r="K228" s="81"/>
+      <c r="L228" s="81"/>
+      <c r="M228" s="81"/>
+      <c r="N228" s="81"/>
       <c r="O228" s="73"/>
       <c r="P228" s="6"/>
       <c r="Q228" s="6"/>
@@ -5720,22 +5729,22 @@
       <c r="A229" s="43" t="s">
         <v>0</v>
       </c>
-      <c r="C229" s="78">
+      <c r="C229" s="81">
         <v>10</v>
       </c>
-      <c r="D229" s="78"/>
-      <c r="E229" s="78"/>
-      <c r="F229" s="78"/>
-      <c r="G229" s="78"/>
-      <c r="H229" s="78"/>
-      <c r="I229" s="78">
+      <c r="D229" s="81"/>
+      <c r="E229" s="81"/>
+      <c r="F229" s="81"/>
+      <c r="G229" s="81"/>
+      <c r="H229" s="81"/>
+      <c r="I229" s="81">
         <v>10</v>
       </c>
-      <c r="J229" s="78"/>
-      <c r="K229" s="78"/>
-      <c r="L229" s="78"/>
-      <c r="M229" s="78"/>
-      <c r="N229" s="78"/>
+      <c r="J229" s="81"/>
+      <c r="K229" s="81"/>
+      <c r="L229" s="81"/>
+      <c r="M229" s="81"/>
+      <c r="N229" s="81"/>
       <c r="O229" s="73"/>
       <c r="Q229" s="6"/>
     </row>
@@ -5743,24 +5752,24 @@
       <c r="A230" s="44" t="s">
         <v>66</v>
       </c>
-      <c r="C230" s="78">
+      <c r="C230" s="81">
         <f>IF(C229="Unlimited", C228, MIN(C228, C229))</f>
         <v>10</v>
       </c>
-      <c r="D230" s="78"/>
-      <c r="E230" s="78"/>
-      <c r="F230" s="78"/>
-      <c r="G230" s="78"/>
-      <c r="H230" s="78"/>
-      <c r="I230" s="78">
+      <c r="D230" s="81"/>
+      <c r="E230" s="81"/>
+      <c r="F230" s="81"/>
+      <c r="G230" s="81"/>
+      <c r="H230" s="81"/>
+      <c r="I230" s="81">
         <f>IF(I229="Unlimited", I228, MIN(I228, I229))</f>
         <v>10</v>
       </c>
-      <c r="J230" s="78"/>
-      <c r="K230" s="78"/>
-      <c r="L230" s="78"/>
-      <c r="M230" s="78"/>
-      <c r="N230" s="78"/>
+      <c r="J230" s="81"/>
+      <c r="K230" s="81"/>
+      <c r="L230" s="81"/>
+      <c r="M230" s="81"/>
+      <c r="N230" s="81"/>
       <c r="O230" s="73"/>
       <c r="P230" s="6"/>
       <c r="Q230" s="6"/>
@@ -5769,22 +5778,22 @@
       <c r="A231" s="43" t="s">
         <v>71</v>
       </c>
-      <c r="C231" s="79">
+      <c r="C231" s="80">
         <v>0.5</v>
       </c>
-      <c r="D231" s="79"/>
-      <c r="E231" s="79"/>
-      <c r="F231" s="79"/>
-      <c r="G231" s="79"/>
-      <c r="H231" s="79"/>
-      <c r="I231" s="79">
+      <c r="D231" s="80"/>
+      <c r="E231" s="80"/>
+      <c r="F231" s="80"/>
+      <c r="G231" s="80"/>
+      <c r="H231" s="80"/>
+      <c r="I231" s="80">
         <v>0.5</v>
       </c>
-      <c r="J231" s="79"/>
-      <c r="K231" s="79"/>
-      <c r="L231" s="79"/>
-      <c r="M231" s="79"/>
-      <c r="N231" s="79"/>
+      <c r="J231" s="80"/>
+      <c r="K231" s="80"/>
+      <c r="L231" s="80"/>
+      <c r="M231" s="80"/>
+      <c r="N231" s="80"/>
       <c r="O231" s="75"/>
       <c r="Q231" s="6"/>
     </row>
@@ -5792,24 +5801,24 @@
       <c r="A232" s="44" t="s">
         <v>72</v>
       </c>
-      <c r="C232" s="78">
+      <c r="C232" s="81">
         <f>C230</f>
         <v>10</v>
       </c>
-      <c r="D232" s="78"/>
-      <c r="E232" s="78"/>
-      <c r="F232" s="78"/>
-      <c r="G232" s="78"/>
-      <c r="H232" s="78"/>
-      <c r="I232" s="78">
+      <c r="D232" s="81"/>
+      <c r="E232" s="81"/>
+      <c r="F232" s="81"/>
+      <c r="G232" s="81"/>
+      <c r="H232" s="81"/>
+      <c r="I232" s="81">
         <f>I230</f>
         <v>10</v>
       </c>
-      <c r="J232" s="78"/>
-      <c r="K232" s="78"/>
-      <c r="L232" s="78"/>
-      <c r="M232" s="78"/>
-      <c r="N232" s="78"/>
+      <c r="J232" s="81"/>
+      <c r="K232" s="81"/>
+      <c r="L232" s="81"/>
+      <c r="M232" s="81"/>
+      <c r="N232" s="81"/>
       <c r="O232" s="73"/>
     </row>
     <row r="233" spans="1:17" x14ac:dyDescent="0.3">
@@ -5957,7 +5966,7 @@
         <v>147</v>
       </c>
       <c r="B239" s="4"/>
-      <c r="C239" s="95" t="s">
+      <c r="C239" s="79" t="s">
         <v>154</v>
       </c>
       <c r="D239" s="77"/>
@@ -6162,7 +6171,7 @@
         <f t="shared" si="38"/>
         <v>12.5</v>
       </c>
-      <c r="O252" s="94">
+      <c r="O252" s="78">
         <f>SUM(C252:N252)</f>
         <v>200</v>
       </c>
@@ -6286,7 +6295,7 @@
         <v>147</v>
       </c>
       <c r="B256" s="4"/>
-      <c r="C256" s="95" t="s">
+      <c r="C256" s="79" t="s">
         <v>155</v>
       </c>
       <c r="D256" s="77"/>
@@ -6458,7 +6467,7 @@
         <f t="shared" si="41"/>
         <v>12.5</v>
       </c>
-      <c r="O269" s="94">
+      <c r="O269" s="78">
         <f>SUM(C269:N269)</f>
         <v>200</v>
       </c>
@@ -6537,14 +6546,14 @@
       </c>
     </row>
     <row r="272" spans="1:16" x14ac:dyDescent="0.3">
-      <c r="C272" s="95"/>
+      <c r="C272" s="79"/>
     </row>
     <row r="273" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A273" s="43" t="s">
         <v>61</v>
       </c>
       <c r="B273" s="4"/>
-      <c r="C273" s="95" t="s">
+      <c r="C273" s="79" t="s">
         <v>156</v>
       </c>
       <c r="N273" s="40"/>
@@ -6706,7 +6715,7 @@
         <f t="shared" si="43"/>
         <v>1.25</v>
       </c>
-      <c r="O285" s="94">
+      <c r="O285" s="78">
         <f>SUM(C285:N285)</f>
         <v>20</v>
       </c>
@@ -6800,134 +6809,134 @@
       <c r="A290" s="43" t="s">
         <v>61</v>
       </c>
-      <c r="C290" s="80">
-        <v>1</v>
-      </c>
-      <c r="D290" s="80"/>
-      <c r="E290" s="78"/>
-      <c r="F290" s="80">
-        <v>1</v>
-      </c>
-      <c r="G290" s="80"/>
-      <c r="H290" s="78"/>
-      <c r="I290" s="80">
-        <v>1</v>
-      </c>
-      <c r="J290" s="80"/>
-      <c r="K290" s="78"/>
-      <c r="L290" s="80">
-        <v>1</v>
-      </c>
-      <c r="M290" s="80"/>
-      <c r="N290" s="78"/>
+      <c r="C290" s="82">
+        <v>1</v>
+      </c>
+      <c r="D290" s="82"/>
+      <c r="E290" s="81"/>
+      <c r="F290" s="82">
+        <v>1</v>
+      </c>
+      <c r="G290" s="82"/>
+      <c r="H290" s="81"/>
+      <c r="I290" s="82">
+        <v>1</v>
+      </c>
+      <c r="J290" s="82"/>
+      <c r="K290" s="81"/>
+      <c r="L290" s="82">
+        <v>1</v>
+      </c>
+      <c r="M290" s="82"/>
+      <c r="N290" s="81"/>
       <c r="O290" s="73"/>
     </row>
     <row r="291" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A291" s="43" t="s">
         <v>62</v>
       </c>
-      <c r="C291" s="80" t="s">
+      <c r="C291" s="82" t="s">
         <v>141</v>
       </c>
-      <c r="D291" s="80"/>
-      <c r="E291" s="78"/>
-      <c r="F291" s="80" t="s">
+      <c r="D291" s="82"/>
+      <c r="E291" s="81"/>
+      <c r="F291" s="82" t="s">
         <v>142</v>
       </c>
-      <c r="G291" s="80"/>
-      <c r="H291" s="78"/>
-      <c r="I291" s="80" t="s">
+      <c r="G291" s="82"/>
+      <c r="H291" s="81"/>
+      <c r="I291" s="82" t="s">
         <v>143</v>
       </c>
-      <c r="J291" s="80"/>
-      <c r="K291" s="78"/>
-      <c r="L291" s="80" t="s">
+      <c r="J291" s="82"/>
+      <c r="K291" s="81"/>
+      <c r="L291" s="82" t="s">
         <v>144</v>
       </c>
-      <c r="M291" s="80"/>
-      <c r="N291" s="78"/>
+      <c r="M291" s="82"/>
+      <c r="N291" s="81"/>
       <c r="O291" s="74"/>
     </row>
     <row r="292" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A292" s="43" t="s">
         <v>63</v>
       </c>
-      <c r="C292" s="80">
-        <v>1</v>
-      </c>
-      <c r="D292" s="80"/>
-      <c r="E292" s="78"/>
-      <c r="F292" s="80">
-        <v>1</v>
-      </c>
-      <c r="G292" s="80"/>
-      <c r="H292" s="78"/>
-      <c r="I292" s="80">
-        <v>1</v>
-      </c>
-      <c r="J292" s="80"/>
-      <c r="K292" s="78"/>
-      <c r="L292" s="80">
-        <v>1</v>
-      </c>
-      <c r="M292" s="80"/>
-      <c r="N292" s="78"/>
+      <c r="C292" s="82">
+        <v>1</v>
+      </c>
+      <c r="D292" s="82"/>
+      <c r="E292" s="81"/>
+      <c r="F292" s="82">
+        <v>1</v>
+      </c>
+      <c r="G292" s="82"/>
+      <c r="H292" s="81"/>
+      <c r="I292" s="82">
+        <v>1</v>
+      </c>
+      <c r="J292" s="82"/>
+      <c r="K292" s="81"/>
+      <c r="L292" s="82">
+        <v>1</v>
+      </c>
+      <c r="M292" s="82"/>
+      <c r="N292" s="81"/>
       <c r="O292" s="73"/>
     </row>
     <row r="293" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A293" s="43" t="s">
         <v>64</v>
       </c>
-      <c r="C293" s="78">
+      <c r="C293" s="81">
         <v>0</v>
       </c>
-      <c r="D293" s="78"/>
-      <c r="E293" s="78"/>
-      <c r="F293" s="78">
+      <c r="D293" s="81"/>
+      <c r="E293" s="81"/>
+      <c r="F293" s="81">
         <v>0</v>
       </c>
-      <c r="G293" s="78"/>
-      <c r="H293" s="78"/>
-      <c r="I293" s="78">
+      <c r="G293" s="81"/>
+      <c r="H293" s="81"/>
+      <c r="I293" s="81">
         <v>0</v>
       </c>
-      <c r="J293" s="78"/>
-      <c r="K293" s="78"/>
-      <c r="L293" s="78">
+      <c r="J293" s="81"/>
+      <c r="K293" s="81"/>
+      <c r="L293" s="81">
         <v>0</v>
       </c>
-      <c r="M293" s="78"/>
-      <c r="N293" s="78"/>
+      <c r="M293" s="81"/>
+      <c r="N293" s="81"/>
       <c r="O293" s="73"/>
     </row>
     <row r="294" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A294" s="44" t="s">
         <v>65</v>
       </c>
-      <c r="C294" s="78">
+      <c r="C294" s="81">
         <f>MAX(0, SUM(C$50:E$50))</f>
         <v>100</v>
       </c>
-      <c r="D294" s="78"/>
-      <c r="E294" s="78"/>
-      <c r="F294" s="78">
+      <c r="D294" s="81"/>
+      <c r="E294" s="81"/>
+      <c r="F294" s="81">
         <f>MAX(0, SUM(F$50:H$50))</f>
         <v>100</v>
       </c>
-      <c r="G294" s="78"/>
-      <c r="H294" s="78"/>
-      <c r="I294" s="78">
+      <c r="G294" s="81"/>
+      <c r="H294" s="81"/>
+      <c r="I294" s="81">
         <f>MAX(0, SUM(I$50:K$50))</f>
         <v>100</v>
       </c>
-      <c r="J294" s="78"/>
-      <c r="K294" s="78"/>
-      <c r="L294" s="78">
+      <c r="J294" s="81"/>
+      <c r="K294" s="81"/>
+      <c r="L294" s="81">
         <f>MAX(0, SUM(L$50:N$50))</f>
         <v>100</v>
       </c>
-      <c r="M294" s="78"/>
-      <c r="N294" s="78"/>
+      <c r="M294" s="81"/>
+      <c r="N294" s="81"/>
       <c r="O294" s="73"/>
       <c r="P294" s="6"/>
       <c r="Q294" s="6"/>
@@ -6936,26 +6945,26 @@
       <c r="A295" s="43" t="s">
         <v>0</v>
       </c>
-      <c r="C295" s="78">
+      <c r="C295" s="81">
         <v>0</v>
       </c>
-      <c r="D295" s="78"/>
-      <c r="E295" s="78"/>
-      <c r="F295" s="78">
+      <c r="D295" s="81"/>
+      <c r="E295" s="81"/>
+      <c r="F295" s="81">
         <v>0</v>
       </c>
-      <c r="G295" s="78"/>
-      <c r="H295" s="78"/>
-      <c r="I295" s="78">
+      <c r="G295" s="81"/>
+      <c r="H295" s="81"/>
+      <c r="I295" s="81">
         <v>0</v>
       </c>
-      <c r="J295" s="78"/>
-      <c r="K295" s="78"/>
-      <c r="L295" s="78">
+      <c r="J295" s="81"/>
+      <c r="K295" s="81"/>
+      <c r="L295" s="81">
         <v>0</v>
       </c>
-      <c r="M295" s="78"/>
-      <c r="N295" s="78"/>
+      <c r="M295" s="81"/>
+      <c r="N295" s="81"/>
       <c r="O295" s="73"/>
       <c r="Q295" s="6"/>
     </row>
@@ -6963,30 +6972,30 @@
       <c r="A296" s="44" t="s">
         <v>66</v>
       </c>
-      <c r="C296" s="78">
+      <c r="C296" s="81">
         <f>C294</f>
         <v>100</v>
       </c>
-      <c r="D296" s="78"/>
-      <c r="E296" s="78"/>
-      <c r="F296" s="78">
+      <c r="D296" s="81"/>
+      <c r="E296" s="81"/>
+      <c r="F296" s="81">
         <f>F294</f>
         <v>100</v>
       </c>
-      <c r="G296" s="78"/>
-      <c r="H296" s="78"/>
-      <c r="I296" s="78">
+      <c r="G296" s="81"/>
+      <c r="H296" s="81"/>
+      <c r="I296" s="81">
         <f>I294</f>
         <v>100</v>
       </c>
-      <c r="J296" s="78"/>
-      <c r="K296" s="78"/>
-      <c r="L296" s="78">
+      <c r="J296" s="81"/>
+      <c r="K296" s="81"/>
+      <c r="L296" s="81">
         <f>L294</f>
         <v>100</v>
       </c>
-      <c r="M296" s="78"/>
-      <c r="N296" s="78"/>
+      <c r="M296" s="81"/>
+      <c r="N296" s="81"/>
       <c r="O296" s="73"/>
       <c r="P296" s="6"/>
       <c r="Q296" s="6"/>
@@ -6995,26 +7004,26 @@
       <c r="A297" s="43" t="s">
         <v>71</v>
       </c>
-      <c r="C297" s="79">
+      <c r="C297" s="80">
         <v>0.1</v>
       </c>
-      <c r="D297" s="79"/>
-      <c r="E297" s="79"/>
-      <c r="F297" s="79">
+      <c r="D297" s="80"/>
+      <c r="E297" s="80"/>
+      <c r="F297" s="80">
         <v>0.1</v>
       </c>
-      <c r="G297" s="79"/>
-      <c r="H297" s="79"/>
-      <c r="I297" s="79">
+      <c r="G297" s="80"/>
+      <c r="H297" s="80"/>
+      <c r="I297" s="80">
         <v>0.1</v>
       </c>
-      <c r="J297" s="79"/>
-      <c r="K297" s="79"/>
-      <c r="L297" s="79">
+      <c r="J297" s="80"/>
+      <c r="K297" s="80"/>
+      <c r="L297" s="80">
         <v>0.1</v>
       </c>
-      <c r="M297" s="79"/>
-      <c r="N297" s="93"/>
+      <c r="M297" s="80"/>
+      <c r="N297" s="84"/>
       <c r="O297" s="75"/>
       <c r="Q297" s="6"/>
     </row>
@@ -7022,30 +7031,30 @@
       <c r="A298" s="44" t="s">
         <v>72</v>
       </c>
-      <c r="C298" s="78">
+      <c r="C298" s="81">
         <f>C297*C296</f>
         <v>10</v>
       </c>
-      <c r="D298" s="78"/>
-      <c r="E298" s="78"/>
-      <c r="F298" s="78">
+      <c r="D298" s="81"/>
+      <c r="E298" s="81"/>
+      <c r="F298" s="81">
         <f t="shared" ref="F298" si="45">F297*F296</f>
         <v>10</v>
       </c>
-      <c r="G298" s="78"/>
-      <c r="H298" s="78"/>
-      <c r="I298" s="78">
+      <c r="G298" s="81"/>
+      <c r="H298" s="81"/>
+      <c r="I298" s="81">
         <f t="shared" ref="I298" si="46">I297*I296</f>
         <v>10</v>
       </c>
-      <c r="J298" s="78"/>
-      <c r="K298" s="78"/>
-      <c r="L298" s="78">
+      <c r="J298" s="81"/>
+      <c r="K298" s="81"/>
+      <c r="L298" s="81">
         <f t="shared" ref="L298" si="47">L297*L296</f>
         <v>10</v>
       </c>
-      <c r="M298" s="78"/>
-      <c r="N298" s="81"/>
+      <c r="M298" s="81"/>
+      <c r="N298" s="83"/>
       <c r="O298" s="73"/>
     </row>
     <row r="299" spans="1:17" x14ac:dyDescent="0.3">
@@ -7204,112 +7213,112 @@
       <c r="A306" s="43" t="s">
         <v>61</v>
       </c>
-      <c r="C306" s="80">
-        <v>1</v>
-      </c>
-      <c r="D306" s="80"/>
-      <c r="E306" s="80"/>
-      <c r="F306" s="80"/>
-      <c r="G306" s="80"/>
-      <c r="H306" s="80"/>
-      <c r="I306" s="80">
-        <v>1</v>
-      </c>
-      <c r="J306" s="80"/>
-      <c r="K306" s="80"/>
-      <c r="L306" s="80"/>
-      <c r="M306" s="80"/>
-      <c r="N306" s="81"/>
+      <c r="C306" s="82">
+        <v>1</v>
+      </c>
+      <c r="D306" s="82"/>
+      <c r="E306" s="82"/>
+      <c r="F306" s="82"/>
+      <c r="G306" s="82"/>
+      <c r="H306" s="82"/>
+      <c r="I306" s="82">
+        <v>1</v>
+      </c>
+      <c r="J306" s="82"/>
+      <c r="K306" s="82"/>
+      <c r="L306" s="82"/>
+      <c r="M306" s="82"/>
+      <c r="N306" s="83"/>
       <c r="O306" s="73"/>
     </row>
     <row r="307" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A307" s="43" t="s">
         <v>62</v>
       </c>
-      <c r="C307" s="80" t="s">
+      <c r="C307" s="82" t="s">
         <v>140</v>
       </c>
-      <c r="D307" s="80"/>
-      <c r="E307" s="80"/>
-      <c r="F307" s="80"/>
-      <c r="G307" s="80"/>
-      <c r="H307" s="80"/>
-      <c r="I307" s="80" t="s">
+      <c r="D307" s="82"/>
+      <c r="E307" s="82"/>
+      <c r="F307" s="82"/>
+      <c r="G307" s="82"/>
+      <c r="H307" s="82"/>
+      <c r="I307" s="82" t="s">
         <v>145</v>
       </c>
-      <c r="J307" s="80"/>
-      <c r="K307" s="80"/>
-      <c r="L307" s="80"/>
-      <c r="M307" s="80"/>
-      <c r="N307" s="81"/>
+      <c r="J307" s="82"/>
+      <c r="K307" s="82"/>
+      <c r="L307" s="82"/>
+      <c r="M307" s="82"/>
+      <c r="N307" s="83"/>
       <c r="O307" s="74"/>
     </row>
     <row r="308" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A308" s="43" t="s">
         <v>63</v>
       </c>
-      <c r="C308" s="80">
-        <v>1</v>
-      </c>
-      <c r="D308" s="80"/>
-      <c r="E308" s="80"/>
-      <c r="F308" s="80"/>
-      <c r="G308" s="80"/>
-      <c r="H308" s="80"/>
-      <c r="I308" s="80">
-        <v>1</v>
-      </c>
-      <c r="J308" s="80"/>
-      <c r="K308" s="80"/>
-      <c r="L308" s="80"/>
-      <c r="M308" s="80"/>
-      <c r="N308" s="80"/>
+      <c r="C308" s="82">
+        <v>1</v>
+      </c>
+      <c r="D308" s="82"/>
+      <c r="E308" s="82"/>
+      <c r="F308" s="82"/>
+      <c r="G308" s="82"/>
+      <c r="H308" s="82"/>
+      <c r="I308" s="82">
+        <v>1</v>
+      </c>
+      <c r="J308" s="82"/>
+      <c r="K308" s="82"/>
+      <c r="L308" s="82"/>
+      <c r="M308" s="82"/>
+      <c r="N308" s="82"/>
       <c r="O308" s="73"/>
     </row>
     <row r="309" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A309" s="43" t="s">
         <v>64</v>
       </c>
-      <c r="C309" s="78">
+      <c r="C309" s="81">
         <v>0</v>
       </c>
-      <c r="D309" s="78"/>
-      <c r="E309" s="78"/>
-      <c r="F309" s="78"/>
-      <c r="G309" s="78"/>
-      <c r="H309" s="78"/>
-      <c r="I309" s="78">
+      <c r="D309" s="81"/>
+      <c r="E309" s="81"/>
+      <c r="F309" s="81"/>
+      <c r="G309" s="81"/>
+      <c r="H309" s="81"/>
+      <c r="I309" s="81">
         <v>0</v>
       </c>
-      <c r="J309" s="78"/>
-      <c r="K309" s="78"/>
-      <c r="L309" s="78"/>
-      <c r="M309" s="78"/>
-      <c r="N309" s="78"/>
+      <c r="J309" s="81"/>
+      <c r="K309" s="81"/>
+      <c r="L309" s="81"/>
+      <c r="M309" s="81"/>
+      <c r="N309" s="81"/>
       <c r="O309" s="73"/>
     </row>
     <row r="310" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A310" s="44" t="s">
         <v>65</v>
       </c>
-      <c r="C310" s="78">
+      <c r="C310" s="81">
         <f>MAX(0, SUM(C$50:H$50))</f>
         <v>200</v>
       </c>
-      <c r="D310" s="78"/>
-      <c r="E310" s="78"/>
-      <c r="F310" s="78"/>
-      <c r="G310" s="78"/>
-      <c r="H310" s="78"/>
-      <c r="I310" s="78">
+      <c r="D310" s="81"/>
+      <c r="E310" s="81"/>
+      <c r="F310" s="81"/>
+      <c r="G310" s="81"/>
+      <c r="H310" s="81"/>
+      <c r="I310" s="81">
         <f>MAX(0, SUM(I$50:N$50))</f>
         <v>200</v>
       </c>
-      <c r="J310" s="78"/>
-      <c r="K310" s="78"/>
-      <c r="L310" s="78"/>
-      <c r="M310" s="78"/>
-      <c r="N310" s="78"/>
+      <c r="J310" s="81"/>
+      <c r="K310" s="81"/>
+      <c r="L310" s="81"/>
+      <c r="M310" s="81"/>
+      <c r="N310" s="81"/>
       <c r="O310" s="73"/>
       <c r="P310" s="6"/>
       <c r="Q310" s="6"/>
@@ -7318,22 +7327,22 @@
       <c r="A311" s="43" t="s">
         <v>0</v>
       </c>
-      <c r="C311" s="78">
+      <c r="C311" s="81">
         <v>0</v>
       </c>
-      <c r="D311" s="78"/>
-      <c r="E311" s="78"/>
-      <c r="F311" s="78"/>
-      <c r="G311" s="78"/>
-      <c r="H311" s="78"/>
-      <c r="I311" s="78">
+      <c r="D311" s="81"/>
+      <c r="E311" s="81"/>
+      <c r="F311" s="81"/>
+      <c r="G311" s="81"/>
+      <c r="H311" s="81"/>
+      <c r="I311" s="81">
         <v>0</v>
       </c>
-      <c r="J311" s="78"/>
-      <c r="K311" s="78"/>
-      <c r="L311" s="78"/>
-      <c r="M311" s="78"/>
-      <c r="N311" s="78"/>
+      <c r="J311" s="81"/>
+      <c r="K311" s="81"/>
+      <c r="L311" s="81"/>
+      <c r="M311" s="81"/>
+      <c r="N311" s="81"/>
       <c r="O311" s="73"/>
       <c r="Q311" s="6"/>
     </row>
@@ -7341,24 +7350,24 @@
       <c r="A312" s="44" t="s">
         <v>66</v>
       </c>
-      <c r="C312" s="78">
+      <c r="C312" s="81">
         <f>IF(C311=0, C310, MIN(C310, C311))</f>
         <v>200</v>
       </c>
-      <c r="D312" s="78"/>
-      <c r="E312" s="78"/>
-      <c r="F312" s="78"/>
-      <c r="G312" s="78"/>
-      <c r="H312" s="78"/>
-      <c r="I312" s="78">
+      <c r="D312" s="81"/>
+      <c r="E312" s="81"/>
+      <c r="F312" s="81"/>
+      <c r="G312" s="81"/>
+      <c r="H312" s="81"/>
+      <c r="I312" s="81">
         <f>IF(I311=0, I310, MIN(I310, I311))</f>
         <v>200</v>
       </c>
-      <c r="J312" s="78"/>
-      <c r="K312" s="78"/>
-      <c r="L312" s="78"/>
-      <c r="M312" s="78"/>
-      <c r="N312" s="78"/>
+      <c r="J312" s="81"/>
+      <c r="K312" s="81"/>
+      <c r="L312" s="81"/>
+      <c r="M312" s="81"/>
+      <c r="N312" s="81"/>
       <c r="O312" s="73"/>
       <c r="P312" s="6"/>
       <c r="Q312" s="6"/>
@@ -7367,22 +7376,22 @@
       <c r="A313" s="43" t="s">
         <v>71</v>
       </c>
-      <c r="C313" s="79">
+      <c r="C313" s="80">
         <v>0.1</v>
       </c>
-      <c r="D313" s="79"/>
-      <c r="E313" s="79"/>
-      <c r="F313" s="79"/>
-      <c r="G313" s="79"/>
-      <c r="H313" s="79"/>
-      <c r="I313" s="79">
+      <c r="D313" s="80"/>
+      <c r="E313" s="80"/>
+      <c r="F313" s="80"/>
+      <c r="G313" s="80"/>
+      <c r="H313" s="80"/>
+      <c r="I313" s="80">
         <v>0.1</v>
       </c>
-      <c r="J313" s="79"/>
-      <c r="K313" s="79"/>
-      <c r="L313" s="79"/>
-      <c r="M313" s="79"/>
-      <c r="N313" s="79"/>
+      <c r="J313" s="80"/>
+      <c r="K313" s="80"/>
+      <c r="L313" s="80"/>
+      <c r="M313" s="80"/>
+      <c r="N313" s="80"/>
       <c r="O313" s="75"/>
       <c r="Q313" s="6"/>
     </row>
@@ -7390,24 +7399,24 @@
       <c r="A314" s="44" t="s">
         <v>72</v>
       </c>
-      <c r="C314" s="78">
+      <c r="C314" s="81">
         <f>C312*C313</f>
         <v>20</v>
       </c>
-      <c r="D314" s="78"/>
-      <c r="E314" s="78"/>
-      <c r="F314" s="78"/>
-      <c r="G314" s="78"/>
-      <c r="H314" s="78"/>
-      <c r="I314" s="78">
+      <c r="D314" s="81"/>
+      <c r="E314" s="81"/>
+      <c r="F314" s="81"/>
+      <c r="G314" s="81"/>
+      <c r="H314" s="81"/>
+      <c r="I314" s="81">
         <f>I312*I313</f>
         <v>20</v>
       </c>
-      <c r="J314" s="78"/>
-      <c r="K314" s="78"/>
-      <c r="L314" s="78"/>
-      <c r="M314" s="78"/>
-      <c r="N314" s="78"/>
+      <c r="J314" s="81"/>
+      <c r="K314" s="81"/>
+      <c r="L314" s="81"/>
+      <c r="M314" s="81"/>
+      <c r="N314" s="81"/>
       <c r="O314" s="73"/>
     </row>
     <row r="315" spans="1:17" x14ac:dyDescent="0.3">
@@ -7566,112 +7575,112 @@
       <c r="A322" s="43" t="s">
         <v>61</v>
       </c>
-      <c r="C322" s="80">
-        <v>1</v>
-      </c>
-      <c r="D322" s="80"/>
-      <c r="E322" s="80"/>
-      <c r="F322" s="80"/>
-      <c r="G322" s="80"/>
-      <c r="H322" s="80"/>
-      <c r="I322" s="80">
-        <v>1</v>
-      </c>
-      <c r="J322" s="80"/>
-      <c r="K322" s="80"/>
-      <c r="L322" s="80"/>
-      <c r="M322" s="80"/>
-      <c r="N322" s="81"/>
+      <c r="C322" s="82">
+        <v>1</v>
+      </c>
+      <c r="D322" s="82"/>
+      <c r="E322" s="82"/>
+      <c r="F322" s="82"/>
+      <c r="G322" s="82"/>
+      <c r="H322" s="82"/>
+      <c r="I322" s="82">
+        <v>1</v>
+      </c>
+      <c r="J322" s="82"/>
+      <c r="K322" s="82"/>
+      <c r="L322" s="82"/>
+      <c r="M322" s="82"/>
+      <c r="N322" s="83"/>
       <c r="O322" s="73"/>
     </row>
     <row r="323" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A323" s="43" t="s">
         <v>62</v>
       </c>
-      <c r="C323" s="80" t="s">
+      <c r="C323" s="82" t="s">
         <v>148</v>
       </c>
-      <c r="D323" s="80"/>
-      <c r="E323" s="80"/>
-      <c r="F323" s="80"/>
-      <c r="G323" s="80"/>
-      <c r="H323" s="80"/>
-      <c r="I323" s="80" t="s">
+      <c r="D323" s="82"/>
+      <c r="E323" s="82"/>
+      <c r="F323" s="82"/>
+      <c r="G323" s="82"/>
+      <c r="H323" s="82"/>
+      <c r="I323" s="82" t="s">
         <v>149</v>
       </c>
-      <c r="J323" s="80"/>
-      <c r="K323" s="80"/>
-      <c r="L323" s="80"/>
-      <c r="M323" s="80"/>
-      <c r="N323" s="81"/>
+      <c r="J323" s="82"/>
+      <c r="K323" s="82"/>
+      <c r="L323" s="82"/>
+      <c r="M323" s="82"/>
+      <c r="N323" s="83"/>
       <c r="O323" s="74"/>
     </row>
     <row r="324" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A324" s="43" t="s">
         <v>63</v>
       </c>
-      <c r="C324" s="80">
-        <v>1</v>
-      </c>
-      <c r="D324" s="80"/>
-      <c r="E324" s="80"/>
-      <c r="F324" s="80"/>
-      <c r="G324" s="80"/>
-      <c r="H324" s="80"/>
-      <c r="I324" s="80">
-        <v>1</v>
-      </c>
-      <c r="J324" s="80"/>
-      <c r="K324" s="80"/>
-      <c r="L324" s="80"/>
-      <c r="M324" s="80"/>
-      <c r="N324" s="80"/>
+      <c r="C324" s="82">
+        <v>1</v>
+      </c>
+      <c r="D324" s="82"/>
+      <c r="E324" s="82"/>
+      <c r="F324" s="82"/>
+      <c r="G324" s="82"/>
+      <c r="H324" s="82"/>
+      <c r="I324" s="82">
+        <v>1</v>
+      </c>
+      <c r="J324" s="82"/>
+      <c r="K324" s="82"/>
+      <c r="L324" s="82"/>
+      <c r="M324" s="82"/>
+      <c r="N324" s="82"/>
       <c r="O324" s="73"/>
     </row>
     <row r="325" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A325" s="43" t="s">
         <v>64</v>
       </c>
-      <c r="C325" s="78">
+      <c r="C325" s="81">
         <v>0</v>
       </c>
-      <c r="D325" s="78"/>
-      <c r="E325" s="78"/>
-      <c r="F325" s="78"/>
-      <c r="G325" s="78"/>
-      <c r="H325" s="78"/>
-      <c r="I325" s="78">
+      <c r="D325" s="81"/>
+      <c r="E325" s="81"/>
+      <c r="F325" s="81"/>
+      <c r="G325" s="81"/>
+      <c r="H325" s="81"/>
+      <c r="I325" s="81">
         <v>0</v>
       </c>
-      <c r="J325" s="78"/>
-      <c r="K325" s="78"/>
-      <c r="L325" s="78"/>
-      <c r="M325" s="78"/>
-      <c r="N325" s="78"/>
+      <c r="J325" s="81"/>
+      <c r="K325" s="81"/>
+      <c r="L325" s="81"/>
+      <c r="M325" s="81"/>
+      <c r="N325" s="81"/>
       <c r="O325" s="73"/>
     </row>
     <row r="326" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A326" s="44" t="s">
         <v>65</v>
       </c>
-      <c r="C326" s="78">
+      <c r="C326" s="81">
         <f>MAX(0, SUM(C$50:H$50))</f>
         <v>200</v>
       </c>
-      <c r="D326" s="78"/>
-      <c r="E326" s="78"/>
-      <c r="F326" s="78"/>
-      <c r="G326" s="78"/>
-      <c r="H326" s="78"/>
-      <c r="I326" s="78">
+      <c r="D326" s="81"/>
+      <c r="E326" s="81"/>
+      <c r="F326" s="81"/>
+      <c r="G326" s="81"/>
+      <c r="H326" s="81"/>
+      <c r="I326" s="81">
         <f>MAX(0, SUM(I$50:N$50))</f>
         <v>200</v>
       </c>
-      <c r="J326" s="78"/>
-      <c r="K326" s="78"/>
-      <c r="L326" s="78"/>
-      <c r="M326" s="78"/>
-      <c r="N326" s="78"/>
+      <c r="J326" s="81"/>
+      <c r="K326" s="81"/>
+      <c r="L326" s="81"/>
+      <c r="M326" s="81"/>
+      <c r="N326" s="81"/>
       <c r="O326" s="73"/>
       <c r="P326" s="6"/>
       <c r="Q326" s="6"/>
@@ -7680,22 +7689,22 @@
       <c r="A327" s="43" t="s">
         <v>0</v>
       </c>
-      <c r="C327" s="78">
+      <c r="C327" s="81">
         <v>0</v>
       </c>
-      <c r="D327" s="78"/>
-      <c r="E327" s="78"/>
-      <c r="F327" s="78"/>
-      <c r="G327" s="78"/>
-      <c r="H327" s="78"/>
-      <c r="I327" s="78">
+      <c r="D327" s="81"/>
+      <c r="E327" s="81"/>
+      <c r="F327" s="81"/>
+      <c r="G327" s="81"/>
+      <c r="H327" s="81"/>
+      <c r="I327" s="81">
         <v>0</v>
       </c>
-      <c r="J327" s="78"/>
-      <c r="K327" s="78"/>
-      <c r="L327" s="78"/>
-      <c r="M327" s="78"/>
-      <c r="N327" s="78"/>
+      <c r="J327" s="81"/>
+      <c r="K327" s="81"/>
+      <c r="L327" s="81"/>
+      <c r="M327" s="81"/>
+      <c r="N327" s="81"/>
       <c r="O327" s="73"/>
       <c r="Q327" s="6"/>
     </row>
@@ -7703,24 +7712,24 @@
       <c r="A328" s="44" t="s">
         <v>66</v>
       </c>
-      <c r="C328" s="78">
+      <c r="C328" s="81">
         <f>IF(C327=0, C326, MIN(C326, C327))</f>
         <v>200</v>
       </c>
-      <c r="D328" s="78"/>
-      <c r="E328" s="78"/>
-      <c r="F328" s="78"/>
-      <c r="G328" s="78"/>
-      <c r="H328" s="78"/>
-      <c r="I328" s="78">
+      <c r="D328" s="81"/>
+      <c r="E328" s="81"/>
+      <c r="F328" s="81"/>
+      <c r="G328" s="81"/>
+      <c r="H328" s="81"/>
+      <c r="I328" s="81">
         <f>IF(I327=0, I326, MIN(I326, I327))</f>
         <v>200</v>
       </c>
-      <c r="J328" s="78"/>
-      <c r="K328" s="78"/>
-      <c r="L328" s="78"/>
-      <c r="M328" s="78"/>
-      <c r="N328" s="78"/>
+      <c r="J328" s="81"/>
+      <c r="K328" s="81"/>
+      <c r="L328" s="81"/>
+      <c r="M328" s="81"/>
+      <c r="N328" s="81"/>
       <c r="O328" s="73"/>
       <c r="P328" s="6"/>
       <c r="Q328" s="6"/>
@@ -7729,22 +7738,22 @@
       <c r="A329" s="43" t="s">
         <v>71</v>
       </c>
-      <c r="C329" s="79">
+      <c r="C329" s="80">
         <v>0.1</v>
       </c>
-      <c r="D329" s="79"/>
-      <c r="E329" s="79"/>
-      <c r="F329" s="79"/>
-      <c r="G329" s="79"/>
-      <c r="H329" s="79"/>
-      <c r="I329" s="79">
+      <c r="D329" s="80"/>
+      <c r="E329" s="80"/>
+      <c r="F329" s="80"/>
+      <c r="G329" s="80"/>
+      <c r="H329" s="80"/>
+      <c r="I329" s="80">
         <v>0.1</v>
       </c>
-      <c r="J329" s="79"/>
-      <c r="K329" s="79"/>
-      <c r="L329" s="79"/>
-      <c r="M329" s="79"/>
-      <c r="N329" s="79"/>
+      <c r="J329" s="80"/>
+      <c r="K329" s="80"/>
+      <c r="L329" s="80"/>
+      <c r="M329" s="80"/>
+      <c r="N329" s="80"/>
       <c r="O329" s="75"/>
       <c r="Q329" s="6"/>
     </row>
@@ -7752,24 +7761,24 @@
       <c r="A330" s="44" t="s">
         <v>72</v>
       </c>
-      <c r="C330" s="78">
+      <c r="C330" s="81">
         <f>C328*C329</f>
         <v>20</v>
       </c>
-      <c r="D330" s="78"/>
-      <c r="E330" s="78"/>
-      <c r="F330" s="78"/>
-      <c r="G330" s="78"/>
-      <c r="H330" s="78"/>
-      <c r="I330" s="78">
+      <c r="D330" s="81"/>
+      <c r="E330" s="81"/>
+      <c r="F330" s="81"/>
+      <c r="G330" s="81"/>
+      <c r="H330" s="81"/>
+      <c r="I330" s="81">
         <f>I328*I329</f>
         <v>20</v>
       </c>
-      <c r="J330" s="78"/>
-      <c r="K330" s="78"/>
-      <c r="L330" s="78"/>
-      <c r="M330" s="78"/>
-      <c r="N330" s="78"/>
+      <c r="J330" s="81"/>
+      <c r="K330" s="81"/>
+      <c r="L330" s="81"/>
+      <c r="M330" s="81"/>
+      <c r="N330" s="81"/>
       <c r="O330" s="73"/>
     </row>
     <row r="331" spans="1:17" x14ac:dyDescent="0.3">
@@ -7912,113 +7921,544 @@
         <v>360</v>
       </c>
     </row>
+    <row r="337" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A337" s="65" t="s">
+        <v>110</v>
+      </c>
+      <c r="B337" s="4"/>
+      <c r="C337" s="79" t="s">
+        <v>162</v>
+      </c>
+      <c r="D337" s="2"/>
+      <c r="H337" s="42"/>
+      <c r="K337" s="42"/>
+      <c r="N337" s="42"/>
+    </row>
+    <row r="338" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A338" s="43" t="s">
+        <v>61</v>
+      </c>
+      <c r="C338" s="2"/>
+      <c r="D338" s="2"/>
+      <c r="E338" s="2">
+        <v>1</v>
+      </c>
+      <c r="F338" s="2">
+        <v>1</v>
+      </c>
+      <c r="G338" s="2"/>
+      <c r="H338" s="2"/>
+      <c r="I338" s="2">
+        <v>1</v>
+      </c>
+      <c r="J338" s="2">
+        <v>1</v>
+      </c>
+      <c r="K338" s="2"/>
+      <c r="L338" s="2"/>
+      <c r="M338" s="2"/>
+      <c r="N338" s="97"/>
+      <c r="O338" s="73"/>
+    </row>
+    <row r="339" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A339" s="43" t="s">
+        <v>62</v>
+      </c>
+      <c r="C339" s="2"/>
+      <c r="D339" s="2"/>
+      <c r="E339" s="2" t="s">
+        <v>148</v>
+      </c>
+      <c r="F339" s="2" t="s">
+        <v>148</v>
+      </c>
+      <c r="G339" s="2"/>
+      <c r="H339" s="2"/>
+      <c r="I339" s="2" t="s">
+        <v>149</v>
+      </c>
+      <c r="J339" s="2" t="s">
+        <v>149</v>
+      </c>
+      <c r="K339" s="2"/>
+      <c r="L339" s="2"/>
+      <c r="M339" s="2"/>
+      <c r="N339" s="97"/>
+      <c r="O339" s="74"/>
+    </row>
+    <row r="340" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A340" s="43" t="s">
+        <v>63</v>
+      </c>
+      <c r="C340" s="2"/>
+      <c r="D340" s="2"/>
+      <c r="E340" s="2">
+        <v>1</v>
+      </c>
+      <c r="F340" s="2">
+        <v>2</v>
+      </c>
+      <c r="G340" s="2"/>
+      <c r="H340" s="2"/>
+      <c r="I340" s="2">
+        <v>1</v>
+      </c>
+      <c r="J340" s="2">
+        <v>2</v>
+      </c>
+      <c r="K340" s="2"/>
+      <c r="L340" s="2"/>
+      <c r="M340" s="2"/>
+      <c r="N340" s="2"/>
+      <c r="O340" s="73"/>
+    </row>
+    <row r="341" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A341" s="43" t="s">
+        <v>64</v>
+      </c>
+      <c r="C341" s="2"/>
+      <c r="D341" s="2"/>
+      <c r="E341" s="6">
+        <v>0</v>
+      </c>
+      <c r="F341" s="6">
+        <v>0</v>
+      </c>
+      <c r="G341" s="6"/>
+      <c r="H341" s="6"/>
+      <c r="I341" s="6">
+        <v>0</v>
+      </c>
+      <c r="J341" s="6">
+        <v>0</v>
+      </c>
+      <c r="K341" s="6"/>
+      <c r="L341" s="6"/>
+      <c r="M341" s="6"/>
+      <c r="N341" s="6"/>
+      <c r="O341" s="73"/>
+    </row>
+    <row r="342" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A342" s="44" t="s">
+        <v>65</v>
+      </c>
+      <c r="C342" s="2"/>
+      <c r="D342" s="2"/>
+      <c r="E342" s="6">
+        <f>MAX(0, SUM(C$50:H$50))</f>
+        <v>200</v>
+      </c>
+      <c r="F342" s="6">
+        <f>MAX(0, SUM(D$50:I$50))</f>
+        <v>200</v>
+      </c>
+      <c r="G342" s="6"/>
+      <c r="H342" s="6"/>
+      <c r="I342" s="6">
+        <f>MAX(0, SUM(I$50:N$50))</f>
+        <v>200</v>
+      </c>
+      <c r="J342" s="6">
+        <f>MAX(0,SUM(I$50:N$50))</f>
+        <v>200</v>
+      </c>
+      <c r="K342" s="6"/>
+      <c r="L342" s="6"/>
+      <c r="M342" s="6"/>
+      <c r="N342" s="6"/>
+      <c r="O342" s="73"/>
+      <c r="P342" s="6"/>
+      <c r="Q342" s="6"/>
+    </row>
+    <row r="343" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A343" s="43" t="s">
+        <v>0</v>
+      </c>
+      <c r="C343" s="2"/>
+      <c r="D343" s="2"/>
+      <c r="E343" s="6">
+        <v>0</v>
+      </c>
+      <c r="F343" s="6">
+        <v>0</v>
+      </c>
+      <c r="G343" s="6"/>
+      <c r="H343" s="6"/>
+      <c r="I343" s="6">
+        <v>0</v>
+      </c>
+      <c r="J343" s="6">
+        <v>0</v>
+      </c>
+      <c r="K343" s="6"/>
+      <c r="L343" s="6"/>
+      <c r="M343" s="6"/>
+      <c r="N343" s="6"/>
+      <c r="O343" s="73"/>
+      <c r="Q343" s="6"/>
+    </row>
+    <row r="344" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A344" s="44" t="s">
+        <v>66</v>
+      </c>
+      <c r="C344" s="2"/>
+      <c r="D344" s="2"/>
+      <c r="E344" s="6">
+        <f>IF(E343=0, E342, MIN(E342, E343))</f>
+        <v>200</v>
+      </c>
+      <c r="F344" s="6">
+        <f>IF(F343=0, F342, MIN(F342, F343))</f>
+        <v>200</v>
+      </c>
+      <c r="G344" s="6"/>
+      <c r="H344" s="6"/>
+      <c r="I344" s="6">
+        <f>IF(I343=0, I342, MIN(I342, I343))</f>
+        <v>200</v>
+      </c>
+      <c r="J344" s="6">
+        <f>IF(J343=0, J342, MIN(J342, J343))</f>
+        <v>200</v>
+      </c>
+      <c r="K344" s="6"/>
+      <c r="L344" s="6"/>
+      <c r="M344" s="6"/>
+      <c r="N344" s="6"/>
+      <c r="O344" s="73"/>
+      <c r="P344" s="6"/>
+      <c r="Q344" s="6"/>
+    </row>
+    <row r="345" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A345" s="43" t="s">
+        <v>71</v>
+      </c>
+      <c r="C345" s="2"/>
+      <c r="D345" s="2"/>
+      <c r="E345" s="96">
+        <v>0.1</v>
+      </c>
+      <c r="F345" s="96">
+        <v>0.2</v>
+      </c>
+      <c r="G345" s="96"/>
+      <c r="H345" s="96"/>
+      <c r="I345" s="96">
+        <v>0.1</v>
+      </c>
+      <c r="J345" s="96">
+        <v>0.2</v>
+      </c>
+      <c r="K345" s="96"/>
+      <c r="L345" s="96"/>
+      <c r="M345" s="96"/>
+      <c r="N345" s="96"/>
+      <c r="O345" s="75"/>
+      <c r="Q345" s="6"/>
+    </row>
+    <row r="346" spans="1:17" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A346" s="44" t="s">
+        <v>72</v>
+      </c>
+      <c r="C346" s="2"/>
+      <c r="D346" s="2"/>
+      <c r="E346" s="6">
+        <f>E344*E345</f>
+        <v>20</v>
+      </c>
+      <c r="F346" s="6">
+        <f>F344*F345</f>
+        <v>40</v>
+      </c>
+      <c r="G346" s="6"/>
+      <c r="H346" s="6"/>
+      <c r="I346" s="6">
+        <f>I344*I345</f>
+        <v>20</v>
+      </c>
+      <c r="J346" s="6">
+        <f>J344*J345</f>
+        <v>40</v>
+      </c>
+      <c r="K346" s="6"/>
+      <c r="L346" s="6"/>
+      <c r="M346" s="6"/>
+      <c r="N346" s="6"/>
+      <c r="O346" s="73"/>
+    </row>
+    <row r="347" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A347" s="43" t="s">
+        <v>3</v>
+      </c>
+      <c r="N347" s="13"/>
+      <c r="O347" s="73"/>
+    </row>
+    <row r="348" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A348" s="43" t="s">
+        <v>67</v>
+      </c>
+      <c r="N348" s="13"/>
+      <c r="O348" s="73"/>
+    </row>
+    <row r="349" spans="1:17" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A349" s="45" t="s">
+        <v>74</v>
+      </c>
+      <c r="C349" s="82">
+        <f>SUM(E346:F346)</f>
+        <v>60</v>
+      </c>
+      <c r="D349" s="82"/>
+      <c r="E349" s="82"/>
+      <c r="F349" s="82"/>
+      <c r="G349" s="82"/>
+      <c r="H349" s="82"/>
+      <c r="I349" s="82">
+        <f>SUM(I346:J346)</f>
+        <v>60</v>
+      </c>
+      <c r="J349" s="82"/>
+      <c r="K349" s="82"/>
+      <c r="L349" s="82"/>
+      <c r="M349" s="82"/>
+      <c r="N349" s="83"/>
+      <c r="O349" s="73">
+        <f>SUM(E346:N346)</f>
+        <v>120</v>
+      </c>
+      <c r="P349" s="6"/>
+      <c r="Q349" s="6"/>
+    </row>
+    <row r="350" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A350" s="44" t="s">
+        <v>136</v>
+      </c>
+      <c r="C350" s="52">
+        <f>$C$349*C$50/SUM($C$50:$H$50)</f>
+        <v>15</v>
+      </c>
+      <c r="D350" s="52">
+        <f t="shared" ref="D350:H350" si="55">$C$349*D$50/SUM($C$50:$H$50)</f>
+        <v>7.5</v>
+      </c>
+      <c r="E350" s="52">
+        <f t="shared" si="55"/>
+        <v>7.5</v>
+      </c>
+      <c r="F350" s="52">
+        <f t="shared" si="55"/>
+        <v>15</v>
+      </c>
+      <c r="G350" s="52">
+        <f t="shared" si="55"/>
+        <v>7.5</v>
+      </c>
+      <c r="H350" s="52">
+        <f t="shared" si="55"/>
+        <v>7.5</v>
+      </c>
+      <c r="I350" s="52">
+        <f>$I$349*I$50/SUM($I$50:$N$50)</f>
+        <v>15</v>
+      </c>
+      <c r="J350" s="52">
+        <f t="shared" ref="J350:N350" si="56">$I$349*J$50/SUM($I$50:$N$50)</f>
+        <v>7.5</v>
+      </c>
+      <c r="K350" s="52">
+        <f t="shared" si="56"/>
+        <v>7.5</v>
+      </c>
+      <c r="L350" s="52">
+        <f t="shared" si="56"/>
+        <v>15</v>
+      </c>
+      <c r="M350" s="52">
+        <f t="shared" si="56"/>
+        <v>7.5</v>
+      </c>
+      <c r="N350" s="52">
+        <f t="shared" si="56"/>
+        <v>7.5</v>
+      </c>
+      <c r="O350" s="76">
+        <f>SUM(C350:N350)</f>
+        <v>120</v>
+      </c>
+    </row>
+    <row r="351" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A351" s="46" t="s">
+        <v>69</v>
+      </c>
+      <c r="C351" s="67">
+        <f>$O$351*C$50/$O$50</f>
+        <v>35</v>
+      </c>
+      <c r="D351" s="67">
+        <f t="shared" ref="D351:N351" si="57">$O$351*D$50/$O$50</f>
+        <v>17.5</v>
+      </c>
+      <c r="E351" s="67">
+        <f t="shared" si="57"/>
+        <v>17.5</v>
+      </c>
+      <c r="F351" s="67">
+        <f t="shared" si="57"/>
+        <v>35</v>
+      </c>
+      <c r="G351" s="67">
+        <f t="shared" si="57"/>
+        <v>17.5</v>
+      </c>
+      <c r="H351" s="67">
+        <f t="shared" si="57"/>
+        <v>17.5</v>
+      </c>
+      <c r="I351" s="67">
+        <f t="shared" si="57"/>
+        <v>35</v>
+      </c>
+      <c r="J351" s="67">
+        <f t="shared" si="57"/>
+        <v>17.5</v>
+      </c>
+      <c r="K351" s="67">
+        <f t="shared" si="57"/>
+        <v>17.5</v>
+      </c>
+      <c r="L351" s="67">
+        <f t="shared" si="57"/>
+        <v>35</v>
+      </c>
+      <c r="M351" s="67">
+        <f t="shared" si="57"/>
+        <v>17.5</v>
+      </c>
+      <c r="N351" s="67">
+        <f t="shared" si="57"/>
+        <v>17.5</v>
+      </c>
+      <c r="O351" s="73">
+        <f>O$50-O349</f>
+        <v>280</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="252">
-    <mergeCell ref="C329:H329"/>
-    <mergeCell ref="I329:N329"/>
-    <mergeCell ref="C330:H330"/>
-    <mergeCell ref="I330:N330"/>
-    <mergeCell ref="C324:H324"/>
-    <mergeCell ref="I324:N324"/>
-    <mergeCell ref="C325:H325"/>
-    <mergeCell ref="I325:N325"/>
-    <mergeCell ref="C326:H326"/>
-    <mergeCell ref="I326:N326"/>
-    <mergeCell ref="C327:H327"/>
-    <mergeCell ref="I327:N327"/>
-    <mergeCell ref="C328:H328"/>
-    <mergeCell ref="I328:N328"/>
-    <mergeCell ref="C312:H312"/>
-    <mergeCell ref="I312:N312"/>
-    <mergeCell ref="C313:H313"/>
-    <mergeCell ref="I313:N313"/>
-    <mergeCell ref="C314:H314"/>
-    <mergeCell ref="I314:N314"/>
-    <mergeCell ref="C322:H322"/>
-    <mergeCell ref="I322:N322"/>
-    <mergeCell ref="C323:H323"/>
-    <mergeCell ref="I323:N323"/>
-    <mergeCell ref="C307:H307"/>
-    <mergeCell ref="I307:N307"/>
-    <mergeCell ref="C308:H308"/>
-    <mergeCell ref="I308:N308"/>
-    <mergeCell ref="C309:H309"/>
-    <mergeCell ref="I309:N309"/>
-    <mergeCell ref="C310:H310"/>
-    <mergeCell ref="I310:N310"/>
-    <mergeCell ref="C311:H311"/>
-    <mergeCell ref="I311:N311"/>
-    <mergeCell ref="C297:E297"/>
-    <mergeCell ref="F297:H297"/>
-    <mergeCell ref="I297:K297"/>
-    <mergeCell ref="L297:N297"/>
-    <mergeCell ref="C298:E298"/>
-    <mergeCell ref="F298:H298"/>
-    <mergeCell ref="I298:K298"/>
-    <mergeCell ref="L298:N298"/>
-    <mergeCell ref="C306:H306"/>
-    <mergeCell ref="I306:N306"/>
-    <mergeCell ref="C294:E294"/>
-    <mergeCell ref="F294:H294"/>
-    <mergeCell ref="I294:K294"/>
-    <mergeCell ref="L294:N294"/>
-    <mergeCell ref="C295:E295"/>
-    <mergeCell ref="F295:H295"/>
-    <mergeCell ref="I295:K295"/>
-    <mergeCell ref="L295:N295"/>
-    <mergeCell ref="C296:E296"/>
-    <mergeCell ref="F296:H296"/>
-    <mergeCell ref="I296:K296"/>
-    <mergeCell ref="L296:N296"/>
-    <mergeCell ref="C291:E291"/>
-    <mergeCell ref="F291:H291"/>
-    <mergeCell ref="I291:K291"/>
-    <mergeCell ref="L291:N291"/>
-    <mergeCell ref="C292:E292"/>
-    <mergeCell ref="F292:H292"/>
-    <mergeCell ref="I292:K292"/>
-    <mergeCell ref="L292:N292"/>
-    <mergeCell ref="C293:E293"/>
-    <mergeCell ref="F293:H293"/>
-    <mergeCell ref="I293:K293"/>
-    <mergeCell ref="L293:N293"/>
-    <mergeCell ref="C290:E290"/>
-    <mergeCell ref="F290:H290"/>
-    <mergeCell ref="I290:K290"/>
-    <mergeCell ref="L290:N290"/>
-    <mergeCell ref="I122:K122"/>
-    <mergeCell ref="I123:K123"/>
-    <mergeCell ref="I117:K117"/>
-    <mergeCell ref="I118:K118"/>
-    <mergeCell ref="I119:K119"/>
-    <mergeCell ref="I120:K120"/>
-    <mergeCell ref="I121:K121"/>
-    <mergeCell ref="I112:K112"/>
-    <mergeCell ref="I113:K113"/>
-    <mergeCell ref="I114:K114"/>
-    <mergeCell ref="I115:K115"/>
-    <mergeCell ref="I116:K116"/>
-    <mergeCell ref="C121:E121"/>
-    <mergeCell ref="F121:H121"/>
-    <mergeCell ref="C122:E122"/>
-    <mergeCell ref="F122:H122"/>
-    <mergeCell ref="C123:E123"/>
-    <mergeCell ref="F123:H123"/>
-    <mergeCell ref="C118:E118"/>
-    <mergeCell ref="F118:H118"/>
-    <mergeCell ref="C119:E119"/>
-    <mergeCell ref="F119:H119"/>
-    <mergeCell ref="C120:E120"/>
-    <mergeCell ref="F120:H120"/>
-    <mergeCell ref="C115:E115"/>
-    <mergeCell ref="F115:H115"/>
-    <mergeCell ref="C116:E116"/>
-    <mergeCell ref="F116:H116"/>
-    <mergeCell ref="C117:E117"/>
-    <mergeCell ref="F117:H117"/>
-    <mergeCell ref="C112:E112"/>
-    <mergeCell ref="F112:H112"/>
-    <mergeCell ref="C113:E113"/>
+  <mergeCells count="254">
+    <mergeCell ref="C349:H349"/>
+    <mergeCell ref="I349:N349"/>
+    <mergeCell ref="C228:H228"/>
+    <mergeCell ref="I228:N228"/>
+    <mergeCell ref="C229:H229"/>
+    <mergeCell ref="I229:N229"/>
+    <mergeCell ref="C230:H230"/>
+    <mergeCell ref="I230:N230"/>
+    <mergeCell ref="C231:H231"/>
+    <mergeCell ref="I231:N231"/>
+    <mergeCell ref="C232:H232"/>
+    <mergeCell ref="I232:N232"/>
+    <mergeCell ref="C225:H225"/>
+    <mergeCell ref="I225:N225"/>
+    <mergeCell ref="C226:H226"/>
+    <mergeCell ref="I226:N226"/>
+    <mergeCell ref="C227:H227"/>
+    <mergeCell ref="I227:N227"/>
+    <mergeCell ref="C224:H224"/>
+    <mergeCell ref="I224:N224"/>
+    <mergeCell ref="C214:H214"/>
+    <mergeCell ref="C215:H215"/>
+    <mergeCell ref="C216:H216"/>
+    <mergeCell ref="I214:N214"/>
+    <mergeCell ref="I215:N215"/>
+    <mergeCell ref="I216:N216"/>
+    <mergeCell ref="F193:H193"/>
+    <mergeCell ref="F194:H194"/>
+    <mergeCell ref="F195:H195"/>
+    <mergeCell ref="C211:H211"/>
+    <mergeCell ref="C212:H212"/>
+    <mergeCell ref="C213:H213"/>
+    <mergeCell ref="I211:N211"/>
+    <mergeCell ref="I212:N212"/>
+    <mergeCell ref="I213:N213"/>
+    <mergeCell ref="C209:H209"/>
+    <mergeCell ref="I209:N209"/>
+    <mergeCell ref="C210:H210"/>
+    <mergeCell ref="I210:N210"/>
+    <mergeCell ref="C198:E198"/>
+    <mergeCell ref="C199:E199"/>
+    <mergeCell ref="C200:E200"/>
+    <mergeCell ref="C208:H208"/>
+    <mergeCell ref="I208:N208"/>
+    <mergeCell ref="L192:N192"/>
+    <mergeCell ref="L193:N193"/>
+    <mergeCell ref="L194:N194"/>
+    <mergeCell ref="L195:N195"/>
+    <mergeCell ref="L196:N196"/>
+    <mergeCell ref="L197:N197"/>
+    <mergeCell ref="L198:N198"/>
+    <mergeCell ref="L199:N199"/>
+    <mergeCell ref="L200:N200"/>
+    <mergeCell ref="I192:K192"/>
+    <mergeCell ref="I193:K193"/>
+    <mergeCell ref="I194:K194"/>
+    <mergeCell ref="I195:K195"/>
+    <mergeCell ref="I196:K196"/>
+    <mergeCell ref="I197:K197"/>
+    <mergeCell ref="I198:K198"/>
+    <mergeCell ref="I199:K199"/>
+    <mergeCell ref="I200:K200"/>
+    <mergeCell ref="F192:H192"/>
+    <mergeCell ref="C35:E35"/>
+    <mergeCell ref="F35:H35"/>
+    <mergeCell ref="I35:K35"/>
+    <mergeCell ref="L35:N35"/>
+    <mergeCell ref="C25:E25"/>
+    <mergeCell ref="F25:H25"/>
+    <mergeCell ref="I25:K25"/>
+    <mergeCell ref="L25:N25"/>
+    <mergeCell ref="C34:E34"/>
+    <mergeCell ref="F34:H34"/>
+    <mergeCell ref="I34:K34"/>
+    <mergeCell ref="L34:N34"/>
+    <mergeCell ref="C68:E68"/>
+    <mergeCell ref="C69:E69"/>
+    <mergeCell ref="C70:E70"/>
+    <mergeCell ref="C71:E71"/>
+    <mergeCell ref="C72:E72"/>
+    <mergeCell ref="C54:E54"/>
+    <mergeCell ref="C53:E53"/>
+    <mergeCell ref="C63:E63"/>
+    <mergeCell ref="C62:E62"/>
+    <mergeCell ref="C64:E64"/>
+    <mergeCell ref="C61:E61"/>
+    <mergeCell ref="C55:E55"/>
+    <mergeCell ref="C56:E56"/>
+    <mergeCell ref="C58:E58"/>
+    <mergeCell ref="C57:E57"/>
+    <mergeCell ref="C59:E59"/>
+    <mergeCell ref="C60:E60"/>
+    <mergeCell ref="C78:E78"/>
+    <mergeCell ref="C79:E79"/>
+    <mergeCell ref="C83:E83"/>
+    <mergeCell ref="C84:E84"/>
+    <mergeCell ref="C85:E85"/>
+    <mergeCell ref="C73:E73"/>
+    <mergeCell ref="C74:E74"/>
+    <mergeCell ref="C75:E75"/>
+    <mergeCell ref="C76:E76"/>
+    <mergeCell ref="C77:E77"/>
+    <mergeCell ref="C102:E102"/>
+    <mergeCell ref="C103:E103"/>
+    <mergeCell ref="C91:E91"/>
+    <mergeCell ref="C92:E92"/>
+    <mergeCell ref="C93:E93"/>
+    <mergeCell ref="C94:E94"/>
+    <mergeCell ref="C98:E98"/>
+    <mergeCell ref="C86:E86"/>
+    <mergeCell ref="C87:E87"/>
+    <mergeCell ref="C88:E88"/>
+    <mergeCell ref="C89:E89"/>
+    <mergeCell ref="C90:E90"/>
     <mergeCell ref="F113:H113"/>
     <mergeCell ref="C114:E114"/>
     <mergeCell ref="F114:H114"/>
@@ -8043,57 +8483,43 @@
     <mergeCell ref="C99:E99"/>
     <mergeCell ref="C100:E100"/>
     <mergeCell ref="C101:E101"/>
-    <mergeCell ref="C102:E102"/>
-    <mergeCell ref="C103:E103"/>
-    <mergeCell ref="C91:E91"/>
-    <mergeCell ref="C92:E92"/>
-    <mergeCell ref="C93:E93"/>
-    <mergeCell ref="C94:E94"/>
-    <mergeCell ref="C98:E98"/>
-    <mergeCell ref="C86:E86"/>
-    <mergeCell ref="C87:E87"/>
-    <mergeCell ref="C88:E88"/>
-    <mergeCell ref="C89:E89"/>
-    <mergeCell ref="C90:E90"/>
-    <mergeCell ref="C78:E78"/>
-    <mergeCell ref="C79:E79"/>
-    <mergeCell ref="C83:E83"/>
-    <mergeCell ref="C84:E84"/>
-    <mergeCell ref="C85:E85"/>
-    <mergeCell ref="C73:E73"/>
-    <mergeCell ref="C74:E74"/>
-    <mergeCell ref="C75:E75"/>
-    <mergeCell ref="C76:E76"/>
-    <mergeCell ref="C77:E77"/>
-    <mergeCell ref="C68:E68"/>
-    <mergeCell ref="C69:E69"/>
-    <mergeCell ref="C70:E70"/>
-    <mergeCell ref="C71:E71"/>
-    <mergeCell ref="C72:E72"/>
-    <mergeCell ref="C54:E54"/>
-    <mergeCell ref="C53:E53"/>
-    <mergeCell ref="C63:E63"/>
-    <mergeCell ref="C62:E62"/>
-    <mergeCell ref="C64:E64"/>
-    <mergeCell ref="C61:E61"/>
-    <mergeCell ref="C55:E55"/>
-    <mergeCell ref="C56:E56"/>
-    <mergeCell ref="C58:E58"/>
-    <mergeCell ref="C57:E57"/>
-    <mergeCell ref="C59:E59"/>
-    <mergeCell ref="C60:E60"/>
-    <mergeCell ref="C35:E35"/>
-    <mergeCell ref="F35:H35"/>
-    <mergeCell ref="I35:K35"/>
-    <mergeCell ref="L35:N35"/>
-    <mergeCell ref="C25:E25"/>
-    <mergeCell ref="F25:H25"/>
-    <mergeCell ref="I25:K25"/>
-    <mergeCell ref="L25:N25"/>
-    <mergeCell ref="C34:E34"/>
-    <mergeCell ref="F34:H34"/>
-    <mergeCell ref="I34:K34"/>
-    <mergeCell ref="L34:N34"/>
+    <mergeCell ref="I112:K112"/>
+    <mergeCell ref="I113:K113"/>
+    <mergeCell ref="I114:K114"/>
+    <mergeCell ref="I115:K115"/>
+    <mergeCell ref="I116:K116"/>
+    <mergeCell ref="C121:E121"/>
+    <mergeCell ref="F121:H121"/>
+    <mergeCell ref="C122:E122"/>
+    <mergeCell ref="F122:H122"/>
+    <mergeCell ref="C118:E118"/>
+    <mergeCell ref="F118:H118"/>
+    <mergeCell ref="C119:E119"/>
+    <mergeCell ref="F119:H119"/>
+    <mergeCell ref="C120:E120"/>
+    <mergeCell ref="F120:H120"/>
+    <mergeCell ref="C115:E115"/>
+    <mergeCell ref="F115:H115"/>
+    <mergeCell ref="C116:E116"/>
+    <mergeCell ref="F116:H116"/>
+    <mergeCell ref="C117:E117"/>
+    <mergeCell ref="F117:H117"/>
+    <mergeCell ref="C112:E112"/>
+    <mergeCell ref="F112:H112"/>
+    <mergeCell ref="C113:E113"/>
+    <mergeCell ref="C290:E290"/>
+    <mergeCell ref="F290:H290"/>
+    <mergeCell ref="I290:K290"/>
+    <mergeCell ref="L290:N290"/>
+    <mergeCell ref="I122:K122"/>
+    <mergeCell ref="I123:K123"/>
+    <mergeCell ref="I117:K117"/>
+    <mergeCell ref="I118:K118"/>
+    <mergeCell ref="I119:K119"/>
+    <mergeCell ref="I120:K120"/>
+    <mergeCell ref="I121:K121"/>
+    <mergeCell ref="C123:E123"/>
+    <mergeCell ref="F123:H123"/>
     <mergeCell ref="F196:H196"/>
     <mergeCell ref="F197:H197"/>
     <mergeCell ref="F198:H198"/>
@@ -8105,67 +8531,74 @@
     <mergeCell ref="C195:E195"/>
     <mergeCell ref="C196:E196"/>
     <mergeCell ref="C197:E197"/>
-    <mergeCell ref="C198:E198"/>
-    <mergeCell ref="C199:E199"/>
-    <mergeCell ref="C200:E200"/>
-    <mergeCell ref="C208:H208"/>
-    <mergeCell ref="I208:N208"/>
-    <mergeCell ref="L192:N192"/>
-    <mergeCell ref="L193:N193"/>
-    <mergeCell ref="L194:N194"/>
-    <mergeCell ref="L195:N195"/>
-    <mergeCell ref="L196:N196"/>
-    <mergeCell ref="L197:N197"/>
-    <mergeCell ref="L198:N198"/>
-    <mergeCell ref="L199:N199"/>
-    <mergeCell ref="L200:N200"/>
-    <mergeCell ref="I192:K192"/>
-    <mergeCell ref="I193:K193"/>
-    <mergeCell ref="I194:K194"/>
-    <mergeCell ref="I195:K195"/>
-    <mergeCell ref="I196:K196"/>
-    <mergeCell ref="I197:K197"/>
-    <mergeCell ref="I198:K198"/>
-    <mergeCell ref="I199:K199"/>
-    <mergeCell ref="I200:K200"/>
-    <mergeCell ref="F192:H192"/>
-    <mergeCell ref="F193:H193"/>
-    <mergeCell ref="F194:H194"/>
-    <mergeCell ref="F195:H195"/>
-    <mergeCell ref="C211:H211"/>
-    <mergeCell ref="C212:H212"/>
-    <mergeCell ref="C213:H213"/>
-    <mergeCell ref="I211:N211"/>
-    <mergeCell ref="I212:N212"/>
-    <mergeCell ref="I213:N213"/>
-    <mergeCell ref="C209:H209"/>
-    <mergeCell ref="I209:N209"/>
-    <mergeCell ref="C210:H210"/>
-    <mergeCell ref="I210:N210"/>
-    <mergeCell ref="C225:H225"/>
-    <mergeCell ref="I225:N225"/>
-    <mergeCell ref="C226:H226"/>
-    <mergeCell ref="I226:N226"/>
-    <mergeCell ref="C227:H227"/>
-    <mergeCell ref="I227:N227"/>
-    <mergeCell ref="C224:H224"/>
-    <mergeCell ref="I224:N224"/>
-    <mergeCell ref="C214:H214"/>
-    <mergeCell ref="C215:H215"/>
-    <mergeCell ref="C216:H216"/>
-    <mergeCell ref="I214:N214"/>
-    <mergeCell ref="I215:N215"/>
-    <mergeCell ref="I216:N216"/>
-    <mergeCell ref="C228:H228"/>
-    <mergeCell ref="I228:N228"/>
-    <mergeCell ref="C229:H229"/>
-    <mergeCell ref="I229:N229"/>
-    <mergeCell ref="C230:H230"/>
-    <mergeCell ref="I230:N230"/>
-    <mergeCell ref="C231:H231"/>
-    <mergeCell ref="I231:N231"/>
-    <mergeCell ref="C232:H232"/>
-    <mergeCell ref="I232:N232"/>
+    <mergeCell ref="C291:E291"/>
+    <mergeCell ref="F291:H291"/>
+    <mergeCell ref="I291:K291"/>
+    <mergeCell ref="L291:N291"/>
+    <mergeCell ref="C292:E292"/>
+    <mergeCell ref="F292:H292"/>
+    <mergeCell ref="I292:K292"/>
+    <mergeCell ref="L292:N292"/>
+    <mergeCell ref="C293:E293"/>
+    <mergeCell ref="F293:H293"/>
+    <mergeCell ref="I293:K293"/>
+    <mergeCell ref="L293:N293"/>
+    <mergeCell ref="C294:E294"/>
+    <mergeCell ref="F294:H294"/>
+    <mergeCell ref="I294:K294"/>
+    <mergeCell ref="L294:N294"/>
+    <mergeCell ref="C295:E295"/>
+    <mergeCell ref="F295:H295"/>
+    <mergeCell ref="I295:K295"/>
+    <mergeCell ref="L295:N295"/>
+    <mergeCell ref="C296:E296"/>
+    <mergeCell ref="F296:H296"/>
+    <mergeCell ref="I296:K296"/>
+    <mergeCell ref="L296:N296"/>
+    <mergeCell ref="C297:E297"/>
+    <mergeCell ref="F297:H297"/>
+    <mergeCell ref="I297:K297"/>
+    <mergeCell ref="L297:N297"/>
+    <mergeCell ref="C298:E298"/>
+    <mergeCell ref="F298:H298"/>
+    <mergeCell ref="I298:K298"/>
+    <mergeCell ref="L298:N298"/>
+    <mergeCell ref="C306:H306"/>
+    <mergeCell ref="I306:N306"/>
+    <mergeCell ref="C307:H307"/>
+    <mergeCell ref="I307:N307"/>
+    <mergeCell ref="C308:H308"/>
+    <mergeCell ref="I308:N308"/>
+    <mergeCell ref="C309:H309"/>
+    <mergeCell ref="I309:N309"/>
+    <mergeCell ref="C310:H310"/>
+    <mergeCell ref="I310:N310"/>
+    <mergeCell ref="C311:H311"/>
+    <mergeCell ref="I311:N311"/>
+    <mergeCell ref="C312:H312"/>
+    <mergeCell ref="I312:N312"/>
+    <mergeCell ref="C313:H313"/>
+    <mergeCell ref="I313:N313"/>
+    <mergeCell ref="C314:H314"/>
+    <mergeCell ref="I314:N314"/>
+    <mergeCell ref="C322:H322"/>
+    <mergeCell ref="I322:N322"/>
+    <mergeCell ref="C323:H323"/>
+    <mergeCell ref="I323:N323"/>
+    <mergeCell ref="C329:H329"/>
+    <mergeCell ref="I329:N329"/>
+    <mergeCell ref="C330:H330"/>
+    <mergeCell ref="I330:N330"/>
+    <mergeCell ref="C324:H324"/>
+    <mergeCell ref="I324:N324"/>
+    <mergeCell ref="C325:H325"/>
+    <mergeCell ref="I325:N325"/>
+    <mergeCell ref="C326:H326"/>
+    <mergeCell ref="I326:N326"/>
+    <mergeCell ref="C327:H327"/>
+    <mergeCell ref="I327:N327"/>
+    <mergeCell ref="C328:H328"/>
+    <mergeCell ref="I328:N328"/>
   </mergeCells>
   <pageMargins left="0.70866141732283472" right="0.70866141732283472" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup paperSize="9" scale="44" orientation="portrait" r:id="rId1"/>
@@ -8183,8 +8616,8 @@
   </sheetPr>
   <dimension ref="A2:M25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -8396,7 +8829,7 @@
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="B3" s="57" t="s">
+      <c r="B3" s="72" t="s">
         <v>80</v>
       </c>
       <c r="C3" s="69" t="s">
@@ -8407,7 +8840,7 @@
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="B4" s="57" t="s">
+      <c r="B4" s="72" t="s">
         <v>84</v>
       </c>
       <c r="C4" s="69" t="s">
@@ -8422,7 +8855,7 @@
       <c r="H4" s="63"/>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="B5" s="57" t="s">
+      <c r="B5" s="72" t="s">
         <v>81</v>
       </c>
       <c r="C5" s="69" t="s">
@@ -8437,7 +8870,7 @@
       <c r="H5" s="64"/>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="B6" s="57" t="s">
+      <c r="B6" s="72" t="s">
         <v>86</v>
       </c>
       <c r="C6" s="69" t="s">
@@ -8452,7 +8885,7 @@
       <c r="H6" s="64"/>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="B7" s="57" t="s">
+      <c r="B7" s="72" t="s">
         <v>104</v>
       </c>
       <c r="C7" s="69" t="s">
@@ -8467,7 +8900,7 @@
       <c r="H7" s="64"/>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="B8" s="57" t="s">
+      <c r="B8" s="72" t="s">
         <v>106</v>
       </c>
       <c r="C8" s="69" t="s">
@@ -8478,7 +8911,7 @@
       </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="B9" s="57" t="s">
+      <c r="B9" s="72" t="s">
         <v>108</v>
       </c>
       <c r="C9" s="69" t="s">
@@ -8489,7 +8922,7 @@
       </c>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="B10" s="57" t="s">
+      <c r="B10" s="72" t="s">
         <v>109</v>
       </c>
       <c r="C10" s="69" t="s">
@@ -8500,7 +8933,7 @@
       </c>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="B11" s="57" t="s">
+      <c r="B11" s="72" t="s">
         <v>110</v>
       </c>
       <c r="C11" s="69" t="s">
@@ -8514,7 +8947,7 @@
       </c>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="B12" s="57" t="s">
+      <c r="B12" s="72" t="s">
         <v>111</v>
       </c>
       <c r="C12" s="69" t="s">
@@ -8528,7 +8961,7 @@
       </c>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="B13" s="57" t="s">
+      <c r="B13" s="72" t="s">
         <v>113</v>
       </c>
       <c r="C13" s="69" t="s">
@@ -8543,7 +8976,7 @@
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A14" s="58"/>
-      <c r="B14" s="57" t="s">
+      <c r="B14" s="72" t="s">
         <v>115</v>
       </c>
       <c r="C14" s="69" t="s">
@@ -8566,7 +8999,7 @@
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A15" s="59"/>
-      <c r="B15" s="57" t="s">
+      <c r="B15" s="72" t="s">
         <v>117</v>
       </c>
       <c r="C15" s="70" t="s">
@@ -8587,7 +9020,7 @@
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A16" s="59"/>
-      <c r="B16" s="57" t="s">
+      <c r="B16" s="72" t="s">
         <v>119</v>
       </c>
       <c r="C16" s="70" t="s">
@@ -8608,7 +9041,7 @@
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A17" s="59"/>
-      <c r="B17" s="57" t="s">
+      <c r="B17" s="72" t="s">
         <v>91</v>
       </c>
       <c r="C17" s="70" t="s">
@@ -8629,7 +9062,7 @@
     </row>
     <row r="18" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A18" s="59"/>
-      <c r="B18" s="57" t="s">
+      <c r="B18" s="72" t="s">
         <v>92</v>
       </c>
       <c r="C18" s="70" t="s">
@@ -8754,6 +9187,24 @@
       <c r="M25" s="62"/>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B3" location="Calculations!A52" display="simple_loc_FAC" xr:uid="{85A23906-AE7A-4EF2-A587-3B038A782F88}"/>
+    <hyperlink ref="B4" location="Calculations!A82" display="simple_pol_FAC" xr:uid="{9285BAC3-BB86-42A0-B8E6-20F9120D36DD}"/>
+    <hyperlink ref="B5" location="Calculations!A67" display="simple_pol_FAC" xr:uid="{40B975F1-6FD7-429E-8BDC-0F843D2E3C47}"/>
+    <hyperlink ref="B6" location="Calculations!A97" display="multiple_FAC" xr:uid="{0784578A-9042-45B5-ABAB-B482A35A09CF}"/>
+    <hyperlink ref="B17" location="Calculations!A126" display="simple_CAT_XL" xr:uid="{0A52529B-26B5-442E-8233-15E02865A61B}"/>
+    <hyperlink ref="B18" location="Calculations!A142" display="multiple_CAT_XL" xr:uid="{9E6C1045-A0E2-4B41-A5D0-647D7EACA04C}"/>
+    <hyperlink ref="B7" location="Calculations!A175" display="simple_QS" xr:uid="{FC997AB8-CE66-4D2F-B594-BC15F84115C6}"/>
+    <hyperlink ref="B12" location="Calculations!A191" display="loc_limit_QS" xr:uid="{6A8534EA-144D-4997-B5BD-DE8E18E63F8E}"/>
+    <hyperlink ref="B13" location="Calculations!A207" display="pol_limit_QS" xr:uid="{8A74CB14-76FB-4238-9C86-A32FC74C0AED}"/>
+    <hyperlink ref="B14" location="Calculations!A223" display="acc_limit_QS" xr:uid="{360EAB9C-846B-49AC-88DC-0CC97F27F6AC}"/>
+    <hyperlink ref="B15" location="Calculations!A239" display="multiple_QS_1" xr:uid="{F39C2C02-C2FE-4C31-951A-C273E3DCEBAB}"/>
+    <hyperlink ref="B16" location="Calculations!A256" display="multiple_QS_2" xr:uid="{7B616093-7274-4F17-902F-8A95113C324C}"/>
+    <hyperlink ref="B8" location="Calculations!A289" display="loc_SS" xr:uid="{7062D54D-F3C2-4409-9C26-81AE9468DB47}"/>
+    <hyperlink ref="B9" location="Calculations!A305" display="pol_SS" xr:uid="{9462480D-4025-45C0-9988-64F65622FE5B}"/>
+    <hyperlink ref="B10" location="Calculations!A355" display="acc_SS" xr:uid="{49A1EF6D-C3F0-446C-89F0-288F81EE0F82}"/>
+    <hyperlink ref="B11" location="Calculations!A337" display="multiple_SS" xr:uid="{E2892C55-32DD-47CB-B12E-68115F56099E}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
updated RiskLevel to ACC #29
</commit_message>
<xml_diff>
--- a/examples/ExamplesComparisonTest.xlsx
+++ b/examples/ExamplesComparisonTest.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\cygwin64\home\Joh\git\ReinsuranceTestTool\examples\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{54AB320C-A4C1-4A17-9777-240427C4237C}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{7667B191-FF57-4398-99FD-3938D52CC375}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="30720" windowHeight="9072" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="491" uniqueCount="162">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="491" uniqueCount="163">
   <si>
     <t>Limit</t>
   </si>
@@ -423,9 +423,6 @@
     <t>GR Loss net of 2nd Order Reins</t>
   </si>
   <si>
-    <t>Treaty 3 on portfolio: 10 xs 0 @50%</t>
-  </si>
-  <si>
     <t>Treaty 1 on portfolio: 50% ceded</t>
   </si>
   <si>
@@ -508,6 +505,12 @@
   </si>
   <si>
     <t>Losses are back-allocated to the coverage level.</t>
+  </si>
+  <si>
+    <t>% placed</t>
+  </si>
+  <si>
+    <t>Treaty 3 on portfolio: 10 xs 0 @100%</t>
   </si>
 </sst>
 </file>
@@ -1046,22 +1049,22 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
@@ -1091,8 +1094,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="6">
@@ -1472,7 +1475,7 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
@@ -1490,7 +1493,7 @@
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="D10" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.3">
@@ -1516,8 +1519,8 @@
   </sheetPr>
   <dimension ref="A1:U368"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="84" zoomScaleNormal="84" workbookViewId="0">
-      <selection activeCell="I186" sqref="I186"/>
+    <sheetView showGridLines="0" topLeftCell="A163" zoomScale="84" zoomScaleNormal="84" workbookViewId="0">
+      <selection activeCell="C188" sqref="C188"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2554,11 +2557,11 @@
       <c r="A53" s="43" t="s">
         <v>61</v>
       </c>
-      <c r="C53" s="86">
-        <v>1</v>
-      </c>
-      <c r="D53" s="86"/>
-      <c r="E53" s="87"/>
+      <c r="C53" s="83">
+        <v>1</v>
+      </c>
+      <c r="D53" s="83"/>
+      <c r="E53" s="84"/>
       <c r="H53" s="40"/>
       <c r="N53" s="40"/>
     </row>
@@ -2566,11 +2569,11 @@
       <c r="A54" s="43" t="s">
         <v>62</v>
       </c>
-      <c r="C54" s="86" t="s">
+      <c r="C54" s="83" t="s">
         <v>70</v>
       </c>
-      <c r="D54" s="86"/>
-      <c r="E54" s="87"/>
+      <c r="D54" s="83"/>
+      <c r="E54" s="84"/>
       <c r="H54" s="40"/>
       <c r="N54" s="40"/>
     </row>
@@ -2578,11 +2581,11 @@
       <c r="A55" s="43" t="s">
         <v>63</v>
       </c>
-      <c r="C55" s="86">
-        <v>1</v>
-      </c>
-      <c r="D55" s="86"/>
-      <c r="E55" s="87"/>
+      <c r="C55" s="83">
+        <v>1</v>
+      </c>
+      <c r="D55" s="83"/>
+      <c r="E55" s="84"/>
       <c r="H55" s="40"/>
       <c r="N55" s="40"/>
     </row>
@@ -2590,11 +2593,11 @@
       <c r="A56" s="43" t="s">
         <v>64</v>
       </c>
-      <c r="C56" s="83">
+      <c r="C56" s="86">
         <v>0</v>
       </c>
-      <c r="D56" s="83"/>
-      <c r="E56" s="87"/>
+      <c r="D56" s="86"/>
+      <c r="E56" s="84"/>
       <c r="H56" s="40"/>
       <c r="N56" s="40"/>
     </row>
@@ -2602,12 +2605,12 @@
       <c r="A57" s="44" t="s">
         <v>65</v>
       </c>
-      <c r="C57" s="83">
+      <c r="C57" s="86">
         <f>MAX(0, SUM(C$50:E$50)-C56)</f>
         <v>100</v>
       </c>
-      <c r="D57" s="83"/>
-      <c r="E57" s="87"/>
+      <c r="D57" s="86"/>
+      <c r="E57" s="84"/>
       <c r="H57" s="40"/>
       <c r="N57" s="40"/>
     </row>
@@ -2615,11 +2618,11 @@
       <c r="A58" s="43" t="s">
         <v>0</v>
       </c>
-      <c r="C58" s="83">
+      <c r="C58" s="86">
         <v>10</v>
       </c>
-      <c r="D58" s="83"/>
-      <c r="E58" s="87"/>
+      <c r="D58" s="86"/>
+      <c r="E58" s="84"/>
       <c r="H58" s="40"/>
       <c r="N58" s="40"/>
     </row>
@@ -2627,12 +2630,12 @@
       <c r="A59" s="44" t="s">
         <v>66</v>
       </c>
-      <c r="C59" s="83">
+      <c r="C59" s="86">
         <f>IF(C58="Unlimited", C57, MIN(C57, C58))</f>
         <v>10</v>
       </c>
-      <c r="D59" s="83"/>
-      <c r="E59" s="87"/>
+      <c r="D59" s="86"/>
+      <c r="E59" s="84"/>
       <c r="H59" s="40"/>
       <c r="N59" s="40"/>
     </row>
@@ -2644,7 +2647,7 @@
         <v>1</v>
       </c>
       <c r="D60" s="85"/>
-      <c r="E60" s="98"/>
+      <c r="E60" s="87"/>
       <c r="H60" s="40"/>
       <c r="N60" s="40"/>
     </row>
@@ -2652,12 +2655,12 @@
       <c r="A61" s="44" t="s">
         <v>72</v>
       </c>
-      <c r="C61" s="83">
+      <c r="C61" s="86">
         <f>C60*C59</f>
         <v>10</v>
       </c>
-      <c r="D61" s="83"/>
-      <c r="E61" s="87"/>
+      <c r="D61" s="86"/>
+      <c r="E61" s="84"/>
       <c r="H61" s="40"/>
       <c r="N61" s="40"/>
     </row>
@@ -2665,9 +2668,9 @@
       <c r="A62" s="43" t="s">
         <v>3</v>
       </c>
-      <c r="C62" s="84"/>
-      <c r="D62" s="84"/>
-      <c r="E62" s="88"/>
+      <c r="C62" s="88"/>
+      <c r="D62" s="88"/>
+      <c r="E62" s="98"/>
       <c r="H62" s="40"/>
       <c r="N62" s="40"/>
     </row>
@@ -2675,9 +2678,9 @@
       <c r="A63" s="43" t="s">
         <v>67</v>
       </c>
-      <c r="C63" s="84"/>
-      <c r="D63" s="84"/>
-      <c r="E63" s="88"/>
+      <c r="C63" s="88"/>
+      <c r="D63" s="88"/>
+      <c r="E63" s="98"/>
       <c r="H63" s="40"/>
       <c r="N63" s="40"/>
     </row>
@@ -2685,12 +2688,12 @@
       <c r="A64" s="45" t="s">
         <v>68</v>
       </c>
-      <c r="C64" s="83">
+      <c r="C64" s="86">
         <f>MIN(C61,IF(OR(C63="Unlimited",C63=""),10^18,C63))</f>
         <v>10</v>
       </c>
-      <c r="D64" s="83"/>
-      <c r="E64" s="87"/>
+      <c r="D64" s="86"/>
+      <c r="E64" s="84"/>
       <c r="H64" s="40"/>
       <c r="N64" s="40"/>
     </row>
@@ -2771,11 +2774,11 @@
       <c r="A68" s="43" t="s">
         <v>61</v>
       </c>
-      <c r="C68" s="86">
-        <v>1</v>
-      </c>
-      <c r="D68" s="86"/>
-      <c r="E68" s="83"/>
+      <c r="C68" s="83">
+        <v>1</v>
+      </c>
+      <c r="D68" s="83"/>
+      <c r="E68" s="86"/>
       <c r="F68" s="13"/>
       <c r="H68" s="40"/>
       <c r="N68" s="40"/>
@@ -2784,11 +2787,11 @@
       <c r="A69" s="43" t="s">
         <v>62</v>
       </c>
-      <c r="C69" s="86" t="s">
+      <c r="C69" s="83" t="s">
         <v>83</v>
       </c>
-      <c r="D69" s="86"/>
-      <c r="E69" s="83"/>
+      <c r="D69" s="83"/>
+      <c r="E69" s="86"/>
       <c r="F69" s="13"/>
       <c r="H69" s="40"/>
       <c r="N69" s="40"/>
@@ -2797,11 +2800,11 @@
       <c r="A70" s="43" t="s">
         <v>63</v>
       </c>
-      <c r="C70" s="86">
-        <v>1</v>
-      </c>
-      <c r="D70" s="86"/>
-      <c r="E70" s="83"/>
+      <c r="C70" s="83">
+        <v>1</v>
+      </c>
+      <c r="D70" s="83"/>
+      <c r="E70" s="86"/>
       <c r="F70" s="13"/>
       <c r="H70" s="40"/>
       <c r="N70" s="40"/>
@@ -2810,11 +2813,11 @@
       <c r="A71" s="43" t="s">
         <v>64</v>
       </c>
-      <c r="C71" s="83">
+      <c r="C71" s="86">
         <v>0</v>
       </c>
-      <c r="D71" s="83"/>
-      <c r="E71" s="83"/>
+      <c r="D71" s="86"/>
+      <c r="E71" s="86"/>
       <c r="F71" s="13"/>
       <c r="H71" s="40"/>
       <c r="N71" s="40"/>
@@ -2823,12 +2826,12 @@
       <c r="A72" s="44" t="s">
         <v>65</v>
       </c>
-      <c r="C72" s="83">
+      <c r="C72" s="86">
         <f>MAX(0, SUM(C$50:H$50)-C71)</f>
         <v>200</v>
       </c>
-      <c r="D72" s="83"/>
-      <c r="E72" s="83"/>
+      <c r="D72" s="86"/>
+      <c r="E72" s="86"/>
       <c r="F72" s="13"/>
       <c r="H72" s="40"/>
       <c r="N72" s="40"/>
@@ -2837,11 +2840,11 @@
       <c r="A73" s="43" t="s">
         <v>0</v>
       </c>
-      <c r="C73" s="83">
+      <c r="C73" s="86">
         <v>10</v>
       </c>
-      <c r="D73" s="83"/>
-      <c r="E73" s="83"/>
+      <c r="D73" s="86"/>
+      <c r="E73" s="86"/>
       <c r="F73" s="13"/>
       <c r="H73" s="40"/>
       <c r="N73" s="40"/>
@@ -2850,12 +2853,12 @@
       <c r="A74" s="44" t="s">
         <v>66</v>
       </c>
-      <c r="C74" s="83">
+      <c r="C74" s="86">
         <f>IF(C73="Unlimited", C72, MIN(C72, C73))</f>
         <v>10</v>
       </c>
-      <c r="D74" s="83"/>
-      <c r="E74" s="83"/>
+      <c r="D74" s="86"/>
+      <c r="E74" s="86"/>
       <c r="F74" s="13"/>
       <c r="H74" s="40"/>
       <c r="N74" s="40"/>
@@ -2877,12 +2880,12 @@
       <c r="A76" s="44" t="s">
         <v>72</v>
       </c>
-      <c r="C76" s="83">
+      <c r="C76" s="86">
         <f>C75*C74</f>
         <v>10</v>
       </c>
-      <c r="D76" s="83"/>
-      <c r="E76" s="83"/>
+      <c r="D76" s="86"/>
+      <c r="E76" s="86"/>
       <c r="F76" s="13"/>
       <c r="H76" s="40"/>
       <c r="N76" s="40"/>
@@ -2891,9 +2894,9 @@
       <c r="A77" s="43" t="s">
         <v>3</v>
       </c>
-      <c r="C77" s="84"/>
-      <c r="D77" s="84"/>
-      <c r="E77" s="84"/>
+      <c r="C77" s="88"/>
+      <c r="D77" s="88"/>
+      <c r="E77" s="88"/>
       <c r="F77" s="13"/>
       <c r="H77" s="40"/>
       <c r="N77" s="40"/>
@@ -2902,9 +2905,9 @@
       <c r="A78" s="43" t="s">
         <v>67</v>
       </c>
-      <c r="C78" s="84"/>
-      <c r="D78" s="84"/>
-      <c r="E78" s="84"/>
+      <c r="C78" s="88"/>
+      <c r="D78" s="88"/>
+      <c r="E78" s="88"/>
       <c r="F78" s="13"/>
       <c r="H78" s="40"/>
       <c r="N78" s="40"/>
@@ -2913,12 +2916,12 @@
       <c r="A79" s="45" t="s">
         <v>68</v>
       </c>
-      <c r="C79" s="83">
+      <c r="C79" s="86">
         <f>MIN(C76,IF(OR(C78="Unlimited",C78=""),10^18,C78))</f>
         <v>10</v>
       </c>
-      <c r="D79" s="83"/>
-      <c r="E79" s="83"/>
+      <c r="D79" s="86"/>
+      <c r="E79" s="86"/>
       <c r="F79" s="13"/>
       <c r="H79" s="40"/>
       <c r="N79" s="40"/>
@@ -3001,11 +3004,11 @@
       <c r="A83" s="43" t="s">
         <v>61</v>
       </c>
-      <c r="C83" s="86">
-        <v>1</v>
-      </c>
-      <c r="D83" s="86"/>
-      <c r="E83" s="83"/>
+      <c r="C83" s="83">
+        <v>1</v>
+      </c>
+      <c r="D83" s="83"/>
+      <c r="E83" s="86"/>
       <c r="F83" s="13"/>
       <c r="H83" s="40"/>
       <c r="N83" s="40"/>
@@ -3014,11 +3017,11 @@
       <c r="A84" s="43" t="s">
         <v>62</v>
       </c>
-      <c r="C84" s="86" t="s">
+      <c r="C84" s="83" t="s">
         <v>85</v>
       </c>
-      <c r="D84" s="86"/>
-      <c r="E84" s="83"/>
+      <c r="D84" s="83"/>
+      <c r="E84" s="86"/>
       <c r="F84" s="13"/>
       <c r="H84" s="40"/>
       <c r="N84" s="40"/>
@@ -3027,11 +3030,11 @@
       <c r="A85" s="43" t="s">
         <v>63</v>
       </c>
-      <c r="C85" s="86">
-        <v>1</v>
-      </c>
-      <c r="D85" s="86"/>
-      <c r="E85" s="83"/>
+      <c r="C85" s="83">
+        <v>1</v>
+      </c>
+      <c r="D85" s="83"/>
+      <c r="E85" s="86"/>
       <c r="F85" s="13"/>
       <c r="H85" s="40"/>
       <c r="N85" s="40"/>
@@ -3040,11 +3043,11 @@
       <c r="A86" s="43" t="s">
         <v>64</v>
       </c>
-      <c r="C86" s="83">
+      <c r="C86" s="86">
         <v>0</v>
       </c>
-      <c r="D86" s="83"/>
-      <c r="E86" s="83"/>
+      <c r="D86" s="86"/>
+      <c r="E86" s="86"/>
       <c r="F86" s="13"/>
       <c r="H86" s="40"/>
       <c r="N86" s="40"/>
@@ -3053,12 +3056,12 @@
       <c r="A87" s="44" t="s">
         <v>65</v>
       </c>
-      <c r="C87" s="83">
+      <c r="C87" s="86">
         <f>MAX(0, SUM(C$50:H$50)-C86)</f>
         <v>200</v>
       </c>
-      <c r="D87" s="83"/>
-      <c r="E87" s="83"/>
+      <c r="D87" s="86"/>
+      <c r="E87" s="86"/>
       <c r="F87" s="13"/>
       <c r="H87" s="40"/>
       <c r="N87" s="40"/>
@@ -3067,11 +3070,11 @@
       <c r="A88" s="43" t="s">
         <v>0</v>
       </c>
-      <c r="C88" s="83">
+      <c r="C88" s="86">
         <v>10</v>
       </c>
-      <c r="D88" s="83"/>
-      <c r="E88" s="83"/>
+      <c r="D88" s="86"/>
+      <c r="E88" s="86"/>
       <c r="F88" s="13"/>
       <c r="H88" s="40"/>
       <c r="N88" s="40"/>
@@ -3080,12 +3083,12 @@
       <c r="A89" s="44" t="s">
         <v>66</v>
       </c>
-      <c r="C89" s="83">
+      <c r="C89" s="86">
         <f>IF(C88="Unlimited", C87, MIN(C87, C88))</f>
         <v>10</v>
       </c>
-      <c r="D89" s="83"/>
-      <c r="E89" s="83"/>
+      <c r="D89" s="86"/>
+      <c r="E89" s="86"/>
       <c r="F89" s="13"/>
       <c r="H89" s="40"/>
       <c r="N89" s="40"/>
@@ -3107,12 +3110,12 @@
       <c r="A91" s="44" t="s">
         <v>72</v>
       </c>
-      <c r="C91" s="83">
+      <c r="C91" s="86">
         <f>C90*C89</f>
         <v>10</v>
       </c>
-      <c r="D91" s="83"/>
-      <c r="E91" s="83"/>
+      <c r="D91" s="86"/>
+      <c r="E91" s="86"/>
       <c r="F91" s="13"/>
       <c r="H91" s="40"/>
       <c r="N91" s="40"/>
@@ -3121,9 +3124,9 @@
       <c r="A92" s="43" t="s">
         <v>3</v>
       </c>
-      <c r="C92" s="84"/>
-      <c r="D92" s="84"/>
-      <c r="E92" s="84"/>
+      <c r="C92" s="88"/>
+      <c r="D92" s="88"/>
+      <c r="E92" s="88"/>
       <c r="F92" s="13"/>
       <c r="H92" s="40"/>
       <c r="N92" s="40"/>
@@ -3132,9 +3135,9 @@
       <c r="A93" s="43" t="s">
         <v>67</v>
       </c>
-      <c r="C93" s="84"/>
-      <c r="D93" s="84"/>
-      <c r="E93" s="84"/>
+      <c r="C93" s="88"/>
+      <c r="D93" s="88"/>
+      <c r="E93" s="88"/>
       <c r="F93" s="13"/>
       <c r="H93" s="40"/>
       <c r="N93" s="40"/>
@@ -3143,12 +3146,12 @@
       <c r="A94" s="45" t="s">
         <v>68</v>
       </c>
-      <c r="C94" s="83">
+      <c r="C94" s="86">
         <f>MIN(C91,IF(OR(C93="Unlimited",C93=""),10^18,C93))</f>
         <v>10</v>
       </c>
-      <c r="D94" s="83"/>
-      <c r="E94" s="83"/>
+      <c r="D94" s="86"/>
+      <c r="E94" s="86"/>
       <c r="F94" s="13"/>
       <c r="H94" s="40"/>
       <c r="N94" s="40"/>
@@ -3234,116 +3237,116 @@
       <c r="A98" s="43" t="s">
         <v>61</v>
       </c>
-      <c r="C98" s="86">
-        <v>1</v>
-      </c>
-      <c r="D98" s="86"/>
-      <c r="E98" s="83"/>
-      <c r="F98" s="86">
-        <v>1</v>
-      </c>
-      <c r="G98" s="86"/>
-      <c r="H98" s="83"/>
+      <c r="C98" s="83">
+        <v>1</v>
+      </c>
+      <c r="D98" s="83"/>
+      <c r="E98" s="86"/>
+      <c r="F98" s="83">
+        <v>1</v>
+      </c>
+      <c r="G98" s="83"/>
+      <c r="H98" s="86"/>
       <c r="N98" s="40"/>
     </row>
     <row r="99" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A99" s="43" t="s">
         <v>62</v>
       </c>
-      <c r="C99" s="86" t="s">
+      <c r="C99" s="83" t="s">
         <v>70</v>
       </c>
-      <c r="D99" s="86"/>
-      <c r="E99" s="83"/>
-      <c r="F99" s="86" t="s">
+      <c r="D99" s="83"/>
+      <c r="E99" s="86"/>
+      <c r="F99" s="83" t="s">
         <v>70</v>
       </c>
-      <c r="G99" s="86"/>
-      <c r="H99" s="83"/>
+      <c r="G99" s="83"/>
+      <c r="H99" s="86"/>
       <c r="N99" s="40"/>
     </row>
     <row r="100" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A100" s="43" t="s">
         <v>63</v>
       </c>
-      <c r="C100" s="86">
-        <v>1</v>
-      </c>
-      <c r="D100" s="86"/>
-      <c r="E100" s="83"/>
-      <c r="F100" s="86">
-        <v>1</v>
-      </c>
-      <c r="G100" s="86"/>
-      <c r="H100" s="83"/>
+      <c r="C100" s="83">
+        <v>1</v>
+      </c>
+      <c r="D100" s="83"/>
+      <c r="E100" s="86"/>
+      <c r="F100" s="83">
+        <v>1</v>
+      </c>
+      <c r="G100" s="83"/>
+      <c r="H100" s="86"/>
       <c r="N100" s="40"/>
     </row>
     <row r="101" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A101" s="43" t="s">
         <v>64</v>
       </c>
-      <c r="C101" s="83">
+      <c r="C101" s="86">
         <v>0</v>
       </c>
-      <c r="D101" s="83"/>
-      <c r="E101" s="83"/>
-      <c r="F101" s="83">
+      <c r="D101" s="86"/>
+      <c r="E101" s="86"/>
+      <c r="F101" s="86">
         <v>0</v>
       </c>
-      <c r="G101" s="83"/>
-      <c r="H101" s="83"/>
+      <c r="G101" s="86"/>
+      <c r="H101" s="86"/>
       <c r="N101" s="40"/>
     </row>
     <row r="102" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A102" s="44" t="s">
         <v>65</v>
       </c>
-      <c r="C102" s="83">
+      <c r="C102" s="86">
         <f>MAX(0, SUM(C$50:E$50)-C101)</f>
         <v>100</v>
       </c>
-      <c r="D102" s="83"/>
-      <c r="E102" s="83"/>
-      <c r="F102" s="83">
+      <c r="D102" s="86"/>
+      <c r="E102" s="86"/>
+      <c r="F102" s="86">
         <f>MAX(0, SUM(F$50:H$50)-F101)</f>
         <v>100</v>
       </c>
-      <c r="G102" s="83"/>
-      <c r="H102" s="83"/>
+      <c r="G102" s="86"/>
+      <c r="H102" s="86"/>
       <c r="N102" s="40"/>
     </row>
     <row r="103" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A103" s="43" t="s">
         <v>0</v>
       </c>
-      <c r="C103" s="83">
+      <c r="C103" s="86">
         <v>10</v>
       </c>
-      <c r="D103" s="83"/>
-      <c r="E103" s="83"/>
-      <c r="F103" s="83">
+      <c r="D103" s="86"/>
+      <c r="E103" s="86"/>
+      <c r="F103" s="86">
         <v>10</v>
       </c>
-      <c r="G103" s="83"/>
-      <c r="H103" s="83"/>
+      <c r="G103" s="86"/>
+      <c r="H103" s="86"/>
       <c r="N103" s="40"/>
     </row>
     <row r="104" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A104" s="44" t="s">
         <v>66</v>
       </c>
-      <c r="C104" s="83">
+      <c r="C104" s="86">
         <f>IF(C103="Unlimited", C102, MIN(C102, C103))</f>
         <v>10</v>
       </c>
-      <c r="D104" s="83"/>
-      <c r="E104" s="83"/>
-      <c r="F104" s="83">
+      <c r="D104" s="86"/>
+      <c r="E104" s="86"/>
+      <c r="F104" s="86">
         <f>IF(F103="Unlimited", F102, MIN(F102, F103))</f>
         <v>10</v>
       </c>
-      <c r="G104" s="83"/>
-      <c r="H104" s="83"/>
+      <c r="G104" s="86"/>
+      <c r="H104" s="86"/>
       <c r="N104" s="40"/>
     </row>
     <row r="105" spans="1:15" x14ac:dyDescent="0.3">
@@ -3366,60 +3369,60 @@
       <c r="A106" s="44" t="s">
         <v>72</v>
       </c>
-      <c r="C106" s="83">
+      <c r="C106" s="86">
         <f>C105*C104</f>
         <v>10</v>
       </c>
-      <c r="D106" s="83"/>
-      <c r="E106" s="83"/>
-      <c r="F106" s="83">
+      <c r="D106" s="86"/>
+      <c r="E106" s="86"/>
+      <c r="F106" s="86">
         <f>F105*F104</f>
         <v>10</v>
       </c>
-      <c r="G106" s="83"/>
-      <c r="H106" s="83"/>
+      <c r="G106" s="86"/>
+      <c r="H106" s="86"/>
       <c r="N106" s="40"/>
     </row>
     <row r="107" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A107" s="43" t="s">
         <v>3</v>
       </c>
-      <c r="C107" s="84"/>
-      <c r="D107" s="84"/>
-      <c r="E107" s="84"/>
-      <c r="F107" s="84"/>
-      <c r="G107" s="84"/>
-      <c r="H107" s="84"/>
+      <c r="C107" s="88"/>
+      <c r="D107" s="88"/>
+      <c r="E107" s="88"/>
+      <c r="F107" s="88"/>
+      <c r="G107" s="88"/>
+      <c r="H107" s="88"/>
       <c r="N107" s="40"/>
     </row>
     <row r="108" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A108" s="43" t="s">
         <v>67</v>
       </c>
-      <c r="C108" s="84"/>
-      <c r="D108" s="84"/>
-      <c r="E108" s="84"/>
-      <c r="F108" s="84"/>
-      <c r="G108" s="84"/>
-      <c r="H108" s="84"/>
+      <c r="C108" s="88"/>
+      <c r="D108" s="88"/>
+      <c r="E108" s="88"/>
+      <c r="F108" s="88"/>
+      <c r="G108" s="88"/>
+      <c r="H108" s="88"/>
       <c r="N108" s="40"/>
     </row>
     <row r="109" spans="1:15" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A109" s="45" t="s">
         <v>68</v>
       </c>
-      <c r="C109" s="83">
+      <c r="C109" s="86">
         <f>MIN(C106,IF(OR(C108="Unlimited",C108=""),10^18,C108))</f>
         <v>10</v>
       </c>
-      <c r="D109" s="83"/>
-      <c r="E109" s="83"/>
-      <c r="F109" s="83">
+      <c r="D109" s="86"/>
+      <c r="E109" s="86"/>
+      <c r="F109" s="86">
         <f>MIN(F106,IF(OR(F108="Unlimited",F108=""),10^18,F108))</f>
         <v>10</v>
       </c>
-      <c r="G109" s="83"/>
-      <c r="H109" s="83"/>
+      <c r="G109" s="86"/>
+      <c r="H109" s="86"/>
       <c r="N109" s="40"/>
     </row>
     <row r="110" spans="1:15" x14ac:dyDescent="0.3">
@@ -3495,121 +3498,121 @@
       <c r="A112" s="43" t="s">
         <v>61</v>
       </c>
-      <c r="C112" s="86">
-        <v>1</v>
-      </c>
-      <c r="D112" s="86"/>
-      <c r="E112" s="83"/>
-      <c r="F112" s="86"/>
-      <c r="G112" s="86"/>
-      <c r="H112" s="83"/>
-      <c r="I112" s="86"/>
-      <c r="J112" s="86"/>
-      <c r="K112" s="83"/>
+      <c r="C112" s="83">
+        <v>1</v>
+      </c>
+      <c r="D112" s="83"/>
+      <c r="E112" s="86"/>
+      <c r="F112" s="83"/>
+      <c r="G112" s="83"/>
+      <c r="H112" s="86"/>
+      <c r="I112" s="83"/>
+      <c r="J112" s="83"/>
+      <c r="K112" s="86"/>
       <c r="N112" s="40"/>
     </row>
     <row r="113" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A113" s="43" t="s">
         <v>62</v>
       </c>
-      <c r="C113" s="86" t="s">
+      <c r="C113" s="83" t="s">
         <v>85</v>
       </c>
-      <c r="D113" s="86"/>
-      <c r="E113" s="83"/>
-      <c r="F113" s="86"/>
-      <c r="G113" s="86"/>
-      <c r="H113" s="83"/>
-      <c r="I113" s="86"/>
-      <c r="J113" s="86"/>
-      <c r="K113" s="83"/>
+      <c r="D113" s="83"/>
+      <c r="E113" s="86"/>
+      <c r="F113" s="83"/>
+      <c r="G113" s="83"/>
+      <c r="H113" s="86"/>
+      <c r="I113" s="83"/>
+      <c r="J113" s="83"/>
+      <c r="K113" s="86"/>
       <c r="N113" s="40"/>
     </row>
     <row r="114" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A114" s="43" t="s">
         <v>63</v>
       </c>
-      <c r="C114" s="86">
-        <v>1</v>
-      </c>
-      <c r="D114" s="86"/>
-      <c r="E114" s="83"/>
-      <c r="F114" s="86"/>
-      <c r="G114" s="86"/>
-      <c r="H114" s="83"/>
-      <c r="I114" s="86"/>
-      <c r="J114" s="86"/>
-      <c r="K114" s="83"/>
+      <c r="C114" s="83">
+        <v>1</v>
+      </c>
+      <c r="D114" s="83"/>
+      <c r="E114" s="86"/>
+      <c r="F114" s="83"/>
+      <c r="G114" s="83"/>
+      <c r="H114" s="86"/>
+      <c r="I114" s="83"/>
+      <c r="J114" s="83"/>
+      <c r="K114" s="86"/>
       <c r="N114" s="40"/>
     </row>
     <row r="115" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A115" s="43" t="s">
         <v>64</v>
       </c>
-      <c r="C115" s="83">
+      <c r="C115" s="86">
         <v>0</v>
       </c>
-      <c r="D115" s="83"/>
-      <c r="E115" s="83"/>
-      <c r="F115" s="83"/>
-      <c r="G115" s="83"/>
-      <c r="H115" s="83"/>
-      <c r="I115" s="83"/>
-      <c r="J115" s="83"/>
-      <c r="K115" s="83"/>
+      <c r="D115" s="86"/>
+      <c r="E115" s="86"/>
+      <c r="F115" s="86"/>
+      <c r="G115" s="86"/>
+      <c r="H115" s="86"/>
+      <c r="I115" s="86"/>
+      <c r="J115" s="86"/>
+      <c r="K115" s="86"/>
       <c r="N115" s="40"/>
     </row>
     <row r="116" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A116" s="44" t="s">
         <v>65</v>
       </c>
-      <c r="C116" s="83">
+      <c r="C116" s="86">
         <f>MAX(0, SUM(C$110:H$110)-C115)</f>
         <v>180</v>
       </c>
-      <c r="D116" s="83"/>
-      <c r="E116" s="83"/>
-      <c r="F116" s="83"/>
-      <c r="G116" s="83"/>
-      <c r="H116" s="83"/>
-      <c r="I116" s="83"/>
-      <c r="J116" s="83"/>
-      <c r="K116" s="83"/>
+      <c r="D116" s="86"/>
+      <c r="E116" s="86"/>
+      <c r="F116" s="86"/>
+      <c r="G116" s="86"/>
+      <c r="H116" s="86"/>
+      <c r="I116" s="86"/>
+      <c r="J116" s="86"/>
+      <c r="K116" s="86"/>
       <c r="N116" s="40"/>
     </row>
     <row r="117" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A117" s="43" t="s">
         <v>0</v>
       </c>
-      <c r="C117" s="83">
+      <c r="C117" s="86">
         <v>10</v>
       </c>
-      <c r="D117" s="83"/>
-      <c r="E117" s="83"/>
-      <c r="F117" s="83"/>
-      <c r="G117" s="83"/>
-      <c r="H117" s="83"/>
-      <c r="I117" s="83"/>
-      <c r="J117" s="83"/>
-      <c r="K117" s="83"/>
+      <c r="D117" s="86"/>
+      <c r="E117" s="86"/>
+      <c r="F117" s="86"/>
+      <c r="G117" s="86"/>
+      <c r="H117" s="86"/>
+      <c r="I117" s="86"/>
+      <c r="J117" s="86"/>
+      <c r="K117" s="86"/>
       <c r="N117" s="40"/>
     </row>
     <row r="118" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A118" s="44" t="s">
         <v>66</v>
       </c>
-      <c r="C118" s="83">
+      <c r="C118" s="86">
         <f>IF(C117="Unlimited", C116, MIN(C116, C117))</f>
         <v>10</v>
       </c>
-      <c r="D118" s="83"/>
-      <c r="E118" s="83"/>
-      <c r="F118" s="83"/>
-      <c r="G118" s="83"/>
-      <c r="H118" s="83"/>
-      <c r="I118" s="83"/>
-      <c r="J118" s="83"/>
-      <c r="K118" s="83"/>
+      <c r="D118" s="86"/>
+      <c r="E118" s="86"/>
+      <c r="F118" s="86"/>
+      <c r="G118" s="86"/>
+      <c r="H118" s="86"/>
+      <c r="I118" s="86"/>
+      <c r="J118" s="86"/>
+      <c r="K118" s="86"/>
       <c r="N118" s="40"/>
     </row>
     <row r="119" spans="1:15" x14ac:dyDescent="0.3">
@@ -3633,66 +3636,66 @@
       <c r="A120" s="44" t="s">
         <v>72</v>
       </c>
-      <c r="C120" s="83">
+      <c r="C120" s="86">
         <f>C119*C118</f>
         <v>10</v>
       </c>
-      <c r="D120" s="83"/>
-      <c r="E120" s="83"/>
-      <c r="F120" s="83"/>
-      <c r="G120" s="83"/>
-      <c r="H120" s="83"/>
-      <c r="I120" s="83"/>
-      <c r="J120" s="83"/>
-      <c r="K120" s="83"/>
+      <c r="D120" s="86"/>
+      <c r="E120" s="86"/>
+      <c r="F120" s="86"/>
+      <c r="G120" s="86"/>
+      <c r="H120" s="86"/>
+      <c r="I120" s="86"/>
+      <c r="J120" s="86"/>
+      <c r="K120" s="86"/>
       <c r="N120" s="40"/>
     </row>
     <row r="121" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A121" s="43" t="s">
         <v>3</v>
       </c>
-      <c r="C121" s="84"/>
-      <c r="D121" s="84"/>
-      <c r="E121" s="84"/>
-      <c r="F121" s="84"/>
-      <c r="G121" s="84"/>
-      <c r="H121" s="84"/>
-      <c r="I121" s="84"/>
-      <c r="J121" s="84"/>
-      <c r="K121" s="84"/>
+      <c r="C121" s="88"/>
+      <c r="D121" s="88"/>
+      <c r="E121" s="88"/>
+      <c r="F121" s="88"/>
+      <c r="G121" s="88"/>
+      <c r="H121" s="88"/>
+      <c r="I121" s="88"/>
+      <c r="J121" s="88"/>
+      <c r="K121" s="88"/>
       <c r="N121" s="40"/>
     </row>
     <row r="122" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A122" s="43" t="s">
         <v>67</v>
       </c>
-      <c r="C122" s="84"/>
-      <c r="D122" s="84"/>
-      <c r="E122" s="84"/>
-      <c r="F122" s="84"/>
-      <c r="G122" s="84"/>
-      <c r="H122" s="84"/>
-      <c r="I122" s="84"/>
-      <c r="J122" s="84"/>
-      <c r="K122" s="84"/>
+      <c r="C122" s="88"/>
+      <c r="D122" s="88"/>
+      <c r="E122" s="88"/>
+      <c r="F122" s="88"/>
+      <c r="G122" s="88"/>
+      <c r="H122" s="88"/>
+      <c r="I122" s="88"/>
+      <c r="J122" s="88"/>
+      <c r="K122" s="88"/>
       <c r="N122" s="40"/>
     </row>
     <row r="123" spans="1:15" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A123" s="45" t="s">
         <v>68</v>
       </c>
-      <c r="C123" s="83">
+      <c r="C123" s="86">
         <f>MIN(C120,IF(OR(C122="Unlimited",C122=""),10^18,C122))</f>
         <v>10</v>
       </c>
-      <c r="D123" s="83"/>
-      <c r="E123" s="83"/>
-      <c r="F123" s="83"/>
-      <c r="G123" s="83"/>
-      <c r="H123" s="83"/>
-      <c r="I123" s="83"/>
-      <c r="J123" s="83"/>
-      <c r="K123" s="83"/>
+      <c r="D123" s="86"/>
+      <c r="E123" s="86"/>
+      <c r="F123" s="86"/>
+      <c r="G123" s="86"/>
+      <c r="H123" s="86"/>
+      <c r="I123" s="86"/>
+      <c r="J123" s="86"/>
+      <c r="K123" s="86"/>
       <c r="N123" s="40"/>
     </row>
     <row r="124" spans="1:15" x14ac:dyDescent="0.3">
@@ -3776,121 +3779,121 @@
       <c r="A127" s="43" t="s">
         <v>61</v>
       </c>
-      <c r="C127" s="86"/>
-      <c r="D127" s="86"/>
-      <c r="E127" s="83"/>
-      <c r="F127" s="86"/>
-      <c r="G127" s="86"/>
-      <c r="H127" s="83"/>
-      <c r="I127" s="86">
-        <v>1</v>
-      </c>
-      <c r="J127" s="86"/>
-      <c r="K127" s="83"/>
+      <c r="C127" s="83"/>
+      <c r="D127" s="83"/>
+      <c r="E127" s="86"/>
+      <c r="F127" s="83"/>
+      <c r="G127" s="83"/>
+      <c r="H127" s="86"/>
+      <c r="I127" s="83">
+        <v>1</v>
+      </c>
+      <c r="J127" s="83"/>
+      <c r="K127" s="86"/>
       <c r="N127" s="40"/>
     </row>
     <row r="128" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A128" s="43" t="s">
         <v>62</v>
       </c>
-      <c r="C128" s="86"/>
-      <c r="D128" s="86"/>
-      <c r="E128" s="83"/>
-      <c r="F128" s="86"/>
-      <c r="G128" s="86"/>
-      <c r="H128" s="83"/>
-      <c r="I128" s="86" t="s">
+      <c r="C128" s="83"/>
+      <c r="D128" s="83"/>
+      <c r="E128" s="86"/>
+      <c r="F128" s="83"/>
+      <c r="G128" s="83"/>
+      <c r="H128" s="86"/>
+      <c r="I128" s="83" t="s">
         <v>83</v>
       </c>
-      <c r="J128" s="86"/>
-      <c r="K128" s="83"/>
+      <c r="J128" s="83"/>
+      <c r="K128" s="86"/>
       <c r="N128" s="40"/>
     </row>
     <row r="129" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A129" s="43" t="s">
         <v>63</v>
       </c>
-      <c r="C129" s="86"/>
-      <c r="D129" s="86"/>
-      <c r="E129" s="83"/>
-      <c r="F129" s="86"/>
-      <c r="G129" s="86"/>
-      <c r="H129" s="83"/>
-      <c r="I129" s="86">
-        <v>1</v>
-      </c>
-      <c r="J129" s="86"/>
-      <c r="K129" s="83"/>
+      <c r="C129" s="83"/>
+      <c r="D129" s="83"/>
+      <c r="E129" s="86"/>
+      <c r="F129" s="83"/>
+      <c r="G129" s="83"/>
+      <c r="H129" s="86"/>
+      <c r="I129" s="83">
+        <v>1</v>
+      </c>
+      <c r="J129" s="83"/>
+      <c r="K129" s="86"/>
       <c r="N129" s="40"/>
     </row>
     <row r="130" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A130" s="43" t="s">
         <v>64</v>
       </c>
-      <c r="C130" s="83"/>
-      <c r="D130" s="83"/>
-      <c r="E130" s="83"/>
-      <c r="F130" s="83"/>
-      <c r="G130" s="83"/>
-      <c r="H130" s="83"/>
-      <c r="I130" s="83">
+      <c r="C130" s="86"/>
+      <c r="D130" s="86"/>
+      <c r="E130" s="86"/>
+      <c r="F130" s="86"/>
+      <c r="G130" s="86"/>
+      <c r="H130" s="86"/>
+      <c r="I130" s="86">
         <v>0</v>
       </c>
-      <c r="J130" s="83"/>
-      <c r="K130" s="83"/>
+      <c r="J130" s="86"/>
+      <c r="K130" s="86"/>
       <c r="N130" s="40"/>
     </row>
     <row r="131" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A131" s="44" t="s">
         <v>65</v>
       </c>
-      <c r="C131" s="83"/>
-      <c r="D131" s="83"/>
-      <c r="E131" s="83"/>
-      <c r="F131" s="83"/>
-      <c r="G131" s="83"/>
-      <c r="H131" s="83"/>
-      <c r="I131" s="83">
+      <c r="C131" s="86"/>
+      <c r="D131" s="86"/>
+      <c r="E131" s="86"/>
+      <c r="F131" s="86"/>
+      <c r="G131" s="86"/>
+      <c r="H131" s="86"/>
+      <c r="I131" s="86">
         <f>MAX(0, SUM(I$124:N$124)-I130)</f>
         <v>200</v>
       </c>
-      <c r="J131" s="83"/>
-      <c r="K131" s="83"/>
+      <c r="J131" s="86"/>
+      <c r="K131" s="86"/>
       <c r="N131" s="40"/>
     </row>
     <row r="132" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A132" s="43" t="s">
         <v>0</v>
       </c>
-      <c r="C132" s="83"/>
-      <c r="D132" s="83"/>
-      <c r="E132" s="83"/>
-      <c r="F132" s="83"/>
-      <c r="G132" s="83"/>
-      <c r="H132" s="83"/>
-      <c r="I132" s="83">
+      <c r="C132" s="86"/>
+      <c r="D132" s="86"/>
+      <c r="E132" s="86"/>
+      <c r="F132" s="86"/>
+      <c r="G132" s="86"/>
+      <c r="H132" s="86"/>
+      <c r="I132" s="86">
         <v>10</v>
       </c>
-      <c r="J132" s="83"/>
-      <c r="K132" s="83"/>
+      <c r="J132" s="86"/>
+      <c r="K132" s="86"/>
       <c r="N132" s="40"/>
     </row>
     <row r="133" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A133" s="44" t="s">
         <v>66</v>
       </c>
-      <c r="C133" s="83"/>
-      <c r="D133" s="83"/>
-      <c r="E133" s="83"/>
-      <c r="F133" s="83"/>
-      <c r="G133" s="83"/>
-      <c r="H133" s="83"/>
-      <c r="I133" s="83">
+      <c r="C133" s="86"/>
+      <c r="D133" s="86"/>
+      <c r="E133" s="86"/>
+      <c r="F133" s="86"/>
+      <c r="G133" s="86"/>
+      <c r="H133" s="86"/>
+      <c r="I133" s="86">
         <f>IF(I132="Unlimited", I131, MIN(I131, I132))</f>
         <v>10</v>
       </c>
-      <c r="J133" s="83"/>
-      <c r="K133" s="83"/>
+      <c r="J133" s="86"/>
+      <c r="K133" s="86"/>
       <c r="N133" s="40"/>
     </row>
     <row r="134" spans="1:15" x14ac:dyDescent="0.3">
@@ -3914,66 +3917,66 @@
       <c r="A135" s="44" t="s">
         <v>72</v>
       </c>
-      <c r="C135" s="83"/>
-      <c r="D135" s="83"/>
-      <c r="E135" s="83"/>
-      <c r="F135" s="83"/>
-      <c r="G135" s="83"/>
-      <c r="H135" s="83"/>
-      <c r="I135" s="83">
+      <c r="C135" s="86"/>
+      <c r="D135" s="86"/>
+      <c r="E135" s="86"/>
+      <c r="F135" s="86"/>
+      <c r="G135" s="86"/>
+      <c r="H135" s="86"/>
+      <c r="I135" s="86">
         <f>I134*I133</f>
         <v>10</v>
       </c>
-      <c r="J135" s="83"/>
-      <c r="K135" s="83"/>
+      <c r="J135" s="86"/>
+      <c r="K135" s="86"/>
       <c r="N135" s="40"/>
     </row>
     <row r="136" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A136" s="43" t="s">
         <v>3</v>
       </c>
-      <c r="C136" s="84"/>
-      <c r="D136" s="84"/>
-      <c r="E136" s="84"/>
-      <c r="F136" s="84"/>
-      <c r="G136" s="84"/>
-      <c r="H136" s="84"/>
-      <c r="I136" s="84"/>
-      <c r="J136" s="84"/>
-      <c r="K136" s="84"/>
+      <c r="C136" s="88"/>
+      <c r="D136" s="88"/>
+      <c r="E136" s="88"/>
+      <c r="F136" s="88"/>
+      <c r="G136" s="88"/>
+      <c r="H136" s="88"/>
+      <c r="I136" s="88"/>
+      <c r="J136" s="88"/>
+      <c r="K136" s="88"/>
       <c r="N136" s="40"/>
     </row>
     <row r="137" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A137" s="43" t="s">
         <v>67</v>
       </c>
-      <c r="C137" s="84"/>
-      <c r="D137" s="84"/>
-      <c r="E137" s="84"/>
-      <c r="F137" s="84"/>
-      <c r="G137" s="84"/>
-      <c r="H137" s="84"/>
-      <c r="I137" s="84"/>
-      <c r="J137" s="84"/>
-      <c r="K137" s="84"/>
+      <c r="C137" s="88"/>
+      <c r="D137" s="88"/>
+      <c r="E137" s="88"/>
+      <c r="F137" s="88"/>
+      <c r="G137" s="88"/>
+      <c r="H137" s="88"/>
+      <c r="I137" s="88"/>
+      <c r="J137" s="88"/>
+      <c r="K137" s="88"/>
       <c r="N137" s="40"/>
     </row>
     <row r="138" spans="1:15" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A138" s="45" t="s">
         <v>68</v>
       </c>
-      <c r="C138" s="83"/>
-      <c r="D138" s="83"/>
-      <c r="E138" s="83"/>
-      <c r="F138" s="83"/>
-      <c r="G138" s="83"/>
-      <c r="H138" s="83"/>
-      <c r="I138" s="83">
+      <c r="C138" s="86"/>
+      <c r="D138" s="86"/>
+      <c r="E138" s="86"/>
+      <c r="F138" s="86"/>
+      <c r="G138" s="86"/>
+      <c r="H138" s="86"/>
+      <c r="I138" s="86">
         <f>MIN(I135,IF(OR(I137="Unlimited",I137=""),10^18,I137))</f>
         <v>10</v>
       </c>
-      <c r="J138" s="83"/>
-      <c r="K138" s="83"/>
+      <c r="J138" s="86"/>
+      <c r="K138" s="86"/>
       <c r="N138" s="40"/>
     </row>
     <row r="139" spans="1:15" x14ac:dyDescent="0.3">
@@ -4121,7 +4124,7 @@
     </row>
     <row r="149" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A149" s="43" t="s">
-        <v>71</v>
+        <v>161</v>
       </c>
       <c r="N149" s="40"/>
       <c r="O149" s="48">
@@ -4393,14 +4396,14 @@
     </row>
     <row r="165" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A165" s="43" t="s">
-        <v>71</v>
+        <v>161</v>
       </c>
       <c r="N165" s="40"/>
       <c r="O165" s="48">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="P165" s="48">
-        <v>1</v>
+        <v>0.5</v>
       </c>
     </row>
     <row r="166" spans="1:17" ht="28.8" x14ac:dyDescent="0.3">
@@ -4410,11 +4413,11 @@
       <c r="N166" s="40"/>
       <c r="O166" s="2">
         <f>O165*O164</f>
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="P166" s="2">
         <f>P165*P164</f>
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="167" spans="1:17" x14ac:dyDescent="0.3">
@@ -4436,15 +4439,15 @@
       <c r="N169" s="40"/>
       <c r="O169" s="6">
         <f>MIN(O166,IF(OR(O168="Unlimited",O168=""),10^18,O168))</f>
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="P169" s="6">
         <f>MIN(P166,IF(OR(P168="Unlimited",P168=""),10^18,P168))</f>
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="Q169" s="2">
         <f>SUM(O169:P169)</f>
-        <v>20</v>
+        <v>10</v>
       </c>
     </row>
     <row r="170" spans="1:17" x14ac:dyDescent="0.3">
@@ -4453,55 +4456,55 @@
       </c>
       <c r="C170" s="52">
         <f>$O$169*C$50/$O$50</f>
-        <v>1.25</v>
+        <v>0.625</v>
       </c>
       <c r="D170" s="52">
         <f t="shared" ref="D170:N170" si="23">$O$169*D$50/$O$50</f>
-        <v>0.625</v>
+        <v>0.3125</v>
       </c>
       <c r="E170" s="52">
         <f t="shared" si="23"/>
-        <v>0.625</v>
+        <v>0.3125</v>
       </c>
       <c r="F170" s="52">
         <f t="shared" si="23"/>
-        <v>1.25</v>
+        <v>0.625</v>
       </c>
       <c r="G170" s="52">
         <f t="shared" si="23"/>
-        <v>0.625</v>
+        <v>0.3125</v>
       </c>
       <c r="H170" s="52">
         <f t="shared" si="23"/>
-        <v>0.625</v>
+        <v>0.3125</v>
       </c>
       <c r="I170" s="52">
         <f t="shared" si="23"/>
-        <v>1.25</v>
+        <v>0.625</v>
       </c>
       <c r="J170" s="52">
         <f t="shared" si="23"/>
-        <v>0.625</v>
+        <v>0.3125</v>
       </c>
       <c r="K170" s="52">
         <f t="shared" si="23"/>
-        <v>0.625</v>
+        <v>0.3125</v>
       </c>
       <c r="L170" s="52">
         <f t="shared" si="23"/>
-        <v>1.25</v>
+        <v>0.625</v>
       </c>
       <c r="M170" s="52">
         <f t="shared" si="23"/>
-        <v>0.625</v>
+        <v>0.3125</v>
       </c>
       <c r="N170" s="53">
         <f t="shared" si="23"/>
-        <v>0.625</v>
+        <v>0.3125</v>
       </c>
       <c r="O170" s="49">
         <f>SUM(C170:N170)</f>
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="171" spans="1:17" x14ac:dyDescent="0.3">
@@ -4510,55 +4513,55 @@
       </c>
       <c r="C171" s="52">
         <f>$P$169*C$50/$O$50</f>
-        <v>1.25</v>
+        <v>0.625</v>
       </c>
       <c r="D171" s="52">
         <f t="shared" ref="D171:N171" si="24">$P$169*D$50/$O$50</f>
-        <v>0.625</v>
+        <v>0.3125</v>
       </c>
       <c r="E171" s="52">
         <f t="shared" si="24"/>
-        <v>0.625</v>
+        <v>0.3125</v>
       </c>
       <c r="F171" s="52">
         <f t="shared" si="24"/>
-        <v>1.25</v>
+        <v>0.625</v>
       </c>
       <c r="G171" s="52">
         <f t="shared" si="24"/>
-        <v>0.625</v>
+        <v>0.3125</v>
       </c>
       <c r="H171" s="52">
         <f t="shared" si="24"/>
-        <v>0.625</v>
+        <v>0.3125</v>
       </c>
       <c r="I171" s="52">
         <f t="shared" si="24"/>
-        <v>1.25</v>
+        <v>0.625</v>
       </c>
       <c r="J171" s="52">
         <f t="shared" si="24"/>
-        <v>0.625</v>
+        <v>0.3125</v>
       </c>
       <c r="K171" s="52">
         <f t="shared" si="24"/>
-        <v>0.625</v>
+        <v>0.3125</v>
       </c>
       <c r="L171" s="52">
         <f t="shared" si="24"/>
-        <v>1.25</v>
+        <v>0.625</v>
       </c>
       <c r="M171" s="52">
         <f t="shared" si="24"/>
-        <v>0.625</v>
+        <v>0.3125</v>
       </c>
       <c r="N171" s="53">
         <f t="shared" si="24"/>
-        <v>0.625</v>
+        <v>0.3125</v>
       </c>
       <c r="O171" s="49">
         <f>SUM(C171:N171)</f>
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="172" spans="1:17" x14ac:dyDescent="0.3">
@@ -4567,55 +4570,55 @@
       </c>
       <c r="C172" s="54">
         <f>$O$172*C50/$O$50</f>
-        <v>47.5</v>
+        <v>48.75</v>
       </c>
       <c r="D172" s="54">
         <f t="shared" ref="D172:N172" si="25">$O$172*D50/$O$50</f>
-        <v>23.75</v>
+        <v>24.375</v>
       </c>
       <c r="E172" s="54">
         <f t="shared" si="25"/>
-        <v>23.75</v>
+        <v>24.375</v>
       </c>
       <c r="F172" s="54">
         <f t="shared" si="25"/>
-        <v>47.5</v>
+        <v>48.75</v>
       </c>
       <c r="G172" s="54">
         <f t="shared" si="25"/>
-        <v>23.75</v>
+        <v>24.375</v>
       </c>
       <c r="H172" s="54">
         <f t="shared" si="25"/>
-        <v>23.75</v>
+        <v>24.375</v>
       </c>
       <c r="I172" s="54">
         <f t="shared" si="25"/>
-        <v>47.5</v>
+        <v>48.75</v>
       </c>
       <c r="J172" s="54">
         <f t="shared" si="25"/>
-        <v>23.75</v>
+        <v>24.375</v>
       </c>
       <c r="K172" s="54">
         <f t="shared" si="25"/>
-        <v>23.75</v>
+        <v>24.375</v>
       </c>
       <c r="L172" s="54">
         <f t="shared" si="25"/>
-        <v>47.5</v>
+        <v>48.75</v>
       </c>
       <c r="M172" s="54">
         <f t="shared" si="25"/>
-        <v>23.75</v>
+        <v>24.375</v>
       </c>
       <c r="N172" s="55">
         <f t="shared" si="25"/>
-        <v>23.75</v>
+        <v>24.375</v>
       </c>
       <c r="O172" s="2">
         <f>O162-Q169</f>
-        <v>380</v>
+        <v>390</v>
       </c>
     </row>
     <row r="174" spans="1:17" x14ac:dyDescent="0.3">
@@ -4623,7 +4626,7 @@
         <v>61</v>
       </c>
       <c r="B174" s="4" t="s">
-        <v>133</v>
+        <v>162</v>
       </c>
       <c r="N174" s="40"/>
       <c r="O174" s="2">
@@ -4665,7 +4668,7 @@
       <c r="N178" s="40"/>
       <c r="O178" s="6">
         <f>MAX(0, O172-O177)</f>
-        <v>380</v>
+        <v>390</v>
       </c>
       <c r="P178" s="6"/>
     </row>
@@ -4691,11 +4694,11 @@
     </row>
     <row r="181" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A181" s="43" t="s">
-        <v>71</v>
+        <v>161</v>
       </c>
       <c r="N181" s="40"/>
       <c r="O181" s="48">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="P181" s="48"/>
     </row>
@@ -4706,7 +4709,7 @@
       <c r="N182" s="40"/>
       <c r="O182" s="2">
         <f>O181*O180</f>
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="183" spans="1:16" x14ac:dyDescent="0.3">
@@ -4728,7 +4731,7 @@
       <c r="N185" s="40"/>
       <c r="O185" s="6">
         <f>MIN(O182,IF(OR(O184="Unlimited",O184=""),10^18,O184))</f>
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="P185" s="6"/>
     </row>
@@ -4738,55 +4741,55 @@
       </c>
       <c r="C186" s="52">
         <f>$O$185*C$36/$O$36</f>
-        <v>1.25</v>
+        <v>0.625</v>
       </c>
       <c r="D186" s="52">
         <f t="shared" ref="D186:N186" si="26">$O$185*D$36/$O$36</f>
-        <v>0.625</v>
+        <v>0.3125</v>
       </c>
       <c r="E186" s="52">
         <f t="shared" si="26"/>
-        <v>0.625</v>
+        <v>0.3125</v>
       </c>
       <c r="F186" s="52">
         <f t="shared" si="26"/>
-        <v>1.25</v>
+        <v>0.625</v>
       </c>
       <c r="G186" s="52">
         <f t="shared" si="26"/>
-        <v>0.625</v>
+        <v>0.3125</v>
       </c>
       <c r="H186" s="52">
         <f t="shared" si="26"/>
-        <v>0.625</v>
+        <v>0.3125</v>
       </c>
       <c r="I186" s="52">
         <f t="shared" si="26"/>
-        <v>1.25</v>
+        <v>0.625</v>
       </c>
       <c r="J186" s="52">
         <f t="shared" si="26"/>
-        <v>0.625</v>
+        <v>0.3125</v>
       </c>
       <c r="K186" s="52">
         <f t="shared" si="26"/>
-        <v>0.625</v>
+        <v>0.3125</v>
       </c>
       <c r="L186" s="52">
         <f t="shared" si="26"/>
-        <v>1.25</v>
+        <v>0.625</v>
       </c>
       <c r="M186" s="52">
         <f t="shared" si="26"/>
-        <v>0.625</v>
+        <v>0.3125</v>
       </c>
       <c r="N186" s="53">
         <f t="shared" si="26"/>
-        <v>0.625</v>
+        <v>0.3125</v>
       </c>
       <c r="O186" s="49">
         <f>SUM(C186:N186)</f>
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="187" spans="1:16" x14ac:dyDescent="0.3">
@@ -4809,57 +4812,57 @@
       <c r="A188" s="46" t="s">
         <v>132</v>
       </c>
-      <c r="C188" s="54">
+      <c r="C188" s="67">
         <f>$O$188*C50/$O$50</f>
-        <v>46.25</v>
-      </c>
-      <c r="D188" s="54">
+        <v>48.125</v>
+      </c>
+      <c r="D188" s="67">
         <f t="shared" ref="D188:N188" si="27">$O$188*D50/$O$50</f>
-        <v>23.125</v>
-      </c>
-      <c r="E188" s="54">
+        <v>24.0625</v>
+      </c>
+      <c r="E188" s="67">
         <f t="shared" si="27"/>
-        <v>23.125</v>
-      </c>
-      <c r="F188" s="54">
+        <v>24.0625</v>
+      </c>
+      <c r="F188" s="67">
         <f t="shared" si="27"/>
-        <v>46.25</v>
-      </c>
-      <c r="G188" s="54">
+        <v>48.125</v>
+      </c>
+      <c r="G188" s="67">
         <f t="shared" si="27"/>
-        <v>23.125</v>
-      </c>
-      <c r="H188" s="54">
+        <v>24.0625</v>
+      </c>
+      <c r="H188" s="67">
         <f t="shared" si="27"/>
-        <v>23.125</v>
-      </c>
-      <c r="I188" s="54">
+        <v>24.0625</v>
+      </c>
+      <c r="I188" s="67">
         <f t="shared" si="27"/>
-        <v>46.25</v>
-      </c>
-      <c r="J188" s="54">
+        <v>48.125</v>
+      </c>
+      <c r="J188" s="67">
         <f t="shared" si="27"/>
-        <v>23.125</v>
-      </c>
-      <c r="K188" s="54">
+        <v>24.0625</v>
+      </c>
+      <c r="K188" s="67">
         <f t="shared" si="27"/>
-        <v>23.125</v>
-      </c>
-      <c r="L188" s="54">
+        <v>24.0625</v>
+      </c>
+      <c r="L188" s="67">
         <f t="shared" si="27"/>
-        <v>46.25</v>
-      </c>
-      <c r="M188" s="54">
+        <v>48.125</v>
+      </c>
+      <c r="M188" s="67">
         <f t="shared" si="27"/>
-        <v>23.125</v>
-      </c>
-      <c r="N188" s="54">
+        <v>24.0625</v>
+      </c>
+      <c r="N188" s="67">
         <f t="shared" si="27"/>
-        <v>23.125</v>
+        <v>24.0625</v>
       </c>
       <c r="O188" s="2">
         <f>O178-O185</f>
-        <v>370</v>
+        <v>385</v>
       </c>
     </row>
     <row r="190" spans="1:16" x14ac:dyDescent="0.3">
@@ -4867,7 +4870,7 @@
         <v>104</v>
       </c>
       <c r="B190" s="4" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="191" spans="1:16" x14ac:dyDescent="0.3">
@@ -4885,7 +4888,7 @@
       </c>
       <c r="N192" s="40"/>
       <c r="O192" s="50" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="193" spans="1:17" x14ac:dyDescent="0.3">
@@ -5104,7 +5107,7 @@
       </c>
       <c r="B206" s="4"/>
       <c r="D206" s="76" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="H206" s="42"/>
       <c r="K206" s="42"/>
@@ -5114,134 +5117,134 @@
       <c r="A207" s="43" t="s">
         <v>61</v>
       </c>
-      <c r="C207" s="86">
-        <v>1</v>
-      </c>
-      <c r="D207" s="86"/>
-      <c r="E207" s="83"/>
-      <c r="F207" s="86">
-        <v>1</v>
-      </c>
-      <c r="G207" s="86"/>
-      <c r="H207" s="83"/>
-      <c r="I207" s="86">
-        <v>1</v>
-      </c>
-      <c r="J207" s="86"/>
-      <c r="K207" s="83"/>
-      <c r="L207" s="86">
-        <v>1</v>
-      </c>
-      <c r="M207" s="86"/>
-      <c r="N207" s="83"/>
+      <c r="C207" s="83">
+        <v>1</v>
+      </c>
+      <c r="D207" s="83"/>
+      <c r="E207" s="86"/>
+      <c r="F207" s="83">
+        <v>1</v>
+      </c>
+      <c r="G207" s="83"/>
+      <c r="H207" s="86"/>
+      <c r="I207" s="83">
+        <v>1</v>
+      </c>
+      <c r="J207" s="83"/>
+      <c r="K207" s="86"/>
+      <c r="L207" s="83">
+        <v>1</v>
+      </c>
+      <c r="M207" s="83"/>
+      <c r="N207" s="86"/>
       <c r="O207" s="72"/>
     </row>
     <row r="208" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A208" s="43" t="s">
         <v>62</v>
       </c>
-      <c r="C208" s="86" t="s">
+      <c r="C208" s="83" t="s">
+        <v>139</v>
+      </c>
+      <c r="D208" s="83"/>
+      <c r="E208" s="86"/>
+      <c r="F208" s="83" t="s">
         <v>140</v>
       </c>
-      <c r="D208" s="86"/>
-      <c r="E208" s="83"/>
-      <c r="F208" s="86" t="s">
+      <c r="G208" s="83"/>
+      <c r="H208" s="86"/>
+      <c r="I208" s="83" t="s">
         <v>141</v>
       </c>
-      <c r="G208" s="86"/>
-      <c r="H208" s="83"/>
-      <c r="I208" s="86" t="s">
+      <c r="J208" s="83"/>
+      <c r="K208" s="86"/>
+      <c r="L208" s="83" t="s">
         <v>142</v>
       </c>
-      <c r="J208" s="86"/>
-      <c r="K208" s="83"/>
-      <c r="L208" s="86" t="s">
-        <v>143</v>
-      </c>
-      <c r="M208" s="86"/>
-      <c r="N208" s="83"/>
+      <c r="M208" s="83"/>
+      <c r="N208" s="86"/>
       <c r="O208" s="73"/>
     </row>
     <row r="209" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A209" s="43" t="s">
         <v>63</v>
       </c>
-      <c r="C209" s="86">
-        <v>1</v>
-      </c>
-      <c r="D209" s="86"/>
-      <c r="E209" s="83"/>
-      <c r="F209" s="86">
-        <v>1</v>
-      </c>
-      <c r="G209" s="86"/>
-      <c r="H209" s="83"/>
-      <c r="I209" s="86">
-        <v>1</v>
-      </c>
-      <c r="J209" s="86"/>
-      <c r="K209" s="83"/>
-      <c r="L209" s="86">
-        <v>1</v>
-      </c>
-      <c r="M209" s="86"/>
-      <c r="N209" s="83"/>
+      <c r="C209" s="83">
+        <v>1</v>
+      </c>
+      <c r="D209" s="83"/>
+      <c r="E209" s="86"/>
+      <c r="F209" s="83">
+        <v>1</v>
+      </c>
+      <c r="G209" s="83"/>
+      <c r="H209" s="86"/>
+      <c r="I209" s="83">
+        <v>1</v>
+      </c>
+      <c r="J209" s="83"/>
+      <c r="K209" s="86"/>
+      <c r="L209" s="83">
+        <v>1</v>
+      </c>
+      <c r="M209" s="83"/>
+      <c r="N209" s="86"/>
       <c r="O209" s="72"/>
     </row>
     <row r="210" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A210" s="43" t="s">
         <v>64</v>
       </c>
-      <c r="C210" s="83">
+      <c r="C210" s="86">
         <v>0</v>
       </c>
-      <c r="D210" s="83"/>
-      <c r="E210" s="83"/>
-      <c r="F210" s="83">
+      <c r="D210" s="86"/>
+      <c r="E210" s="86"/>
+      <c r="F210" s="86">
         <v>0</v>
       </c>
-      <c r="G210" s="83"/>
-      <c r="H210" s="83"/>
-      <c r="I210" s="83">
+      <c r="G210" s="86"/>
+      <c r="H210" s="86"/>
+      <c r="I210" s="86">
         <v>0</v>
       </c>
-      <c r="J210" s="83"/>
-      <c r="K210" s="83"/>
-      <c r="L210" s="83">
+      <c r="J210" s="86"/>
+      <c r="K210" s="86"/>
+      <c r="L210" s="86">
         <v>0</v>
       </c>
-      <c r="M210" s="83"/>
-      <c r="N210" s="83"/>
+      <c r="M210" s="86"/>
+      <c r="N210" s="86"/>
       <c r="O210" s="72"/>
     </row>
     <row r="211" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A211" s="44" t="s">
         <v>65</v>
       </c>
-      <c r="C211" s="83">
+      <c r="C211" s="86">
         <f>MAX(0, SUM(C$50:E$50)*C214-C210)</f>
         <v>50</v>
       </c>
-      <c r="D211" s="83"/>
-      <c r="E211" s="83"/>
-      <c r="F211" s="83">
+      <c r="D211" s="86"/>
+      <c r="E211" s="86"/>
+      <c r="F211" s="86">
         <f>MAX(0, SUM(F$50:H$50)-F210)</f>
         <v>100</v>
       </c>
-      <c r="G211" s="83"/>
-      <c r="H211" s="83"/>
-      <c r="I211" s="83">
+      <c r="G211" s="86"/>
+      <c r="H211" s="86"/>
+      <c r="I211" s="86">
         <f>MAX(0, SUM(I$50:K$50)-I210)</f>
         <v>100</v>
       </c>
-      <c r="J211" s="83"/>
-      <c r="K211" s="83"/>
-      <c r="L211" s="83">
+      <c r="J211" s="86"/>
+      <c r="K211" s="86"/>
+      <c r="L211" s="86">
         <f>MAX(0, SUM(L$50:N$50)-L210)</f>
         <v>100</v>
       </c>
-      <c r="M211" s="83"/>
-      <c r="N211" s="83"/>
+      <c r="M211" s="86"/>
+      <c r="N211" s="86"/>
       <c r="O211" s="72"/>
       <c r="P211" s="6"/>
       <c r="Q211" s="6"/>
@@ -5250,26 +5253,26 @@
       <c r="A212" s="43" t="s">
         <v>0</v>
       </c>
-      <c r="C212" s="83">
+      <c r="C212" s="86">
         <v>10</v>
       </c>
-      <c r="D212" s="83"/>
-      <c r="E212" s="83"/>
-      <c r="F212" s="83">
+      <c r="D212" s="86"/>
+      <c r="E212" s="86"/>
+      <c r="F212" s="86">
         <v>10</v>
       </c>
-      <c r="G212" s="83"/>
-      <c r="H212" s="83"/>
-      <c r="I212" s="83">
+      <c r="G212" s="86"/>
+      <c r="H212" s="86"/>
+      <c r="I212" s="86">
         <v>10</v>
       </c>
-      <c r="J212" s="83"/>
-      <c r="K212" s="83"/>
-      <c r="L212" s="83">
+      <c r="J212" s="86"/>
+      <c r="K212" s="86"/>
+      <c r="L212" s="86">
         <v>10</v>
       </c>
-      <c r="M212" s="83"/>
-      <c r="N212" s="83"/>
+      <c r="M212" s="86"/>
+      <c r="N212" s="86"/>
       <c r="O212" s="72"/>
       <c r="Q212" s="6"/>
     </row>
@@ -5277,30 +5280,30 @@
       <c r="A213" s="44" t="s">
         <v>66</v>
       </c>
-      <c r="C213" s="83">
+      <c r="C213" s="86">
         <f>IF(C212="Unlimited", C211, MIN(C211, C212))</f>
         <v>10</v>
       </c>
-      <c r="D213" s="83"/>
-      <c r="E213" s="83"/>
-      <c r="F213" s="83">
+      <c r="D213" s="86"/>
+      <c r="E213" s="86"/>
+      <c r="F213" s="86">
         <f>IF(F212="Unlimited", F211, MIN(F211, F212))</f>
         <v>10</v>
       </c>
-      <c r="G213" s="83"/>
-      <c r="H213" s="83"/>
-      <c r="I213" s="83">
+      <c r="G213" s="86"/>
+      <c r="H213" s="86"/>
+      <c r="I213" s="86">
         <f>IF(I212="Unlimited", I211, MIN(I211, I212))</f>
         <v>10</v>
       </c>
-      <c r="J213" s="83"/>
-      <c r="K213" s="83"/>
-      <c r="L213" s="83">
+      <c r="J213" s="86"/>
+      <c r="K213" s="86"/>
+      <c r="L213" s="86">
         <f>IF(L212="Unlimited", L211, MIN(L211, L212))</f>
         <v>10</v>
       </c>
-      <c r="M213" s="83"/>
-      <c r="N213" s="83"/>
+      <c r="M213" s="86"/>
+      <c r="N213" s="86"/>
       <c r="O213" s="72"/>
       <c r="P213" s="6"/>
       <c r="Q213" s="6"/>
@@ -5336,30 +5339,30 @@
       <c r="A215" s="44" t="s">
         <v>72</v>
       </c>
-      <c r="C215" s="83">
+      <c r="C215" s="86">
         <f>C213</f>
         <v>10</v>
       </c>
-      <c r="D215" s="83"/>
-      <c r="E215" s="83"/>
-      <c r="F215" s="83">
+      <c r="D215" s="86"/>
+      <c r="E215" s="86"/>
+      <c r="F215" s="86">
         <f t="shared" ref="F215" si="30">F213</f>
         <v>10</v>
       </c>
-      <c r="G215" s="83"/>
-      <c r="H215" s="83"/>
-      <c r="I215" s="83">
+      <c r="G215" s="86"/>
+      <c r="H215" s="86"/>
+      <c r="I215" s="86">
         <f t="shared" ref="I215" si="31">I213</f>
         <v>10</v>
       </c>
-      <c r="J215" s="83"/>
-      <c r="K215" s="83"/>
-      <c r="L215" s="83">
+      <c r="J215" s="86"/>
+      <c r="K215" s="86"/>
+      <c r="L215" s="86">
         <f t="shared" ref="L215" si="32">L213</f>
         <v>10</v>
       </c>
-      <c r="M215" s="83"/>
-      <c r="N215" s="87"/>
+      <c r="M215" s="86"/>
+      <c r="N215" s="84"/>
       <c r="O215" s="72"/>
     </row>
     <row r="216" spans="1:17" x14ac:dyDescent="0.3">
@@ -5508,7 +5511,7 @@
       </c>
       <c r="B222" s="4"/>
       <c r="D222" s="76" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="H222" s="42"/>
       <c r="K222" s="42"/>
@@ -5518,112 +5521,112 @@
       <c r="A223" s="43" t="s">
         <v>61</v>
       </c>
-      <c r="C223" s="86">
-        <v>1</v>
-      </c>
-      <c r="D223" s="86"/>
-      <c r="E223" s="86"/>
-      <c r="F223" s="86"/>
-      <c r="G223" s="86"/>
-      <c r="H223" s="86"/>
-      <c r="I223" s="86">
-        <v>1</v>
-      </c>
-      <c r="J223" s="86"/>
-      <c r="K223" s="86"/>
-      <c r="L223" s="86"/>
-      <c r="M223" s="86"/>
-      <c r="N223" s="87"/>
+      <c r="C223" s="83">
+        <v>1</v>
+      </c>
+      <c r="D223" s="83"/>
+      <c r="E223" s="83"/>
+      <c r="F223" s="83"/>
+      <c r="G223" s="83"/>
+      <c r="H223" s="83"/>
+      <c r="I223" s="83">
+        <v>1</v>
+      </c>
+      <c r="J223" s="83"/>
+      <c r="K223" s="83"/>
+      <c r="L223" s="83"/>
+      <c r="M223" s="83"/>
+      <c r="N223" s="84"/>
       <c r="O223" s="72"/>
     </row>
     <row r="224" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A224" s="43" t="s">
         <v>62</v>
       </c>
-      <c r="C224" s="86" t="s">
-        <v>139</v>
-      </c>
-      <c r="D224" s="86"/>
-      <c r="E224" s="86"/>
-      <c r="F224" s="86"/>
-      <c r="G224" s="86"/>
-      <c r="H224" s="86"/>
-      <c r="I224" s="86" t="s">
-        <v>144</v>
-      </c>
-      <c r="J224" s="86"/>
-      <c r="K224" s="86"/>
-      <c r="L224" s="86"/>
-      <c r="M224" s="86"/>
-      <c r="N224" s="87"/>
+      <c r="C224" s="83" t="s">
+        <v>138</v>
+      </c>
+      <c r="D224" s="83"/>
+      <c r="E224" s="83"/>
+      <c r="F224" s="83"/>
+      <c r="G224" s="83"/>
+      <c r="H224" s="83"/>
+      <c r="I224" s="83" t="s">
+        <v>143</v>
+      </c>
+      <c r="J224" s="83"/>
+      <c r="K224" s="83"/>
+      <c r="L224" s="83"/>
+      <c r="M224" s="83"/>
+      <c r="N224" s="84"/>
       <c r="O224" s="73"/>
     </row>
     <row r="225" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A225" s="43" t="s">
         <v>63</v>
       </c>
-      <c r="C225" s="86">
-        <v>1</v>
-      </c>
-      <c r="D225" s="86"/>
-      <c r="E225" s="86"/>
-      <c r="F225" s="86"/>
-      <c r="G225" s="86"/>
-      <c r="H225" s="86"/>
-      <c r="I225" s="86">
-        <v>1</v>
-      </c>
-      <c r="J225" s="86"/>
-      <c r="K225" s="86"/>
-      <c r="L225" s="86"/>
-      <c r="M225" s="86"/>
-      <c r="N225" s="86"/>
+      <c r="C225" s="83">
+        <v>1</v>
+      </c>
+      <c r="D225" s="83"/>
+      <c r="E225" s="83"/>
+      <c r="F225" s="83"/>
+      <c r="G225" s="83"/>
+      <c r="H225" s="83"/>
+      <c r="I225" s="83">
+        <v>1</v>
+      </c>
+      <c r="J225" s="83"/>
+      <c r="K225" s="83"/>
+      <c r="L225" s="83"/>
+      <c r="M225" s="83"/>
+      <c r="N225" s="83"/>
       <c r="O225" s="72"/>
     </row>
     <row r="226" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A226" s="43" t="s">
         <v>64</v>
       </c>
-      <c r="C226" s="83">
+      <c r="C226" s="86">
         <v>0</v>
       </c>
-      <c r="D226" s="83"/>
-      <c r="E226" s="83"/>
-      <c r="F226" s="83"/>
-      <c r="G226" s="83"/>
-      <c r="H226" s="83"/>
-      <c r="I226" s="83">
+      <c r="D226" s="86"/>
+      <c r="E226" s="86"/>
+      <c r="F226" s="86"/>
+      <c r="G226" s="86"/>
+      <c r="H226" s="86"/>
+      <c r="I226" s="86">
         <v>0</v>
       </c>
-      <c r="J226" s="83"/>
-      <c r="K226" s="83"/>
-      <c r="L226" s="83"/>
-      <c r="M226" s="83"/>
-      <c r="N226" s="83"/>
+      <c r="J226" s="86"/>
+      <c r="K226" s="86"/>
+      <c r="L226" s="86"/>
+      <c r="M226" s="86"/>
+      <c r="N226" s="86"/>
       <c r="O226" s="72"/>
     </row>
     <row r="227" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A227" s="44" t="s">
         <v>65</v>
       </c>
-      <c r="C227" s="83">
+      <c r="C227" s="86">
         <f>MAX(0, SUM(C$50:H$50)*C230-C226)</f>
         <v>100</v>
       </c>
-      <c r="D227" s="83"/>
-      <c r="E227" s="83"/>
-      <c r="F227" s="83"/>
-      <c r="G227" s="83"/>
-      <c r="H227" s="83"/>
-      <c r="I227" s="83">
+      <c r="D227" s="86"/>
+      <c r="E227" s="86"/>
+      <c r="F227" s="86"/>
+      <c r="G227" s="86"/>
+      <c r="H227" s="86"/>
+      <c r="I227" s="86">
         <f>MAX(0, SUM(I$50:K$50)*I230-I226)</f>
         <v>50</v>
       </c>
-      <c r="J227" s="83"/>
-      <c r="K227" s="83"/>
-      <c r="L227" s="83"/>
-      <c r="M227" s="83"/>
-      <c r="N227" s="83"/>
+      <c r="J227" s="86"/>
+      <c r="K227" s="86"/>
+      <c r="L227" s="86"/>
+      <c r="M227" s="86"/>
+      <c r="N227" s="86"/>
       <c r="O227" s="72"/>
       <c r="P227" s="6"/>
       <c r="Q227" s="6"/>
@@ -5632,22 +5635,22 @@
       <c r="A228" s="43" t="s">
         <v>0</v>
       </c>
-      <c r="C228" s="83">
+      <c r="C228" s="86">
         <v>10</v>
       </c>
-      <c r="D228" s="83"/>
-      <c r="E228" s="83"/>
-      <c r="F228" s="83"/>
-      <c r="G228" s="83"/>
-      <c r="H228" s="83"/>
-      <c r="I228" s="83">
+      <c r="D228" s="86"/>
+      <c r="E228" s="86"/>
+      <c r="F228" s="86"/>
+      <c r="G228" s="86"/>
+      <c r="H228" s="86"/>
+      <c r="I228" s="86">
         <v>10</v>
       </c>
-      <c r="J228" s="83"/>
-      <c r="K228" s="83"/>
-      <c r="L228" s="83"/>
-      <c r="M228" s="83"/>
-      <c r="N228" s="83"/>
+      <c r="J228" s="86"/>
+      <c r="K228" s="86"/>
+      <c r="L228" s="86"/>
+      <c r="M228" s="86"/>
+      <c r="N228" s="86"/>
       <c r="O228" s="72"/>
       <c r="Q228" s="6"/>
     </row>
@@ -5655,24 +5658,24 @@
       <c r="A229" s="44" t="s">
         <v>66</v>
       </c>
-      <c r="C229" s="83">
+      <c r="C229" s="86">
         <f>IF(C228="Unlimited", C227, MIN(C227, C228))</f>
         <v>10</v>
       </c>
-      <c r="D229" s="83"/>
-      <c r="E229" s="83"/>
-      <c r="F229" s="83"/>
-      <c r="G229" s="83"/>
-      <c r="H229" s="83"/>
-      <c r="I229" s="83">
+      <c r="D229" s="86"/>
+      <c r="E229" s="86"/>
+      <c r="F229" s="86"/>
+      <c r="G229" s="86"/>
+      <c r="H229" s="86"/>
+      <c r="I229" s="86">
         <f>IF(I228="Unlimited", I227, MIN(I227, I228))</f>
         <v>10</v>
       </c>
-      <c r="J229" s="83"/>
-      <c r="K229" s="83"/>
-      <c r="L229" s="83"/>
-      <c r="M229" s="83"/>
-      <c r="N229" s="83"/>
+      <c r="J229" s="86"/>
+      <c r="K229" s="86"/>
+      <c r="L229" s="86"/>
+      <c r="M229" s="86"/>
+      <c r="N229" s="86"/>
       <c r="O229" s="72"/>
       <c r="P229" s="6"/>
       <c r="Q229" s="6"/>
@@ -5704,24 +5707,24 @@
       <c r="A231" s="44" t="s">
         <v>72</v>
       </c>
-      <c r="C231" s="83">
+      <c r="C231" s="86">
         <f>C229</f>
         <v>10</v>
       </c>
-      <c r="D231" s="83"/>
-      <c r="E231" s="83"/>
-      <c r="F231" s="83"/>
-      <c r="G231" s="83"/>
-      <c r="H231" s="83"/>
-      <c r="I231" s="83">
+      <c r="D231" s="86"/>
+      <c r="E231" s="86"/>
+      <c r="F231" s="86"/>
+      <c r="G231" s="86"/>
+      <c r="H231" s="86"/>
+      <c r="I231" s="86">
         <f>I229</f>
         <v>10</v>
       </c>
-      <c r="J231" s="83"/>
-      <c r="K231" s="83"/>
-      <c r="L231" s="83"/>
-      <c r="M231" s="83"/>
-      <c r="N231" s="83"/>
+      <c r="J231" s="86"/>
+      <c r="K231" s="86"/>
+      <c r="L231" s="86"/>
+      <c r="M231" s="86"/>
+      <c r="N231" s="86"/>
       <c r="O231" s="72"/>
     </row>
     <row r="232" spans="1:17" x14ac:dyDescent="0.3">
@@ -5752,7 +5755,7 @@
     </row>
     <row r="235" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A235" s="44" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C235" s="52">
         <f>$C$231*C$50/SUM($C$50:$H$50)</f>
@@ -5870,7 +5873,7 @@
       </c>
       <c r="B238" s="4"/>
       <c r="D238" s="76" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="H238" s="42"/>
       <c r="K238" s="42"/>
@@ -5880,112 +5883,112 @@
       <c r="A239" s="43" t="s">
         <v>61</v>
       </c>
-      <c r="C239" s="86">
-        <v>1</v>
-      </c>
-      <c r="D239" s="86"/>
-      <c r="E239" s="86"/>
-      <c r="F239" s="86"/>
-      <c r="G239" s="86"/>
-      <c r="H239" s="86"/>
-      <c r="I239" s="86">
-        <v>1</v>
-      </c>
-      <c r="J239" s="86"/>
-      <c r="K239" s="86"/>
-      <c r="L239" s="86"/>
-      <c r="M239" s="86"/>
-      <c r="N239" s="87"/>
+      <c r="C239" s="83">
+        <v>1</v>
+      </c>
+      <c r="D239" s="83"/>
+      <c r="E239" s="83"/>
+      <c r="F239" s="83"/>
+      <c r="G239" s="83"/>
+      <c r="H239" s="83"/>
+      <c r="I239" s="83">
+        <v>1</v>
+      </c>
+      <c r="J239" s="83"/>
+      <c r="K239" s="83"/>
+      <c r="L239" s="83"/>
+      <c r="M239" s="83"/>
+      <c r="N239" s="84"/>
       <c r="O239" s="72"/>
     </row>
     <row r="240" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A240" s="43" t="s">
         <v>62</v>
       </c>
-      <c r="C240" s="86" t="s">
+      <c r="C240" s="83" t="s">
+        <v>146</v>
+      </c>
+      <c r="D240" s="83"/>
+      <c r="E240" s="83"/>
+      <c r="F240" s="83"/>
+      <c r="G240" s="83"/>
+      <c r="H240" s="83"/>
+      <c r="I240" s="83" t="s">
         <v>147</v>
       </c>
-      <c r="D240" s="86"/>
-      <c r="E240" s="86"/>
-      <c r="F240" s="86"/>
-      <c r="G240" s="86"/>
-      <c r="H240" s="86"/>
-      <c r="I240" s="86" t="s">
-        <v>148</v>
-      </c>
-      <c r="J240" s="86"/>
-      <c r="K240" s="86"/>
-      <c r="L240" s="86"/>
-      <c r="M240" s="86"/>
-      <c r="N240" s="87"/>
+      <c r="J240" s="83"/>
+      <c r="K240" s="83"/>
+      <c r="L240" s="83"/>
+      <c r="M240" s="83"/>
+      <c r="N240" s="84"/>
       <c r="O240" s="73"/>
     </row>
     <row r="241" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A241" s="43" t="s">
         <v>63</v>
       </c>
-      <c r="C241" s="86">
-        <v>1</v>
-      </c>
-      <c r="D241" s="86"/>
-      <c r="E241" s="86"/>
-      <c r="F241" s="86"/>
-      <c r="G241" s="86"/>
-      <c r="H241" s="86"/>
-      <c r="I241" s="86">
-        <v>1</v>
-      </c>
-      <c r="J241" s="86"/>
-      <c r="K241" s="86"/>
-      <c r="L241" s="86"/>
-      <c r="M241" s="86"/>
-      <c r="N241" s="86"/>
+      <c r="C241" s="83">
+        <v>1</v>
+      </c>
+      <c r="D241" s="83"/>
+      <c r="E241" s="83"/>
+      <c r="F241" s="83"/>
+      <c r="G241" s="83"/>
+      <c r="H241" s="83"/>
+      <c r="I241" s="83">
+        <v>1</v>
+      </c>
+      <c r="J241" s="83"/>
+      <c r="K241" s="83"/>
+      <c r="L241" s="83"/>
+      <c r="M241" s="83"/>
+      <c r="N241" s="83"/>
       <c r="O241" s="72"/>
     </row>
     <row r="242" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A242" s="43" t="s">
         <v>64</v>
       </c>
-      <c r="C242" s="83">
+      <c r="C242" s="86">
         <v>0</v>
       </c>
-      <c r="D242" s="83"/>
-      <c r="E242" s="83"/>
-      <c r="F242" s="83"/>
-      <c r="G242" s="83"/>
-      <c r="H242" s="83"/>
-      <c r="I242" s="83">
+      <c r="D242" s="86"/>
+      <c r="E242" s="86"/>
+      <c r="F242" s="86"/>
+      <c r="G242" s="86"/>
+      <c r="H242" s="86"/>
+      <c r="I242" s="86">
         <v>0</v>
       </c>
-      <c r="J242" s="83"/>
-      <c r="K242" s="83"/>
-      <c r="L242" s="83"/>
-      <c r="M242" s="83"/>
-      <c r="N242" s="83"/>
+      <c r="J242" s="86"/>
+      <c r="K242" s="86"/>
+      <c r="L242" s="86"/>
+      <c r="M242" s="86"/>
+      <c r="N242" s="86"/>
       <c r="O242" s="72"/>
     </row>
     <row r="243" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A243" s="44" t="s">
         <v>65</v>
       </c>
-      <c r="C243" s="83">
+      <c r="C243" s="86">
         <f>MAX(0, SUM(C$50:H$50)*C246-C242)</f>
         <v>100</v>
       </c>
-      <c r="D243" s="83"/>
-      <c r="E243" s="83"/>
-      <c r="F243" s="83"/>
-      <c r="G243" s="83"/>
-      <c r="H243" s="83"/>
-      <c r="I243" s="83">
+      <c r="D243" s="86"/>
+      <c r="E243" s="86"/>
+      <c r="F243" s="86"/>
+      <c r="G243" s="86"/>
+      <c r="H243" s="86"/>
+      <c r="I243" s="86">
         <f>MAX(0, SUM(I$50:K$50)*I246-I242)</f>
         <v>50</v>
       </c>
-      <c r="J243" s="83"/>
-      <c r="K243" s="83"/>
-      <c r="L243" s="83"/>
-      <c r="M243" s="83"/>
-      <c r="N243" s="83"/>
+      <c r="J243" s="86"/>
+      <c r="K243" s="86"/>
+      <c r="L243" s="86"/>
+      <c r="M243" s="86"/>
+      <c r="N243" s="86"/>
       <c r="O243" s="72"/>
       <c r="P243" s="6"/>
       <c r="Q243" s="6"/>
@@ -5994,22 +5997,22 @@
       <c r="A244" s="43" t="s">
         <v>0</v>
       </c>
-      <c r="C244" s="83">
+      <c r="C244" s="86">
         <v>10</v>
       </c>
-      <c r="D244" s="83"/>
-      <c r="E244" s="83"/>
-      <c r="F244" s="83"/>
-      <c r="G244" s="83"/>
-      <c r="H244" s="83"/>
-      <c r="I244" s="83">
+      <c r="D244" s="86"/>
+      <c r="E244" s="86"/>
+      <c r="F244" s="86"/>
+      <c r="G244" s="86"/>
+      <c r="H244" s="86"/>
+      <c r="I244" s="86">
         <v>10</v>
       </c>
-      <c r="J244" s="83"/>
-      <c r="K244" s="83"/>
-      <c r="L244" s="83"/>
-      <c r="M244" s="83"/>
-      <c r="N244" s="83"/>
+      <c r="J244" s="86"/>
+      <c r="K244" s="86"/>
+      <c r="L244" s="86"/>
+      <c r="M244" s="86"/>
+      <c r="N244" s="86"/>
       <c r="O244" s="72"/>
       <c r="Q244" s="6"/>
     </row>
@@ -6017,24 +6020,24 @@
       <c r="A245" s="44" t="s">
         <v>66</v>
       </c>
-      <c r="C245" s="83">
+      <c r="C245" s="86">
         <f>IF(C244="Unlimited", C243, MIN(C243, C244))</f>
         <v>10</v>
       </c>
-      <c r="D245" s="83"/>
-      <c r="E245" s="83"/>
-      <c r="F245" s="83"/>
-      <c r="G245" s="83"/>
-      <c r="H245" s="83"/>
-      <c r="I245" s="83">
+      <c r="D245" s="86"/>
+      <c r="E245" s="86"/>
+      <c r="F245" s="86"/>
+      <c r="G245" s="86"/>
+      <c r="H245" s="86"/>
+      <c r="I245" s="86">
         <f>IF(I244="Unlimited", I243, MIN(I243, I244))</f>
         <v>10</v>
       </c>
-      <c r="J245" s="83"/>
-      <c r="K245" s="83"/>
-      <c r="L245" s="83"/>
-      <c r="M245" s="83"/>
-      <c r="N245" s="83"/>
+      <c r="J245" s="86"/>
+      <c r="K245" s="86"/>
+      <c r="L245" s="86"/>
+      <c r="M245" s="86"/>
+      <c r="N245" s="86"/>
       <c r="O245" s="72"/>
       <c r="P245" s="6"/>
       <c r="Q245" s="6"/>
@@ -6066,24 +6069,24 @@
       <c r="A247" s="44" t="s">
         <v>72</v>
       </c>
-      <c r="C247" s="83">
+      <c r="C247" s="86">
         <f>C245</f>
         <v>10</v>
       </c>
-      <c r="D247" s="83"/>
-      <c r="E247" s="83"/>
-      <c r="F247" s="83"/>
-      <c r="G247" s="83"/>
-      <c r="H247" s="83"/>
-      <c r="I247" s="83">
+      <c r="D247" s="86"/>
+      <c r="E247" s="86"/>
+      <c r="F247" s="86"/>
+      <c r="G247" s="86"/>
+      <c r="H247" s="86"/>
+      <c r="I247" s="86">
         <f>I245</f>
         <v>10</v>
       </c>
-      <c r="J247" s="83"/>
-      <c r="K247" s="83"/>
-      <c r="L247" s="83"/>
-      <c r="M247" s="83"/>
-      <c r="N247" s="83"/>
+      <c r="J247" s="86"/>
+      <c r="K247" s="86"/>
+      <c r="L247" s="86"/>
+      <c r="M247" s="86"/>
+      <c r="N247" s="86"/>
       <c r="O247" s="72"/>
     </row>
     <row r="248" spans="1:17" x14ac:dyDescent="0.3">
@@ -6114,7 +6117,7 @@
     </row>
     <row r="251" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A251" s="44" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C251" s="52">
         <f>$C$247*C$50/SUM($C$50:$H$50)</f>
@@ -6228,11 +6231,11 @@
     </row>
     <row r="254" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A254" s="65" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B254" s="4"/>
       <c r="C254" s="78" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="D254" s="76"/>
       <c r="H254" s="42"/>
@@ -6258,10 +6261,10 @@
       </c>
       <c r="N256" s="40"/>
       <c r="O256" s="50" t="s">
+        <v>148</v>
+      </c>
+      <c r="P256" s="50" t="s">
         <v>149</v>
-      </c>
-      <c r="P256" s="50" t="s">
-        <v>150</v>
       </c>
     </row>
     <row r="257" spans="1:17" x14ac:dyDescent="0.3">
@@ -6557,11 +6560,11 @@
     </row>
     <row r="271" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A271" s="65" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B271" s="4"/>
       <c r="C271" s="78" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="D271" s="76"/>
       <c r="H271" s="42"/>
@@ -6584,7 +6587,7 @@
       </c>
       <c r="N273" s="40"/>
       <c r="O273" s="50" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="P273" s="50"/>
     </row>
@@ -6819,7 +6822,7 @@
       </c>
       <c r="B288" s="4"/>
       <c r="C288" s="78" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="N288" s="40"/>
       <c r="O288" s="2">
@@ -6832,7 +6835,7 @@
       </c>
       <c r="N289" s="40"/>
       <c r="O289" s="50" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="P289" s="50"/>
     </row>
@@ -7064,7 +7067,7 @@
       </c>
       <c r="B304" s="4"/>
       <c r="D304" s="76" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="H304" s="42"/>
       <c r="K304" s="42"/>
@@ -7074,134 +7077,134 @@
       <c r="A305" s="43" t="s">
         <v>61</v>
       </c>
-      <c r="C305" s="86">
-        <v>1</v>
-      </c>
-      <c r="D305" s="86"/>
-      <c r="E305" s="83"/>
-      <c r="F305" s="86">
-        <v>1</v>
-      </c>
-      <c r="G305" s="86"/>
-      <c r="H305" s="83"/>
-      <c r="I305" s="86">
-        <v>1</v>
-      </c>
-      <c r="J305" s="86"/>
-      <c r="K305" s="83"/>
-      <c r="L305" s="86">
-        <v>1</v>
-      </c>
-      <c r="M305" s="86"/>
-      <c r="N305" s="83"/>
+      <c r="C305" s="83">
+        <v>1</v>
+      </c>
+      <c r="D305" s="83"/>
+      <c r="E305" s="86"/>
+      <c r="F305" s="83">
+        <v>1</v>
+      </c>
+      <c r="G305" s="83"/>
+      <c r="H305" s="86"/>
+      <c r="I305" s="83">
+        <v>1</v>
+      </c>
+      <c r="J305" s="83"/>
+      <c r="K305" s="86"/>
+      <c r="L305" s="83">
+        <v>1</v>
+      </c>
+      <c r="M305" s="83"/>
+      <c r="N305" s="86"/>
       <c r="O305" s="72"/>
     </row>
     <row r="306" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A306" s="43" t="s">
         <v>62</v>
       </c>
-      <c r="C306" s="86" t="s">
+      <c r="C306" s="83" t="s">
+        <v>139</v>
+      </c>
+      <c r="D306" s="83"/>
+      <c r="E306" s="86"/>
+      <c r="F306" s="83" t="s">
         <v>140</v>
       </c>
-      <c r="D306" s="86"/>
-      <c r="E306" s="83"/>
-      <c r="F306" s="86" t="s">
+      <c r="G306" s="83"/>
+      <c r="H306" s="86"/>
+      <c r="I306" s="83" t="s">
         <v>141</v>
       </c>
-      <c r="G306" s="86"/>
-      <c r="H306" s="83"/>
-      <c r="I306" s="86" t="s">
+      <c r="J306" s="83"/>
+      <c r="K306" s="86"/>
+      <c r="L306" s="83" t="s">
         <v>142</v>
       </c>
-      <c r="J306" s="86"/>
-      <c r="K306" s="83"/>
-      <c r="L306" s="86" t="s">
-        <v>143</v>
-      </c>
-      <c r="M306" s="86"/>
-      <c r="N306" s="83"/>
+      <c r="M306" s="83"/>
+      <c r="N306" s="86"/>
       <c r="O306" s="73"/>
     </row>
     <row r="307" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A307" s="43" t="s">
         <v>63</v>
       </c>
-      <c r="C307" s="86">
-        <v>1</v>
-      </c>
-      <c r="D307" s="86"/>
-      <c r="E307" s="83"/>
-      <c r="F307" s="86">
-        <v>1</v>
-      </c>
-      <c r="G307" s="86"/>
-      <c r="H307" s="83"/>
-      <c r="I307" s="86">
-        <v>1</v>
-      </c>
-      <c r="J307" s="86"/>
-      <c r="K307" s="83"/>
-      <c r="L307" s="86">
-        <v>1</v>
-      </c>
-      <c r="M307" s="86"/>
-      <c r="N307" s="83"/>
+      <c r="C307" s="83">
+        <v>1</v>
+      </c>
+      <c r="D307" s="83"/>
+      <c r="E307" s="86"/>
+      <c r="F307" s="83">
+        <v>1</v>
+      </c>
+      <c r="G307" s="83"/>
+      <c r="H307" s="86"/>
+      <c r="I307" s="83">
+        <v>1</v>
+      </c>
+      <c r="J307" s="83"/>
+      <c r="K307" s="86"/>
+      <c r="L307" s="83">
+        <v>1</v>
+      </c>
+      <c r="M307" s="83"/>
+      <c r="N307" s="86"/>
       <c r="O307" s="72"/>
     </row>
     <row r="308" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A308" s="43" t="s">
         <v>64</v>
       </c>
-      <c r="C308" s="83">
+      <c r="C308" s="86">
         <v>0</v>
       </c>
-      <c r="D308" s="83"/>
-      <c r="E308" s="83"/>
-      <c r="F308" s="83">
+      <c r="D308" s="86"/>
+      <c r="E308" s="86"/>
+      <c r="F308" s="86">
         <v>0</v>
       </c>
-      <c r="G308" s="83"/>
-      <c r="H308" s="83"/>
-      <c r="I308" s="83">
+      <c r="G308" s="86"/>
+      <c r="H308" s="86"/>
+      <c r="I308" s="86">
         <v>0</v>
       </c>
-      <c r="J308" s="83"/>
-      <c r="K308" s="83"/>
-      <c r="L308" s="83">
+      <c r="J308" s="86"/>
+      <c r="K308" s="86"/>
+      <c r="L308" s="86">
         <v>0</v>
       </c>
-      <c r="M308" s="83"/>
-      <c r="N308" s="83"/>
+      <c r="M308" s="86"/>
+      <c r="N308" s="86"/>
       <c r="O308" s="72"/>
     </row>
     <row r="309" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A309" s="44" t="s">
         <v>65</v>
       </c>
-      <c r="C309" s="83">
+      <c r="C309" s="86">
         <f>MAX(0, SUM(C$50:E$50))</f>
         <v>100</v>
       </c>
-      <c r="D309" s="83"/>
-      <c r="E309" s="83"/>
-      <c r="F309" s="83">
+      <c r="D309" s="86"/>
+      <c r="E309" s="86"/>
+      <c r="F309" s="86">
         <f>MAX(0, SUM(F$50:H$50))</f>
         <v>100</v>
       </c>
-      <c r="G309" s="83"/>
-      <c r="H309" s="83"/>
-      <c r="I309" s="83">
+      <c r="G309" s="86"/>
+      <c r="H309" s="86"/>
+      <c r="I309" s="86">
         <f>MAX(0, SUM(I$50:K$50))</f>
         <v>100</v>
       </c>
-      <c r="J309" s="83"/>
-      <c r="K309" s="83"/>
-      <c r="L309" s="83">
+      <c r="J309" s="86"/>
+      <c r="K309" s="86"/>
+      <c r="L309" s="86">
         <f>MAX(0, SUM(L$50:N$50))</f>
         <v>100</v>
       </c>
-      <c r="M309" s="83"/>
-      <c r="N309" s="83"/>
+      <c r="M309" s="86"/>
+      <c r="N309" s="86"/>
       <c r="O309" s="72"/>
       <c r="P309" s="6"/>
       <c r="Q309" s="6"/>
@@ -7210,26 +7213,26 @@
       <c r="A310" s="43" t="s">
         <v>0</v>
       </c>
-      <c r="C310" s="83">
+      <c r="C310" s="86">
         <v>0</v>
       </c>
-      <c r="D310" s="83"/>
-      <c r="E310" s="83"/>
-      <c r="F310" s="83">
+      <c r="D310" s="86"/>
+      <c r="E310" s="86"/>
+      <c r="F310" s="86">
         <v>0</v>
       </c>
-      <c r="G310" s="83"/>
-      <c r="H310" s="83"/>
-      <c r="I310" s="83">
+      <c r="G310" s="86"/>
+      <c r="H310" s="86"/>
+      <c r="I310" s="86">
         <v>0</v>
       </c>
-      <c r="J310" s="83"/>
-      <c r="K310" s="83"/>
-      <c r="L310" s="83">
+      <c r="J310" s="86"/>
+      <c r="K310" s="86"/>
+      <c r="L310" s="86">
         <v>0</v>
       </c>
-      <c r="M310" s="83"/>
-      <c r="N310" s="83"/>
+      <c r="M310" s="86"/>
+      <c r="N310" s="86"/>
       <c r="O310" s="72"/>
       <c r="Q310" s="6"/>
     </row>
@@ -7237,30 +7240,30 @@
       <c r="A311" s="44" t="s">
         <v>66</v>
       </c>
-      <c r="C311" s="83">
+      <c r="C311" s="86">
         <f>C309</f>
         <v>100</v>
       </c>
-      <c r="D311" s="83"/>
-      <c r="E311" s="83"/>
-      <c r="F311" s="83">
+      <c r="D311" s="86"/>
+      <c r="E311" s="86"/>
+      <c r="F311" s="86">
         <f>F309</f>
         <v>100</v>
       </c>
-      <c r="G311" s="83"/>
-      <c r="H311" s="83"/>
-      <c r="I311" s="83">
+      <c r="G311" s="86"/>
+      <c r="H311" s="86"/>
+      <c r="I311" s="86">
         <f>I309</f>
         <v>100</v>
       </c>
-      <c r="J311" s="83"/>
-      <c r="K311" s="83"/>
-      <c r="L311" s="83">
+      <c r="J311" s="86"/>
+      <c r="K311" s="86"/>
+      <c r="L311" s="86">
         <f>L309</f>
         <v>100</v>
       </c>
-      <c r="M311" s="83"/>
-      <c r="N311" s="83"/>
+      <c r="M311" s="86"/>
+      <c r="N311" s="86"/>
       <c r="O311" s="72"/>
       <c r="P311" s="6"/>
       <c r="Q311" s="6"/>
@@ -7288,7 +7291,7 @@
         <v>0.1</v>
       </c>
       <c r="M312" s="85"/>
-      <c r="N312" s="98"/>
+      <c r="N312" s="87"/>
       <c r="O312" s="74"/>
       <c r="Q312" s="6"/>
     </row>
@@ -7296,30 +7299,30 @@
       <c r="A313" s="44" t="s">
         <v>72</v>
       </c>
-      <c r="C313" s="83">
+      <c r="C313" s="86">
         <f>C312*C311</f>
         <v>10</v>
       </c>
-      <c r="D313" s="83"/>
-      <c r="E313" s="83"/>
-      <c r="F313" s="83">
+      <c r="D313" s="86"/>
+      <c r="E313" s="86"/>
+      <c r="F313" s="86">
         <f t="shared" ref="F313" si="47">F312*F311</f>
         <v>10</v>
       </c>
-      <c r="G313" s="83"/>
-      <c r="H313" s="83"/>
-      <c r="I313" s="83">
+      <c r="G313" s="86"/>
+      <c r="H313" s="86"/>
+      <c r="I313" s="86">
         <f t="shared" ref="I313" si="48">I312*I311</f>
         <v>10</v>
       </c>
-      <c r="J313" s="83"/>
-      <c r="K313" s="83"/>
-      <c r="L313" s="83">
+      <c r="J313" s="86"/>
+      <c r="K313" s="86"/>
+      <c r="L313" s="86">
         <f t="shared" ref="L313" si="49">L312*L311</f>
         <v>10</v>
       </c>
-      <c r="M313" s="83"/>
-      <c r="N313" s="87"/>
+      <c r="M313" s="86"/>
+      <c r="N313" s="84"/>
       <c r="O313" s="72"/>
     </row>
     <row r="314" spans="1:17" x14ac:dyDescent="0.3">
@@ -7468,7 +7471,7 @@
       </c>
       <c r="B320" s="4"/>
       <c r="D320" s="76" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="H320" s="42"/>
       <c r="K320" s="42"/>
@@ -7478,112 +7481,112 @@
       <c r="A321" s="43" t="s">
         <v>61</v>
       </c>
-      <c r="C321" s="86">
-        <v>1</v>
-      </c>
-      <c r="D321" s="86"/>
-      <c r="E321" s="86"/>
-      <c r="F321" s="86"/>
-      <c r="G321" s="86"/>
-      <c r="H321" s="86"/>
-      <c r="I321" s="86">
-        <v>1</v>
-      </c>
-      <c r="J321" s="86"/>
-      <c r="K321" s="86"/>
-      <c r="L321" s="86"/>
-      <c r="M321" s="86"/>
-      <c r="N321" s="87"/>
+      <c r="C321" s="83">
+        <v>1</v>
+      </c>
+      <c r="D321" s="83"/>
+      <c r="E321" s="83"/>
+      <c r="F321" s="83"/>
+      <c r="G321" s="83"/>
+      <c r="H321" s="83"/>
+      <c r="I321" s="83">
+        <v>1</v>
+      </c>
+      <c r="J321" s="83"/>
+      <c r="K321" s="83"/>
+      <c r="L321" s="83"/>
+      <c r="M321" s="83"/>
+      <c r="N321" s="84"/>
       <c r="O321" s="72"/>
     </row>
     <row r="322" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A322" s="43" t="s">
         <v>62</v>
       </c>
-      <c r="C322" s="86" t="s">
-        <v>139</v>
-      </c>
-      <c r="D322" s="86"/>
-      <c r="E322" s="86"/>
-      <c r="F322" s="86"/>
-      <c r="G322" s="86"/>
-      <c r="H322" s="86"/>
-      <c r="I322" s="86" t="s">
-        <v>144</v>
-      </c>
-      <c r="J322" s="86"/>
-      <c r="K322" s="86"/>
-      <c r="L322" s="86"/>
-      <c r="M322" s="86"/>
-      <c r="N322" s="87"/>
+      <c r="C322" s="83" t="s">
+        <v>138</v>
+      </c>
+      <c r="D322" s="83"/>
+      <c r="E322" s="83"/>
+      <c r="F322" s="83"/>
+      <c r="G322" s="83"/>
+      <c r="H322" s="83"/>
+      <c r="I322" s="83" t="s">
+        <v>143</v>
+      </c>
+      <c r="J322" s="83"/>
+      <c r="K322" s="83"/>
+      <c r="L322" s="83"/>
+      <c r="M322" s="83"/>
+      <c r="N322" s="84"/>
       <c r="O322" s="73"/>
     </row>
     <row r="323" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A323" s="43" t="s">
         <v>63</v>
       </c>
-      <c r="C323" s="86">
-        <v>1</v>
-      </c>
-      <c r="D323" s="86"/>
-      <c r="E323" s="86"/>
-      <c r="F323" s="86"/>
-      <c r="G323" s="86"/>
-      <c r="H323" s="86"/>
-      <c r="I323" s="86">
-        <v>1</v>
-      </c>
-      <c r="J323" s="86"/>
-      <c r="K323" s="86"/>
-      <c r="L323" s="86"/>
-      <c r="M323" s="86"/>
-      <c r="N323" s="86"/>
+      <c r="C323" s="83">
+        <v>1</v>
+      </c>
+      <c r="D323" s="83"/>
+      <c r="E323" s="83"/>
+      <c r="F323" s="83"/>
+      <c r="G323" s="83"/>
+      <c r="H323" s="83"/>
+      <c r="I323" s="83">
+        <v>1</v>
+      </c>
+      <c r="J323" s="83"/>
+      <c r="K323" s="83"/>
+      <c r="L323" s="83"/>
+      <c r="M323" s="83"/>
+      <c r="N323" s="83"/>
       <c r="O323" s="72"/>
     </row>
     <row r="324" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A324" s="43" t="s">
         <v>64</v>
       </c>
-      <c r="C324" s="83">
+      <c r="C324" s="86">
         <v>0</v>
       </c>
-      <c r="D324" s="83"/>
-      <c r="E324" s="83"/>
-      <c r="F324" s="83"/>
-      <c r="G324" s="83"/>
-      <c r="H324" s="83"/>
-      <c r="I324" s="83">
+      <c r="D324" s="86"/>
+      <c r="E324" s="86"/>
+      <c r="F324" s="86"/>
+      <c r="G324" s="86"/>
+      <c r="H324" s="86"/>
+      <c r="I324" s="86">
         <v>0</v>
       </c>
-      <c r="J324" s="83"/>
-      <c r="K324" s="83"/>
-      <c r="L324" s="83"/>
-      <c r="M324" s="83"/>
-      <c r="N324" s="83"/>
+      <c r="J324" s="86"/>
+      <c r="K324" s="86"/>
+      <c r="L324" s="86"/>
+      <c r="M324" s="86"/>
+      <c r="N324" s="86"/>
       <c r="O324" s="72"/>
     </row>
     <row r="325" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A325" s="44" t="s">
         <v>65</v>
       </c>
-      <c r="C325" s="83">
+      <c r="C325" s="86">
         <f>MAX(0, SUM(C$50:H$50))</f>
         <v>200</v>
       </c>
-      <c r="D325" s="83"/>
-      <c r="E325" s="83"/>
-      <c r="F325" s="83"/>
-      <c r="G325" s="83"/>
-      <c r="H325" s="83"/>
-      <c r="I325" s="83">
+      <c r="D325" s="86"/>
+      <c r="E325" s="86"/>
+      <c r="F325" s="86"/>
+      <c r="G325" s="86"/>
+      <c r="H325" s="86"/>
+      <c r="I325" s="86">
         <f>MAX(0, SUM(I$50:N$50))</f>
         <v>200</v>
       </c>
-      <c r="J325" s="83"/>
-      <c r="K325" s="83"/>
-      <c r="L325" s="83"/>
-      <c r="M325" s="83"/>
-      <c r="N325" s="83"/>
+      <c r="J325" s="86"/>
+      <c r="K325" s="86"/>
+      <c r="L325" s="86"/>
+      <c r="M325" s="86"/>
+      <c r="N325" s="86"/>
       <c r="O325" s="72"/>
       <c r="P325" s="6"/>
       <c r="Q325" s="6"/>
@@ -7592,22 +7595,22 @@
       <c r="A326" s="43" t="s">
         <v>0</v>
       </c>
-      <c r="C326" s="83">
+      <c r="C326" s="86">
         <v>0</v>
       </c>
-      <c r="D326" s="83"/>
-      <c r="E326" s="83"/>
-      <c r="F326" s="83"/>
-      <c r="G326" s="83"/>
-      <c r="H326" s="83"/>
-      <c r="I326" s="83">
+      <c r="D326" s="86"/>
+      <c r="E326" s="86"/>
+      <c r="F326" s="86"/>
+      <c r="G326" s="86"/>
+      <c r="H326" s="86"/>
+      <c r="I326" s="86">
         <v>0</v>
       </c>
-      <c r="J326" s="83"/>
-      <c r="K326" s="83"/>
-      <c r="L326" s="83"/>
-      <c r="M326" s="83"/>
-      <c r="N326" s="83"/>
+      <c r="J326" s="86"/>
+      <c r="K326" s="86"/>
+      <c r="L326" s="86"/>
+      <c r="M326" s="86"/>
+      <c r="N326" s="86"/>
       <c r="O326" s="72"/>
       <c r="Q326" s="6"/>
     </row>
@@ -7615,24 +7618,24 @@
       <c r="A327" s="44" t="s">
         <v>66</v>
       </c>
-      <c r="C327" s="83">
+      <c r="C327" s="86">
         <f>IF(C326=0, C325, MIN(C325, C326))</f>
         <v>200</v>
       </c>
-      <c r="D327" s="83"/>
-      <c r="E327" s="83"/>
-      <c r="F327" s="83"/>
-      <c r="G327" s="83"/>
-      <c r="H327" s="83"/>
-      <c r="I327" s="83">
+      <c r="D327" s="86"/>
+      <c r="E327" s="86"/>
+      <c r="F327" s="86"/>
+      <c r="G327" s="86"/>
+      <c r="H327" s="86"/>
+      <c r="I327" s="86">
         <f>IF(I326=0, I325, MIN(I325, I326))</f>
         <v>200</v>
       </c>
-      <c r="J327" s="83"/>
-      <c r="K327" s="83"/>
-      <c r="L327" s="83"/>
-      <c r="M327" s="83"/>
-      <c r="N327" s="83"/>
+      <c r="J327" s="86"/>
+      <c r="K327" s="86"/>
+      <c r="L327" s="86"/>
+      <c r="M327" s="86"/>
+      <c r="N327" s="86"/>
       <c r="O327" s="72"/>
       <c r="P327" s="6"/>
       <c r="Q327" s="6"/>
@@ -7664,24 +7667,24 @@
       <c r="A329" s="44" t="s">
         <v>72</v>
       </c>
-      <c r="C329" s="83">
+      <c r="C329" s="86">
         <f>C327*C328</f>
         <v>20</v>
       </c>
-      <c r="D329" s="83"/>
-      <c r="E329" s="83"/>
-      <c r="F329" s="83"/>
-      <c r="G329" s="83"/>
-      <c r="H329" s="83"/>
-      <c r="I329" s="83">
+      <c r="D329" s="86"/>
+      <c r="E329" s="86"/>
+      <c r="F329" s="86"/>
+      <c r="G329" s="86"/>
+      <c r="H329" s="86"/>
+      <c r="I329" s="86">
         <f>I327*I328</f>
         <v>20</v>
       </c>
-      <c r="J329" s="83"/>
-      <c r="K329" s="83"/>
-      <c r="L329" s="83"/>
-      <c r="M329" s="83"/>
-      <c r="N329" s="83"/>
+      <c r="J329" s="86"/>
+      <c r="K329" s="86"/>
+      <c r="L329" s="86"/>
+      <c r="M329" s="86"/>
+      <c r="N329" s="86"/>
       <c r="O329" s="72"/>
     </row>
     <row r="330" spans="1:17" x14ac:dyDescent="0.3">
@@ -7712,7 +7715,7 @@
     </row>
     <row r="333" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A333" s="44" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C333" s="52">
         <f>$C$329*C$50/SUM($C$50:$H$50)</f>
@@ -7830,7 +7833,7 @@
       </c>
       <c r="B336" s="4"/>
       <c r="D336" s="76" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="H336" s="42"/>
       <c r="K336" s="42"/>
@@ -7840,112 +7843,112 @@
       <c r="A337" s="43" t="s">
         <v>61</v>
       </c>
-      <c r="C337" s="86">
-        <v>1</v>
-      </c>
-      <c r="D337" s="86"/>
-      <c r="E337" s="86"/>
-      <c r="F337" s="86"/>
-      <c r="G337" s="86"/>
-      <c r="H337" s="86"/>
-      <c r="I337" s="86">
-        <v>1</v>
-      </c>
-      <c r="J337" s="86"/>
-      <c r="K337" s="86"/>
-      <c r="L337" s="86"/>
-      <c r="M337" s="86"/>
-      <c r="N337" s="87"/>
+      <c r="C337" s="83">
+        <v>1</v>
+      </c>
+      <c r="D337" s="83"/>
+      <c r="E337" s="83"/>
+      <c r="F337" s="83"/>
+      <c r="G337" s="83"/>
+      <c r="H337" s="83"/>
+      <c r="I337" s="83">
+        <v>1</v>
+      </c>
+      <c r="J337" s="83"/>
+      <c r="K337" s="83"/>
+      <c r="L337" s="83"/>
+      <c r="M337" s="83"/>
+      <c r="N337" s="84"/>
       <c r="O337" s="72"/>
     </row>
     <row r="338" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A338" s="43" t="s">
         <v>62</v>
       </c>
-      <c r="C338" s="86" t="s">
+      <c r="C338" s="83" t="s">
+        <v>146</v>
+      </c>
+      <c r="D338" s="83"/>
+      <c r="E338" s="83"/>
+      <c r="F338" s="83"/>
+      <c r="G338" s="83"/>
+      <c r="H338" s="83"/>
+      <c r="I338" s="83" t="s">
         <v>147</v>
       </c>
-      <c r="D338" s="86"/>
-      <c r="E338" s="86"/>
-      <c r="F338" s="86"/>
-      <c r="G338" s="86"/>
-      <c r="H338" s="86"/>
-      <c r="I338" s="86" t="s">
-        <v>148</v>
-      </c>
-      <c r="J338" s="86"/>
-      <c r="K338" s="86"/>
-      <c r="L338" s="86"/>
-      <c r="M338" s="86"/>
-      <c r="N338" s="87"/>
+      <c r="J338" s="83"/>
+      <c r="K338" s="83"/>
+      <c r="L338" s="83"/>
+      <c r="M338" s="83"/>
+      <c r="N338" s="84"/>
       <c r="O338" s="73"/>
     </row>
     <row r="339" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A339" s="43" t="s">
         <v>63</v>
       </c>
-      <c r="C339" s="86">
-        <v>1</v>
-      </c>
-      <c r="D339" s="86"/>
-      <c r="E339" s="86"/>
-      <c r="F339" s="86"/>
-      <c r="G339" s="86"/>
-      <c r="H339" s="86"/>
-      <c r="I339" s="86">
-        <v>1</v>
-      </c>
-      <c r="J339" s="86"/>
-      <c r="K339" s="86"/>
-      <c r="L339" s="86"/>
-      <c r="M339" s="86"/>
-      <c r="N339" s="86"/>
+      <c r="C339" s="83">
+        <v>1</v>
+      </c>
+      <c r="D339" s="83"/>
+      <c r="E339" s="83"/>
+      <c r="F339" s="83"/>
+      <c r="G339" s="83"/>
+      <c r="H339" s="83"/>
+      <c r="I339" s="83">
+        <v>1</v>
+      </c>
+      <c r="J339" s="83"/>
+      <c r="K339" s="83"/>
+      <c r="L339" s="83"/>
+      <c r="M339" s="83"/>
+      <c r="N339" s="83"/>
       <c r="O339" s="72"/>
     </row>
     <row r="340" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A340" s="43" t="s">
         <v>64</v>
       </c>
-      <c r="C340" s="83">
+      <c r="C340" s="86">
         <v>0</v>
       </c>
-      <c r="D340" s="83"/>
-      <c r="E340" s="83"/>
-      <c r="F340" s="83"/>
-      <c r="G340" s="83"/>
-      <c r="H340" s="83"/>
-      <c r="I340" s="83">
+      <c r="D340" s="86"/>
+      <c r="E340" s="86"/>
+      <c r="F340" s="86"/>
+      <c r="G340" s="86"/>
+      <c r="H340" s="86"/>
+      <c r="I340" s="86">
         <v>0</v>
       </c>
-      <c r="J340" s="83"/>
-      <c r="K340" s="83"/>
-      <c r="L340" s="83"/>
-      <c r="M340" s="83"/>
-      <c r="N340" s="83"/>
+      <c r="J340" s="86"/>
+      <c r="K340" s="86"/>
+      <c r="L340" s="86"/>
+      <c r="M340" s="86"/>
+      <c r="N340" s="86"/>
       <c r="O340" s="72"/>
     </row>
     <row r="341" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A341" s="44" t="s">
         <v>65</v>
       </c>
-      <c r="C341" s="83">
+      <c r="C341" s="86">
         <f>MAX(0, SUM(C$50:H$50))</f>
         <v>200</v>
       </c>
-      <c r="D341" s="83"/>
-      <c r="E341" s="83"/>
-      <c r="F341" s="83"/>
-      <c r="G341" s="83"/>
-      <c r="H341" s="83"/>
-      <c r="I341" s="83">
+      <c r="D341" s="86"/>
+      <c r="E341" s="86"/>
+      <c r="F341" s="86"/>
+      <c r="G341" s="86"/>
+      <c r="H341" s="86"/>
+      <c r="I341" s="86">
         <f>MAX(0, SUM(I$50:N$50))</f>
         <v>200</v>
       </c>
-      <c r="J341" s="83"/>
-      <c r="K341" s="83"/>
-      <c r="L341" s="83"/>
-      <c r="M341" s="83"/>
-      <c r="N341" s="83"/>
+      <c r="J341" s="86"/>
+      <c r="K341" s="86"/>
+      <c r="L341" s="86"/>
+      <c r="M341" s="86"/>
+      <c r="N341" s="86"/>
       <c r="O341" s="72"/>
       <c r="P341" s="6"/>
       <c r="Q341" s="6"/>
@@ -7954,22 +7957,22 @@
       <c r="A342" s="43" t="s">
         <v>0</v>
       </c>
-      <c r="C342" s="83">
+      <c r="C342" s="86">
         <v>0</v>
       </c>
-      <c r="D342" s="83"/>
-      <c r="E342" s="83"/>
-      <c r="F342" s="83"/>
-      <c r="G342" s="83"/>
-      <c r="H342" s="83"/>
-      <c r="I342" s="83">
+      <c r="D342" s="86"/>
+      <c r="E342" s="86"/>
+      <c r="F342" s="86"/>
+      <c r="G342" s="86"/>
+      <c r="H342" s="86"/>
+      <c r="I342" s="86">
         <v>0</v>
       </c>
-      <c r="J342" s="83"/>
-      <c r="K342" s="83"/>
-      <c r="L342" s="83"/>
-      <c r="M342" s="83"/>
-      <c r="N342" s="83"/>
+      <c r="J342" s="86"/>
+      <c r="K342" s="86"/>
+      <c r="L342" s="86"/>
+      <c r="M342" s="86"/>
+      <c r="N342" s="86"/>
       <c r="O342" s="72"/>
       <c r="Q342" s="6"/>
     </row>
@@ -7977,24 +7980,24 @@
       <c r="A343" s="44" t="s">
         <v>66</v>
       </c>
-      <c r="C343" s="83">
+      <c r="C343" s="86">
         <f>IF(C342=0, C341, MIN(C341, C342))</f>
         <v>200</v>
       </c>
-      <c r="D343" s="83"/>
-      <c r="E343" s="83"/>
-      <c r="F343" s="83"/>
-      <c r="G343" s="83"/>
-      <c r="H343" s="83"/>
-      <c r="I343" s="83">
+      <c r="D343" s="86"/>
+      <c r="E343" s="86"/>
+      <c r="F343" s="86"/>
+      <c r="G343" s="86"/>
+      <c r="H343" s="86"/>
+      <c r="I343" s="86">
         <f>IF(I342=0, I341, MIN(I341, I342))</f>
         <v>200</v>
       </c>
-      <c r="J343" s="83"/>
-      <c r="K343" s="83"/>
-      <c r="L343" s="83"/>
-      <c r="M343" s="83"/>
-      <c r="N343" s="83"/>
+      <c r="J343" s="86"/>
+      <c r="K343" s="86"/>
+      <c r="L343" s="86"/>
+      <c r="M343" s="86"/>
+      <c r="N343" s="86"/>
       <c r="O343" s="72"/>
       <c r="P343" s="6"/>
       <c r="Q343" s="6"/>
@@ -8026,24 +8029,24 @@
       <c r="A345" s="44" t="s">
         <v>72</v>
       </c>
-      <c r="C345" s="83">
+      <c r="C345" s="86">
         <f>C343*C344</f>
         <v>20</v>
       </c>
-      <c r="D345" s="83"/>
-      <c r="E345" s="83"/>
-      <c r="F345" s="83"/>
-      <c r="G345" s="83"/>
-      <c r="H345" s="83"/>
-      <c r="I345" s="83">
+      <c r="D345" s="86"/>
+      <c r="E345" s="86"/>
+      <c r="F345" s="86"/>
+      <c r="G345" s="86"/>
+      <c r="H345" s="86"/>
+      <c r="I345" s="86">
         <f>I343*I344</f>
         <v>20</v>
       </c>
-      <c r="J345" s="83"/>
-      <c r="K345" s="83"/>
-      <c r="L345" s="83"/>
-      <c r="M345" s="83"/>
-      <c r="N345" s="83"/>
+      <c r="J345" s="86"/>
+      <c r="K345" s="86"/>
+      <c r="L345" s="86"/>
+      <c r="M345" s="86"/>
+      <c r="N345" s="86"/>
       <c r="O345" s="72"/>
     </row>
     <row r="346" spans="1:17" x14ac:dyDescent="0.3">
@@ -8074,7 +8077,7 @@
     </row>
     <row r="349" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A349" s="44" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C349" s="52">
         <f>$C$329*C$50/SUM($C$50:$H$50)</f>
@@ -8192,7 +8195,7 @@
       </c>
       <c r="B352" s="4"/>
       <c r="C352" s="78" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="D352" s="2"/>
       <c r="H352" s="42"/>
@@ -8238,31 +8241,31 @@
         <v>62</v>
       </c>
       <c r="C354" s="2" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="D354" s="2" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="E354" s="2"/>
       <c r="F354" s="2" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="G354" s="2" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="H354" s="2"/>
       <c r="I354" s="2" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="J354" s="2" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="K354" s="2"/>
       <c r="L354" s="2" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="M354" s="2" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="N354" s="81"/>
       <c r="O354" s="73"/>
@@ -8553,18 +8556,18 @@
       <c r="A364" s="45" t="s">
         <v>74</v>
       </c>
-      <c r="C364" s="86"/>
-      <c r="D364" s="86"/>
-      <c r="E364" s="86"/>
-      <c r="F364" s="86"/>
-      <c r="G364" s="86"/>
-      <c r="H364" s="86"/>
-      <c r="I364" s="86"/>
-      <c r="J364" s="86"/>
-      <c r="K364" s="86"/>
-      <c r="L364" s="86"/>
-      <c r="M364" s="86"/>
-      <c r="N364" s="86"/>
+      <c r="C364" s="83"/>
+      <c r="D364" s="83"/>
+      <c r="E364" s="83"/>
+      <c r="F364" s="83"/>
+      <c r="G364" s="83"/>
+      <c r="H364" s="83"/>
+      <c r="I364" s="83"/>
+      <c r="J364" s="83"/>
+      <c r="K364" s="83"/>
+      <c r="L364" s="83"/>
+      <c r="M364" s="83"/>
+      <c r="N364" s="83"/>
       <c r="O364" s="72">
         <f>SUM(C361:M361)</f>
         <v>120</v>
@@ -8765,70 +8768,210 @@
     </row>
   </sheetData>
   <mergeCells count="292">
-    <mergeCell ref="C364:E364"/>
-    <mergeCell ref="F364:H364"/>
-    <mergeCell ref="I364:K364"/>
-    <mergeCell ref="L364:N364"/>
-    <mergeCell ref="C338:H338"/>
-    <mergeCell ref="I338:N338"/>
-    <mergeCell ref="C344:H344"/>
-    <mergeCell ref="I344:N344"/>
-    <mergeCell ref="C345:H345"/>
-    <mergeCell ref="I345:N345"/>
-    <mergeCell ref="C339:H339"/>
-    <mergeCell ref="I339:N339"/>
-    <mergeCell ref="C340:H340"/>
-    <mergeCell ref="I340:N340"/>
-    <mergeCell ref="C341:H341"/>
-    <mergeCell ref="I341:N341"/>
-    <mergeCell ref="C342:H342"/>
-    <mergeCell ref="I342:N342"/>
-    <mergeCell ref="C343:H343"/>
-    <mergeCell ref="I343:N343"/>
-    <mergeCell ref="C326:H326"/>
-    <mergeCell ref="I326:N326"/>
-    <mergeCell ref="C327:H327"/>
-    <mergeCell ref="I327:N327"/>
-    <mergeCell ref="C328:H328"/>
-    <mergeCell ref="I328:N328"/>
-    <mergeCell ref="C329:H329"/>
-    <mergeCell ref="I329:N329"/>
-    <mergeCell ref="C337:H337"/>
-    <mergeCell ref="I337:N337"/>
-    <mergeCell ref="C321:H321"/>
-    <mergeCell ref="I321:N321"/>
-    <mergeCell ref="C322:H322"/>
-    <mergeCell ref="I322:N322"/>
-    <mergeCell ref="C323:H323"/>
-    <mergeCell ref="I323:N323"/>
-    <mergeCell ref="C324:H324"/>
-    <mergeCell ref="I324:N324"/>
-    <mergeCell ref="C325:H325"/>
-    <mergeCell ref="I325:N325"/>
-    <mergeCell ref="C311:E311"/>
-    <mergeCell ref="F311:H311"/>
-    <mergeCell ref="I311:K311"/>
-    <mergeCell ref="L311:N311"/>
-    <mergeCell ref="C312:E312"/>
-    <mergeCell ref="F312:H312"/>
-    <mergeCell ref="I312:K312"/>
-    <mergeCell ref="L312:N312"/>
-    <mergeCell ref="C313:E313"/>
-    <mergeCell ref="F313:H313"/>
-    <mergeCell ref="I313:K313"/>
-    <mergeCell ref="L313:N313"/>
-    <mergeCell ref="L308:N308"/>
-    <mergeCell ref="C309:E309"/>
-    <mergeCell ref="F309:H309"/>
-    <mergeCell ref="I309:K309"/>
-    <mergeCell ref="L309:N309"/>
-    <mergeCell ref="C310:E310"/>
-    <mergeCell ref="F310:H310"/>
-    <mergeCell ref="I310:K310"/>
-    <mergeCell ref="L310:N310"/>
-    <mergeCell ref="C308:E308"/>
-    <mergeCell ref="F308:H308"/>
-    <mergeCell ref="I308:K308"/>
+    <mergeCell ref="C138:E138"/>
+    <mergeCell ref="F138:H138"/>
+    <mergeCell ref="I138:K138"/>
+    <mergeCell ref="C135:E135"/>
+    <mergeCell ref="F135:H135"/>
+    <mergeCell ref="I135:K135"/>
+    <mergeCell ref="C136:E136"/>
+    <mergeCell ref="F136:H136"/>
+    <mergeCell ref="I136:K136"/>
+    <mergeCell ref="C137:E137"/>
+    <mergeCell ref="F137:H137"/>
+    <mergeCell ref="I137:K137"/>
+    <mergeCell ref="F131:H131"/>
+    <mergeCell ref="I131:K131"/>
+    <mergeCell ref="C132:E132"/>
+    <mergeCell ref="F132:H132"/>
+    <mergeCell ref="I132:K132"/>
+    <mergeCell ref="C133:E133"/>
+    <mergeCell ref="F133:H133"/>
+    <mergeCell ref="I133:K133"/>
+    <mergeCell ref="C134:E134"/>
+    <mergeCell ref="F134:H134"/>
+    <mergeCell ref="I134:K134"/>
+    <mergeCell ref="C305:E305"/>
+    <mergeCell ref="F305:H305"/>
+    <mergeCell ref="I305:K305"/>
+    <mergeCell ref="L305:N305"/>
+    <mergeCell ref="L306:N306"/>
+    <mergeCell ref="C307:E307"/>
+    <mergeCell ref="F307:H307"/>
+    <mergeCell ref="I307:K307"/>
+    <mergeCell ref="L307:N307"/>
+    <mergeCell ref="C243:H243"/>
+    <mergeCell ref="I243:N243"/>
+    <mergeCell ref="C244:H244"/>
+    <mergeCell ref="I244:N244"/>
+    <mergeCell ref="C245:H245"/>
+    <mergeCell ref="I245:N245"/>
+    <mergeCell ref="C246:H246"/>
+    <mergeCell ref="I246:N246"/>
+    <mergeCell ref="C247:H247"/>
+    <mergeCell ref="I247:N247"/>
+    <mergeCell ref="C240:H240"/>
+    <mergeCell ref="I240:N240"/>
+    <mergeCell ref="C241:H241"/>
+    <mergeCell ref="I241:N241"/>
+    <mergeCell ref="C242:H242"/>
+    <mergeCell ref="I242:N242"/>
+    <mergeCell ref="C239:H239"/>
+    <mergeCell ref="I239:N239"/>
+    <mergeCell ref="C229:H229"/>
+    <mergeCell ref="C230:H230"/>
+    <mergeCell ref="C231:H231"/>
+    <mergeCell ref="I229:N229"/>
+    <mergeCell ref="I230:N230"/>
+    <mergeCell ref="I231:N231"/>
+    <mergeCell ref="I224:N224"/>
+    <mergeCell ref="C225:H225"/>
+    <mergeCell ref="I225:N225"/>
+    <mergeCell ref="C213:E213"/>
+    <mergeCell ref="C214:E214"/>
+    <mergeCell ref="C215:E215"/>
+    <mergeCell ref="C223:H223"/>
+    <mergeCell ref="I223:N223"/>
+    <mergeCell ref="F211:H211"/>
+    <mergeCell ref="F212:H212"/>
+    <mergeCell ref="F213:H213"/>
+    <mergeCell ref="F214:H214"/>
+    <mergeCell ref="F215:H215"/>
+    <mergeCell ref="L207:N207"/>
+    <mergeCell ref="L208:N208"/>
+    <mergeCell ref="L209:N209"/>
+    <mergeCell ref="L210:N210"/>
+    <mergeCell ref="L211:N211"/>
+    <mergeCell ref="L212:N212"/>
+    <mergeCell ref="L213:N213"/>
+    <mergeCell ref="L214:N214"/>
+    <mergeCell ref="L215:N215"/>
+    <mergeCell ref="C54:E54"/>
+    <mergeCell ref="C53:E53"/>
+    <mergeCell ref="C63:E63"/>
+    <mergeCell ref="C62:E62"/>
+    <mergeCell ref="C64:E64"/>
+    <mergeCell ref="C61:E61"/>
+    <mergeCell ref="I207:K207"/>
+    <mergeCell ref="I208:K208"/>
+    <mergeCell ref="I209:K209"/>
+    <mergeCell ref="F208:H208"/>
+    <mergeCell ref="F209:H209"/>
+    <mergeCell ref="C127:E127"/>
+    <mergeCell ref="F127:H127"/>
+    <mergeCell ref="I127:K127"/>
+    <mergeCell ref="C128:E128"/>
+    <mergeCell ref="F128:H128"/>
+    <mergeCell ref="I128:K128"/>
+    <mergeCell ref="C129:E129"/>
+    <mergeCell ref="F129:H129"/>
+    <mergeCell ref="I129:K129"/>
+    <mergeCell ref="C130:E130"/>
+    <mergeCell ref="F130:H130"/>
+    <mergeCell ref="I130:K130"/>
+    <mergeCell ref="C131:E131"/>
+    <mergeCell ref="C35:E35"/>
+    <mergeCell ref="F35:H35"/>
+    <mergeCell ref="I35:K35"/>
+    <mergeCell ref="L35:N35"/>
+    <mergeCell ref="C25:E25"/>
+    <mergeCell ref="F25:H25"/>
+    <mergeCell ref="I25:K25"/>
+    <mergeCell ref="L25:N25"/>
+    <mergeCell ref="C34:E34"/>
+    <mergeCell ref="F34:H34"/>
+    <mergeCell ref="I34:K34"/>
+    <mergeCell ref="L34:N34"/>
+    <mergeCell ref="C55:E55"/>
+    <mergeCell ref="C56:E56"/>
+    <mergeCell ref="C58:E58"/>
+    <mergeCell ref="C57:E57"/>
+    <mergeCell ref="C59:E59"/>
+    <mergeCell ref="C60:E60"/>
+    <mergeCell ref="C78:E78"/>
+    <mergeCell ref="C79:E79"/>
+    <mergeCell ref="C83:E83"/>
+    <mergeCell ref="C68:E68"/>
+    <mergeCell ref="C69:E69"/>
+    <mergeCell ref="C70:E70"/>
+    <mergeCell ref="C71:E71"/>
+    <mergeCell ref="C72:E72"/>
+    <mergeCell ref="C84:E84"/>
+    <mergeCell ref="C85:E85"/>
+    <mergeCell ref="C73:E73"/>
+    <mergeCell ref="C74:E74"/>
+    <mergeCell ref="C75:E75"/>
+    <mergeCell ref="C76:E76"/>
+    <mergeCell ref="C77:E77"/>
+    <mergeCell ref="C102:E102"/>
+    <mergeCell ref="C103:E103"/>
+    <mergeCell ref="C91:E91"/>
+    <mergeCell ref="C92:E92"/>
+    <mergeCell ref="C93:E93"/>
+    <mergeCell ref="C94:E94"/>
+    <mergeCell ref="C98:E98"/>
+    <mergeCell ref="C86:E86"/>
+    <mergeCell ref="C87:E87"/>
+    <mergeCell ref="C88:E88"/>
+    <mergeCell ref="C89:E89"/>
+    <mergeCell ref="C90:E90"/>
+    <mergeCell ref="F113:H113"/>
+    <mergeCell ref="C114:E114"/>
+    <mergeCell ref="F114:H114"/>
+    <mergeCell ref="C109:E109"/>
+    <mergeCell ref="F98:H98"/>
+    <mergeCell ref="F99:H99"/>
+    <mergeCell ref="F100:H100"/>
+    <mergeCell ref="F101:H101"/>
+    <mergeCell ref="F102:H102"/>
+    <mergeCell ref="F103:H103"/>
+    <mergeCell ref="F104:H104"/>
+    <mergeCell ref="F105:H105"/>
+    <mergeCell ref="F106:H106"/>
+    <mergeCell ref="F107:H107"/>
+    <mergeCell ref="F108:H108"/>
+    <mergeCell ref="F109:H109"/>
+    <mergeCell ref="C104:E104"/>
+    <mergeCell ref="C105:E105"/>
+    <mergeCell ref="C106:E106"/>
+    <mergeCell ref="C107:E107"/>
+    <mergeCell ref="C108:E108"/>
+    <mergeCell ref="C99:E99"/>
+    <mergeCell ref="C100:E100"/>
+    <mergeCell ref="C101:E101"/>
+    <mergeCell ref="I112:K112"/>
+    <mergeCell ref="I113:K113"/>
+    <mergeCell ref="I114:K114"/>
+    <mergeCell ref="I115:K115"/>
+    <mergeCell ref="I116:K116"/>
+    <mergeCell ref="C121:E121"/>
+    <mergeCell ref="F121:H121"/>
+    <mergeCell ref="C122:E122"/>
+    <mergeCell ref="F122:H122"/>
+    <mergeCell ref="C118:E118"/>
+    <mergeCell ref="F118:H118"/>
+    <mergeCell ref="C119:E119"/>
+    <mergeCell ref="F119:H119"/>
+    <mergeCell ref="C120:E120"/>
+    <mergeCell ref="F120:H120"/>
+    <mergeCell ref="C115:E115"/>
+    <mergeCell ref="F115:H115"/>
+    <mergeCell ref="C116:E116"/>
+    <mergeCell ref="F116:H116"/>
+    <mergeCell ref="C117:E117"/>
+    <mergeCell ref="F117:H117"/>
+    <mergeCell ref="C112:E112"/>
+    <mergeCell ref="F112:H112"/>
+    <mergeCell ref="C113:E113"/>
+    <mergeCell ref="I122:K122"/>
+    <mergeCell ref="I123:K123"/>
+    <mergeCell ref="I117:K117"/>
+    <mergeCell ref="I118:K118"/>
+    <mergeCell ref="I119:K119"/>
+    <mergeCell ref="I120:K120"/>
+    <mergeCell ref="I121:K121"/>
+    <mergeCell ref="C123:E123"/>
+    <mergeCell ref="F123:H123"/>
     <mergeCell ref="C207:E207"/>
     <mergeCell ref="C208:E208"/>
     <mergeCell ref="C209:E209"/>
@@ -8853,210 +8996,70 @@
     <mergeCell ref="I227:N227"/>
     <mergeCell ref="I228:N228"/>
     <mergeCell ref="C224:H224"/>
-    <mergeCell ref="I122:K122"/>
-    <mergeCell ref="I123:K123"/>
-    <mergeCell ref="I117:K117"/>
-    <mergeCell ref="I118:K118"/>
-    <mergeCell ref="I119:K119"/>
-    <mergeCell ref="I120:K120"/>
-    <mergeCell ref="I121:K121"/>
-    <mergeCell ref="C123:E123"/>
-    <mergeCell ref="F123:H123"/>
-    <mergeCell ref="I112:K112"/>
-    <mergeCell ref="I113:K113"/>
-    <mergeCell ref="I114:K114"/>
-    <mergeCell ref="I115:K115"/>
-    <mergeCell ref="I116:K116"/>
-    <mergeCell ref="C121:E121"/>
-    <mergeCell ref="F121:H121"/>
-    <mergeCell ref="C122:E122"/>
-    <mergeCell ref="F122:H122"/>
-    <mergeCell ref="C118:E118"/>
-    <mergeCell ref="F118:H118"/>
-    <mergeCell ref="C119:E119"/>
-    <mergeCell ref="F119:H119"/>
-    <mergeCell ref="C120:E120"/>
-    <mergeCell ref="F120:H120"/>
-    <mergeCell ref="C115:E115"/>
-    <mergeCell ref="F115:H115"/>
-    <mergeCell ref="C116:E116"/>
-    <mergeCell ref="F116:H116"/>
-    <mergeCell ref="C117:E117"/>
-    <mergeCell ref="F117:H117"/>
-    <mergeCell ref="C112:E112"/>
-    <mergeCell ref="F112:H112"/>
-    <mergeCell ref="C113:E113"/>
-    <mergeCell ref="F113:H113"/>
-    <mergeCell ref="C114:E114"/>
-    <mergeCell ref="F114:H114"/>
-    <mergeCell ref="C109:E109"/>
-    <mergeCell ref="F98:H98"/>
-    <mergeCell ref="F99:H99"/>
-    <mergeCell ref="F100:H100"/>
-    <mergeCell ref="F101:H101"/>
-    <mergeCell ref="F102:H102"/>
-    <mergeCell ref="F103:H103"/>
-    <mergeCell ref="F104:H104"/>
-    <mergeCell ref="F105:H105"/>
-    <mergeCell ref="F106:H106"/>
-    <mergeCell ref="F107:H107"/>
-    <mergeCell ref="F108:H108"/>
-    <mergeCell ref="F109:H109"/>
-    <mergeCell ref="C104:E104"/>
-    <mergeCell ref="C105:E105"/>
-    <mergeCell ref="C106:E106"/>
-    <mergeCell ref="C107:E107"/>
-    <mergeCell ref="C108:E108"/>
-    <mergeCell ref="C99:E99"/>
-    <mergeCell ref="C100:E100"/>
-    <mergeCell ref="C101:E101"/>
-    <mergeCell ref="C84:E84"/>
-    <mergeCell ref="C85:E85"/>
-    <mergeCell ref="C73:E73"/>
-    <mergeCell ref="C74:E74"/>
-    <mergeCell ref="C75:E75"/>
-    <mergeCell ref="C76:E76"/>
-    <mergeCell ref="C77:E77"/>
-    <mergeCell ref="C102:E102"/>
-    <mergeCell ref="C103:E103"/>
-    <mergeCell ref="C91:E91"/>
-    <mergeCell ref="C92:E92"/>
-    <mergeCell ref="C93:E93"/>
-    <mergeCell ref="C94:E94"/>
-    <mergeCell ref="C98:E98"/>
-    <mergeCell ref="C86:E86"/>
-    <mergeCell ref="C87:E87"/>
-    <mergeCell ref="C88:E88"/>
-    <mergeCell ref="C89:E89"/>
-    <mergeCell ref="C90:E90"/>
-    <mergeCell ref="C55:E55"/>
-    <mergeCell ref="C56:E56"/>
-    <mergeCell ref="C58:E58"/>
-    <mergeCell ref="C57:E57"/>
-    <mergeCell ref="C59:E59"/>
-    <mergeCell ref="C60:E60"/>
-    <mergeCell ref="C78:E78"/>
-    <mergeCell ref="C79:E79"/>
-    <mergeCell ref="C83:E83"/>
-    <mergeCell ref="C68:E68"/>
-    <mergeCell ref="C69:E69"/>
-    <mergeCell ref="C70:E70"/>
-    <mergeCell ref="C71:E71"/>
-    <mergeCell ref="C72:E72"/>
-    <mergeCell ref="C35:E35"/>
-    <mergeCell ref="F35:H35"/>
-    <mergeCell ref="I35:K35"/>
-    <mergeCell ref="L35:N35"/>
-    <mergeCell ref="C25:E25"/>
-    <mergeCell ref="F25:H25"/>
-    <mergeCell ref="I25:K25"/>
-    <mergeCell ref="L25:N25"/>
-    <mergeCell ref="C34:E34"/>
-    <mergeCell ref="F34:H34"/>
-    <mergeCell ref="I34:K34"/>
-    <mergeCell ref="L34:N34"/>
-    <mergeCell ref="C54:E54"/>
-    <mergeCell ref="C53:E53"/>
-    <mergeCell ref="C63:E63"/>
-    <mergeCell ref="C62:E62"/>
-    <mergeCell ref="C64:E64"/>
-    <mergeCell ref="C61:E61"/>
-    <mergeCell ref="I207:K207"/>
-    <mergeCell ref="I208:K208"/>
-    <mergeCell ref="I209:K209"/>
-    <mergeCell ref="F208:H208"/>
-    <mergeCell ref="F209:H209"/>
-    <mergeCell ref="C127:E127"/>
-    <mergeCell ref="F127:H127"/>
-    <mergeCell ref="I127:K127"/>
-    <mergeCell ref="C128:E128"/>
-    <mergeCell ref="F128:H128"/>
-    <mergeCell ref="I128:K128"/>
-    <mergeCell ref="C129:E129"/>
-    <mergeCell ref="F129:H129"/>
-    <mergeCell ref="I129:K129"/>
-    <mergeCell ref="C130:E130"/>
-    <mergeCell ref="F130:H130"/>
-    <mergeCell ref="I130:K130"/>
-    <mergeCell ref="C131:E131"/>
-    <mergeCell ref="L207:N207"/>
-    <mergeCell ref="L208:N208"/>
-    <mergeCell ref="L209:N209"/>
-    <mergeCell ref="L210:N210"/>
-    <mergeCell ref="L211:N211"/>
-    <mergeCell ref="L212:N212"/>
-    <mergeCell ref="L213:N213"/>
-    <mergeCell ref="L214:N214"/>
-    <mergeCell ref="L215:N215"/>
-    <mergeCell ref="I224:N224"/>
-    <mergeCell ref="C225:H225"/>
-    <mergeCell ref="I225:N225"/>
-    <mergeCell ref="C213:E213"/>
-    <mergeCell ref="C214:E214"/>
-    <mergeCell ref="C215:E215"/>
-    <mergeCell ref="C223:H223"/>
-    <mergeCell ref="I223:N223"/>
-    <mergeCell ref="F211:H211"/>
-    <mergeCell ref="F212:H212"/>
-    <mergeCell ref="F213:H213"/>
-    <mergeCell ref="F214:H214"/>
-    <mergeCell ref="F215:H215"/>
-    <mergeCell ref="C240:H240"/>
-    <mergeCell ref="I240:N240"/>
-    <mergeCell ref="C241:H241"/>
-    <mergeCell ref="I241:N241"/>
-    <mergeCell ref="C242:H242"/>
-    <mergeCell ref="I242:N242"/>
-    <mergeCell ref="C239:H239"/>
-    <mergeCell ref="I239:N239"/>
-    <mergeCell ref="C229:H229"/>
-    <mergeCell ref="C230:H230"/>
-    <mergeCell ref="C231:H231"/>
-    <mergeCell ref="I229:N229"/>
-    <mergeCell ref="I230:N230"/>
-    <mergeCell ref="I231:N231"/>
-    <mergeCell ref="C243:H243"/>
-    <mergeCell ref="I243:N243"/>
-    <mergeCell ref="C244:H244"/>
-    <mergeCell ref="I244:N244"/>
-    <mergeCell ref="C245:H245"/>
-    <mergeCell ref="I245:N245"/>
-    <mergeCell ref="C246:H246"/>
-    <mergeCell ref="I246:N246"/>
-    <mergeCell ref="C247:H247"/>
-    <mergeCell ref="I247:N247"/>
-    <mergeCell ref="C305:E305"/>
-    <mergeCell ref="F305:H305"/>
-    <mergeCell ref="I305:K305"/>
-    <mergeCell ref="L305:N305"/>
-    <mergeCell ref="L306:N306"/>
-    <mergeCell ref="C307:E307"/>
-    <mergeCell ref="F307:H307"/>
-    <mergeCell ref="I307:K307"/>
-    <mergeCell ref="L307:N307"/>
-    <mergeCell ref="F131:H131"/>
-    <mergeCell ref="I131:K131"/>
-    <mergeCell ref="C132:E132"/>
-    <mergeCell ref="F132:H132"/>
-    <mergeCell ref="I132:K132"/>
-    <mergeCell ref="C133:E133"/>
-    <mergeCell ref="F133:H133"/>
-    <mergeCell ref="I133:K133"/>
-    <mergeCell ref="C134:E134"/>
-    <mergeCell ref="F134:H134"/>
-    <mergeCell ref="I134:K134"/>
-    <mergeCell ref="C138:E138"/>
-    <mergeCell ref="F138:H138"/>
-    <mergeCell ref="I138:K138"/>
-    <mergeCell ref="C135:E135"/>
-    <mergeCell ref="F135:H135"/>
-    <mergeCell ref="I135:K135"/>
-    <mergeCell ref="C136:E136"/>
-    <mergeCell ref="F136:H136"/>
-    <mergeCell ref="I136:K136"/>
-    <mergeCell ref="C137:E137"/>
-    <mergeCell ref="F137:H137"/>
-    <mergeCell ref="I137:K137"/>
+    <mergeCell ref="L308:N308"/>
+    <mergeCell ref="C309:E309"/>
+    <mergeCell ref="F309:H309"/>
+    <mergeCell ref="I309:K309"/>
+    <mergeCell ref="L309:N309"/>
+    <mergeCell ref="C310:E310"/>
+    <mergeCell ref="F310:H310"/>
+    <mergeCell ref="I310:K310"/>
+    <mergeCell ref="L310:N310"/>
+    <mergeCell ref="C308:E308"/>
+    <mergeCell ref="F308:H308"/>
+    <mergeCell ref="I308:K308"/>
+    <mergeCell ref="C311:E311"/>
+    <mergeCell ref="F311:H311"/>
+    <mergeCell ref="I311:K311"/>
+    <mergeCell ref="L311:N311"/>
+    <mergeCell ref="C312:E312"/>
+    <mergeCell ref="F312:H312"/>
+    <mergeCell ref="I312:K312"/>
+    <mergeCell ref="L312:N312"/>
+    <mergeCell ref="C313:E313"/>
+    <mergeCell ref="F313:H313"/>
+    <mergeCell ref="I313:K313"/>
+    <mergeCell ref="L313:N313"/>
+    <mergeCell ref="C321:H321"/>
+    <mergeCell ref="I321:N321"/>
+    <mergeCell ref="C322:H322"/>
+    <mergeCell ref="I322:N322"/>
+    <mergeCell ref="C323:H323"/>
+    <mergeCell ref="I323:N323"/>
+    <mergeCell ref="C324:H324"/>
+    <mergeCell ref="I324:N324"/>
+    <mergeCell ref="C325:H325"/>
+    <mergeCell ref="I325:N325"/>
+    <mergeCell ref="C326:H326"/>
+    <mergeCell ref="I326:N326"/>
+    <mergeCell ref="C327:H327"/>
+    <mergeCell ref="I327:N327"/>
+    <mergeCell ref="C328:H328"/>
+    <mergeCell ref="I328:N328"/>
+    <mergeCell ref="C329:H329"/>
+    <mergeCell ref="I329:N329"/>
+    <mergeCell ref="C337:H337"/>
+    <mergeCell ref="I337:N337"/>
+    <mergeCell ref="C364:E364"/>
+    <mergeCell ref="F364:H364"/>
+    <mergeCell ref="I364:K364"/>
+    <mergeCell ref="L364:N364"/>
+    <mergeCell ref="C338:H338"/>
+    <mergeCell ref="I338:N338"/>
+    <mergeCell ref="C344:H344"/>
+    <mergeCell ref="I344:N344"/>
+    <mergeCell ref="C345:H345"/>
+    <mergeCell ref="I345:N345"/>
+    <mergeCell ref="C339:H339"/>
+    <mergeCell ref="I339:N339"/>
+    <mergeCell ref="C340:H340"/>
+    <mergeCell ref="I340:N340"/>
+    <mergeCell ref="C341:H341"/>
+    <mergeCell ref="I341:N341"/>
+    <mergeCell ref="C342:H342"/>
+    <mergeCell ref="I342:N342"/>
+    <mergeCell ref="C343:H343"/>
+    <mergeCell ref="I343:N343"/>
   </mergeCells>
   <pageMargins left="0.70866141732283472" right="0.70866141732283472" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup paperSize="9" scale="44" orientation="portrait" r:id="rId1"/>
@@ -9075,7 +9078,7 @@
   <dimension ref="A2:M25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -9393,7 +9396,7 @@
         <v>110</v>
       </c>
       <c r="C11" s="69" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="D11" s="69" t="s">
         <v>126</v>

</xml_diff>

<commit_message>
QS examples with Risk and Occ Limits
</commit_message>
<xml_diff>
--- a/examples/ExamplesComparisonTest.xlsx
+++ b/examples/ExamplesComparisonTest.xlsx
@@ -8,21 +8,21 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\cygwin64\home\Joh\git\ReinsuranceTestTool\examples\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{73C30931-8FDF-4480-84FF-5921110E1EFD}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{AC3A4699-4CB5-4707-B5EB-30619582D45C}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="30720" windowHeight="9072" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="30720" windowHeight="9072" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Information" sheetId="18" r:id="rId1"/>
     <sheet name="Calculations" sheetId="15" r:id="rId2"/>
     <sheet name="OED examples list" sheetId="17" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="162913" iterateDelta="1E-4"/>
+  <calcPr calcId="162913"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="491" uniqueCount="163">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="563" uniqueCount="181">
   <si>
     <t>Limit</t>
   </si>
@@ -511,6 +511,60 @@
   </si>
   <si>
     <t>Treaty 3 on portfolio: 10 xs 0 @100%</t>
+  </si>
+  <si>
+    <t>Subject Loss net of % ceded</t>
+  </si>
+  <si>
+    <t>Ceded Loss (Subj Loss net of % ceded, % placed)</t>
+  </si>
+  <si>
+    <t>placed_acc_QS</t>
+  </si>
+  <si>
+    <t>Treaty 1 on each account: 50% ceded, 80% placed</t>
+  </si>
+  <si>
+    <t>Treaty 1 on account 1: 50% ceded, 80% placed</t>
+  </si>
+  <si>
+    <t>placed_acc_1_QS</t>
+  </si>
+  <si>
+    <t>QS with % ceded and % placed applied to all accounts</t>
+  </si>
+  <si>
+    <t>QS with % ceded and % placed applied to account 1</t>
+  </si>
+  <si>
+    <t>In progress</t>
+  </si>
+  <si>
+    <t>placed_acc_limit_QS</t>
+  </si>
+  <si>
+    <t>placed_acc_1_limit_QS</t>
+  </si>
+  <si>
+    <t>QS with % ceded and % placed applied to account 1 with risk and occ limits</t>
+  </si>
+  <si>
+    <t>QS with % ceded and % placed applied to all accounts with risk and occ limits</t>
+  </si>
+  <si>
+    <t>Subj Loss net of % ceded &amp; lim</t>
+  </si>
+  <si>
+    <t>Treaty 1 on each account: 50% ceded Risk Limit 50, Occ Limit 90, 80% placed</t>
+  </si>
+  <si>
+    <t>Treaty 1 on account 1: 50% ceded Risk Limit 50, Occ Limit 40, 80% placed</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Single surplus share at policy level.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Single surplus share at account level.</t>
   </si>
 </sst>
 </file>
@@ -811,7 +865,7 @@
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="99">
+  <cellXfs count="103">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
@@ -1049,20 +1103,32 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="165" fontId="13" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="5" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1517,10 +1583,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:U368"/>
+  <dimension ref="A1:U420"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A236" zoomScale="84" zoomScaleNormal="84" workbookViewId="0">
-      <selection activeCell="I254" sqref="I254"/>
+    <sheetView showGridLines="0" topLeftCell="A391" zoomScale="84" zoomScaleNormal="84" workbookViewId="0">
+      <selection activeCell="C419" sqref="C419:H419"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1906,26 +1972,26 @@
       <c r="B25" s="25" t="s">
         <v>48</v>
       </c>
-      <c r="C25" s="93">
+      <c r="C25" s="97">
         <v>100</v>
       </c>
-      <c r="D25" s="93"/>
-      <c r="E25" s="94"/>
-      <c r="F25" s="93">
+      <c r="D25" s="97"/>
+      <c r="E25" s="98"/>
+      <c r="F25" s="97">
         <v>100</v>
       </c>
-      <c r="G25" s="93"/>
-      <c r="H25" s="94"/>
-      <c r="I25" s="95">
+      <c r="G25" s="97"/>
+      <c r="H25" s="98"/>
+      <c r="I25" s="99">
         <v>100</v>
       </c>
-      <c r="J25" s="93"/>
-      <c r="K25" s="94"/>
-      <c r="L25" s="93">
+      <c r="J25" s="97"/>
+      <c r="K25" s="98"/>
+      <c r="L25" s="97">
         <v>100</v>
       </c>
-      <c r="M25" s="93"/>
-      <c r="N25" s="94"/>
+      <c r="M25" s="97"/>
+      <c r="N25" s="98"/>
       <c r="O25" s="8"/>
       <c r="P25" s="8"/>
       <c r="Q25" s="11"/>
@@ -2166,30 +2232,30 @@
       <c r="B34" s="8" t="s">
         <v>50</v>
       </c>
-      <c r="C34" s="96">
+      <c r="C34" s="100">
         <f>SUMIF($C$21:$N$21,C21,$C$31:$N$31)</f>
         <v>2000</v>
       </c>
-      <c r="D34" s="96"/>
-      <c r="E34" s="97"/>
-      <c r="F34" s="96">
+      <c r="D34" s="100"/>
+      <c r="E34" s="101"/>
+      <c r="F34" s="100">
         <f>SUMIF($C$21:$N$21,F21,$C$31:$N$31)</f>
         <v>2000</v>
       </c>
-      <c r="G34" s="96"/>
-      <c r="H34" s="97"/>
-      <c r="I34" s="96">
+      <c r="G34" s="100"/>
+      <c r="H34" s="101"/>
+      <c r="I34" s="100">
         <f>SUMIF($C$21:$N$21,I21,$C$31:$N$31)</f>
         <v>2000</v>
       </c>
-      <c r="J34" s="96"/>
-      <c r="K34" s="97"/>
-      <c r="L34" s="96">
+      <c r="J34" s="100"/>
+      <c r="K34" s="101"/>
+      <c r="L34" s="100">
         <f>SUMIF($C$21:$N$21,L21,$C$31:$N$31)</f>
         <v>2000</v>
       </c>
-      <c r="M34" s="96"/>
-      <c r="N34" s="97"/>
+      <c r="M34" s="100"/>
+      <c r="N34" s="101"/>
       <c r="O34" s="8"/>
       <c r="P34" s="23"/>
       <c r="Q34" s="11"/>
@@ -2201,30 +2267,30 @@
       <c r="B35" s="36" t="s">
         <v>52</v>
       </c>
-      <c r="C35" s="89">
+      <c r="C35" s="93">
         <f>MIN(C34, C25)</f>
         <v>100</v>
       </c>
-      <c r="D35" s="90"/>
-      <c r="E35" s="91"/>
-      <c r="F35" s="89">
+      <c r="D35" s="94"/>
+      <c r="E35" s="95"/>
+      <c r="F35" s="93">
         <f>MIN(F34, F25)</f>
         <v>100</v>
       </c>
-      <c r="G35" s="90"/>
-      <c r="H35" s="91"/>
-      <c r="I35" s="89">
+      <c r="G35" s="94"/>
+      <c r="H35" s="95"/>
+      <c r="I35" s="93">
         <f>MIN(I34, I25)</f>
         <v>100</v>
       </c>
-      <c r="J35" s="90"/>
-      <c r="K35" s="91"/>
-      <c r="L35" s="92">
+      <c r="J35" s="94"/>
+      <c r="K35" s="95"/>
+      <c r="L35" s="96">
         <f>MIN(L34, L25)</f>
         <v>100</v>
       </c>
-      <c r="M35" s="90"/>
-      <c r="N35" s="91"/>
+      <c r="M35" s="94"/>
+      <c r="N35" s="95"/>
       <c r="O35" s="12">
         <f>SUM(C35:N35)</f>
         <v>400</v>
@@ -2593,10 +2659,10 @@
       <c r="A56" s="43" t="s">
         <v>64</v>
       </c>
-      <c r="C56" s="83">
+      <c r="C56" s="89">
         <v>0</v>
       </c>
-      <c r="D56" s="83"/>
+      <c r="D56" s="89"/>
       <c r="E56" s="87"/>
       <c r="H56" s="40"/>
       <c r="N56" s="40"/>
@@ -2605,11 +2671,11 @@
       <c r="A57" s="44" t="s">
         <v>65</v>
       </c>
-      <c r="C57" s="83">
+      <c r="C57" s="89">
         <f>MAX(0, SUM(C$50:E$50)-C56)</f>
         <v>100</v>
       </c>
-      <c r="D57" s="83"/>
+      <c r="D57" s="89"/>
       <c r="E57" s="87"/>
       <c r="H57" s="40"/>
       <c r="N57" s="40"/>
@@ -2618,10 +2684,10 @@
       <c r="A58" s="43" t="s">
         <v>0</v>
       </c>
-      <c r="C58" s="83">
+      <c r="C58" s="89">
         <v>10</v>
       </c>
-      <c r="D58" s="83"/>
+      <c r="D58" s="89"/>
       <c r="E58" s="87"/>
       <c r="H58" s="40"/>
       <c r="N58" s="40"/>
@@ -2630,11 +2696,11 @@
       <c r="A59" s="44" t="s">
         <v>66</v>
       </c>
-      <c r="C59" s="83">
+      <c r="C59" s="89">
         <f>IF(C58="Unlimited", C57, MIN(C57, C58))</f>
         <v>10</v>
       </c>
-      <c r="D59" s="83"/>
+      <c r="D59" s="89"/>
       <c r="E59" s="87"/>
       <c r="H59" s="40"/>
       <c r="N59" s="40"/>
@@ -2643,11 +2709,11 @@
       <c r="A60" s="43" t="s">
         <v>71</v>
       </c>
-      <c r="C60" s="85">
-        <v>1</v>
-      </c>
-      <c r="D60" s="85"/>
-      <c r="E60" s="98"/>
+      <c r="C60" s="88">
+        <v>1</v>
+      </c>
+      <c r="D60" s="88"/>
+      <c r="E60" s="102"/>
       <c r="H60" s="40"/>
       <c r="N60" s="40"/>
     </row>
@@ -2655,11 +2721,11 @@
       <c r="A61" s="44" t="s">
         <v>72</v>
       </c>
-      <c r="C61" s="83">
+      <c r="C61" s="89">
         <f>C60*C59</f>
         <v>10</v>
       </c>
-      <c r="D61" s="83"/>
+      <c r="D61" s="89"/>
       <c r="E61" s="87"/>
       <c r="H61" s="40"/>
       <c r="N61" s="40"/>
@@ -2668,9 +2734,9 @@
       <c r="A62" s="43" t="s">
         <v>3</v>
       </c>
-      <c r="C62" s="84"/>
-      <c r="D62" s="84"/>
-      <c r="E62" s="88"/>
+      <c r="C62" s="91"/>
+      <c r="D62" s="91"/>
+      <c r="E62" s="92"/>
       <c r="H62" s="40"/>
       <c r="N62" s="40"/>
     </row>
@@ -2678,9 +2744,9 @@
       <c r="A63" s="43" t="s">
         <v>67</v>
       </c>
-      <c r="C63" s="84"/>
-      <c r="D63" s="84"/>
-      <c r="E63" s="88"/>
+      <c r="C63" s="91"/>
+      <c r="D63" s="91"/>
+      <c r="E63" s="92"/>
       <c r="H63" s="40"/>
       <c r="N63" s="40"/>
     </row>
@@ -2688,11 +2754,11 @@
       <c r="A64" s="45" t="s">
         <v>68</v>
       </c>
-      <c r="C64" s="83">
+      <c r="C64" s="89">
         <f>MIN(C61,IF(OR(C63="Unlimited",C63=""),10^18,C63))</f>
         <v>10</v>
       </c>
-      <c r="D64" s="83"/>
+      <c r="D64" s="89"/>
       <c r="E64" s="87"/>
       <c r="H64" s="40"/>
       <c r="N64" s="40"/>
@@ -2778,7 +2844,7 @@
         <v>1</v>
       </c>
       <c r="D68" s="86"/>
-      <c r="E68" s="83"/>
+      <c r="E68" s="89"/>
       <c r="F68" s="13"/>
       <c r="H68" s="40"/>
       <c r="N68" s="40"/>
@@ -2791,7 +2857,7 @@
         <v>83</v>
       </c>
       <c r="D69" s="86"/>
-      <c r="E69" s="83"/>
+      <c r="E69" s="89"/>
       <c r="F69" s="13"/>
       <c r="H69" s="40"/>
       <c r="N69" s="40"/>
@@ -2804,7 +2870,7 @@
         <v>1</v>
       </c>
       <c r="D70" s="86"/>
-      <c r="E70" s="83"/>
+      <c r="E70" s="89"/>
       <c r="F70" s="13"/>
       <c r="H70" s="40"/>
       <c r="N70" s="40"/>
@@ -2813,11 +2879,11 @@
       <c r="A71" s="43" t="s">
         <v>64</v>
       </c>
-      <c r="C71" s="83">
+      <c r="C71" s="89">
         <v>0</v>
       </c>
-      <c r="D71" s="83"/>
-      <c r="E71" s="83"/>
+      <c r="D71" s="89"/>
+      <c r="E71" s="89"/>
       <c r="F71" s="13"/>
       <c r="H71" s="40"/>
       <c r="N71" s="40"/>
@@ -2826,12 +2892,12 @@
       <c r="A72" s="44" t="s">
         <v>65</v>
       </c>
-      <c r="C72" s="83">
+      <c r="C72" s="89">
         <f>MAX(0, SUM(C$50:H$50)-C71)</f>
         <v>200</v>
       </c>
-      <c r="D72" s="83"/>
-      <c r="E72" s="83"/>
+      <c r="D72" s="89"/>
+      <c r="E72" s="89"/>
       <c r="F72" s="13"/>
       <c r="H72" s="40"/>
       <c r="N72" s="40"/>
@@ -2840,11 +2906,11 @@
       <c r="A73" s="43" t="s">
         <v>0</v>
       </c>
-      <c r="C73" s="83">
+      <c r="C73" s="89">
         <v>10</v>
       </c>
-      <c r="D73" s="83"/>
-      <c r="E73" s="83"/>
+      <c r="D73" s="89"/>
+      <c r="E73" s="89"/>
       <c r="F73" s="13"/>
       <c r="H73" s="40"/>
       <c r="N73" s="40"/>
@@ -2853,12 +2919,12 @@
       <c r="A74" s="44" t="s">
         <v>66</v>
       </c>
-      <c r="C74" s="83">
+      <c r="C74" s="89">
         <f>IF(C73="Unlimited", C72, MIN(C72, C73))</f>
         <v>10</v>
       </c>
-      <c r="D74" s="83"/>
-      <c r="E74" s="83"/>
+      <c r="D74" s="89"/>
+      <c r="E74" s="89"/>
       <c r="F74" s="13"/>
       <c r="H74" s="40"/>
       <c r="N74" s="40"/>
@@ -2867,11 +2933,11 @@
       <c r="A75" s="43" t="s">
         <v>71</v>
       </c>
-      <c r="C75" s="85">
-        <v>1</v>
-      </c>
-      <c r="D75" s="85"/>
-      <c r="E75" s="85"/>
+      <c r="C75" s="88">
+        <v>1</v>
+      </c>
+      <c r="D75" s="88"/>
+      <c r="E75" s="88"/>
       <c r="F75" s="13"/>
       <c r="H75" s="40"/>
       <c r="N75" s="40"/>
@@ -2880,12 +2946,12 @@
       <c r="A76" s="44" t="s">
         <v>72</v>
       </c>
-      <c r="C76" s="83">
+      <c r="C76" s="89">
         <f>C75*C74</f>
         <v>10</v>
       </c>
-      <c r="D76" s="83"/>
-      <c r="E76" s="83"/>
+      <c r="D76" s="89"/>
+      <c r="E76" s="89"/>
       <c r="F76" s="13"/>
       <c r="H76" s="40"/>
       <c r="N76" s="40"/>
@@ -2894,9 +2960,9 @@
       <c r="A77" s="43" t="s">
         <v>3</v>
       </c>
-      <c r="C77" s="84"/>
-      <c r="D77" s="84"/>
-      <c r="E77" s="84"/>
+      <c r="C77" s="91"/>
+      <c r="D77" s="91"/>
+      <c r="E77" s="91"/>
       <c r="F77" s="13"/>
       <c r="H77" s="40"/>
       <c r="N77" s="40"/>
@@ -2905,9 +2971,9 @@
       <c r="A78" s="43" t="s">
         <v>67</v>
       </c>
-      <c r="C78" s="84"/>
-      <c r="D78" s="84"/>
-      <c r="E78" s="84"/>
+      <c r="C78" s="91"/>
+      <c r="D78" s="91"/>
+      <c r="E78" s="91"/>
       <c r="F78" s="13"/>
       <c r="H78" s="40"/>
       <c r="N78" s="40"/>
@@ -2916,12 +2982,12 @@
       <c r="A79" s="45" t="s">
         <v>68</v>
       </c>
-      <c r="C79" s="83">
+      <c r="C79" s="89">
         <f>MIN(C76,IF(OR(C78="Unlimited",C78=""),10^18,C78))</f>
         <v>10</v>
       </c>
-      <c r="D79" s="83"/>
-      <c r="E79" s="83"/>
+      <c r="D79" s="89"/>
+      <c r="E79" s="89"/>
       <c r="F79" s="13"/>
       <c r="H79" s="40"/>
       <c r="N79" s="40"/>
@@ -3008,7 +3074,7 @@
         <v>1</v>
       </c>
       <c r="D83" s="86"/>
-      <c r="E83" s="83"/>
+      <c r="E83" s="89"/>
       <c r="F83" s="13"/>
       <c r="H83" s="40"/>
       <c r="N83" s="40"/>
@@ -3021,7 +3087,7 @@
         <v>85</v>
       </c>
       <c r="D84" s="86"/>
-      <c r="E84" s="83"/>
+      <c r="E84" s="89"/>
       <c r="F84" s="13"/>
       <c r="H84" s="40"/>
       <c r="N84" s="40"/>
@@ -3034,7 +3100,7 @@
         <v>1</v>
       </c>
       <c r="D85" s="86"/>
-      <c r="E85" s="83"/>
+      <c r="E85" s="89"/>
       <c r="F85" s="13"/>
       <c r="H85" s="40"/>
       <c r="N85" s="40"/>
@@ -3043,11 +3109,11 @@
       <c r="A86" s="43" t="s">
         <v>64</v>
       </c>
-      <c r="C86" s="83">
+      <c r="C86" s="89">
         <v>0</v>
       </c>
-      <c r="D86" s="83"/>
-      <c r="E86" s="83"/>
+      <c r="D86" s="89"/>
+      <c r="E86" s="89"/>
       <c r="F86" s="13"/>
       <c r="H86" s="40"/>
       <c r="N86" s="40"/>
@@ -3056,12 +3122,12 @@
       <c r="A87" s="44" t="s">
         <v>65</v>
       </c>
-      <c r="C87" s="83">
+      <c r="C87" s="89">
         <f>MAX(0, SUM(C$50:H$50)-C86)</f>
         <v>200</v>
       </c>
-      <c r="D87" s="83"/>
-      <c r="E87" s="83"/>
+      <c r="D87" s="89"/>
+      <c r="E87" s="89"/>
       <c r="F87" s="13"/>
       <c r="H87" s="40"/>
       <c r="N87" s="40"/>
@@ -3070,11 +3136,11 @@
       <c r="A88" s="43" t="s">
         <v>0</v>
       </c>
-      <c r="C88" s="83">
+      <c r="C88" s="89">
         <v>10</v>
       </c>
-      <c r="D88" s="83"/>
-      <c r="E88" s="83"/>
+      <c r="D88" s="89"/>
+      <c r="E88" s="89"/>
       <c r="F88" s="13"/>
       <c r="H88" s="40"/>
       <c r="N88" s="40"/>
@@ -3083,12 +3149,12 @@
       <c r="A89" s="44" t="s">
         <v>66</v>
       </c>
-      <c r="C89" s="83">
+      <c r="C89" s="89">
         <f>IF(C88="Unlimited", C87, MIN(C87, C88))</f>
         <v>10</v>
       </c>
-      <c r="D89" s="83"/>
-      <c r="E89" s="83"/>
+      <c r="D89" s="89"/>
+      <c r="E89" s="89"/>
       <c r="F89" s="13"/>
       <c r="H89" s="40"/>
       <c r="N89" s="40"/>
@@ -3097,11 +3163,11 @@
       <c r="A90" s="43" t="s">
         <v>71</v>
       </c>
-      <c r="C90" s="85">
-        <v>1</v>
-      </c>
-      <c r="D90" s="85"/>
-      <c r="E90" s="85"/>
+      <c r="C90" s="88">
+        <v>1</v>
+      </c>
+      <c r="D90" s="88"/>
+      <c r="E90" s="88"/>
       <c r="F90" s="13"/>
       <c r="H90" s="40"/>
       <c r="N90" s="40"/>
@@ -3110,12 +3176,12 @@
       <c r="A91" s="44" t="s">
         <v>72</v>
       </c>
-      <c r="C91" s="83">
+      <c r="C91" s="89">
         <f>C90*C89</f>
         <v>10</v>
       </c>
-      <c r="D91" s="83"/>
-      <c r="E91" s="83"/>
+      <c r="D91" s="89"/>
+      <c r="E91" s="89"/>
       <c r="F91" s="13"/>
       <c r="H91" s="40"/>
       <c r="N91" s="40"/>
@@ -3124,9 +3190,9 @@
       <c r="A92" s="43" t="s">
         <v>3</v>
       </c>
-      <c r="C92" s="84"/>
-      <c r="D92" s="84"/>
-      <c r="E92" s="84"/>
+      <c r="C92" s="91"/>
+      <c r="D92" s="91"/>
+      <c r="E92" s="91"/>
       <c r="F92" s="13"/>
       <c r="H92" s="40"/>
       <c r="N92" s="40"/>
@@ -3135,9 +3201,9 @@
       <c r="A93" s="43" t="s">
         <v>67</v>
       </c>
-      <c r="C93" s="84"/>
-      <c r="D93" s="84"/>
-      <c r="E93" s="84"/>
+      <c r="C93" s="91"/>
+      <c r="D93" s="91"/>
+      <c r="E93" s="91"/>
       <c r="F93" s="13"/>
       <c r="H93" s="40"/>
       <c r="N93" s="40"/>
@@ -3146,12 +3212,12 @@
       <c r="A94" s="45" t="s">
         <v>68</v>
       </c>
-      <c r="C94" s="83">
+      <c r="C94" s="89">
         <f>MIN(C91,IF(OR(C93="Unlimited",C93=""),10^18,C93))</f>
         <v>10</v>
       </c>
-      <c r="D94" s="83"/>
-      <c r="E94" s="83"/>
+      <c r="D94" s="89"/>
+      <c r="E94" s="89"/>
       <c r="F94" s="13"/>
       <c r="H94" s="40"/>
       <c r="N94" s="40"/>
@@ -3241,12 +3307,12 @@
         <v>1</v>
       </c>
       <c r="D98" s="86"/>
-      <c r="E98" s="83"/>
+      <c r="E98" s="89"/>
       <c r="F98" s="86">
         <v>1</v>
       </c>
       <c r="G98" s="86"/>
-      <c r="H98" s="83"/>
+      <c r="H98" s="89"/>
       <c r="N98" s="40"/>
     </row>
     <row r="99" spans="1:15" x14ac:dyDescent="0.3">
@@ -3257,12 +3323,12 @@
         <v>70</v>
       </c>
       <c r="D99" s="86"/>
-      <c r="E99" s="83"/>
+      <c r="E99" s="89"/>
       <c r="F99" s="86" t="s">
         <v>70</v>
       </c>
       <c r="G99" s="86"/>
-      <c r="H99" s="83"/>
+      <c r="H99" s="89"/>
       <c r="N99" s="40"/>
     </row>
     <row r="100" spans="1:15" x14ac:dyDescent="0.3">
@@ -3273,156 +3339,156 @@
         <v>1</v>
       </c>
       <c r="D100" s="86"/>
-      <c r="E100" s="83"/>
+      <c r="E100" s="89"/>
       <c r="F100" s="86">
         <v>1</v>
       </c>
       <c r="G100" s="86"/>
-      <c r="H100" s="83"/>
+      <c r="H100" s="89"/>
       <c r="N100" s="40"/>
     </row>
     <row r="101" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A101" s="43" t="s">
         <v>64</v>
       </c>
-      <c r="C101" s="83">
+      <c r="C101" s="89">
         <v>0</v>
       </c>
-      <c r="D101" s="83"/>
-      <c r="E101" s="83"/>
-      <c r="F101" s="83">
+      <c r="D101" s="89"/>
+      <c r="E101" s="89"/>
+      <c r="F101" s="89">
         <v>0</v>
       </c>
-      <c r="G101" s="83"/>
-      <c r="H101" s="83"/>
+      <c r="G101" s="89"/>
+      <c r="H101" s="89"/>
       <c r="N101" s="40"/>
     </row>
     <row r="102" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A102" s="44" t="s">
         <v>65</v>
       </c>
-      <c r="C102" s="83">
+      <c r="C102" s="89">
         <f>MAX(0, SUM(C$50:E$50)-C101)</f>
         <v>100</v>
       </c>
-      <c r="D102" s="83"/>
-      <c r="E102" s="83"/>
-      <c r="F102" s="83">
+      <c r="D102" s="89"/>
+      <c r="E102" s="89"/>
+      <c r="F102" s="89">
         <f>MAX(0, SUM(F$50:H$50)-F101)</f>
         <v>100</v>
       </c>
-      <c r="G102" s="83"/>
-      <c r="H102" s="83"/>
+      <c r="G102" s="89"/>
+      <c r="H102" s="89"/>
       <c r="N102" s="40"/>
     </row>
     <row r="103" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A103" s="43" t="s">
         <v>0</v>
       </c>
-      <c r="C103" s="83">
+      <c r="C103" s="89">
         <v>10</v>
       </c>
-      <c r="D103" s="83"/>
-      <c r="E103" s="83"/>
-      <c r="F103" s="83">
+      <c r="D103" s="89"/>
+      <c r="E103" s="89"/>
+      <c r="F103" s="89">
         <v>10</v>
       </c>
-      <c r="G103" s="83"/>
-      <c r="H103" s="83"/>
+      <c r="G103" s="89"/>
+      <c r="H103" s="89"/>
       <c r="N103" s="40"/>
     </row>
     <row r="104" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A104" s="44" t="s">
         <v>66</v>
       </c>
-      <c r="C104" s="83">
+      <c r="C104" s="89">
         <f>IF(C103="Unlimited", C102, MIN(C102, C103))</f>
         <v>10</v>
       </c>
-      <c r="D104" s="83"/>
-      <c r="E104" s="83"/>
-      <c r="F104" s="83">
+      <c r="D104" s="89"/>
+      <c r="E104" s="89"/>
+      <c r="F104" s="89">
         <f>IF(F103="Unlimited", F102, MIN(F102, F103))</f>
         <v>10</v>
       </c>
-      <c r="G104" s="83"/>
-      <c r="H104" s="83"/>
+      <c r="G104" s="89"/>
+      <c r="H104" s="89"/>
       <c r="N104" s="40"/>
     </row>
     <row r="105" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A105" s="43" t="s">
         <v>71</v>
       </c>
-      <c r="C105" s="85">
-        <v>1</v>
-      </c>
-      <c r="D105" s="85"/>
-      <c r="E105" s="85"/>
-      <c r="F105" s="85">
-        <v>1</v>
-      </c>
-      <c r="G105" s="85"/>
-      <c r="H105" s="85"/>
+      <c r="C105" s="88">
+        <v>1</v>
+      </c>
+      <c r="D105" s="88"/>
+      <c r="E105" s="88"/>
+      <c r="F105" s="88">
+        <v>1</v>
+      </c>
+      <c r="G105" s="88"/>
+      <c r="H105" s="88"/>
       <c r="N105" s="40"/>
     </row>
     <row r="106" spans="1:15" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A106" s="44" t="s">
         <v>72</v>
       </c>
-      <c r="C106" s="83">
+      <c r="C106" s="89">
         <f>C105*C104</f>
         <v>10</v>
       </c>
-      <c r="D106" s="83"/>
-      <c r="E106" s="83"/>
-      <c r="F106" s="83">
+      <c r="D106" s="89"/>
+      <c r="E106" s="89"/>
+      <c r="F106" s="89">
         <f>F105*F104</f>
         <v>10</v>
       </c>
-      <c r="G106" s="83"/>
-      <c r="H106" s="83"/>
+      <c r="G106" s="89"/>
+      <c r="H106" s="89"/>
       <c r="N106" s="40"/>
     </row>
     <row r="107" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A107" s="43" t="s">
         <v>3</v>
       </c>
-      <c r="C107" s="84"/>
-      <c r="D107" s="84"/>
-      <c r="E107" s="84"/>
-      <c r="F107" s="84"/>
-      <c r="G107" s="84"/>
-      <c r="H107" s="84"/>
+      <c r="C107" s="91"/>
+      <c r="D107" s="91"/>
+      <c r="E107" s="91"/>
+      <c r="F107" s="91"/>
+      <c r="G107" s="91"/>
+      <c r="H107" s="91"/>
       <c r="N107" s="40"/>
     </row>
     <row r="108" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A108" s="43" t="s">
         <v>67</v>
       </c>
-      <c r="C108" s="84"/>
-      <c r="D108" s="84"/>
-      <c r="E108" s="84"/>
-      <c r="F108" s="84"/>
-      <c r="G108" s="84"/>
-      <c r="H108" s="84"/>
+      <c r="C108" s="91"/>
+      <c r="D108" s="91"/>
+      <c r="E108" s="91"/>
+      <c r="F108" s="91"/>
+      <c r="G108" s="91"/>
+      <c r="H108" s="91"/>
       <c r="N108" s="40"/>
     </row>
     <row r="109" spans="1:15" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A109" s="45" t="s">
         <v>68</v>
       </c>
-      <c r="C109" s="83">
+      <c r="C109" s="89">
         <f>MIN(C106,IF(OR(C108="Unlimited",C108=""),10^18,C108))</f>
         <v>10</v>
       </c>
-      <c r="D109" s="83"/>
-      <c r="E109" s="83"/>
-      <c r="F109" s="83">
+      <c r="D109" s="89"/>
+      <c r="E109" s="89"/>
+      <c r="F109" s="89">
         <f>MIN(F106,IF(OR(F108="Unlimited",F108=""),10^18,F108))</f>
         <v>10</v>
       </c>
-      <c r="G109" s="83"/>
-      <c r="H109" s="83"/>
+      <c r="G109" s="89"/>
+      <c r="H109" s="89"/>
       <c r="N109" s="40"/>
     </row>
     <row r="110" spans="1:15" x14ac:dyDescent="0.3">
@@ -3502,13 +3568,13 @@
         <v>1</v>
       </c>
       <c r="D112" s="86"/>
-      <c r="E112" s="83"/>
+      <c r="E112" s="89"/>
       <c r="F112" s="86"/>
       <c r="G112" s="86"/>
-      <c r="H112" s="83"/>
+      <c r="H112" s="89"/>
       <c r="I112" s="86"/>
       <c r="J112" s="86"/>
-      <c r="K112" s="83"/>
+      <c r="K112" s="89"/>
       <c r="N112" s="40"/>
     </row>
     <row r="113" spans="1:15" x14ac:dyDescent="0.3">
@@ -3519,13 +3585,13 @@
         <v>85</v>
       </c>
       <c r="D113" s="86"/>
-      <c r="E113" s="83"/>
+      <c r="E113" s="89"/>
       <c r="F113" s="86"/>
       <c r="G113" s="86"/>
-      <c r="H113" s="83"/>
+      <c r="H113" s="89"/>
       <c r="I113" s="86"/>
       <c r="J113" s="86"/>
-      <c r="K113" s="83"/>
+      <c r="K113" s="89"/>
       <c r="N113" s="40"/>
     </row>
     <row r="114" spans="1:15" x14ac:dyDescent="0.3">
@@ -3536,166 +3602,166 @@
         <v>1</v>
       </c>
       <c r="D114" s="86"/>
-      <c r="E114" s="83"/>
+      <c r="E114" s="89"/>
       <c r="F114" s="86"/>
       <c r="G114" s="86"/>
-      <c r="H114" s="83"/>
+      <c r="H114" s="89"/>
       <c r="I114" s="86"/>
       <c r="J114" s="86"/>
-      <c r="K114" s="83"/>
+      <c r="K114" s="89"/>
       <c r="N114" s="40"/>
     </row>
     <row r="115" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A115" s="43" t="s">
         <v>64</v>
       </c>
-      <c r="C115" s="83">
+      <c r="C115" s="89">
         <v>0</v>
       </c>
-      <c r="D115" s="83"/>
-      <c r="E115" s="83"/>
-      <c r="F115" s="83"/>
-      <c r="G115" s="83"/>
-      <c r="H115" s="83"/>
-      <c r="I115" s="83"/>
-      <c r="J115" s="83"/>
-      <c r="K115" s="83"/>
+      <c r="D115" s="89"/>
+      <c r="E115" s="89"/>
+      <c r="F115" s="89"/>
+      <c r="G115" s="89"/>
+      <c r="H115" s="89"/>
+      <c r="I115" s="89"/>
+      <c r="J115" s="89"/>
+      <c r="K115" s="89"/>
       <c r="N115" s="40"/>
     </row>
     <row r="116" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A116" s="44" t="s">
         <v>65</v>
       </c>
-      <c r="C116" s="83">
+      <c r="C116" s="89">
         <f>MAX(0, SUM(C$110:H$110)-C115)</f>
         <v>180</v>
       </c>
-      <c r="D116" s="83"/>
-      <c r="E116" s="83"/>
-      <c r="F116" s="83"/>
-      <c r="G116" s="83"/>
-      <c r="H116" s="83"/>
-      <c r="I116" s="83"/>
-      <c r="J116" s="83"/>
-      <c r="K116" s="83"/>
+      <c r="D116" s="89"/>
+      <c r="E116" s="89"/>
+      <c r="F116" s="89"/>
+      <c r="G116" s="89"/>
+      <c r="H116" s="89"/>
+      <c r="I116" s="89"/>
+      <c r="J116" s="89"/>
+      <c r="K116" s="89"/>
       <c r="N116" s="40"/>
     </row>
     <row r="117" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A117" s="43" t="s">
         <v>0</v>
       </c>
-      <c r="C117" s="83">
+      <c r="C117" s="89">
         <v>10</v>
       </c>
-      <c r="D117" s="83"/>
-      <c r="E117" s="83"/>
-      <c r="F117" s="83"/>
-      <c r="G117" s="83"/>
-      <c r="H117" s="83"/>
-      <c r="I117" s="83"/>
-      <c r="J117" s="83"/>
-      <c r="K117" s="83"/>
+      <c r="D117" s="89"/>
+      <c r="E117" s="89"/>
+      <c r="F117" s="89"/>
+      <c r="G117" s="89"/>
+      <c r="H117" s="89"/>
+      <c r="I117" s="89"/>
+      <c r="J117" s="89"/>
+      <c r="K117" s="89"/>
       <c r="N117" s="40"/>
     </row>
     <row r="118" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A118" s="44" t="s">
         <v>66</v>
       </c>
-      <c r="C118" s="83">
+      <c r="C118" s="89">
         <f>IF(C117="Unlimited", C116, MIN(C116, C117))</f>
         <v>10</v>
       </c>
-      <c r="D118" s="83"/>
-      <c r="E118" s="83"/>
-      <c r="F118" s="83"/>
-      <c r="G118" s="83"/>
-      <c r="H118" s="83"/>
-      <c r="I118" s="83"/>
-      <c r="J118" s="83"/>
-      <c r="K118" s="83"/>
+      <c r="D118" s="89"/>
+      <c r="E118" s="89"/>
+      <c r="F118" s="89"/>
+      <c r="G118" s="89"/>
+      <c r="H118" s="89"/>
+      <c r="I118" s="89"/>
+      <c r="J118" s="89"/>
+      <c r="K118" s="89"/>
       <c r="N118" s="40"/>
     </row>
     <row r="119" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A119" s="43" t="s">
         <v>71</v>
       </c>
-      <c r="C119" s="85">
-        <v>1</v>
-      </c>
-      <c r="D119" s="85"/>
-      <c r="E119" s="85"/>
-      <c r="F119" s="85"/>
-      <c r="G119" s="85"/>
-      <c r="H119" s="85"/>
-      <c r="I119" s="85"/>
-      <c r="J119" s="85"/>
-      <c r="K119" s="85"/>
+      <c r="C119" s="88">
+        <v>1</v>
+      </c>
+      <c r="D119" s="88"/>
+      <c r="E119" s="88"/>
+      <c r="F119" s="88"/>
+      <c r="G119" s="88"/>
+      <c r="H119" s="88"/>
+      <c r="I119" s="88"/>
+      <c r="J119" s="88"/>
+      <c r="K119" s="88"/>
       <c r="N119" s="40"/>
     </row>
     <row r="120" spans="1:15" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A120" s="44" t="s">
         <v>72</v>
       </c>
-      <c r="C120" s="83">
+      <c r="C120" s="89">
         <f>C119*C118</f>
         <v>10</v>
       </c>
-      <c r="D120" s="83"/>
-      <c r="E120" s="83"/>
-      <c r="F120" s="83"/>
-      <c r="G120" s="83"/>
-      <c r="H120" s="83"/>
-      <c r="I120" s="83"/>
-      <c r="J120" s="83"/>
-      <c r="K120" s="83"/>
+      <c r="D120" s="89"/>
+      <c r="E120" s="89"/>
+      <c r="F120" s="89"/>
+      <c r="G120" s="89"/>
+      <c r="H120" s="89"/>
+      <c r="I120" s="89"/>
+      <c r="J120" s="89"/>
+      <c r="K120" s="89"/>
       <c r="N120" s="40"/>
     </row>
     <row r="121" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A121" s="43" t="s">
         <v>3</v>
       </c>
-      <c r="C121" s="84"/>
-      <c r="D121" s="84"/>
-      <c r="E121" s="84"/>
-      <c r="F121" s="84"/>
-      <c r="G121" s="84"/>
-      <c r="H121" s="84"/>
-      <c r="I121" s="84"/>
-      <c r="J121" s="84"/>
-      <c r="K121" s="84"/>
+      <c r="C121" s="91"/>
+      <c r="D121" s="91"/>
+      <c r="E121" s="91"/>
+      <c r="F121" s="91"/>
+      <c r="G121" s="91"/>
+      <c r="H121" s="91"/>
+      <c r="I121" s="91"/>
+      <c r="J121" s="91"/>
+      <c r="K121" s="91"/>
       <c r="N121" s="40"/>
     </row>
     <row r="122" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A122" s="43" t="s">
         <v>67</v>
       </c>
-      <c r="C122" s="84"/>
-      <c r="D122" s="84"/>
-      <c r="E122" s="84"/>
-      <c r="F122" s="84"/>
-      <c r="G122" s="84"/>
-      <c r="H122" s="84"/>
-      <c r="I122" s="84"/>
-      <c r="J122" s="84"/>
-      <c r="K122" s="84"/>
+      <c r="C122" s="91"/>
+      <c r="D122" s="91"/>
+      <c r="E122" s="91"/>
+      <c r="F122" s="91"/>
+      <c r="G122" s="91"/>
+      <c r="H122" s="91"/>
+      <c r="I122" s="91"/>
+      <c r="J122" s="91"/>
+      <c r="K122" s="91"/>
       <c r="N122" s="40"/>
     </row>
     <row r="123" spans="1:15" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A123" s="45" t="s">
         <v>68</v>
       </c>
-      <c r="C123" s="83">
+      <c r="C123" s="89">
         <f>MIN(C120,IF(OR(C122="Unlimited",C122=""),10^18,C122))</f>
         <v>10</v>
       </c>
-      <c r="D123" s="83"/>
-      <c r="E123" s="83"/>
-      <c r="F123" s="83"/>
-      <c r="G123" s="83"/>
-      <c r="H123" s="83"/>
-      <c r="I123" s="83"/>
-      <c r="J123" s="83"/>
-      <c r="K123" s="83"/>
+      <c r="D123" s="89"/>
+      <c r="E123" s="89"/>
+      <c r="F123" s="89"/>
+      <c r="G123" s="89"/>
+      <c r="H123" s="89"/>
+      <c r="I123" s="89"/>
+      <c r="J123" s="89"/>
+      <c r="K123" s="89"/>
       <c r="N123" s="40"/>
     </row>
     <row r="124" spans="1:15" x14ac:dyDescent="0.3">
@@ -3781,15 +3847,15 @@
       </c>
       <c r="C127" s="86"/>
       <c r="D127" s="86"/>
-      <c r="E127" s="83"/>
+      <c r="E127" s="89"/>
       <c r="F127" s="86"/>
       <c r="G127" s="86"/>
-      <c r="H127" s="83"/>
+      <c r="H127" s="89"/>
       <c r="I127" s="86">
         <v>1</v>
       </c>
       <c r="J127" s="86"/>
-      <c r="K127" s="83"/>
+      <c r="K127" s="89"/>
       <c r="N127" s="40"/>
     </row>
     <row r="128" spans="1:15" x14ac:dyDescent="0.3">
@@ -3798,15 +3864,15 @@
       </c>
       <c r="C128" s="86"/>
       <c r="D128" s="86"/>
-      <c r="E128" s="83"/>
+      <c r="E128" s="89"/>
       <c r="F128" s="86"/>
       <c r="G128" s="86"/>
-      <c r="H128" s="83"/>
+      <c r="H128" s="89"/>
       <c r="I128" s="86" t="s">
         <v>83</v>
       </c>
       <c r="J128" s="86"/>
-      <c r="K128" s="83"/>
+      <c r="K128" s="89"/>
       <c r="N128" s="40"/>
     </row>
     <row r="129" spans="1:15" x14ac:dyDescent="0.3">
@@ -3815,168 +3881,168 @@
       </c>
       <c r="C129" s="86"/>
       <c r="D129" s="86"/>
-      <c r="E129" s="83"/>
+      <c r="E129" s="89"/>
       <c r="F129" s="86"/>
       <c r="G129" s="86"/>
-      <c r="H129" s="83"/>
+      <c r="H129" s="89"/>
       <c r="I129" s="86">
         <v>1</v>
       </c>
       <c r="J129" s="86"/>
-      <c r="K129" s="83"/>
+      <c r="K129" s="89"/>
       <c r="N129" s="40"/>
     </row>
     <row r="130" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A130" s="43" t="s">
         <v>64</v>
       </c>
-      <c r="C130" s="83"/>
-      <c r="D130" s="83"/>
-      <c r="E130" s="83"/>
-      <c r="F130" s="83"/>
-      <c r="G130" s="83"/>
-      <c r="H130" s="83"/>
-      <c r="I130" s="83">
+      <c r="C130" s="89"/>
+      <c r="D130" s="89"/>
+      <c r="E130" s="89"/>
+      <c r="F130" s="89"/>
+      <c r="G130" s="89"/>
+      <c r="H130" s="89"/>
+      <c r="I130" s="89">
         <v>0</v>
       </c>
-      <c r="J130" s="83"/>
-      <c r="K130" s="83"/>
+      <c r="J130" s="89"/>
+      <c r="K130" s="89"/>
       <c r="N130" s="40"/>
     </row>
     <row r="131" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A131" s="44" t="s">
         <v>65</v>
       </c>
-      <c r="C131" s="83"/>
-      <c r="D131" s="83"/>
-      <c r="E131" s="83"/>
-      <c r="F131" s="83"/>
-      <c r="G131" s="83"/>
-      <c r="H131" s="83"/>
-      <c r="I131" s="83">
+      <c r="C131" s="89"/>
+      <c r="D131" s="89"/>
+      <c r="E131" s="89"/>
+      <c r="F131" s="89"/>
+      <c r="G131" s="89"/>
+      <c r="H131" s="89"/>
+      <c r="I131" s="89">
         <f>MAX(0, SUM(I$124:N$124)-I130)</f>
         <v>200</v>
       </c>
-      <c r="J131" s="83"/>
-      <c r="K131" s="83"/>
+      <c r="J131" s="89"/>
+      <c r="K131" s="89"/>
       <c r="N131" s="40"/>
     </row>
     <row r="132" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A132" s="43" t="s">
         <v>0</v>
       </c>
-      <c r="C132" s="83"/>
-      <c r="D132" s="83"/>
-      <c r="E132" s="83"/>
-      <c r="F132" s="83"/>
-      <c r="G132" s="83"/>
-      <c r="H132" s="83"/>
-      <c r="I132" s="83">
+      <c r="C132" s="89"/>
+      <c r="D132" s="89"/>
+      <c r="E132" s="89"/>
+      <c r="F132" s="89"/>
+      <c r="G132" s="89"/>
+      <c r="H132" s="89"/>
+      <c r="I132" s="89">
         <v>10</v>
       </c>
-      <c r="J132" s="83"/>
-      <c r="K132" s="83"/>
+      <c r="J132" s="89"/>
+      <c r="K132" s="89"/>
       <c r="N132" s="40"/>
     </row>
     <row r="133" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A133" s="44" t="s">
         <v>66</v>
       </c>
-      <c r="C133" s="83"/>
-      <c r="D133" s="83"/>
-      <c r="E133" s="83"/>
-      <c r="F133" s="83"/>
-      <c r="G133" s="83"/>
-      <c r="H133" s="83"/>
-      <c r="I133" s="83">
+      <c r="C133" s="89"/>
+      <c r="D133" s="89"/>
+      <c r="E133" s="89"/>
+      <c r="F133" s="89"/>
+      <c r="G133" s="89"/>
+      <c r="H133" s="89"/>
+      <c r="I133" s="89">
         <f>IF(I132="Unlimited", I131, MIN(I131, I132))</f>
         <v>10</v>
       </c>
-      <c r="J133" s="83"/>
-      <c r="K133" s="83"/>
+      <c r="J133" s="89"/>
+      <c r="K133" s="89"/>
       <c r="N133" s="40"/>
     </row>
     <row r="134" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A134" s="43" t="s">
         <v>71</v>
       </c>
-      <c r="C134" s="85"/>
-      <c r="D134" s="85"/>
-      <c r="E134" s="85"/>
-      <c r="F134" s="85"/>
-      <c r="G134" s="85"/>
-      <c r="H134" s="85"/>
-      <c r="I134" s="85">
-        <v>1</v>
-      </c>
-      <c r="J134" s="85"/>
-      <c r="K134" s="85"/>
+      <c r="C134" s="88"/>
+      <c r="D134" s="88"/>
+      <c r="E134" s="88"/>
+      <c r="F134" s="88"/>
+      <c r="G134" s="88"/>
+      <c r="H134" s="88"/>
+      <c r="I134" s="88">
+        <v>1</v>
+      </c>
+      <c r="J134" s="88"/>
+      <c r="K134" s="88"/>
       <c r="N134" s="40"/>
     </row>
     <row r="135" spans="1:15" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A135" s="44" t="s">
         <v>72</v>
       </c>
-      <c r="C135" s="83"/>
-      <c r="D135" s="83"/>
-      <c r="E135" s="83"/>
-      <c r="F135" s="83"/>
-      <c r="G135" s="83"/>
-      <c r="H135" s="83"/>
-      <c r="I135" s="83">
+      <c r="C135" s="89"/>
+      <c r="D135" s="89"/>
+      <c r="E135" s="89"/>
+      <c r="F135" s="89"/>
+      <c r="G135" s="89"/>
+      <c r="H135" s="89"/>
+      <c r="I135" s="89">
         <f>I134*I133</f>
         <v>10</v>
       </c>
-      <c r="J135" s="83"/>
-      <c r="K135" s="83"/>
+      <c r="J135" s="89"/>
+      <c r="K135" s="89"/>
       <c r="N135" s="40"/>
     </row>
     <row r="136" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A136" s="43" t="s">
         <v>3</v>
       </c>
-      <c r="C136" s="84"/>
-      <c r="D136" s="84"/>
-      <c r="E136" s="84"/>
-      <c r="F136" s="84"/>
-      <c r="G136" s="84"/>
-      <c r="H136" s="84"/>
-      <c r="I136" s="84"/>
-      <c r="J136" s="84"/>
-      <c r="K136" s="84"/>
+      <c r="C136" s="91"/>
+      <c r="D136" s="91"/>
+      <c r="E136" s="91"/>
+      <c r="F136" s="91"/>
+      <c r="G136" s="91"/>
+      <c r="H136" s="91"/>
+      <c r="I136" s="91"/>
+      <c r="J136" s="91"/>
+      <c r="K136" s="91"/>
       <c r="N136" s="40"/>
     </row>
     <row r="137" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A137" s="43" t="s">
         <v>67</v>
       </c>
-      <c r="C137" s="84"/>
-      <c r="D137" s="84"/>
-      <c r="E137" s="84"/>
-      <c r="F137" s="84"/>
-      <c r="G137" s="84"/>
-      <c r="H137" s="84"/>
-      <c r="I137" s="84"/>
-      <c r="J137" s="84"/>
-      <c r="K137" s="84"/>
+      <c r="C137" s="91"/>
+      <c r="D137" s="91"/>
+      <c r="E137" s="91"/>
+      <c r="F137" s="91"/>
+      <c r="G137" s="91"/>
+      <c r="H137" s="91"/>
+      <c r="I137" s="91"/>
+      <c r="J137" s="91"/>
+      <c r="K137" s="91"/>
       <c r="N137" s="40"/>
     </row>
     <row r="138" spans="1:15" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A138" s="45" t="s">
         <v>68</v>
       </c>
-      <c r="C138" s="83"/>
-      <c r="D138" s="83"/>
-      <c r="E138" s="83"/>
-      <c r="F138" s="83"/>
-      <c r="G138" s="83"/>
-      <c r="H138" s="83"/>
-      <c r="I138" s="83">
+      <c r="C138" s="89"/>
+      <c r="D138" s="89"/>
+      <c r="E138" s="89"/>
+      <c r="F138" s="89"/>
+      <c r="G138" s="89"/>
+      <c r="H138" s="89"/>
+      <c r="I138" s="89">
         <f>MIN(I135,IF(OR(I137="Unlimited",I137=""),10^18,I137))</f>
         <v>10</v>
       </c>
-      <c r="J138" s="83"/>
-      <c r="K138" s="83"/>
+      <c r="J138" s="89"/>
+      <c r="K138" s="89"/>
       <c r="N138" s="40"/>
     </row>
     <row r="139" spans="1:15" x14ac:dyDescent="0.3">
@@ -5121,22 +5187,22 @@
         <v>1</v>
       </c>
       <c r="D207" s="86"/>
-      <c r="E207" s="83"/>
+      <c r="E207" s="89"/>
       <c r="F207" s="86">
         <v>1</v>
       </c>
       <c r="G207" s="86"/>
-      <c r="H207" s="83"/>
+      <c r="H207" s="89"/>
       <c r="I207" s="86">
         <v>1</v>
       </c>
       <c r="J207" s="86"/>
-      <c r="K207" s="83"/>
+      <c r="K207" s="89"/>
       <c r="L207" s="86">
         <v>1</v>
       </c>
       <c r="M207" s="86"/>
-      <c r="N207" s="83"/>
+      <c r="N207" s="89"/>
       <c r="O207" s="72"/>
     </row>
     <row r="208" spans="1:17" x14ac:dyDescent="0.3">
@@ -5147,22 +5213,22 @@
         <v>139</v>
       </c>
       <c r="D208" s="86"/>
-      <c r="E208" s="83"/>
+      <c r="E208" s="89"/>
       <c r="F208" s="86" t="s">
         <v>140</v>
       </c>
       <c r="G208" s="86"/>
-      <c r="H208" s="83"/>
+      <c r="H208" s="89"/>
       <c r="I208" s="86" t="s">
         <v>141</v>
       </c>
       <c r="J208" s="86"/>
-      <c r="K208" s="83"/>
+      <c r="K208" s="89"/>
       <c r="L208" s="86" t="s">
         <v>142</v>
       </c>
       <c r="M208" s="86"/>
-      <c r="N208" s="83"/>
+      <c r="N208" s="89"/>
       <c r="O208" s="73"/>
     </row>
     <row r="209" spans="1:17" x14ac:dyDescent="0.3">
@@ -5173,78 +5239,78 @@
         <v>1</v>
       </c>
       <c r="D209" s="86"/>
-      <c r="E209" s="83"/>
+      <c r="E209" s="89"/>
       <c r="F209" s="86">
         <v>1</v>
       </c>
       <c r="G209" s="86"/>
-      <c r="H209" s="83"/>
+      <c r="H209" s="89"/>
       <c r="I209" s="86">
         <v>1</v>
       </c>
       <c r="J209" s="86"/>
-      <c r="K209" s="83"/>
+      <c r="K209" s="89"/>
       <c r="L209" s="86">
         <v>1</v>
       </c>
       <c r="M209" s="86"/>
-      <c r="N209" s="83"/>
+      <c r="N209" s="89"/>
       <c r="O209" s="72"/>
     </row>
     <row r="210" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A210" s="43" t="s">
         <v>64</v>
       </c>
-      <c r="C210" s="83">
+      <c r="C210" s="89">
         <v>0</v>
       </c>
-      <c r="D210" s="83"/>
-      <c r="E210" s="83"/>
-      <c r="F210" s="83">
+      <c r="D210" s="89"/>
+      <c r="E210" s="89"/>
+      <c r="F210" s="89">
         <v>0</v>
       </c>
-      <c r="G210" s="83"/>
-      <c r="H210" s="83"/>
-      <c r="I210" s="83">
+      <c r="G210" s="89"/>
+      <c r="H210" s="89"/>
+      <c r="I210" s="89">
         <v>0</v>
       </c>
-      <c r="J210" s="83"/>
-      <c r="K210" s="83"/>
-      <c r="L210" s="83">
+      <c r="J210" s="89"/>
+      <c r="K210" s="89"/>
+      <c r="L210" s="89">
         <v>0</v>
       </c>
-      <c r="M210" s="83"/>
-      <c r="N210" s="83"/>
+      <c r="M210" s="89"/>
+      <c r="N210" s="89"/>
       <c r="O210" s="72"/>
     </row>
     <row r="211" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A211" s="44" t="s">
         <v>65</v>
       </c>
-      <c r="C211" s="83">
+      <c r="C211" s="89">
         <f>MAX(0, SUM(C$50:E$50)*C214-C210)</f>
         <v>50</v>
       </c>
-      <c r="D211" s="83"/>
-      <c r="E211" s="83"/>
-      <c r="F211" s="83">
+      <c r="D211" s="89"/>
+      <c r="E211" s="89"/>
+      <c r="F211" s="89">
         <f>MAX(0, SUM(F$50:H$50)-F210)</f>
         <v>100</v>
       </c>
-      <c r="G211" s="83"/>
-      <c r="H211" s="83"/>
-      <c r="I211" s="83">
+      <c r="G211" s="89"/>
+      <c r="H211" s="89"/>
+      <c r="I211" s="89">
         <f>MAX(0, SUM(I$50:K$50)-I210)</f>
         <v>100</v>
       </c>
-      <c r="J211" s="83"/>
-      <c r="K211" s="83"/>
-      <c r="L211" s="83">
+      <c r="J211" s="89"/>
+      <c r="K211" s="89"/>
+      <c r="L211" s="89">
         <f>MAX(0, SUM(L$50:N$50)-L210)</f>
         <v>100</v>
       </c>
-      <c r="M211" s="83"/>
-      <c r="N211" s="83"/>
+      <c r="M211" s="89"/>
+      <c r="N211" s="89"/>
       <c r="O211" s="72"/>
       <c r="P211" s="6"/>
       <c r="Q211" s="6"/>
@@ -5253,26 +5319,26 @@
       <c r="A212" s="43" t="s">
         <v>0</v>
       </c>
-      <c r="C212" s="83">
+      <c r="C212" s="89">
         <v>10</v>
       </c>
-      <c r="D212" s="83"/>
-      <c r="E212" s="83"/>
-      <c r="F212" s="83">
+      <c r="D212" s="89"/>
+      <c r="E212" s="89"/>
+      <c r="F212" s="89">
         <v>10</v>
       </c>
-      <c r="G212" s="83"/>
-      <c r="H212" s="83"/>
-      <c r="I212" s="83">
+      <c r="G212" s="89"/>
+      <c r="H212" s="89"/>
+      <c r="I212" s="89">
         <v>10</v>
       </c>
-      <c r="J212" s="83"/>
-      <c r="K212" s="83"/>
-      <c r="L212" s="83">
+      <c r="J212" s="89"/>
+      <c r="K212" s="89"/>
+      <c r="L212" s="89">
         <v>10</v>
       </c>
-      <c r="M212" s="83"/>
-      <c r="N212" s="83"/>
+      <c r="M212" s="89"/>
+      <c r="N212" s="89"/>
       <c r="O212" s="72"/>
       <c r="Q212" s="6"/>
     </row>
@@ -5280,30 +5346,30 @@
       <c r="A213" s="44" t="s">
         <v>66</v>
       </c>
-      <c r="C213" s="83">
+      <c r="C213" s="89">
         <f>IF(C212="Unlimited", C211, MIN(C211, C212))</f>
         <v>10</v>
       </c>
-      <c r="D213" s="83"/>
-      <c r="E213" s="83"/>
-      <c r="F213" s="83">
+      <c r="D213" s="89"/>
+      <c r="E213" s="89"/>
+      <c r="F213" s="89">
         <f>IF(F212="Unlimited", F211, MIN(F211, F212))</f>
         <v>10</v>
       </c>
-      <c r="G213" s="83"/>
-      <c r="H213" s="83"/>
-      <c r="I213" s="83">
+      <c r="G213" s="89"/>
+      <c r="H213" s="89"/>
+      <c r="I213" s="89">
         <f>IF(I212="Unlimited", I211, MIN(I211, I212))</f>
         <v>10</v>
       </c>
-      <c r="J213" s="83"/>
-      <c r="K213" s="83"/>
-      <c r="L213" s="83">
+      <c r="J213" s="89"/>
+      <c r="K213" s="89"/>
+      <c r="L213" s="89">
         <f>IF(L212="Unlimited", L211, MIN(L211, L212))</f>
         <v>10</v>
       </c>
-      <c r="M213" s="83"/>
-      <c r="N213" s="83"/>
+      <c r="M213" s="89"/>
+      <c r="N213" s="89"/>
       <c r="O213" s="72"/>
       <c r="P213" s="6"/>
       <c r="Q213" s="6"/>
@@ -5312,26 +5378,26 @@
       <c r="A214" s="43" t="s">
         <v>71</v>
       </c>
-      <c r="C214" s="85">
+      <c r="C214" s="88">
         <v>0.5</v>
       </c>
-      <c r="D214" s="85"/>
-      <c r="E214" s="85"/>
-      <c r="F214" s="85">
+      <c r="D214" s="88"/>
+      <c r="E214" s="88"/>
+      <c r="F214" s="88">
         <v>0.5</v>
       </c>
-      <c r="G214" s="85"/>
-      <c r="H214" s="85"/>
-      <c r="I214" s="85">
+      <c r="G214" s="88"/>
+      <c r="H214" s="88"/>
+      <c r="I214" s="88">
         <v>0.5</v>
       </c>
-      <c r="J214" s="85"/>
-      <c r="K214" s="85"/>
-      <c r="L214" s="85">
+      <c r="J214" s="88"/>
+      <c r="K214" s="88"/>
+      <c r="L214" s="88">
         <v>0.5</v>
       </c>
-      <c r="M214" s="85"/>
-      <c r="N214" s="85"/>
+      <c r="M214" s="88"/>
+      <c r="N214" s="88"/>
       <c r="O214" s="74"/>
       <c r="Q214" s="6"/>
     </row>
@@ -5339,29 +5405,29 @@
       <c r="A215" s="44" t="s">
         <v>72</v>
       </c>
-      <c r="C215" s="83">
+      <c r="C215" s="89">
         <f>C213</f>
         <v>10</v>
       </c>
-      <c r="D215" s="83"/>
-      <c r="E215" s="83"/>
-      <c r="F215" s="83">
+      <c r="D215" s="89"/>
+      <c r="E215" s="89"/>
+      <c r="F215" s="89">
         <f t="shared" ref="F215" si="30">F213</f>
         <v>10</v>
       </c>
-      <c r="G215" s="83"/>
-      <c r="H215" s="83"/>
-      <c r="I215" s="83">
+      <c r="G215" s="89"/>
+      <c r="H215" s="89"/>
+      <c r="I215" s="89">
         <f t="shared" ref="I215" si="31">I213</f>
         <v>10</v>
       </c>
-      <c r="J215" s="83"/>
-      <c r="K215" s="83"/>
-      <c r="L215" s="83">
+      <c r="J215" s="89"/>
+      <c r="K215" s="89"/>
+      <c r="L215" s="89">
         <f t="shared" ref="L215" si="32">L213</f>
         <v>10</v>
       </c>
-      <c r="M215" s="83"/>
+      <c r="M215" s="89"/>
       <c r="N215" s="87"/>
       <c r="O215" s="72"/>
     </row>
@@ -5587,46 +5653,46 @@
       <c r="A226" s="43" t="s">
         <v>64</v>
       </c>
-      <c r="C226" s="83">
+      <c r="C226" s="89">
         <v>0</v>
       </c>
-      <c r="D226" s="83"/>
-      <c r="E226" s="83"/>
-      <c r="F226" s="83"/>
-      <c r="G226" s="83"/>
-      <c r="H226" s="83"/>
-      <c r="I226" s="83">
+      <c r="D226" s="89"/>
+      <c r="E226" s="89"/>
+      <c r="F226" s="89"/>
+      <c r="G226" s="89"/>
+      <c r="H226" s="89"/>
+      <c r="I226" s="89">
         <v>0</v>
       </c>
-      <c r="J226" s="83"/>
-      <c r="K226" s="83"/>
-      <c r="L226" s="83"/>
-      <c r="M226" s="83"/>
-      <c r="N226" s="83"/>
+      <c r="J226" s="89"/>
+      <c r="K226" s="89"/>
+      <c r="L226" s="89"/>
+      <c r="M226" s="89"/>
+      <c r="N226" s="89"/>
       <c r="O226" s="72"/>
     </row>
     <row r="227" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A227" s="44" t="s">
         <v>65</v>
       </c>
-      <c r="C227" s="83">
+      <c r="C227" s="89">
         <f>MAX(0, SUM(C$50:H$50)*C230-C226)</f>
         <v>100</v>
       </c>
-      <c r="D227" s="83"/>
-      <c r="E227" s="83"/>
-      <c r="F227" s="83"/>
-      <c r="G227" s="83"/>
-      <c r="H227" s="83"/>
-      <c r="I227" s="83">
+      <c r="D227" s="89"/>
+      <c r="E227" s="89"/>
+      <c r="F227" s="89"/>
+      <c r="G227" s="89"/>
+      <c r="H227" s="89"/>
+      <c r="I227" s="89">
         <f>MAX(0, SUM(I$50:K$50)*I230-I226)</f>
         <v>50</v>
       </c>
-      <c r="J227" s="83"/>
-      <c r="K227" s="83"/>
-      <c r="L227" s="83"/>
-      <c r="M227" s="83"/>
-      <c r="N227" s="83"/>
+      <c r="J227" s="89"/>
+      <c r="K227" s="89"/>
+      <c r="L227" s="89"/>
+      <c r="M227" s="89"/>
+      <c r="N227" s="89"/>
       <c r="O227" s="72"/>
       <c r="P227" s="6"/>
       <c r="Q227" s="6"/>
@@ -5635,22 +5701,22 @@
       <c r="A228" s="43" t="s">
         <v>0</v>
       </c>
-      <c r="C228" s="83">
+      <c r="C228" s="89">
         <v>10</v>
       </c>
-      <c r="D228" s="83"/>
-      <c r="E228" s="83"/>
-      <c r="F228" s="83"/>
-      <c r="G228" s="83"/>
-      <c r="H228" s="83"/>
-      <c r="I228" s="83">
+      <c r="D228" s="89"/>
+      <c r="E228" s="89"/>
+      <c r="F228" s="89"/>
+      <c r="G228" s="89"/>
+      <c r="H228" s="89"/>
+      <c r="I228" s="89">
         <v>10</v>
       </c>
-      <c r="J228" s="83"/>
-      <c r="K228" s="83"/>
-      <c r="L228" s="83"/>
-      <c r="M228" s="83"/>
-      <c r="N228" s="83"/>
+      <c r="J228" s="89"/>
+      <c r="K228" s="89"/>
+      <c r="L228" s="89"/>
+      <c r="M228" s="89"/>
+      <c r="N228" s="89"/>
       <c r="O228" s="72"/>
       <c r="Q228" s="6"/>
     </row>
@@ -5658,24 +5724,24 @@
       <c r="A229" s="44" t="s">
         <v>66</v>
       </c>
-      <c r="C229" s="83">
+      <c r="C229" s="89">
         <f>IF(C228="Unlimited", C227, MIN(C227, C228))</f>
         <v>10</v>
       </c>
-      <c r="D229" s="83"/>
-      <c r="E229" s="83"/>
-      <c r="F229" s="83"/>
-      <c r="G229" s="83"/>
-      <c r="H229" s="83"/>
-      <c r="I229" s="83">
+      <c r="D229" s="89"/>
+      <c r="E229" s="89"/>
+      <c r="F229" s="89"/>
+      <c r="G229" s="89"/>
+      <c r="H229" s="89"/>
+      <c r="I229" s="89">
         <f>IF(I228="Unlimited", I227, MIN(I227, I228))</f>
         <v>10</v>
       </c>
-      <c r="J229" s="83"/>
-      <c r="K229" s="83"/>
-      <c r="L229" s="83"/>
-      <c r="M229" s="83"/>
-      <c r="N229" s="83"/>
+      <c r="J229" s="89"/>
+      <c r="K229" s="89"/>
+      <c r="L229" s="89"/>
+      <c r="M229" s="89"/>
+      <c r="N229" s="89"/>
       <c r="O229" s="72"/>
       <c r="P229" s="6"/>
       <c r="Q229" s="6"/>
@@ -5684,22 +5750,22 @@
       <c r="A230" s="43" t="s">
         <v>71</v>
       </c>
-      <c r="C230" s="85">
+      <c r="C230" s="88">
         <v>0.5</v>
       </c>
-      <c r="D230" s="85"/>
-      <c r="E230" s="85"/>
-      <c r="F230" s="85"/>
-      <c r="G230" s="85"/>
-      <c r="H230" s="85"/>
-      <c r="I230" s="85">
+      <c r="D230" s="88"/>
+      <c r="E230" s="88"/>
+      <c r="F230" s="88"/>
+      <c r="G230" s="88"/>
+      <c r="H230" s="88"/>
+      <c r="I230" s="88">
         <v>0.5</v>
       </c>
-      <c r="J230" s="85"/>
-      <c r="K230" s="85"/>
-      <c r="L230" s="85"/>
-      <c r="M230" s="85"/>
-      <c r="N230" s="85"/>
+      <c r="J230" s="88"/>
+      <c r="K230" s="88"/>
+      <c r="L230" s="88"/>
+      <c r="M230" s="88"/>
+      <c r="N230" s="88"/>
       <c r="O230" s="74"/>
       <c r="Q230" s="6"/>
     </row>
@@ -5707,24 +5773,24 @@
       <c r="A231" s="44" t="s">
         <v>72</v>
       </c>
-      <c r="C231" s="83">
+      <c r="C231" s="89">
         <f>C229</f>
         <v>10</v>
       </c>
-      <c r="D231" s="83"/>
-      <c r="E231" s="83"/>
-      <c r="F231" s="83"/>
-      <c r="G231" s="83"/>
-      <c r="H231" s="83"/>
-      <c r="I231" s="83">
+      <c r="D231" s="89"/>
+      <c r="E231" s="89"/>
+      <c r="F231" s="89"/>
+      <c r="G231" s="89"/>
+      <c r="H231" s="89"/>
+      <c r="I231" s="89">
         <f>I229</f>
         <v>10</v>
       </c>
-      <c r="J231" s="83"/>
-      <c r="K231" s="83"/>
-      <c r="L231" s="83"/>
-      <c r="M231" s="83"/>
-      <c r="N231" s="83"/>
+      <c r="J231" s="89"/>
+      <c r="K231" s="89"/>
+      <c r="L231" s="89"/>
+      <c r="M231" s="89"/>
+      <c r="N231" s="89"/>
       <c r="O231" s="72"/>
     </row>
     <row r="232" spans="1:17" x14ac:dyDescent="0.3">
@@ -5949,46 +6015,46 @@
       <c r="A242" s="43" t="s">
         <v>64</v>
       </c>
-      <c r="C242" s="83">
+      <c r="C242" s="89">
         <v>0</v>
       </c>
-      <c r="D242" s="83"/>
-      <c r="E242" s="83"/>
-      <c r="F242" s="83"/>
-      <c r="G242" s="83"/>
-      <c r="H242" s="83"/>
-      <c r="I242" s="83">
+      <c r="D242" s="89"/>
+      <c r="E242" s="89"/>
+      <c r="F242" s="89"/>
+      <c r="G242" s="89"/>
+      <c r="H242" s="89"/>
+      <c r="I242" s="89">
         <v>0</v>
       </c>
-      <c r="J242" s="83"/>
-      <c r="K242" s="83"/>
-      <c r="L242" s="83"/>
-      <c r="M242" s="83"/>
-      <c r="N242" s="83"/>
+      <c r="J242" s="89"/>
+      <c r="K242" s="89"/>
+      <c r="L242" s="89"/>
+      <c r="M242" s="89"/>
+      <c r="N242" s="89"/>
       <c r="O242" s="72"/>
     </row>
     <row r="243" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A243" s="44" t="s">
         <v>65</v>
       </c>
-      <c r="C243" s="83">
+      <c r="C243" s="89">
         <f>MAX(0, SUM(C$50:H$50)*C246-C242)</f>
         <v>100</v>
       </c>
-      <c r="D243" s="83"/>
-      <c r="E243" s="83"/>
-      <c r="F243" s="83"/>
-      <c r="G243" s="83"/>
-      <c r="H243" s="83"/>
-      <c r="I243" s="83">
+      <c r="D243" s="89"/>
+      <c r="E243" s="89"/>
+      <c r="F243" s="89"/>
+      <c r="G243" s="89"/>
+      <c r="H243" s="89"/>
+      <c r="I243" s="89">
         <f>MAX(0, SUM(I$50:N$50)*I246-I242)</f>
         <v>100</v>
       </c>
-      <c r="J243" s="83"/>
-      <c r="K243" s="83"/>
-      <c r="L243" s="83"/>
-      <c r="M243" s="83"/>
-      <c r="N243" s="83"/>
+      <c r="J243" s="89"/>
+      <c r="K243" s="89"/>
+      <c r="L243" s="89"/>
+      <c r="M243" s="89"/>
+      <c r="N243" s="89"/>
       <c r="O243" s="72"/>
       <c r="P243" s="6"/>
       <c r="Q243" s="6"/>
@@ -5997,22 +6063,22 @@
       <c r="A244" s="43" t="s">
         <v>0</v>
       </c>
-      <c r="C244" s="83">
+      <c r="C244" s="89">
         <v>10</v>
       </c>
-      <c r="D244" s="83"/>
-      <c r="E244" s="83"/>
-      <c r="F244" s="83"/>
-      <c r="G244" s="83"/>
-      <c r="H244" s="83"/>
-      <c r="I244" s="83">
+      <c r="D244" s="89"/>
+      <c r="E244" s="89"/>
+      <c r="F244" s="89"/>
+      <c r="G244" s="89"/>
+      <c r="H244" s="89"/>
+      <c r="I244" s="89">
         <v>10</v>
       </c>
-      <c r="J244" s="83"/>
-      <c r="K244" s="83"/>
-      <c r="L244" s="83"/>
-      <c r="M244" s="83"/>
-      <c r="N244" s="83"/>
+      <c r="J244" s="89"/>
+      <c r="K244" s="89"/>
+      <c r="L244" s="89"/>
+      <c r="M244" s="89"/>
+      <c r="N244" s="89"/>
       <c r="O244" s="72"/>
       <c r="Q244" s="6"/>
     </row>
@@ -6020,24 +6086,24 @@
       <c r="A245" s="44" t="s">
         <v>66</v>
       </c>
-      <c r="C245" s="83">
+      <c r="C245" s="89">
         <f>IF(C244="Unlimited", C243, MIN(C243, C244))</f>
         <v>10</v>
       </c>
-      <c r="D245" s="83"/>
-      <c r="E245" s="83"/>
-      <c r="F245" s="83"/>
-      <c r="G245" s="83"/>
-      <c r="H245" s="83"/>
-      <c r="I245" s="83">
+      <c r="D245" s="89"/>
+      <c r="E245" s="89"/>
+      <c r="F245" s="89"/>
+      <c r="G245" s="89"/>
+      <c r="H245" s="89"/>
+      <c r="I245" s="89">
         <f>IF(I244="Unlimited", I243, MIN(I243, I244))</f>
         <v>10</v>
       </c>
-      <c r="J245" s="83"/>
-      <c r="K245" s="83"/>
-      <c r="L245" s="83"/>
-      <c r="M245" s="83"/>
-      <c r="N245" s="83"/>
+      <c r="J245" s="89"/>
+      <c r="K245" s="89"/>
+      <c r="L245" s="89"/>
+      <c r="M245" s="89"/>
+      <c r="N245" s="89"/>
       <c r="O245" s="72"/>
       <c r="P245" s="6"/>
       <c r="Q245" s="6"/>
@@ -6046,22 +6112,22 @@
       <c r="A246" s="43" t="s">
         <v>71</v>
       </c>
-      <c r="C246" s="85">
+      <c r="C246" s="88">
         <v>0.5</v>
       </c>
-      <c r="D246" s="85"/>
-      <c r="E246" s="85"/>
-      <c r="F246" s="85"/>
-      <c r="G246" s="85"/>
-      <c r="H246" s="85"/>
-      <c r="I246" s="85">
+      <c r="D246" s="88"/>
+      <c r="E246" s="88"/>
+      <c r="F246" s="88"/>
+      <c r="G246" s="88"/>
+      <c r="H246" s="88"/>
+      <c r="I246" s="88">
         <v>0.5</v>
       </c>
-      <c r="J246" s="85"/>
-      <c r="K246" s="85"/>
-      <c r="L246" s="85"/>
-      <c r="M246" s="85"/>
-      <c r="N246" s="85"/>
+      <c r="J246" s="88"/>
+      <c r="K246" s="88"/>
+      <c r="L246" s="88"/>
+      <c r="M246" s="88"/>
+      <c r="N246" s="88"/>
       <c r="O246" s="74"/>
       <c r="Q246" s="6"/>
     </row>
@@ -6069,24 +6135,24 @@
       <c r="A247" s="44" t="s">
         <v>72</v>
       </c>
-      <c r="C247" s="83">
+      <c r="C247" s="89">
         <f>C245</f>
         <v>10</v>
       </c>
-      <c r="D247" s="83"/>
-      <c r="E247" s="83"/>
-      <c r="F247" s="83"/>
-      <c r="G247" s="83"/>
-      <c r="H247" s="83"/>
-      <c r="I247" s="83">
+      <c r="D247" s="89"/>
+      <c r="E247" s="89"/>
+      <c r="F247" s="89"/>
+      <c r="G247" s="89"/>
+      <c r="H247" s="89"/>
+      <c r="I247" s="89">
         <f>I245</f>
         <v>10</v>
       </c>
-      <c r="J247" s="83"/>
-      <c r="K247" s="83"/>
-      <c r="L247" s="83"/>
-      <c r="M247" s="83"/>
-      <c r="N247" s="83"/>
+      <c r="J247" s="89"/>
+      <c r="K247" s="89"/>
+      <c r="L247" s="89"/>
+      <c r="M247" s="89"/>
+      <c r="N247" s="89"/>
       <c r="O247" s="72"/>
     </row>
     <row r="248" spans="1:17" x14ac:dyDescent="0.3">
@@ -7081,22 +7147,22 @@
         <v>1</v>
       </c>
       <c r="D305" s="86"/>
-      <c r="E305" s="83"/>
+      <c r="E305" s="89"/>
       <c r="F305" s="86">
         <v>1</v>
       </c>
       <c r="G305" s="86"/>
-      <c r="H305" s="83"/>
+      <c r="H305" s="89"/>
       <c r="I305" s="86">
         <v>1</v>
       </c>
       <c r="J305" s="86"/>
-      <c r="K305" s="83"/>
+      <c r="K305" s="89"/>
       <c r="L305" s="86">
         <v>1</v>
       </c>
       <c r="M305" s="86"/>
-      <c r="N305" s="83"/>
+      <c r="N305" s="89"/>
       <c r="O305" s="72"/>
     </row>
     <row r="306" spans="1:17" x14ac:dyDescent="0.3">
@@ -7107,22 +7173,22 @@
         <v>139</v>
       </c>
       <c r="D306" s="86"/>
-      <c r="E306" s="83"/>
+      <c r="E306" s="89"/>
       <c r="F306" s="86" t="s">
         <v>140</v>
       </c>
       <c r="G306" s="86"/>
-      <c r="H306" s="83"/>
+      <c r="H306" s="89"/>
       <c r="I306" s="86" t="s">
         <v>141</v>
       </c>
       <c r="J306" s="86"/>
-      <c r="K306" s="83"/>
+      <c r="K306" s="89"/>
       <c r="L306" s="86" t="s">
         <v>142</v>
       </c>
       <c r="M306" s="86"/>
-      <c r="N306" s="83"/>
+      <c r="N306" s="89"/>
       <c r="O306" s="73"/>
     </row>
     <row r="307" spans="1:17" x14ac:dyDescent="0.3">
@@ -7133,78 +7199,78 @@
         <v>1</v>
       </c>
       <c r="D307" s="86"/>
-      <c r="E307" s="83"/>
+      <c r="E307" s="89"/>
       <c r="F307" s="86">
         <v>1</v>
       </c>
       <c r="G307" s="86"/>
-      <c r="H307" s="83"/>
+      <c r="H307" s="89"/>
       <c r="I307" s="86">
         <v>1</v>
       </c>
       <c r="J307" s="86"/>
-      <c r="K307" s="83"/>
+      <c r="K307" s="89"/>
       <c r="L307" s="86">
         <v>1</v>
       </c>
       <c r="M307" s="86"/>
-      <c r="N307" s="83"/>
+      <c r="N307" s="89"/>
       <c r="O307" s="72"/>
     </row>
     <row r="308" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A308" s="43" t="s">
         <v>64</v>
       </c>
-      <c r="C308" s="83">
+      <c r="C308" s="89">
         <v>0</v>
       </c>
-      <c r="D308" s="83"/>
-      <c r="E308" s="83"/>
-      <c r="F308" s="83">
+      <c r="D308" s="89"/>
+      <c r="E308" s="89"/>
+      <c r="F308" s="89">
         <v>0</v>
       </c>
-      <c r="G308" s="83"/>
-      <c r="H308" s="83"/>
-      <c r="I308" s="83">
+      <c r="G308" s="89"/>
+      <c r="H308" s="89"/>
+      <c r="I308" s="89">
         <v>0</v>
       </c>
-      <c r="J308" s="83"/>
-      <c r="K308" s="83"/>
-      <c r="L308" s="83">
+      <c r="J308" s="89"/>
+      <c r="K308" s="89"/>
+      <c r="L308" s="89">
         <v>0</v>
       </c>
-      <c r="M308" s="83"/>
-      <c r="N308" s="83"/>
+      <c r="M308" s="89"/>
+      <c r="N308" s="89"/>
       <c r="O308" s="72"/>
     </row>
     <row r="309" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A309" s="44" t="s">
         <v>65</v>
       </c>
-      <c r="C309" s="83">
+      <c r="C309" s="89">
         <f>MAX(0, SUM(C$50:E$50))</f>
         <v>100</v>
       </c>
-      <c r="D309" s="83"/>
-      <c r="E309" s="83"/>
-      <c r="F309" s="83">
+      <c r="D309" s="89"/>
+      <c r="E309" s="89"/>
+      <c r="F309" s="89">
         <f>MAX(0, SUM(F$50:H$50))</f>
         <v>100</v>
       </c>
-      <c r="G309" s="83"/>
-      <c r="H309" s="83"/>
-      <c r="I309" s="83">
+      <c r="G309" s="89"/>
+      <c r="H309" s="89"/>
+      <c r="I309" s="89">
         <f>MAX(0, SUM(I$50:K$50))</f>
         <v>100</v>
       </c>
-      <c r="J309" s="83"/>
-      <c r="K309" s="83"/>
-      <c r="L309" s="83">
+      <c r="J309" s="89"/>
+      <c r="K309" s="89"/>
+      <c r="L309" s="89">
         <f>MAX(0, SUM(L$50:N$50))</f>
         <v>100</v>
       </c>
-      <c r="M309" s="83"/>
-      <c r="N309" s="83"/>
+      <c r="M309" s="89"/>
+      <c r="N309" s="89"/>
       <c r="O309" s="72"/>
       <c r="P309" s="6"/>
       <c r="Q309" s="6"/>
@@ -7213,26 +7279,26 @@
       <c r="A310" s="43" t="s">
         <v>0</v>
       </c>
-      <c r="C310" s="83">
+      <c r="C310" s="89">
         <v>0</v>
       </c>
-      <c r="D310" s="83"/>
-      <c r="E310" s="83"/>
-      <c r="F310" s="83">
+      <c r="D310" s="89"/>
+      <c r="E310" s="89"/>
+      <c r="F310" s="89">
         <v>0</v>
       </c>
-      <c r="G310" s="83"/>
-      <c r="H310" s="83"/>
-      <c r="I310" s="83">
+      <c r="G310" s="89"/>
+      <c r="H310" s="89"/>
+      <c r="I310" s="89">
         <v>0</v>
       </c>
-      <c r="J310" s="83"/>
-      <c r="K310" s="83"/>
-      <c r="L310" s="83">
+      <c r="J310" s="89"/>
+      <c r="K310" s="89"/>
+      <c r="L310" s="89">
         <v>0</v>
       </c>
-      <c r="M310" s="83"/>
-      <c r="N310" s="83"/>
+      <c r="M310" s="89"/>
+      <c r="N310" s="89"/>
       <c r="O310" s="72"/>
       <c r="Q310" s="6"/>
     </row>
@@ -7240,30 +7306,30 @@
       <c r="A311" s="44" t="s">
         <v>66</v>
       </c>
-      <c r="C311" s="83">
+      <c r="C311" s="89">
         <f>C309</f>
         <v>100</v>
       </c>
-      <c r="D311" s="83"/>
-      <c r="E311" s="83"/>
-      <c r="F311" s="83">
+      <c r="D311" s="89"/>
+      <c r="E311" s="89"/>
+      <c r="F311" s="89">
         <f>F309</f>
         <v>100</v>
       </c>
-      <c r="G311" s="83"/>
-      <c r="H311" s="83"/>
-      <c r="I311" s="83">
+      <c r="G311" s="89"/>
+      <c r="H311" s="89"/>
+      <c r="I311" s="89">
         <f>I309</f>
         <v>100</v>
       </c>
-      <c r="J311" s="83"/>
-      <c r="K311" s="83"/>
-      <c r="L311" s="83">
+      <c r="J311" s="89"/>
+      <c r="K311" s="89"/>
+      <c r="L311" s="89">
         <f>L309</f>
         <v>100</v>
       </c>
-      <c r="M311" s="83"/>
-      <c r="N311" s="83"/>
+      <c r="M311" s="89"/>
+      <c r="N311" s="89"/>
       <c r="O311" s="72"/>
       <c r="P311" s="6"/>
       <c r="Q311" s="6"/>
@@ -7272,26 +7338,26 @@
       <c r="A312" s="43" t="s">
         <v>71</v>
       </c>
-      <c r="C312" s="85">
+      <c r="C312" s="88">
         <v>0.1</v>
       </c>
-      <c r="D312" s="85"/>
-      <c r="E312" s="85"/>
-      <c r="F312" s="85">
+      <c r="D312" s="88"/>
+      <c r="E312" s="88"/>
+      <c r="F312" s="88">
         <v>0.1</v>
       </c>
-      <c r="G312" s="85"/>
-      <c r="H312" s="85"/>
-      <c r="I312" s="85">
+      <c r="G312" s="88"/>
+      <c r="H312" s="88"/>
+      <c r="I312" s="88">
         <v>0.1</v>
       </c>
-      <c r="J312" s="85"/>
-      <c r="K312" s="85"/>
-      <c r="L312" s="85">
+      <c r="J312" s="88"/>
+      <c r="K312" s="88"/>
+      <c r="L312" s="88">
         <v>0.1</v>
       </c>
-      <c r="M312" s="85"/>
-      <c r="N312" s="98"/>
+      <c r="M312" s="88"/>
+      <c r="N312" s="102"/>
       <c r="O312" s="74"/>
       <c r="Q312" s="6"/>
     </row>
@@ -7299,29 +7365,29 @@
       <c r="A313" s="44" t="s">
         <v>72</v>
       </c>
-      <c r="C313" s="83">
+      <c r="C313" s="89">
         <f>C312*C311</f>
         <v>10</v>
       </c>
-      <c r="D313" s="83"/>
-      <c r="E313" s="83"/>
-      <c r="F313" s="83">
+      <c r="D313" s="89"/>
+      <c r="E313" s="89"/>
+      <c r="F313" s="89">
         <f t="shared" ref="F313" si="47">F312*F311</f>
         <v>10</v>
       </c>
-      <c r="G313" s="83"/>
-      <c r="H313" s="83"/>
-      <c r="I313" s="83">
+      <c r="G313" s="89"/>
+      <c r="H313" s="89"/>
+      <c r="I313" s="89">
         <f t="shared" ref="I313" si="48">I312*I311</f>
         <v>10</v>
       </c>
-      <c r="J313" s="83"/>
-      <c r="K313" s="83"/>
-      <c r="L313" s="83">
+      <c r="J313" s="89"/>
+      <c r="K313" s="89"/>
+      <c r="L313" s="89">
         <f t="shared" ref="L313" si="49">L312*L311</f>
         <v>10</v>
       </c>
-      <c r="M313" s="83"/>
+      <c r="M313" s="89"/>
       <c r="N313" s="87"/>
       <c r="O313" s="72"/>
     </row>
@@ -7547,46 +7613,46 @@
       <c r="A324" s="43" t="s">
         <v>64</v>
       </c>
-      <c r="C324" s="83">
+      <c r="C324" s="89">
         <v>0</v>
       </c>
-      <c r="D324" s="83"/>
-      <c r="E324" s="83"/>
-      <c r="F324" s="83"/>
-      <c r="G324" s="83"/>
-      <c r="H324" s="83"/>
-      <c r="I324" s="83">
+      <c r="D324" s="89"/>
+      <c r="E324" s="89"/>
+      <c r="F324" s="89"/>
+      <c r="G324" s="89"/>
+      <c r="H324" s="89"/>
+      <c r="I324" s="89">
         <v>0</v>
       </c>
-      <c r="J324" s="83"/>
-      <c r="K324" s="83"/>
-      <c r="L324" s="83"/>
-      <c r="M324" s="83"/>
-      <c r="N324" s="83"/>
+      <c r="J324" s="89"/>
+      <c r="K324" s="89"/>
+      <c r="L324" s="89"/>
+      <c r="M324" s="89"/>
+      <c r="N324" s="89"/>
       <c r="O324" s="72"/>
     </row>
     <row r="325" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A325" s="44" t="s">
         <v>65</v>
       </c>
-      <c r="C325" s="83">
+      <c r="C325" s="89">
         <f>MAX(0, SUM(C$50:H$50))</f>
         <v>200</v>
       </c>
-      <c r="D325" s="83"/>
-      <c r="E325" s="83"/>
-      <c r="F325" s="83"/>
-      <c r="G325" s="83"/>
-      <c r="H325" s="83"/>
-      <c r="I325" s="83">
+      <c r="D325" s="89"/>
+      <c r="E325" s="89"/>
+      <c r="F325" s="89"/>
+      <c r="G325" s="89"/>
+      <c r="H325" s="89"/>
+      <c r="I325" s="89">
         <f>MAX(0, SUM(I$50:N$50))</f>
         <v>200</v>
       </c>
-      <c r="J325" s="83"/>
-      <c r="K325" s="83"/>
-      <c r="L325" s="83"/>
-      <c r="M325" s="83"/>
-      <c r="N325" s="83"/>
+      <c r="J325" s="89"/>
+      <c r="K325" s="89"/>
+      <c r="L325" s="89"/>
+      <c r="M325" s="89"/>
+      <c r="N325" s="89"/>
       <c r="O325" s="72"/>
       <c r="P325" s="6"/>
       <c r="Q325" s="6"/>
@@ -7595,22 +7661,22 @@
       <c r="A326" s="43" t="s">
         <v>0</v>
       </c>
-      <c r="C326" s="83">
+      <c r="C326" s="89">
         <v>0</v>
       </c>
-      <c r="D326" s="83"/>
-      <c r="E326" s="83"/>
-      <c r="F326" s="83"/>
-      <c r="G326" s="83"/>
-      <c r="H326" s="83"/>
-      <c r="I326" s="83">
+      <c r="D326" s="89"/>
+      <c r="E326" s="89"/>
+      <c r="F326" s="89"/>
+      <c r="G326" s="89"/>
+      <c r="H326" s="89"/>
+      <c r="I326" s="89">
         <v>0</v>
       </c>
-      <c r="J326" s="83"/>
-      <c r="K326" s="83"/>
-      <c r="L326" s="83"/>
-      <c r="M326" s="83"/>
-      <c r="N326" s="83"/>
+      <c r="J326" s="89"/>
+      <c r="K326" s="89"/>
+      <c r="L326" s="89"/>
+      <c r="M326" s="89"/>
+      <c r="N326" s="89"/>
       <c r="O326" s="72"/>
       <c r="Q326" s="6"/>
     </row>
@@ -7618,24 +7684,24 @@
       <c r="A327" s="44" t="s">
         <v>66</v>
       </c>
-      <c r="C327" s="83">
+      <c r="C327" s="89">
         <f>IF(C326=0, C325, MIN(C325, C326))</f>
         <v>200</v>
       </c>
-      <c r="D327" s="83"/>
-      <c r="E327" s="83"/>
-      <c r="F327" s="83"/>
-      <c r="G327" s="83"/>
-      <c r="H327" s="83"/>
-      <c r="I327" s="83">
+      <c r="D327" s="89"/>
+      <c r="E327" s="89"/>
+      <c r="F327" s="89"/>
+      <c r="G327" s="89"/>
+      <c r="H327" s="89"/>
+      <c r="I327" s="89">
         <f>IF(I326=0, I325, MIN(I325, I326))</f>
         <v>200</v>
       </c>
-      <c r="J327" s="83"/>
-      <c r="K327" s="83"/>
-      <c r="L327" s="83"/>
-      <c r="M327" s="83"/>
-      <c r="N327" s="83"/>
+      <c r="J327" s="89"/>
+      <c r="K327" s="89"/>
+      <c r="L327" s="89"/>
+      <c r="M327" s="89"/>
+      <c r="N327" s="89"/>
       <c r="O327" s="72"/>
       <c r="P327" s="6"/>
       <c r="Q327" s="6"/>
@@ -7644,22 +7710,22 @@
       <c r="A328" s="43" t="s">
         <v>71</v>
       </c>
-      <c r="C328" s="85">
+      <c r="C328" s="88">
         <v>0.1</v>
       </c>
-      <c r="D328" s="85"/>
-      <c r="E328" s="85"/>
-      <c r="F328" s="85"/>
-      <c r="G328" s="85"/>
-      <c r="H328" s="85"/>
-      <c r="I328" s="85">
+      <c r="D328" s="88"/>
+      <c r="E328" s="88"/>
+      <c r="F328" s="88"/>
+      <c r="G328" s="88"/>
+      <c r="H328" s="88"/>
+      <c r="I328" s="88">
         <v>0.1</v>
       </c>
-      <c r="J328" s="85"/>
-      <c r="K328" s="85"/>
-      <c r="L328" s="85"/>
-      <c r="M328" s="85"/>
-      <c r="N328" s="85"/>
+      <c r="J328" s="88"/>
+      <c r="K328" s="88"/>
+      <c r="L328" s="88"/>
+      <c r="M328" s="88"/>
+      <c r="N328" s="88"/>
       <c r="O328" s="74"/>
       <c r="Q328" s="6"/>
     </row>
@@ -7667,24 +7733,24 @@
       <c r="A329" s="44" t="s">
         <v>72</v>
       </c>
-      <c r="C329" s="83">
+      <c r="C329" s="89">
         <f>C327*C328</f>
         <v>20</v>
       </c>
-      <c r="D329" s="83"/>
-      <c r="E329" s="83"/>
-      <c r="F329" s="83"/>
-      <c r="G329" s="83"/>
-      <c r="H329" s="83"/>
-      <c r="I329" s="83">
+      <c r="D329" s="89"/>
+      <c r="E329" s="89"/>
+      <c r="F329" s="89"/>
+      <c r="G329" s="89"/>
+      <c r="H329" s="89"/>
+      <c r="I329" s="89">
         <f>I327*I328</f>
         <v>20</v>
       </c>
-      <c r="J329" s="83"/>
-      <c r="K329" s="83"/>
-      <c r="L329" s="83"/>
-      <c r="M329" s="83"/>
-      <c r="N329" s="83"/>
+      <c r="J329" s="89"/>
+      <c r="K329" s="89"/>
+      <c r="L329" s="89"/>
+      <c r="M329" s="89"/>
+      <c r="N329" s="89"/>
       <c r="O329" s="72"/>
     </row>
     <row r="330" spans="1:17" x14ac:dyDescent="0.3">
@@ -7909,46 +7975,46 @@
       <c r="A340" s="43" t="s">
         <v>64</v>
       </c>
-      <c r="C340" s="83">
+      <c r="C340" s="89">
         <v>0</v>
       </c>
-      <c r="D340" s="83"/>
-      <c r="E340" s="83"/>
-      <c r="F340" s="83"/>
-      <c r="G340" s="83"/>
-      <c r="H340" s="83"/>
-      <c r="I340" s="83">
+      <c r="D340" s="89"/>
+      <c r="E340" s="89"/>
+      <c r="F340" s="89"/>
+      <c r="G340" s="89"/>
+      <c r="H340" s="89"/>
+      <c r="I340" s="89">
         <v>0</v>
       </c>
-      <c r="J340" s="83"/>
-      <c r="K340" s="83"/>
-      <c r="L340" s="83"/>
-      <c r="M340" s="83"/>
-      <c r="N340" s="83"/>
+      <c r="J340" s="89"/>
+      <c r="K340" s="89"/>
+      <c r="L340" s="89"/>
+      <c r="M340" s="89"/>
+      <c r="N340" s="89"/>
       <c r="O340" s="72"/>
     </row>
     <row r="341" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A341" s="44" t="s">
         <v>65</v>
       </c>
-      <c r="C341" s="83">
+      <c r="C341" s="89">
         <f>MAX(0, SUM(C$50:H$50))</f>
         <v>200</v>
       </c>
-      <c r="D341" s="83"/>
-      <c r="E341" s="83"/>
-      <c r="F341" s="83"/>
-      <c r="G341" s="83"/>
-      <c r="H341" s="83"/>
-      <c r="I341" s="83">
+      <c r="D341" s="89"/>
+      <c r="E341" s="89"/>
+      <c r="F341" s="89"/>
+      <c r="G341" s="89"/>
+      <c r="H341" s="89"/>
+      <c r="I341" s="89">
         <f>MAX(0, SUM(I$50:N$50))</f>
         <v>200</v>
       </c>
-      <c r="J341" s="83"/>
-      <c r="K341" s="83"/>
-      <c r="L341" s="83"/>
-      <c r="M341" s="83"/>
-      <c r="N341" s="83"/>
+      <c r="J341" s="89"/>
+      <c r="K341" s="89"/>
+      <c r="L341" s="89"/>
+      <c r="M341" s="89"/>
+      <c r="N341" s="89"/>
       <c r="O341" s="72"/>
       <c r="P341" s="6"/>
       <c r="Q341" s="6"/>
@@ -7957,22 +8023,22 @@
       <c r="A342" s="43" t="s">
         <v>0</v>
       </c>
-      <c r="C342" s="83">
+      <c r="C342" s="89">
         <v>0</v>
       </c>
-      <c r="D342" s="83"/>
-      <c r="E342" s="83"/>
-      <c r="F342" s="83"/>
-      <c r="G342" s="83"/>
-      <c r="H342" s="83"/>
-      <c r="I342" s="83">
+      <c r="D342" s="89"/>
+      <c r="E342" s="89"/>
+      <c r="F342" s="89"/>
+      <c r="G342" s="89"/>
+      <c r="H342" s="89"/>
+      <c r="I342" s="89">
         <v>0</v>
       </c>
-      <c r="J342" s="83"/>
-      <c r="K342" s="83"/>
-      <c r="L342" s="83"/>
-      <c r="M342" s="83"/>
-      <c r="N342" s="83"/>
+      <c r="J342" s="89"/>
+      <c r="K342" s="89"/>
+      <c r="L342" s="89"/>
+      <c r="M342" s="89"/>
+      <c r="N342" s="89"/>
       <c r="O342" s="72"/>
       <c r="Q342" s="6"/>
     </row>
@@ -7980,24 +8046,24 @@
       <c r="A343" s="44" t="s">
         <v>66</v>
       </c>
-      <c r="C343" s="83">
+      <c r="C343" s="89">
         <f>IF(C342=0, C341, MIN(C341, C342))</f>
         <v>200</v>
       </c>
-      <c r="D343" s="83"/>
-      <c r="E343" s="83"/>
-      <c r="F343" s="83"/>
-      <c r="G343" s="83"/>
-      <c r="H343" s="83"/>
-      <c r="I343" s="83">
+      <c r="D343" s="89"/>
+      <c r="E343" s="89"/>
+      <c r="F343" s="89"/>
+      <c r="G343" s="89"/>
+      <c r="H343" s="89"/>
+      <c r="I343" s="89">
         <f>IF(I342=0, I341, MIN(I341, I342))</f>
         <v>200</v>
       </c>
-      <c r="J343" s="83"/>
-      <c r="K343" s="83"/>
-      <c r="L343" s="83"/>
-      <c r="M343" s="83"/>
-      <c r="N343" s="83"/>
+      <c r="J343" s="89"/>
+      <c r="K343" s="89"/>
+      <c r="L343" s="89"/>
+      <c r="M343" s="89"/>
+      <c r="N343" s="89"/>
       <c r="O343" s="72"/>
       <c r="P343" s="6"/>
       <c r="Q343" s="6"/>
@@ -8006,22 +8072,22 @@
       <c r="A344" s="43" t="s">
         <v>71</v>
       </c>
-      <c r="C344" s="85">
+      <c r="C344" s="88">
         <v>0.1</v>
       </c>
-      <c r="D344" s="85"/>
-      <c r="E344" s="85"/>
-      <c r="F344" s="85"/>
-      <c r="G344" s="85"/>
-      <c r="H344" s="85"/>
-      <c r="I344" s="85">
+      <c r="D344" s="88"/>
+      <c r="E344" s="88"/>
+      <c r="F344" s="88"/>
+      <c r="G344" s="88"/>
+      <c r="H344" s="88"/>
+      <c r="I344" s="88">
         <v>0.1</v>
       </c>
-      <c r="J344" s="85"/>
-      <c r="K344" s="85"/>
-      <c r="L344" s="85"/>
-      <c r="M344" s="85"/>
-      <c r="N344" s="85"/>
+      <c r="J344" s="88"/>
+      <c r="K344" s="88"/>
+      <c r="L344" s="88"/>
+      <c r="M344" s="88"/>
+      <c r="N344" s="88"/>
       <c r="O344" s="74"/>
       <c r="Q344" s="6"/>
     </row>
@@ -8029,24 +8095,24 @@
       <c r="A345" s="44" t="s">
         <v>72</v>
       </c>
-      <c r="C345" s="83">
+      <c r="C345" s="89">
         <f>C343*C344</f>
         <v>20</v>
       </c>
-      <c r="D345" s="83"/>
-      <c r="E345" s="83"/>
-      <c r="F345" s="83"/>
-      <c r="G345" s="83"/>
-      <c r="H345" s="83"/>
-      <c r="I345" s="83">
+      <c r="D345" s="89"/>
+      <c r="E345" s="89"/>
+      <c r="F345" s="89"/>
+      <c r="G345" s="89"/>
+      <c r="H345" s="89"/>
+      <c r="I345" s="89">
         <f>I343*I344</f>
         <v>20</v>
       </c>
-      <c r="J345" s="83"/>
-      <c r="K345" s="83"/>
-      <c r="L345" s="83"/>
-      <c r="M345" s="83"/>
-      <c r="N345" s="83"/>
+      <c r="J345" s="89"/>
+      <c r="K345" s="89"/>
+      <c r="L345" s="89"/>
+      <c r="M345" s="89"/>
+      <c r="N345" s="89"/>
       <c r="O345" s="72"/>
     </row>
     <row r="346" spans="1:17" x14ac:dyDescent="0.3">
@@ -8766,8 +8832,1289 @@
         <v>280</v>
       </c>
     </row>
+    <row r="370" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A370" s="65" t="s">
+        <v>165</v>
+      </c>
+      <c r="B370" s="4"/>
+      <c r="D370" s="76" t="s">
+        <v>166</v>
+      </c>
+      <c r="H370" s="42"/>
+      <c r="K370" s="42"/>
+      <c r="N370" s="42"/>
+    </row>
+    <row r="371" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A371" s="43" t="s">
+        <v>61</v>
+      </c>
+      <c r="C371" s="86">
+        <v>1</v>
+      </c>
+      <c r="D371" s="86"/>
+      <c r="E371" s="86"/>
+      <c r="F371" s="86"/>
+      <c r="G371" s="86"/>
+      <c r="H371" s="86"/>
+      <c r="I371" s="86">
+        <v>1</v>
+      </c>
+      <c r="J371" s="86"/>
+      <c r="K371" s="86"/>
+      <c r="L371" s="86"/>
+      <c r="M371" s="86"/>
+      <c r="N371" s="87"/>
+      <c r="O371" s="72"/>
+    </row>
+    <row r="372" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A372" s="43" t="s">
+        <v>62</v>
+      </c>
+      <c r="C372" s="86" t="s">
+        <v>146</v>
+      </c>
+      <c r="D372" s="86"/>
+      <c r="E372" s="86"/>
+      <c r="F372" s="86"/>
+      <c r="G372" s="86"/>
+      <c r="H372" s="86"/>
+      <c r="I372" s="86" t="s">
+        <v>147</v>
+      </c>
+      <c r="J372" s="86"/>
+      <c r="K372" s="86"/>
+      <c r="L372" s="86"/>
+      <c r="M372" s="86"/>
+      <c r="N372" s="87"/>
+      <c r="O372" s="73"/>
+    </row>
+    <row r="373" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A373" s="43" t="s">
+        <v>63</v>
+      </c>
+      <c r="C373" s="86">
+        <v>1</v>
+      </c>
+      <c r="D373" s="86"/>
+      <c r="E373" s="86"/>
+      <c r="F373" s="86"/>
+      <c r="G373" s="86"/>
+      <c r="H373" s="86"/>
+      <c r="I373" s="86">
+        <v>1</v>
+      </c>
+      <c r="J373" s="86"/>
+      <c r="K373" s="86"/>
+      <c r="L373" s="86"/>
+      <c r="M373" s="86"/>
+      <c r="N373" s="86"/>
+      <c r="O373" s="72"/>
+    </row>
+    <row r="374" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A374" s="43" t="s">
+        <v>71</v>
+      </c>
+      <c r="C374" s="88">
+        <v>0.5</v>
+      </c>
+      <c r="D374" s="88"/>
+      <c r="E374" s="88"/>
+      <c r="F374" s="88"/>
+      <c r="G374" s="88"/>
+      <c r="H374" s="88"/>
+      <c r="I374" s="88">
+        <v>0.5</v>
+      </c>
+      <c r="J374" s="88"/>
+      <c r="K374" s="88"/>
+      <c r="L374" s="88"/>
+      <c r="M374" s="88"/>
+      <c r="N374" s="88"/>
+      <c r="O374" s="72"/>
+    </row>
+    <row r="375" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A375" s="44" t="s">
+        <v>163</v>
+      </c>
+      <c r="C375" s="89">
+        <f>SUM(C$50:H$50)*C374</f>
+        <v>100</v>
+      </c>
+      <c r="D375" s="89"/>
+      <c r="E375" s="89"/>
+      <c r="F375" s="89"/>
+      <c r="G375" s="89"/>
+      <c r="H375" s="89"/>
+      <c r="I375" s="89">
+        <f>SUM(I$50:N$50)*I374</f>
+        <v>100</v>
+      </c>
+      <c r="J375" s="89"/>
+      <c r="K375" s="89"/>
+      <c r="L375" s="89"/>
+      <c r="M375" s="89"/>
+      <c r="N375" s="89"/>
+      <c r="O375" s="72">
+        <f>SUM(C375:N375)</f>
+        <v>200</v>
+      </c>
+      <c r="P375" s="6"/>
+      <c r="Q375" s="6"/>
+    </row>
+    <row r="376" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A376" s="43" t="s">
+        <v>67</v>
+      </c>
+      <c r="N376" s="13"/>
+      <c r="O376" s="72"/>
+    </row>
+    <row r="377" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A377" s="43" t="s">
+        <v>161</v>
+      </c>
+      <c r="N377" s="13"/>
+      <c r="O377" s="83">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="378" spans="1:17" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A378" s="45" t="s">
+        <v>164</v>
+      </c>
+      <c r="C378" s="86">
+        <f>O$378*C375/$O375</f>
+        <v>80</v>
+      </c>
+      <c r="D378" s="86"/>
+      <c r="E378" s="86"/>
+      <c r="F378" s="86"/>
+      <c r="G378" s="86"/>
+      <c r="H378" s="86"/>
+      <c r="I378" s="86">
+        <f>O$378*I375/$O375</f>
+        <v>80</v>
+      </c>
+      <c r="J378" s="86"/>
+      <c r="K378" s="86"/>
+      <c r="L378" s="86"/>
+      <c r="M378" s="86"/>
+      <c r="N378" s="86"/>
+      <c r="O378" s="72">
+        <f>O377*O375</f>
+        <v>160</v>
+      </c>
+      <c r="P378" s="6"/>
+      <c r="Q378" s="6"/>
+    </row>
+    <row r="379" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A379" s="44" t="s">
+        <v>135</v>
+      </c>
+      <c r="C379" s="52">
+        <f>$C378*C$50/SUM($C$50:$H$50)</f>
+        <v>20</v>
+      </c>
+      <c r="D379" s="52">
+        <f t="shared" ref="D379:H379" si="70">$C378*D$50/SUM($C$50:$H$50)</f>
+        <v>10</v>
+      </c>
+      <c r="E379" s="52">
+        <f t="shared" si="70"/>
+        <v>10</v>
+      </c>
+      <c r="F379" s="52">
+        <f t="shared" si="70"/>
+        <v>20</v>
+      </c>
+      <c r="G379" s="52">
+        <f t="shared" si="70"/>
+        <v>10</v>
+      </c>
+      <c r="H379" s="52">
+        <f t="shared" si="70"/>
+        <v>10</v>
+      </c>
+      <c r="I379" s="52">
+        <f>$I378*I$50/SUM($C$50:$H$50)</f>
+        <v>20</v>
+      </c>
+      <c r="J379" s="52">
+        <f t="shared" ref="J379:N379" si="71">$I378*J$50/SUM($C$50:$H$50)</f>
+        <v>10</v>
+      </c>
+      <c r="K379" s="52">
+        <f t="shared" si="71"/>
+        <v>10</v>
+      </c>
+      <c r="L379" s="52">
+        <f t="shared" si="71"/>
+        <v>20</v>
+      </c>
+      <c r="M379" s="52">
+        <f t="shared" si="71"/>
+        <v>10</v>
+      </c>
+      <c r="N379" s="52">
+        <f t="shared" si="71"/>
+        <v>10</v>
+      </c>
+      <c r="O379" s="75">
+        <f>SUM(C379:N379)</f>
+        <v>160</v>
+      </c>
+    </row>
+    <row r="380" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A380" s="46" t="s">
+        <v>69</v>
+      </c>
+      <c r="C380" s="67">
+        <f>$O380*C$50/$O$50</f>
+        <v>30</v>
+      </c>
+      <c r="D380" s="67">
+        <f t="shared" ref="D380:N380" si="72">$O380*D$50/$O$50</f>
+        <v>15</v>
+      </c>
+      <c r="E380" s="67">
+        <f t="shared" si="72"/>
+        <v>15</v>
+      </c>
+      <c r="F380" s="67">
+        <f t="shared" si="72"/>
+        <v>30</v>
+      </c>
+      <c r="G380" s="67">
+        <f t="shared" si="72"/>
+        <v>15</v>
+      </c>
+      <c r="H380" s="67">
+        <f t="shared" si="72"/>
+        <v>15</v>
+      </c>
+      <c r="I380" s="67">
+        <f t="shared" si="72"/>
+        <v>30</v>
+      </c>
+      <c r="J380" s="67">
+        <f t="shared" si="72"/>
+        <v>15</v>
+      </c>
+      <c r="K380" s="67">
+        <f t="shared" si="72"/>
+        <v>15</v>
+      </c>
+      <c r="L380" s="67">
+        <f t="shared" si="72"/>
+        <v>30</v>
+      </c>
+      <c r="M380" s="67">
+        <f t="shared" si="72"/>
+        <v>15</v>
+      </c>
+      <c r="N380" s="67">
+        <f t="shared" si="72"/>
+        <v>15</v>
+      </c>
+      <c r="O380" s="72">
+        <f>O$50-O378</f>
+        <v>240</v>
+      </c>
+    </row>
+    <row r="382" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A382" s="65" t="s">
+        <v>168</v>
+      </c>
+      <c r="B382" s="4"/>
+      <c r="D382" s="76" t="s">
+        <v>167</v>
+      </c>
+      <c r="H382" s="42"/>
+      <c r="K382" s="42"/>
+      <c r="N382" s="42"/>
+    </row>
+    <row r="383" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A383" s="43" t="s">
+        <v>61</v>
+      </c>
+      <c r="C383" s="86">
+        <v>1</v>
+      </c>
+      <c r="D383" s="86"/>
+      <c r="E383" s="86"/>
+      <c r="F383" s="86"/>
+      <c r="G383" s="86"/>
+      <c r="H383" s="86"/>
+      <c r="I383" s="86"/>
+      <c r="J383" s="86"/>
+      <c r="K383" s="86"/>
+      <c r="L383" s="86"/>
+      <c r="M383" s="86"/>
+      <c r="N383" s="87"/>
+      <c r="O383" s="72"/>
+    </row>
+    <row r="384" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A384" s="43" t="s">
+        <v>62</v>
+      </c>
+      <c r="C384" s="86" t="s">
+        <v>146</v>
+      </c>
+      <c r="D384" s="86"/>
+      <c r="E384" s="86"/>
+      <c r="F384" s="86"/>
+      <c r="G384" s="86"/>
+      <c r="H384" s="86"/>
+      <c r="I384" s="86" t="s">
+        <v>147</v>
+      </c>
+      <c r="J384" s="86"/>
+      <c r="K384" s="86"/>
+      <c r="L384" s="86"/>
+      <c r="M384" s="86"/>
+      <c r="N384" s="87"/>
+      <c r="O384" s="73"/>
+    </row>
+    <row r="385" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A385" s="43" t="s">
+        <v>63</v>
+      </c>
+      <c r="C385" s="86">
+        <v>1</v>
+      </c>
+      <c r="D385" s="86"/>
+      <c r="E385" s="86"/>
+      <c r="F385" s="86"/>
+      <c r="G385" s="86"/>
+      <c r="H385" s="86"/>
+      <c r="I385" s="86"/>
+      <c r="J385" s="86"/>
+      <c r="K385" s="86"/>
+      <c r="L385" s="86"/>
+      <c r="M385" s="86"/>
+      <c r="N385" s="86"/>
+      <c r="O385" s="72"/>
+    </row>
+    <row r="386" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A386" s="43" t="s">
+        <v>71</v>
+      </c>
+      <c r="C386" s="88">
+        <v>0.5</v>
+      </c>
+      <c r="D386" s="88"/>
+      <c r="E386" s="88"/>
+      <c r="F386" s="88"/>
+      <c r="G386" s="88"/>
+      <c r="H386" s="88"/>
+      <c r="I386" s="88"/>
+      <c r="J386" s="88"/>
+      <c r="K386" s="88"/>
+      <c r="L386" s="88"/>
+      <c r="M386" s="88"/>
+      <c r="N386" s="88"/>
+      <c r="O386" s="72"/>
+    </row>
+    <row r="387" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A387" s="44" t="s">
+        <v>163</v>
+      </c>
+      <c r="C387" s="89">
+        <f>SUM(C$50:H$50)*C386</f>
+        <v>100</v>
+      </c>
+      <c r="D387" s="89"/>
+      <c r="E387" s="89"/>
+      <c r="F387" s="89"/>
+      <c r="G387" s="89"/>
+      <c r="H387" s="89"/>
+      <c r="I387" s="89"/>
+      <c r="J387" s="89"/>
+      <c r="K387" s="89"/>
+      <c r="L387" s="89"/>
+      <c r="M387" s="89"/>
+      <c r="N387" s="89"/>
+      <c r="O387" s="72">
+        <f>SUM(C387:N387)</f>
+        <v>100</v>
+      </c>
+      <c r="P387" s="6"/>
+      <c r="Q387" s="6"/>
+    </row>
+    <row r="388" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A388" s="43" t="s">
+        <v>67</v>
+      </c>
+      <c r="N388" s="13"/>
+      <c r="O388" s="72"/>
+    </row>
+    <row r="389" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A389" s="43" t="s">
+        <v>161</v>
+      </c>
+      <c r="C389" s="90">
+        <v>0.8</v>
+      </c>
+      <c r="D389" s="86"/>
+      <c r="E389" s="86"/>
+      <c r="F389" s="86"/>
+      <c r="G389" s="86"/>
+      <c r="H389" s="86"/>
+      <c r="N389" s="13"/>
+      <c r="O389" s="83">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="390" spans="1:17" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A390" s="45" t="s">
+        <v>164</v>
+      </c>
+      <c r="C390" s="86">
+        <f>C389*C387</f>
+        <v>80</v>
+      </c>
+      <c r="D390" s="86"/>
+      <c r="E390" s="86"/>
+      <c r="F390" s="86"/>
+      <c r="G390" s="86"/>
+      <c r="H390" s="86"/>
+      <c r="I390" s="86"/>
+      <c r="J390" s="86"/>
+      <c r="K390" s="86"/>
+      <c r="L390" s="86"/>
+      <c r="M390" s="86"/>
+      <c r="N390" s="86"/>
+      <c r="O390" s="72">
+        <f>SUM(C390:N390)</f>
+        <v>80</v>
+      </c>
+      <c r="P390" s="6"/>
+      <c r="Q390" s="6"/>
+    </row>
+    <row r="391" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A391" s="44" t="s">
+        <v>135</v>
+      </c>
+      <c r="C391" s="52">
+        <f>$C390*C$50/SUM($C$50:$H$50)</f>
+        <v>20</v>
+      </c>
+      <c r="D391" s="52">
+        <f t="shared" ref="D391" si="73">$C390*D$50/SUM($C$50:$H$50)</f>
+        <v>10</v>
+      </c>
+      <c r="E391" s="52">
+        <f t="shared" ref="E391" si="74">$C390*E$50/SUM($C$50:$H$50)</f>
+        <v>10</v>
+      </c>
+      <c r="F391" s="52">
+        <f t="shared" ref="F391" si="75">$C390*F$50/SUM($C$50:$H$50)</f>
+        <v>20</v>
+      </c>
+      <c r="G391" s="52">
+        <f t="shared" ref="G391" si="76">$C390*G$50/SUM($C$50:$H$50)</f>
+        <v>10</v>
+      </c>
+      <c r="H391" s="52">
+        <f t="shared" ref="H391" si="77">$C390*H$50/SUM($C$50:$H$50)</f>
+        <v>10</v>
+      </c>
+      <c r="I391" s="52">
+        <f>$I390*I$50/SUM($I$50:$N$50)</f>
+        <v>0</v>
+      </c>
+      <c r="J391" s="52">
+        <f t="shared" ref="J391" si="78">$I390*J$50/SUM($C$50:$H$50)</f>
+        <v>0</v>
+      </c>
+      <c r="K391" s="52">
+        <f t="shared" ref="K391" si="79">$I390*K$50/SUM($C$50:$H$50)</f>
+        <v>0</v>
+      </c>
+      <c r="L391" s="52">
+        <f t="shared" ref="L391" si="80">$I390*L$50/SUM($C$50:$H$50)</f>
+        <v>0</v>
+      </c>
+      <c r="M391" s="52">
+        <f t="shared" ref="M391" si="81">$I390*M$50/SUM($C$50:$H$50)</f>
+        <v>0</v>
+      </c>
+      <c r="N391" s="52">
+        <f t="shared" ref="N391" si="82">$I390*N$50/SUM($C$50:$H$50)</f>
+        <v>0</v>
+      </c>
+      <c r="O391" s="84">
+        <f>SUM(C391:N391)</f>
+        <v>80</v>
+      </c>
+    </row>
+    <row r="392" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A392" s="46" t="s">
+        <v>69</v>
+      </c>
+      <c r="C392" s="67">
+        <f>($O392-$C390)*C$50/$O$50</f>
+        <v>30</v>
+      </c>
+      <c r="D392" s="67">
+        <f t="shared" ref="D392:H392" si="83">($O392-$C390)*D$50/$O$50</f>
+        <v>15</v>
+      </c>
+      <c r="E392" s="67">
+        <f t="shared" si="83"/>
+        <v>15</v>
+      </c>
+      <c r="F392" s="67">
+        <f t="shared" si="83"/>
+        <v>30</v>
+      </c>
+      <c r="G392" s="67">
+        <f t="shared" si="83"/>
+        <v>15</v>
+      </c>
+      <c r="H392" s="67">
+        <f t="shared" si="83"/>
+        <v>15</v>
+      </c>
+      <c r="I392" s="67">
+        <f>I$50</f>
+        <v>50</v>
+      </c>
+      <c r="J392" s="67">
+        <f t="shared" ref="J392:N392" si="84">J$50</f>
+        <v>25</v>
+      </c>
+      <c r="K392" s="67">
+        <f t="shared" si="84"/>
+        <v>25</v>
+      </c>
+      <c r="L392" s="67">
+        <f t="shared" si="84"/>
+        <v>50</v>
+      </c>
+      <c r="M392" s="67">
+        <f t="shared" si="84"/>
+        <v>25</v>
+      </c>
+      <c r="N392" s="67">
+        <f t="shared" si="84"/>
+        <v>25</v>
+      </c>
+      <c r="O392" s="72">
+        <f>O$50-O390</f>
+        <v>320</v>
+      </c>
+    </row>
+    <row r="394" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A394" s="65" t="s">
+        <v>172</v>
+      </c>
+      <c r="B394" s="78" t="s">
+        <v>177</v>
+      </c>
+      <c r="D394" s="2"/>
+      <c r="H394" s="42"/>
+      <c r="K394" s="42"/>
+      <c r="N394" s="42"/>
+    </row>
+    <row r="395" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A395" s="43" t="s">
+        <v>61</v>
+      </c>
+      <c r="C395" s="86">
+        <v>1</v>
+      </c>
+      <c r="D395" s="86"/>
+      <c r="E395" s="86"/>
+      <c r="F395" s="86"/>
+      <c r="G395" s="86"/>
+      <c r="H395" s="86"/>
+      <c r="I395" s="86">
+        <v>1</v>
+      </c>
+      <c r="J395" s="86"/>
+      <c r="K395" s="86"/>
+      <c r="L395" s="86"/>
+      <c r="M395" s="86"/>
+      <c r="N395" s="87"/>
+      <c r="O395" s="72"/>
+    </row>
+    <row r="396" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A396" s="43" t="s">
+        <v>62</v>
+      </c>
+      <c r="C396" s="86" t="s">
+        <v>146</v>
+      </c>
+      <c r="D396" s="86"/>
+      <c r="E396" s="86"/>
+      <c r="F396" s="86"/>
+      <c r="G396" s="86"/>
+      <c r="H396" s="86"/>
+      <c r="I396" s="86" t="s">
+        <v>147</v>
+      </c>
+      <c r="J396" s="86"/>
+      <c r="K396" s="86"/>
+      <c r="L396" s="86"/>
+      <c r="M396" s="86"/>
+      <c r="N396" s="87"/>
+      <c r="O396" s="73"/>
+    </row>
+    <row r="397" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A397" s="43" t="s">
+        <v>63</v>
+      </c>
+      <c r="C397" s="86">
+        <v>1</v>
+      </c>
+      <c r="D397" s="86"/>
+      <c r="E397" s="86"/>
+      <c r="F397" s="86"/>
+      <c r="G397" s="86"/>
+      <c r="H397" s="86"/>
+      <c r="I397" s="86">
+        <v>1</v>
+      </c>
+      <c r="J397" s="86"/>
+      <c r="K397" s="86"/>
+      <c r="L397" s="86"/>
+      <c r="M397" s="86"/>
+      <c r="N397" s="86"/>
+      <c r="O397" s="72"/>
+    </row>
+    <row r="398" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A398" s="43" t="s">
+        <v>71</v>
+      </c>
+      <c r="C398" s="88">
+        <v>0.5</v>
+      </c>
+      <c r="D398" s="88"/>
+      <c r="E398" s="88"/>
+      <c r="F398" s="88"/>
+      <c r="G398" s="88"/>
+      <c r="H398" s="88"/>
+      <c r="I398" s="88">
+        <v>0.5</v>
+      </c>
+      <c r="J398" s="88"/>
+      <c r="K398" s="88"/>
+      <c r="L398" s="88"/>
+      <c r="M398" s="88"/>
+      <c r="N398" s="88"/>
+      <c r="O398" s="72"/>
+    </row>
+    <row r="399" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A399" s="44" t="s">
+        <v>163</v>
+      </c>
+      <c r="C399" s="89">
+        <f>SUM(C$50:H$50)*C398</f>
+        <v>100</v>
+      </c>
+      <c r="D399" s="89"/>
+      <c r="E399" s="89"/>
+      <c r="F399" s="89"/>
+      <c r="G399" s="89"/>
+      <c r="H399" s="89"/>
+      <c r="I399" s="89">
+        <f>SUM(I$50:N$50)*I398</f>
+        <v>100</v>
+      </c>
+      <c r="J399" s="89"/>
+      <c r="K399" s="89"/>
+      <c r="L399" s="89"/>
+      <c r="M399" s="89"/>
+      <c r="N399" s="89"/>
+      <c r="O399" s="72"/>
+      <c r="P399" s="6"/>
+      <c r="Q399" s="6"/>
+    </row>
+    <row r="400" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A400" s="43" t="s">
+        <v>0</v>
+      </c>
+      <c r="C400" s="89">
+        <v>50</v>
+      </c>
+      <c r="D400" s="89"/>
+      <c r="E400" s="89"/>
+      <c r="F400" s="89"/>
+      <c r="G400" s="89"/>
+      <c r="H400" s="89"/>
+      <c r="I400" s="89">
+        <v>50</v>
+      </c>
+      <c r="J400" s="89"/>
+      <c r="K400" s="89"/>
+      <c r="L400" s="89"/>
+      <c r="M400" s="89"/>
+      <c r="N400" s="89"/>
+      <c r="O400" s="72"/>
+      <c r="Q400" s="6"/>
+    </row>
+    <row r="401" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A401" s="44" t="s">
+        <v>176</v>
+      </c>
+      <c r="C401" s="89">
+        <f>IF(C400=0, C399, MIN(C399, C400))</f>
+        <v>50</v>
+      </c>
+      <c r="D401" s="89"/>
+      <c r="E401" s="89"/>
+      <c r="F401" s="89"/>
+      <c r="G401" s="89"/>
+      <c r="H401" s="89"/>
+      <c r="I401" s="89">
+        <f>IF(I400=0, I399, MIN(I399, I400))</f>
+        <v>50</v>
+      </c>
+      <c r="J401" s="89"/>
+      <c r="K401" s="89"/>
+      <c r="L401" s="89"/>
+      <c r="M401" s="89"/>
+      <c r="N401" s="89"/>
+      <c r="O401" s="72">
+        <f>SUM(C401:N401)</f>
+        <v>100</v>
+      </c>
+      <c r="P401" s="6"/>
+      <c r="Q401" s="6"/>
+    </row>
+    <row r="402" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A402" s="43" t="s">
+        <v>67</v>
+      </c>
+      <c r="N402" s="13"/>
+      <c r="O402" s="72">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="403" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A403" s="43" t="s">
+        <v>161</v>
+      </c>
+      <c r="N403" s="13"/>
+      <c r="O403" s="83">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="404" spans="1:17" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A404" s="45" t="s">
+        <v>164</v>
+      </c>
+      <c r="C404" s="86">
+        <f>O$404*C401/$O401</f>
+        <v>36</v>
+      </c>
+      <c r="D404" s="86"/>
+      <c r="E404" s="86"/>
+      <c r="F404" s="86"/>
+      <c r="G404" s="86"/>
+      <c r="H404" s="86"/>
+      <c r="I404" s="86">
+        <f>O$404*I401/$O401</f>
+        <v>36</v>
+      </c>
+      <c r="J404" s="86"/>
+      <c r="K404" s="86"/>
+      <c r="L404" s="86"/>
+      <c r="M404" s="86"/>
+      <c r="N404" s="86"/>
+      <c r="O404" s="72">
+        <f>O403*MIN(O401,O402)</f>
+        <v>72</v>
+      </c>
+      <c r="P404" s="6"/>
+      <c r="Q404" s="6"/>
+    </row>
+    <row r="405" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A405" s="44" t="s">
+        <v>135</v>
+      </c>
+      <c r="C405" s="52">
+        <f>$C404*C$50/SUM($C$50:$H$50)</f>
+        <v>9</v>
+      </c>
+      <c r="D405" s="52">
+        <f t="shared" ref="D405:H405" si="85">$C404*D$50/SUM($C$50:$H$50)</f>
+        <v>4.5</v>
+      </c>
+      <c r="E405" s="52">
+        <f t="shared" si="85"/>
+        <v>4.5</v>
+      </c>
+      <c r="F405" s="52">
+        <f t="shared" si="85"/>
+        <v>9</v>
+      </c>
+      <c r="G405" s="52">
+        <f t="shared" si="85"/>
+        <v>4.5</v>
+      </c>
+      <c r="H405" s="52">
+        <f t="shared" si="85"/>
+        <v>4.5</v>
+      </c>
+      <c r="I405" s="52">
+        <f>$I404*I$50/SUM($C$50:$H$50)</f>
+        <v>9</v>
+      </c>
+      <c r="J405" s="52">
+        <f t="shared" ref="J405:N405" si="86">$I404*J$50/SUM($C$50:$H$50)</f>
+        <v>4.5</v>
+      </c>
+      <c r="K405" s="52">
+        <f t="shared" si="86"/>
+        <v>4.5</v>
+      </c>
+      <c r="L405" s="52">
+        <f t="shared" si="86"/>
+        <v>9</v>
+      </c>
+      <c r="M405" s="52">
+        <f t="shared" si="86"/>
+        <v>4.5</v>
+      </c>
+      <c r="N405" s="52">
+        <f t="shared" si="86"/>
+        <v>4.5</v>
+      </c>
+      <c r="O405" s="75">
+        <f>SUM(C405:N405)</f>
+        <v>72</v>
+      </c>
+    </row>
+    <row r="406" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A406" s="46" t="s">
+        <v>69</v>
+      </c>
+      <c r="C406" s="67">
+        <f>$O406*C$50/$O$50</f>
+        <v>41</v>
+      </c>
+      <c r="D406" s="67">
+        <f t="shared" ref="D406:N406" si="87">$O406*D$50/$O$50</f>
+        <v>20.5</v>
+      </c>
+      <c r="E406" s="67">
+        <f t="shared" si="87"/>
+        <v>20.5</v>
+      </c>
+      <c r="F406" s="67">
+        <f t="shared" si="87"/>
+        <v>41</v>
+      </c>
+      <c r="G406" s="67">
+        <f t="shared" si="87"/>
+        <v>20.5</v>
+      </c>
+      <c r="H406" s="67">
+        <f t="shared" si="87"/>
+        <v>20.5</v>
+      </c>
+      <c r="I406" s="67">
+        <f t="shared" si="87"/>
+        <v>41</v>
+      </c>
+      <c r="J406" s="67">
+        <f t="shared" si="87"/>
+        <v>20.5</v>
+      </c>
+      <c r="K406" s="67">
+        <f t="shared" si="87"/>
+        <v>20.5</v>
+      </c>
+      <c r="L406" s="67">
+        <f t="shared" si="87"/>
+        <v>41</v>
+      </c>
+      <c r="M406" s="67">
+        <f t="shared" si="87"/>
+        <v>20.5</v>
+      </c>
+      <c r="N406" s="67">
+        <f t="shared" si="87"/>
+        <v>20.5</v>
+      </c>
+      <c r="O406" s="72">
+        <f>O$50-O404</f>
+        <v>328</v>
+      </c>
+    </row>
+    <row r="408" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A408" s="65" t="s">
+        <v>173</v>
+      </c>
+      <c r="B408" s="78" t="s">
+        <v>178</v>
+      </c>
+      <c r="D408" s="2"/>
+      <c r="H408" s="42"/>
+      <c r="K408" s="42"/>
+      <c r="N408" s="42"/>
+    </row>
+    <row r="409" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A409" s="43" t="s">
+        <v>61</v>
+      </c>
+      <c r="C409" s="86">
+        <v>1</v>
+      </c>
+      <c r="D409" s="86"/>
+      <c r="E409" s="86"/>
+      <c r="F409" s="86"/>
+      <c r="G409" s="86"/>
+      <c r="H409" s="86"/>
+      <c r="I409" s="86"/>
+      <c r="J409" s="86"/>
+      <c r="K409" s="86"/>
+      <c r="L409" s="86"/>
+      <c r="M409" s="86"/>
+      <c r="N409" s="87"/>
+      <c r="O409" s="72"/>
+    </row>
+    <row r="410" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A410" s="43" t="s">
+        <v>62</v>
+      </c>
+      <c r="C410" s="86" t="s">
+        <v>146</v>
+      </c>
+      <c r="D410" s="86"/>
+      <c r="E410" s="86"/>
+      <c r="F410" s="86"/>
+      <c r="G410" s="86"/>
+      <c r="H410" s="86"/>
+      <c r="I410" s="86" t="s">
+        <v>147</v>
+      </c>
+      <c r="J410" s="86"/>
+      <c r="K410" s="86"/>
+      <c r="L410" s="86"/>
+      <c r="M410" s="86"/>
+      <c r="N410" s="87"/>
+      <c r="O410" s="73"/>
+    </row>
+    <row r="411" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A411" s="43" t="s">
+        <v>63</v>
+      </c>
+      <c r="C411" s="86">
+        <v>1</v>
+      </c>
+      <c r="D411" s="86"/>
+      <c r="E411" s="86"/>
+      <c r="F411" s="86"/>
+      <c r="G411" s="86"/>
+      <c r="H411" s="86"/>
+      <c r="I411" s="86"/>
+      <c r="J411" s="86"/>
+      <c r="K411" s="86"/>
+      <c r="L411" s="86"/>
+      <c r="M411" s="86"/>
+      <c r="N411" s="86"/>
+      <c r="O411" s="72"/>
+    </row>
+    <row r="412" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A412" s="43" t="s">
+        <v>71</v>
+      </c>
+      <c r="C412" s="88">
+        <v>0.5</v>
+      </c>
+      <c r="D412" s="88"/>
+      <c r="E412" s="88"/>
+      <c r="F412" s="88"/>
+      <c r="G412" s="88"/>
+      <c r="H412" s="88"/>
+      <c r="I412" s="88"/>
+      <c r="J412" s="88"/>
+      <c r="K412" s="88"/>
+      <c r="L412" s="88"/>
+      <c r="M412" s="88"/>
+      <c r="N412" s="88"/>
+      <c r="O412" s="72"/>
+    </row>
+    <row r="413" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A413" s="44" t="s">
+        <v>163</v>
+      </c>
+      <c r="C413" s="89">
+        <f>SUM(C$50:H$50)*C412</f>
+        <v>100</v>
+      </c>
+      <c r="D413" s="89"/>
+      <c r="E413" s="89"/>
+      <c r="F413" s="89"/>
+      <c r="G413" s="89"/>
+      <c r="H413" s="89"/>
+      <c r="I413" s="89"/>
+      <c r="J413" s="89"/>
+      <c r="K413" s="89"/>
+      <c r="L413" s="89"/>
+      <c r="M413" s="89"/>
+      <c r="N413" s="89"/>
+      <c r="O413" s="72">
+        <f>SUM(C413:N413)</f>
+        <v>100</v>
+      </c>
+      <c r="P413" s="6"/>
+      <c r="Q413" s="6"/>
+    </row>
+    <row r="414" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A414" s="43" t="s">
+        <v>0</v>
+      </c>
+      <c r="C414" s="89">
+        <v>50</v>
+      </c>
+      <c r="D414" s="89"/>
+      <c r="E414" s="89"/>
+      <c r="F414" s="89"/>
+      <c r="G414" s="89"/>
+      <c r="H414" s="89"/>
+      <c r="I414" s="89"/>
+      <c r="J414" s="89"/>
+      <c r="K414" s="89"/>
+      <c r="L414" s="89"/>
+      <c r="M414" s="89"/>
+      <c r="N414" s="89"/>
+      <c r="O414" s="72"/>
+      <c r="Q414" s="6"/>
+    </row>
+    <row r="415" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A415" s="44" t="s">
+        <v>176</v>
+      </c>
+      <c r="C415" s="89">
+        <f>IF(C414=0, C413, MIN(C413, C414))</f>
+        <v>50</v>
+      </c>
+      <c r="D415" s="89"/>
+      <c r="E415" s="89"/>
+      <c r="F415" s="89"/>
+      <c r="G415" s="89"/>
+      <c r="H415" s="89"/>
+      <c r="I415" s="89"/>
+      <c r="J415" s="89"/>
+      <c r="K415" s="89"/>
+      <c r="L415" s="89"/>
+      <c r="M415" s="89"/>
+      <c r="N415" s="89"/>
+      <c r="O415" s="72"/>
+      <c r="P415" s="6"/>
+      <c r="Q415" s="6"/>
+    </row>
+    <row r="416" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A416" s="43" t="s">
+        <v>67</v>
+      </c>
+      <c r="C416" s="89">
+        <v>40</v>
+      </c>
+      <c r="D416" s="89"/>
+      <c r="E416" s="89"/>
+      <c r="F416" s="89"/>
+      <c r="G416" s="89"/>
+      <c r="H416" s="89"/>
+      <c r="N416" s="13"/>
+      <c r="O416" s="72"/>
+    </row>
+    <row r="417" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A417" s="43" t="s">
+        <v>161</v>
+      </c>
+      <c r="C417" s="90">
+        <v>0.8</v>
+      </c>
+      <c r="D417" s="86"/>
+      <c r="E417" s="86"/>
+      <c r="F417" s="86"/>
+      <c r="G417" s="86"/>
+      <c r="H417" s="86"/>
+      <c r="N417" s="13"/>
+      <c r="O417" s="83">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="418" spans="1:17" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A418" s="45" t="s">
+        <v>164</v>
+      </c>
+      <c r="C418" s="86">
+        <f>C417*C416</f>
+        <v>32</v>
+      </c>
+      <c r="D418" s="86"/>
+      <c r="E418" s="86"/>
+      <c r="F418" s="86"/>
+      <c r="G418" s="86"/>
+      <c r="H418" s="86"/>
+      <c r="I418" s="86"/>
+      <c r="J418" s="86"/>
+      <c r="K418" s="86"/>
+      <c r="L418" s="86"/>
+      <c r="M418" s="86"/>
+      <c r="N418" s="86"/>
+      <c r="O418" s="72">
+        <f>SUM(C418:N418)</f>
+        <v>32</v>
+      </c>
+      <c r="P418" s="6"/>
+      <c r="Q418" s="6"/>
+    </row>
+    <row r="419" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A419" s="44" t="s">
+        <v>135</v>
+      </c>
+      <c r="C419" s="52">
+        <f>$C418*C$50/SUM($C$50:$H$50)</f>
+        <v>8</v>
+      </c>
+      <c r="D419" s="52">
+        <f t="shared" ref="D419:H419" si="88">$C418*D$50/SUM($C$50:$H$50)</f>
+        <v>4</v>
+      </c>
+      <c r="E419" s="52">
+        <f t="shared" si="88"/>
+        <v>4</v>
+      </c>
+      <c r="F419" s="52">
+        <f t="shared" si="88"/>
+        <v>8</v>
+      </c>
+      <c r="G419" s="52">
+        <f t="shared" si="88"/>
+        <v>4</v>
+      </c>
+      <c r="H419" s="52">
+        <f t="shared" si="88"/>
+        <v>4</v>
+      </c>
+      <c r="I419" s="52">
+        <f>$I418*I$50/SUM($I$50:$N$50)</f>
+        <v>0</v>
+      </c>
+      <c r="J419" s="52">
+        <f t="shared" ref="J419:N419" si="89">$I418*J$50/SUM($C$50:$H$50)</f>
+        <v>0</v>
+      </c>
+      <c r="K419" s="52">
+        <f t="shared" si="89"/>
+        <v>0</v>
+      </c>
+      <c r="L419" s="52">
+        <f t="shared" si="89"/>
+        <v>0</v>
+      </c>
+      <c r="M419" s="52">
+        <f t="shared" si="89"/>
+        <v>0</v>
+      </c>
+      <c r="N419" s="52">
+        <f t="shared" si="89"/>
+        <v>0</v>
+      </c>
+      <c r="O419" s="84">
+        <f>SUM(C419:N419)</f>
+        <v>32</v>
+      </c>
+    </row>
+    <row r="420" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A420" s="46" t="s">
+        <v>69</v>
+      </c>
+      <c r="C420" s="67">
+        <f>($O420-$C418)*C$50/$O$50</f>
+        <v>42</v>
+      </c>
+      <c r="D420" s="67">
+        <f t="shared" ref="D420:H420" si="90">($O420-$C418)*D$50/$O$50</f>
+        <v>21</v>
+      </c>
+      <c r="E420" s="67">
+        <f t="shared" si="90"/>
+        <v>21</v>
+      </c>
+      <c r="F420" s="67">
+        <f t="shared" si="90"/>
+        <v>42</v>
+      </c>
+      <c r="G420" s="67">
+        <f t="shared" si="90"/>
+        <v>21</v>
+      </c>
+      <c r="H420" s="67">
+        <f t="shared" si="90"/>
+        <v>21</v>
+      </c>
+      <c r="I420" s="67">
+        <f>I$50</f>
+        <v>50</v>
+      </c>
+      <c r="J420" s="67">
+        <f t="shared" ref="J420:N420" si="91">J$50</f>
+        <v>25</v>
+      </c>
+      <c r="K420" s="67">
+        <f t="shared" si="91"/>
+        <v>25</v>
+      </c>
+      <c r="L420" s="67">
+        <f t="shared" si="91"/>
+        <v>50</v>
+      </c>
+      <c r="M420" s="67">
+        <f t="shared" si="91"/>
+        <v>25</v>
+      </c>
+      <c r="N420" s="67">
+        <f t="shared" si="91"/>
+        <v>25</v>
+      </c>
+      <c r="O420" s="72">
+        <f>O$50-O418</f>
+        <v>368</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="292">
+  <mergeCells count="351">
+    <mergeCell ref="C400:H400"/>
+    <mergeCell ref="I400:N400"/>
+    <mergeCell ref="C401:H401"/>
+    <mergeCell ref="I401:N401"/>
+    <mergeCell ref="C416:H416"/>
+    <mergeCell ref="C413:H413"/>
+    <mergeCell ref="I413:N413"/>
+    <mergeCell ref="C417:H417"/>
+    <mergeCell ref="C418:H418"/>
+    <mergeCell ref="I418:N418"/>
+    <mergeCell ref="C414:H414"/>
+    <mergeCell ref="I414:N414"/>
+    <mergeCell ref="C415:H415"/>
+    <mergeCell ref="I415:N415"/>
+    <mergeCell ref="C404:H404"/>
+    <mergeCell ref="I404:N404"/>
+    <mergeCell ref="C409:H409"/>
+    <mergeCell ref="I409:N409"/>
+    <mergeCell ref="C410:H410"/>
+    <mergeCell ref="I410:N410"/>
+    <mergeCell ref="C411:H411"/>
+    <mergeCell ref="I411:N411"/>
+    <mergeCell ref="C412:H412"/>
+    <mergeCell ref="I412:N412"/>
+    <mergeCell ref="C395:H395"/>
+    <mergeCell ref="I395:N395"/>
+    <mergeCell ref="C396:H396"/>
+    <mergeCell ref="I396:N396"/>
+    <mergeCell ref="C397:H397"/>
+    <mergeCell ref="I397:N397"/>
+    <mergeCell ref="C398:H398"/>
+    <mergeCell ref="I398:N398"/>
+    <mergeCell ref="C399:H399"/>
+    <mergeCell ref="I399:N399"/>
     <mergeCell ref="C364:E364"/>
     <mergeCell ref="F364:H364"/>
     <mergeCell ref="I364:K364"/>
@@ -9060,6 +10407,31 @@
     <mergeCell ref="C137:E137"/>
     <mergeCell ref="F137:H137"/>
     <mergeCell ref="I137:K137"/>
+    <mergeCell ref="C378:H378"/>
+    <mergeCell ref="I378:N378"/>
+    <mergeCell ref="C383:H383"/>
+    <mergeCell ref="I383:N383"/>
+    <mergeCell ref="C371:H371"/>
+    <mergeCell ref="I371:N371"/>
+    <mergeCell ref="C372:H372"/>
+    <mergeCell ref="I372:N372"/>
+    <mergeCell ref="C373:H373"/>
+    <mergeCell ref="I373:N373"/>
+    <mergeCell ref="C374:H374"/>
+    <mergeCell ref="I374:N374"/>
+    <mergeCell ref="C375:H375"/>
+    <mergeCell ref="I375:N375"/>
+    <mergeCell ref="C384:H384"/>
+    <mergeCell ref="I384:N384"/>
+    <mergeCell ref="C385:H385"/>
+    <mergeCell ref="I385:N385"/>
+    <mergeCell ref="C386:H386"/>
+    <mergeCell ref="I386:N386"/>
+    <mergeCell ref="C387:H387"/>
+    <mergeCell ref="I387:N387"/>
+    <mergeCell ref="C390:H390"/>
+    <mergeCell ref="I390:N390"/>
+    <mergeCell ref="C389:H389"/>
   </mergeCells>
   <pageMargins left="0.70866141732283472" right="0.70866141732283472" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup paperSize="9" scale="44" orientation="portrait" r:id="rId1"/>
@@ -9077,15 +10449,15 @@
   </sheetPr>
   <dimension ref="A2:M25"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="18.21875" style="57" customWidth="1"/>
-    <col min="2" max="2" width="16.6640625" style="57" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="40.88671875" style="57" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20.109375" style="57" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="63.6640625" style="57" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="16.109375" style="57" customWidth="1"/>
     <col min="5" max="5" width="19.33203125" style="57" customWidth="1"/>
     <col min="6" max="6" width="19.88671875" style="57" customWidth="1"/>
@@ -9374,7 +10746,7 @@
         <v>108</v>
       </c>
       <c r="C9" s="69" t="s">
-        <v>107</v>
+        <v>179</v>
       </c>
       <c r="D9" s="69" t="s">
         <v>126</v>
@@ -9385,7 +10757,7 @@
         <v>109</v>
       </c>
       <c r="C10" s="69" t="s">
-        <v>107</v>
+        <v>180</v>
       </c>
       <c r="D10" s="69" t="s">
         <v>126</v>
@@ -9530,9 +10902,15 @@
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A19" s="59"/>
-      <c r="B19" s="56"/>
-      <c r="C19" s="56"/>
-      <c r="D19" s="56"/>
+      <c r="B19" s="85" t="s">
+        <v>165</v>
+      </c>
+      <c r="C19" s="70" t="s">
+        <v>169</v>
+      </c>
+      <c r="D19" s="70" t="s">
+        <v>171</v>
+      </c>
       <c r="E19"/>
       <c r="F19" s="56"/>
       <c r="G19" s="56"/>
@@ -9545,9 +10923,15 @@
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A20" s="59"/>
-      <c r="B20" s="56"/>
-      <c r="C20" s="56"/>
-      <c r="D20" s="56"/>
+      <c r="B20" s="85" t="s">
+        <v>168</v>
+      </c>
+      <c r="C20" s="70" t="s">
+        <v>170</v>
+      </c>
+      <c r="D20" s="70" t="s">
+        <v>171</v>
+      </c>
       <c r="E20"/>
       <c r="F20" s="56"/>
       <c r="G20" s="56"/>
@@ -9560,9 +10944,15 @@
     </row>
     <row r="21" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A21" s="59"/>
-      <c r="B21" s="56"/>
-      <c r="C21" s="56"/>
-      <c r="D21" s="56"/>
+      <c r="B21" s="85" t="s">
+        <v>172</v>
+      </c>
+      <c r="C21" s="70" t="s">
+        <v>175</v>
+      </c>
+      <c r="D21" s="70" t="s">
+        <v>171</v>
+      </c>
       <c r="E21"/>
       <c r="F21" s="56"/>
       <c r="G21" s="56"/>
@@ -9575,9 +10965,15 @@
     </row>
     <row r="22" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A22" s="59"/>
-      <c r="B22" s="56"/>
-      <c r="C22" s="56"/>
-      <c r="D22" s="56"/>
+      <c r="B22" s="85" t="s">
+        <v>173</v>
+      </c>
+      <c r="C22" s="70" t="s">
+        <v>174</v>
+      </c>
+      <c r="D22" s="70" t="s">
+        <v>171</v>
+      </c>
       <c r="E22"/>
       <c r="F22" s="56"/>
       <c r="G22" s="56"/>
@@ -9651,6 +11047,10 @@
     <hyperlink ref="B9" location="Calculations!A320" display="pol_SS" xr:uid="{9462480D-4025-45C0-9988-64F65622FE5B}"/>
     <hyperlink ref="B10" location="Calculations!A336" display="acc_SS" xr:uid="{49A1EF6D-C3F0-446C-89F0-288F81EE0F82}"/>
     <hyperlink ref="B11" location="Calculations!A352" display="multiple_SS" xr:uid="{E2892C55-32DD-47CB-B12E-68115F56099E}"/>
+    <hyperlink ref="B19" location="Calculations!A370" display="placed_acc_QS" xr:uid="{A3E79680-34CE-4365-AF36-79E1FF3FA450}"/>
+    <hyperlink ref="B20" location="Calculations!A382" display="placed_acc_1_QS" xr:uid="{A79DF74C-D25E-4A32-8A4A-D13193F5A6FA}"/>
+    <hyperlink ref="B21" location="Calculations!A394" display="placed_acc_limit_QS" xr:uid="{9198C94E-94B3-4F7C-B637-F7D17172365D}"/>
+    <hyperlink ref="B22" location="Calculations!A408" display="placed_acc_1_limit_QS" xr:uid="{37046EE5-CB2C-4C4C-8B2D-470EF59821CE}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
CAT XL with account filter
</commit_message>
<xml_diff>
--- a/examples/ExamplesComparisonTest.xlsx
+++ b/examples/ExamplesComparisonTest.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\cygwin64\home\Joh\git\ReinsuranceTestTool\examples\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{66B9626A-3F3F-4DA1-B705-AEBD080B7FC5}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{1E47A683-FB85-449E-ADC5-2AF0BED43271}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="30720" windowHeight="9072" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="611" uniqueCount="188">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="630" uniqueCount="191">
   <si>
     <t>Limit</t>
   </si>
@@ -586,6 +586,15 @@
   </si>
   <si>
     <t>SS with % ceded by location, occurrence limit and % placed</t>
+  </si>
+  <si>
+    <t>Treaty 1 on portfolio with filter on account 1: 1000 xs 50 @100%</t>
+  </si>
+  <si>
+    <t>acc_1_CAT_XL</t>
+  </si>
+  <si>
+    <t>Single CAT XL with filter on account 1</t>
   </si>
 </sst>
 </file>
@@ -886,7 +895,7 @@
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="103">
+  <cellXfs count="109">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
@@ -1136,12 +1145,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
@@ -1151,7 +1154,16 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
@@ -1181,8 +1193,23 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="6">
@@ -1604,10 +1631,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:U454"/>
+  <dimension ref="A1:U470"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A418" zoomScale="84" zoomScaleNormal="84" workbookViewId="0">
-      <selection activeCell="A422" activeCellId="1" sqref="A439 A422"/>
+    <sheetView showGridLines="0" topLeftCell="A446" zoomScale="84" zoomScaleNormal="84" workbookViewId="0">
+      <selection activeCell="A456" sqref="A456"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1993,26 +2020,26 @@
       <c r="B25" s="25" t="s">
         <v>48</v>
       </c>
-      <c r="C25" s="97">
+      <c r="C25" s="98">
         <v>100</v>
       </c>
-      <c r="D25" s="97"/>
-      <c r="E25" s="98"/>
-      <c r="F25" s="97">
+      <c r="D25" s="98"/>
+      <c r="E25" s="99"/>
+      <c r="F25" s="98">
         <v>100</v>
       </c>
-      <c r="G25" s="97"/>
-      <c r="H25" s="98"/>
-      <c r="I25" s="99">
+      <c r="G25" s="98"/>
+      <c r="H25" s="99"/>
+      <c r="I25" s="100">
         <v>100</v>
       </c>
-      <c r="J25" s="97"/>
-      <c r="K25" s="98"/>
-      <c r="L25" s="97">
+      <c r="J25" s="98"/>
+      <c r="K25" s="99"/>
+      <c r="L25" s="98">
         <v>100</v>
       </c>
-      <c r="M25" s="97"/>
-      <c r="N25" s="98"/>
+      <c r="M25" s="98"/>
+      <c r="N25" s="99"/>
       <c r="O25" s="8"/>
       <c r="P25" s="8"/>
       <c r="Q25" s="11"/>
@@ -2253,30 +2280,30 @@
       <c r="B34" s="8" t="s">
         <v>50</v>
       </c>
-      <c r="C34" s="100">
+      <c r="C34" s="101">
         <f>SUMIF($C$21:$N$21,C21,$C$31:$N$31)</f>
         <v>2000</v>
       </c>
-      <c r="D34" s="100"/>
-      <c r="E34" s="101"/>
-      <c r="F34" s="100">
+      <c r="D34" s="101"/>
+      <c r="E34" s="102"/>
+      <c r="F34" s="101">
         <f>SUMIF($C$21:$N$21,F21,$C$31:$N$31)</f>
         <v>2000</v>
       </c>
-      <c r="G34" s="100"/>
-      <c r="H34" s="101"/>
-      <c r="I34" s="100">
+      <c r="G34" s="101"/>
+      <c r="H34" s="102"/>
+      <c r="I34" s="101">
         <f>SUMIF($C$21:$N$21,I21,$C$31:$N$31)</f>
         <v>2000</v>
       </c>
-      <c r="J34" s="100"/>
-      <c r="K34" s="101"/>
-      <c r="L34" s="100">
+      <c r="J34" s="101"/>
+      <c r="K34" s="102"/>
+      <c r="L34" s="101">
         <f>SUMIF($C$21:$N$21,L21,$C$31:$N$31)</f>
         <v>2000</v>
       </c>
-      <c r="M34" s="100"/>
-      <c r="N34" s="101"/>
+      <c r="M34" s="101"/>
+      <c r="N34" s="102"/>
       <c r="O34" s="8"/>
       <c r="P34" s="23"/>
       <c r="Q34" s="11"/>
@@ -2288,30 +2315,30 @@
       <c r="B35" s="36" t="s">
         <v>52</v>
       </c>
-      <c r="C35" s="93">
+      <c r="C35" s="94">
         <f>MIN(C34, C25)</f>
         <v>100</v>
       </c>
-      <c r="D35" s="94"/>
-      <c r="E35" s="95"/>
-      <c r="F35" s="93">
+      <c r="D35" s="95"/>
+      <c r="E35" s="96"/>
+      <c r="F35" s="94">
         <f>MIN(F34, F25)</f>
         <v>100</v>
       </c>
-      <c r="G35" s="94"/>
-      <c r="H35" s="95"/>
-      <c r="I35" s="93">
+      <c r="G35" s="95"/>
+      <c r="H35" s="96"/>
+      <c r="I35" s="94">
         <f>MIN(I34, I25)</f>
         <v>100</v>
       </c>
-      <c r="J35" s="94"/>
-      <c r="K35" s="95"/>
-      <c r="L35" s="96">
+      <c r="J35" s="95"/>
+      <c r="K35" s="96"/>
+      <c r="L35" s="97">
         <f>MIN(L34, L25)</f>
         <v>100</v>
       </c>
-      <c r="M35" s="94"/>
-      <c r="N35" s="95"/>
+      <c r="M35" s="95"/>
+      <c r="N35" s="96"/>
       <c r="O35" s="12">
         <f>SUM(C35:N35)</f>
         <v>400</v>
@@ -2644,11 +2671,11 @@
       <c r="A53" s="43" t="s">
         <v>61</v>
       </c>
-      <c r="C53" s="88">
-        <v>1</v>
-      </c>
-      <c r="D53" s="88"/>
-      <c r="E53" s="89"/>
+      <c r="C53" s="90">
+        <v>1</v>
+      </c>
+      <c r="D53" s="90"/>
+      <c r="E53" s="87"/>
       <c r="H53" s="40"/>
       <c r="N53" s="40"/>
     </row>
@@ -2656,11 +2683,11 @@
       <c r="A54" s="43" t="s">
         <v>62</v>
       </c>
-      <c r="C54" s="88" t="s">
+      <c r="C54" s="90" t="s">
         <v>70</v>
       </c>
-      <c r="D54" s="88"/>
-      <c r="E54" s="89"/>
+      <c r="D54" s="90"/>
+      <c r="E54" s="87"/>
       <c r="H54" s="40"/>
       <c r="N54" s="40"/>
     </row>
@@ -2668,11 +2695,11 @@
       <c r="A55" s="43" t="s">
         <v>63</v>
       </c>
-      <c r="C55" s="88">
-        <v>1</v>
-      </c>
-      <c r="D55" s="88"/>
-      <c r="E55" s="89"/>
+      <c r="C55" s="90">
+        <v>1</v>
+      </c>
+      <c r="D55" s="90"/>
+      <c r="E55" s="87"/>
       <c r="H55" s="40"/>
       <c r="N55" s="40"/>
     </row>
@@ -2684,7 +2711,7 @@
         <v>0</v>
       </c>
       <c r="D56" s="86"/>
-      <c r="E56" s="89"/>
+      <c r="E56" s="87"/>
       <c r="H56" s="40"/>
       <c r="N56" s="40"/>
     </row>
@@ -2697,7 +2724,7 @@
         <v>100</v>
       </c>
       <c r="D57" s="86"/>
-      <c r="E57" s="89"/>
+      <c r="E57" s="87"/>
       <c r="H57" s="40"/>
       <c r="N57" s="40"/>
     </row>
@@ -2709,7 +2736,7 @@
         <v>10</v>
       </c>
       <c r="D58" s="86"/>
-      <c r="E58" s="89"/>
+      <c r="E58" s="87"/>
       <c r="H58" s="40"/>
       <c r="N58" s="40"/>
     </row>
@@ -2722,7 +2749,7 @@
         <v>10</v>
       </c>
       <c r="D59" s="86"/>
-      <c r="E59" s="89"/>
+      <c r="E59" s="87"/>
       <c r="H59" s="40"/>
       <c r="N59" s="40"/>
     </row>
@@ -2730,11 +2757,11 @@
       <c r="A60" s="43" t="s">
         <v>71</v>
       </c>
-      <c r="C60" s="90">
-        <v>1</v>
-      </c>
-      <c r="D60" s="90"/>
-      <c r="E60" s="91"/>
+      <c r="C60" s="88">
+        <v>1</v>
+      </c>
+      <c r="D60" s="88"/>
+      <c r="E60" s="89"/>
       <c r="H60" s="40"/>
       <c r="N60" s="40"/>
     </row>
@@ -2747,7 +2774,7 @@
         <v>10</v>
       </c>
       <c r="D61" s="86"/>
-      <c r="E61" s="89"/>
+      <c r="E61" s="87"/>
       <c r="H61" s="40"/>
       <c r="N61" s="40"/>
     </row>
@@ -2757,7 +2784,7 @@
       </c>
       <c r="C62" s="92"/>
       <c r="D62" s="92"/>
-      <c r="E62" s="102"/>
+      <c r="E62" s="93"/>
       <c r="H62" s="40"/>
       <c r="N62" s="40"/>
     </row>
@@ -2767,7 +2794,7 @@
       </c>
       <c r="C63" s="92"/>
       <c r="D63" s="92"/>
-      <c r="E63" s="102"/>
+      <c r="E63" s="93"/>
       <c r="H63" s="40"/>
       <c r="N63" s="40"/>
     </row>
@@ -2780,7 +2807,7 @@
         <v>10</v>
       </c>
       <c r="D64" s="86"/>
-      <c r="E64" s="89"/>
+      <c r="E64" s="87"/>
       <c r="H64" s="40"/>
       <c r="N64" s="40"/>
     </row>
@@ -2861,10 +2888,10 @@
       <c r="A68" s="43" t="s">
         <v>61</v>
       </c>
-      <c r="C68" s="88">
-        <v>1</v>
-      </c>
-      <c r="D68" s="88"/>
+      <c r="C68" s="90">
+        <v>1</v>
+      </c>
+      <c r="D68" s="90"/>
       <c r="E68" s="86"/>
       <c r="F68" s="13"/>
       <c r="H68" s="40"/>
@@ -2874,10 +2901,10 @@
       <c r="A69" s="43" t="s">
         <v>62</v>
       </c>
-      <c r="C69" s="88" t="s">
+      <c r="C69" s="90" t="s">
         <v>83</v>
       </c>
-      <c r="D69" s="88"/>
+      <c r="D69" s="90"/>
       <c r="E69" s="86"/>
       <c r="F69" s="13"/>
       <c r="H69" s="40"/>
@@ -2887,10 +2914,10 @@
       <c r="A70" s="43" t="s">
         <v>63</v>
       </c>
-      <c r="C70" s="88">
-        <v>1</v>
-      </c>
-      <c r="D70" s="88"/>
+      <c r="C70" s="90">
+        <v>1</v>
+      </c>
+      <c r="D70" s="90"/>
       <c r="E70" s="86"/>
       <c r="F70" s="13"/>
       <c r="H70" s="40"/>
@@ -2954,11 +2981,11 @@
       <c r="A75" s="43" t="s">
         <v>71</v>
       </c>
-      <c r="C75" s="90">
-        <v>1</v>
-      </c>
-      <c r="D75" s="90"/>
-      <c r="E75" s="90"/>
+      <c r="C75" s="88">
+        <v>1</v>
+      </c>
+      <c r="D75" s="88"/>
+      <c r="E75" s="88"/>
       <c r="F75" s="13"/>
       <c r="H75" s="40"/>
       <c r="N75" s="40"/>
@@ -3091,10 +3118,10 @@
       <c r="A83" s="43" t="s">
         <v>61</v>
       </c>
-      <c r="C83" s="88">
-        <v>1</v>
-      </c>
-      <c r="D83" s="88"/>
+      <c r="C83" s="90">
+        <v>1</v>
+      </c>
+      <c r="D83" s="90"/>
       <c r="E83" s="86"/>
       <c r="F83" s="13"/>
       <c r="H83" s="40"/>
@@ -3104,10 +3131,10 @@
       <c r="A84" s="43" t="s">
         <v>62</v>
       </c>
-      <c r="C84" s="88" t="s">
+      <c r="C84" s="90" t="s">
         <v>85</v>
       </c>
-      <c r="D84" s="88"/>
+      <c r="D84" s="90"/>
       <c r="E84" s="86"/>
       <c r="F84" s="13"/>
       <c r="H84" s="40"/>
@@ -3117,10 +3144,10 @@
       <c r="A85" s="43" t="s">
         <v>63</v>
       </c>
-      <c r="C85" s="88">
-        <v>1</v>
-      </c>
-      <c r="D85" s="88"/>
+      <c r="C85" s="90">
+        <v>1</v>
+      </c>
+      <c r="D85" s="90"/>
       <c r="E85" s="86"/>
       <c r="F85" s="13"/>
       <c r="H85" s="40"/>
@@ -3184,11 +3211,11 @@
       <c r="A90" s="43" t="s">
         <v>71</v>
       </c>
-      <c r="C90" s="90">
-        <v>1</v>
-      </c>
-      <c r="D90" s="90"/>
-      <c r="E90" s="90"/>
+      <c r="C90" s="88">
+        <v>1</v>
+      </c>
+      <c r="D90" s="88"/>
+      <c r="E90" s="88"/>
       <c r="F90" s="13"/>
       <c r="H90" s="40"/>
       <c r="N90" s="40"/>
@@ -3324,15 +3351,15 @@
       <c r="A98" s="43" t="s">
         <v>61</v>
       </c>
-      <c r="C98" s="88">
-        <v>1</v>
-      </c>
-      <c r="D98" s="88"/>
+      <c r="C98" s="90">
+        <v>1</v>
+      </c>
+      <c r="D98" s="90"/>
       <c r="E98" s="86"/>
-      <c r="F98" s="88">
-        <v>1</v>
-      </c>
-      <c r="G98" s="88"/>
+      <c r="F98" s="90">
+        <v>1</v>
+      </c>
+      <c r="G98" s="90"/>
       <c r="H98" s="86"/>
       <c r="N98" s="40"/>
     </row>
@@ -3340,15 +3367,15 @@
       <c r="A99" s="43" t="s">
         <v>62</v>
       </c>
-      <c r="C99" s="88" t="s">
+      <c r="C99" s="90" t="s">
         <v>70</v>
       </c>
-      <c r="D99" s="88"/>
+      <c r="D99" s="90"/>
       <c r="E99" s="86"/>
-      <c r="F99" s="88" t="s">
+      <c r="F99" s="90" t="s">
         <v>70</v>
       </c>
-      <c r="G99" s="88"/>
+      <c r="G99" s="90"/>
       <c r="H99" s="86"/>
       <c r="N99" s="40"/>
     </row>
@@ -3356,15 +3383,15 @@
       <c r="A100" s="43" t="s">
         <v>63</v>
       </c>
-      <c r="C100" s="88">
-        <v>1</v>
-      </c>
-      <c r="D100" s="88"/>
+      <c r="C100" s="90">
+        <v>1</v>
+      </c>
+      <c r="D100" s="90"/>
       <c r="E100" s="86"/>
-      <c r="F100" s="88">
-        <v>1</v>
-      </c>
-      <c r="G100" s="88"/>
+      <c r="F100" s="90">
+        <v>1</v>
+      </c>
+      <c r="G100" s="90"/>
       <c r="H100" s="86"/>
       <c r="N100" s="40"/>
     </row>
@@ -3440,16 +3467,16 @@
       <c r="A105" s="43" t="s">
         <v>71</v>
       </c>
-      <c r="C105" s="90">
-        <v>1</v>
-      </c>
-      <c r="D105" s="90"/>
-      <c r="E105" s="90"/>
-      <c r="F105" s="90">
-        <v>1</v>
-      </c>
-      <c r="G105" s="90"/>
-      <c r="H105" s="90"/>
+      <c r="C105" s="88">
+        <v>1</v>
+      </c>
+      <c r="D105" s="88"/>
+      <c r="E105" s="88"/>
+      <c r="F105" s="88">
+        <v>1</v>
+      </c>
+      <c r="G105" s="88"/>
+      <c r="H105" s="88"/>
       <c r="N105" s="40"/>
     </row>
     <row r="106" spans="1:15" ht="28.8" x14ac:dyDescent="0.3">
@@ -3585,16 +3612,16 @@
       <c r="A112" s="43" t="s">
         <v>61</v>
       </c>
-      <c r="C112" s="88">
-        <v>1</v>
-      </c>
-      <c r="D112" s="88"/>
+      <c r="C112" s="90">
+        <v>1</v>
+      </c>
+      <c r="D112" s="90"/>
       <c r="E112" s="86"/>
-      <c r="F112" s="88"/>
-      <c r="G112" s="88"/>
+      <c r="F112" s="90"/>
+      <c r="G112" s="90"/>
       <c r="H112" s="86"/>
-      <c r="I112" s="88"/>
-      <c r="J112" s="88"/>
+      <c r="I112" s="90"/>
+      <c r="J112" s="90"/>
       <c r="K112" s="86"/>
       <c r="N112" s="40"/>
     </row>
@@ -3602,16 +3629,16 @@
       <c r="A113" s="43" t="s">
         <v>62</v>
       </c>
-      <c r="C113" s="88" t="s">
+      <c r="C113" s="90" t="s">
         <v>85</v>
       </c>
-      <c r="D113" s="88"/>
+      <c r="D113" s="90"/>
       <c r="E113" s="86"/>
-      <c r="F113" s="88"/>
-      <c r="G113" s="88"/>
+      <c r="F113" s="90"/>
+      <c r="G113" s="90"/>
       <c r="H113" s="86"/>
-      <c r="I113" s="88"/>
-      <c r="J113" s="88"/>
+      <c r="I113" s="90"/>
+      <c r="J113" s="90"/>
       <c r="K113" s="86"/>
       <c r="N113" s="40"/>
     </row>
@@ -3619,16 +3646,16 @@
       <c r="A114" s="43" t="s">
         <v>63</v>
       </c>
-      <c r="C114" s="88">
-        <v>1</v>
-      </c>
-      <c r="D114" s="88"/>
+      <c r="C114" s="90">
+        <v>1</v>
+      </c>
+      <c r="D114" s="90"/>
       <c r="E114" s="86"/>
-      <c r="F114" s="88"/>
-      <c r="G114" s="88"/>
+      <c r="F114" s="90"/>
+      <c r="G114" s="90"/>
       <c r="H114" s="86"/>
-      <c r="I114" s="88"/>
-      <c r="J114" s="88"/>
+      <c r="I114" s="90"/>
+      <c r="J114" s="90"/>
       <c r="K114" s="86"/>
       <c r="N114" s="40"/>
     </row>
@@ -3706,17 +3733,17 @@
       <c r="A119" s="43" t="s">
         <v>71</v>
       </c>
-      <c r="C119" s="90">
-        <v>1</v>
-      </c>
-      <c r="D119" s="90"/>
-      <c r="E119" s="90"/>
-      <c r="F119" s="90"/>
-      <c r="G119" s="90"/>
-      <c r="H119" s="90"/>
-      <c r="I119" s="90"/>
-      <c r="J119" s="90"/>
-      <c r="K119" s="90"/>
+      <c r="C119" s="88">
+        <v>1</v>
+      </c>
+      <c r="D119" s="88"/>
+      <c r="E119" s="88"/>
+      <c r="F119" s="88"/>
+      <c r="G119" s="88"/>
+      <c r="H119" s="88"/>
+      <c r="I119" s="88"/>
+      <c r="J119" s="88"/>
+      <c r="K119" s="88"/>
       <c r="N119" s="40"/>
     </row>
     <row r="120" spans="1:15" ht="28.8" x14ac:dyDescent="0.3">
@@ -3866,16 +3893,16 @@
       <c r="A127" s="43" t="s">
         <v>61</v>
       </c>
-      <c r="C127" s="88"/>
-      <c r="D127" s="88"/>
+      <c r="C127" s="90"/>
+      <c r="D127" s="90"/>
       <c r="E127" s="86"/>
-      <c r="F127" s="88"/>
-      <c r="G127" s="88"/>
+      <c r="F127" s="90"/>
+      <c r="G127" s="90"/>
       <c r="H127" s="86"/>
-      <c r="I127" s="88">
-        <v>1</v>
-      </c>
-      <c r="J127" s="88"/>
+      <c r="I127" s="90">
+        <v>1</v>
+      </c>
+      <c r="J127" s="90"/>
       <c r="K127" s="86"/>
       <c r="N127" s="40"/>
     </row>
@@ -3883,16 +3910,16 @@
       <c r="A128" s="43" t="s">
         <v>62</v>
       </c>
-      <c r="C128" s="88"/>
-      <c r="D128" s="88"/>
+      <c r="C128" s="90"/>
+      <c r="D128" s="90"/>
       <c r="E128" s="86"/>
-      <c r="F128" s="88"/>
-      <c r="G128" s="88"/>
+      <c r="F128" s="90"/>
+      <c r="G128" s="90"/>
       <c r="H128" s="86"/>
-      <c r="I128" s="88" t="s">
+      <c r="I128" s="90" t="s">
         <v>83</v>
       </c>
-      <c r="J128" s="88"/>
+      <c r="J128" s="90"/>
       <c r="K128" s="86"/>
       <c r="N128" s="40"/>
     </row>
@@ -3900,16 +3927,16 @@
       <c r="A129" s="43" t="s">
         <v>63</v>
       </c>
-      <c r="C129" s="88"/>
-      <c r="D129" s="88"/>
+      <c r="C129" s="90"/>
+      <c r="D129" s="90"/>
       <c r="E129" s="86"/>
-      <c r="F129" s="88"/>
-      <c r="G129" s="88"/>
+      <c r="F129" s="90"/>
+      <c r="G129" s="90"/>
       <c r="H129" s="86"/>
-      <c r="I129" s="88">
-        <v>1</v>
-      </c>
-      <c r="J129" s="88"/>
+      <c r="I129" s="90">
+        <v>1</v>
+      </c>
+      <c r="J129" s="90"/>
       <c r="K129" s="86"/>
       <c r="N129" s="40"/>
     </row>
@@ -3987,17 +4014,17 @@
       <c r="A134" s="43" t="s">
         <v>71</v>
       </c>
-      <c r="C134" s="90"/>
-      <c r="D134" s="90"/>
-      <c r="E134" s="90"/>
-      <c r="F134" s="90"/>
-      <c r="G134" s="90"/>
-      <c r="H134" s="90"/>
-      <c r="I134" s="90">
-        <v>1</v>
-      </c>
-      <c r="J134" s="90"/>
-      <c r="K134" s="90"/>
+      <c r="C134" s="88"/>
+      <c r="D134" s="88"/>
+      <c r="E134" s="88"/>
+      <c r="F134" s="88"/>
+      <c r="G134" s="88"/>
+      <c r="H134" s="88"/>
+      <c r="I134" s="88">
+        <v>1</v>
+      </c>
+      <c r="J134" s="88"/>
+      <c r="K134" s="88"/>
       <c r="N134" s="40"/>
     </row>
     <row r="135" spans="1:15" ht="28.8" x14ac:dyDescent="0.3">
@@ -5204,25 +5231,25 @@
       <c r="A207" s="43" t="s">
         <v>61</v>
       </c>
-      <c r="C207" s="88">
-        <v>1</v>
-      </c>
-      <c r="D207" s="88"/>
+      <c r="C207" s="90">
+        <v>1</v>
+      </c>
+      <c r="D207" s="90"/>
       <c r="E207" s="86"/>
-      <c r="F207" s="88">
-        <v>1</v>
-      </c>
-      <c r="G207" s="88"/>
+      <c r="F207" s="90">
+        <v>1</v>
+      </c>
+      <c r="G207" s="90"/>
       <c r="H207" s="86"/>
-      <c r="I207" s="88">
-        <v>1</v>
-      </c>
-      <c r="J207" s="88"/>
+      <c r="I207" s="90">
+        <v>1</v>
+      </c>
+      <c r="J207" s="90"/>
       <c r="K207" s="86"/>
-      <c r="L207" s="88">
-        <v>1</v>
-      </c>
-      <c r="M207" s="88"/>
+      <c r="L207" s="90">
+        <v>1</v>
+      </c>
+      <c r="M207" s="90"/>
       <c r="N207" s="86"/>
       <c r="O207" s="72"/>
     </row>
@@ -5230,25 +5257,25 @@
       <c r="A208" s="43" t="s">
         <v>62</v>
       </c>
-      <c r="C208" s="88" t="s">
+      <c r="C208" s="90" t="s">
         <v>139</v>
       </c>
-      <c r="D208" s="88"/>
+      <c r="D208" s="90"/>
       <c r="E208" s="86"/>
-      <c r="F208" s="88" t="s">
+      <c r="F208" s="90" t="s">
         <v>140</v>
       </c>
-      <c r="G208" s="88"/>
+      <c r="G208" s="90"/>
       <c r="H208" s="86"/>
-      <c r="I208" s="88" t="s">
+      <c r="I208" s="90" t="s">
         <v>141</v>
       </c>
-      <c r="J208" s="88"/>
+      <c r="J208" s="90"/>
       <c r="K208" s="86"/>
-      <c r="L208" s="88" t="s">
+      <c r="L208" s="90" t="s">
         <v>142</v>
       </c>
-      <c r="M208" s="88"/>
+      <c r="M208" s="90"/>
       <c r="N208" s="86"/>
       <c r="O208" s="73"/>
     </row>
@@ -5256,25 +5283,25 @@
       <c r="A209" s="43" t="s">
         <v>63</v>
       </c>
-      <c r="C209" s="88">
-        <v>1</v>
-      </c>
-      <c r="D209" s="88"/>
+      <c r="C209" s="90">
+        <v>1</v>
+      </c>
+      <c r="D209" s="90"/>
       <c r="E209" s="86"/>
-      <c r="F209" s="88">
-        <v>1</v>
-      </c>
-      <c r="G209" s="88"/>
+      <c r="F209" s="90">
+        <v>1</v>
+      </c>
+      <c r="G209" s="90"/>
       <c r="H209" s="86"/>
-      <c r="I209" s="88">
-        <v>1</v>
-      </c>
-      <c r="J209" s="88"/>
+      <c r="I209" s="90">
+        <v>1</v>
+      </c>
+      <c r="J209" s="90"/>
       <c r="K209" s="86"/>
-      <c r="L209" s="88">
-        <v>1</v>
-      </c>
-      <c r="M209" s="88"/>
+      <c r="L209" s="90">
+        <v>1</v>
+      </c>
+      <c r="M209" s="90"/>
       <c r="N209" s="86"/>
       <c r="O209" s="72"/>
     </row>
@@ -5399,26 +5426,26 @@
       <c r="A214" s="43" t="s">
         <v>71</v>
       </c>
-      <c r="C214" s="90">
+      <c r="C214" s="88">
         <v>0.5</v>
       </c>
-      <c r="D214" s="90"/>
-      <c r="E214" s="90"/>
-      <c r="F214" s="90">
+      <c r="D214" s="88"/>
+      <c r="E214" s="88"/>
+      <c r="F214" s="88">
         <v>0.5</v>
       </c>
-      <c r="G214" s="90"/>
-      <c r="H214" s="90"/>
-      <c r="I214" s="90">
+      <c r="G214" s="88"/>
+      <c r="H214" s="88"/>
+      <c r="I214" s="88">
         <v>0.5</v>
       </c>
-      <c r="J214" s="90"/>
-      <c r="K214" s="90"/>
-      <c r="L214" s="90">
+      <c r="J214" s="88"/>
+      <c r="K214" s="88"/>
+      <c r="L214" s="88">
         <v>0.5</v>
       </c>
-      <c r="M214" s="90"/>
-      <c r="N214" s="90"/>
+      <c r="M214" s="88"/>
+      <c r="N214" s="88"/>
       <c r="O214" s="74"/>
       <c r="Q214" s="6"/>
     </row>
@@ -5449,7 +5476,7 @@
         <v>10</v>
       </c>
       <c r="M215" s="86"/>
-      <c r="N215" s="89"/>
+      <c r="N215" s="87"/>
       <c r="O215" s="72"/>
     </row>
     <row r="216" spans="1:17" x14ac:dyDescent="0.3">
@@ -5608,66 +5635,66 @@
       <c r="A223" s="43" t="s">
         <v>61</v>
       </c>
-      <c r="C223" s="88">
-        <v>1</v>
-      </c>
-      <c r="D223" s="88"/>
-      <c r="E223" s="88"/>
-      <c r="F223" s="88"/>
-      <c r="G223" s="88"/>
-      <c r="H223" s="88"/>
-      <c r="I223" s="88">
-        <v>1</v>
-      </c>
-      <c r="J223" s="88"/>
-      <c r="K223" s="88"/>
-      <c r="L223" s="88"/>
-      <c r="M223" s="88"/>
-      <c r="N223" s="89"/>
+      <c r="C223" s="90">
+        <v>1</v>
+      </c>
+      <c r="D223" s="90"/>
+      <c r="E223" s="90"/>
+      <c r="F223" s="90"/>
+      <c r="G223" s="90"/>
+      <c r="H223" s="90"/>
+      <c r="I223" s="90">
+        <v>1</v>
+      </c>
+      <c r="J223" s="90"/>
+      <c r="K223" s="90"/>
+      <c r="L223" s="90"/>
+      <c r="M223" s="90"/>
+      <c r="N223" s="87"/>
       <c r="O223" s="72"/>
     </row>
     <row r="224" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A224" s="43" t="s">
         <v>62</v>
       </c>
-      <c r="C224" s="88" t="s">
+      <c r="C224" s="90" t="s">
         <v>138</v>
       </c>
-      <c r="D224" s="88"/>
-      <c r="E224" s="88"/>
-      <c r="F224" s="88"/>
-      <c r="G224" s="88"/>
-      <c r="H224" s="88"/>
-      <c r="I224" s="88" t="s">
+      <c r="D224" s="90"/>
+      <c r="E224" s="90"/>
+      <c r="F224" s="90"/>
+      <c r="G224" s="90"/>
+      <c r="H224" s="90"/>
+      <c r="I224" s="90" t="s">
         <v>143</v>
       </c>
-      <c r="J224" s="88"/>
-      <c r="K224" s="88"/>
-      <c r="L224" s="88"/>
-      <c r="M224" s="88"/>
-      <c r="N224" s="89"/>
+      <c r="J224" s="90"/>
+      <c r="K224" s="90"/>
+      <c r="L224" s="90"/>
+      <c r="M224" s="90"/>
+      <c r="N224" s="87"/>
       <c r="O224" s="73"/>
     </row>
     <row r="225" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A225" s="43" t="s">
         <v>63</v>
       </c>
-      <c r="C225" s="88">
-        <v>1</v>
-      </c>
-      <c r="D225" s="88"/>
-      <c r="E225" s="88"/>
-      <c r="F225" s="88"/>
-      <c r="G225" s="88"/>
-      <c r="H225" s="88"/>
-      <c r="I225" s="88">
-        <v>1</v>
-      </c>
-      <c r="J225" s="88"/>
-      <c r="K225" s="88"/>
-      <c r="L225" s="88"/>
-      <c r="M225" s="88"/>
-      <c r="N225" s="88"/>
+      <c r="C225" s="90">
+        <v>1</v>
+      </c>
+      <c r="D225" s="90"/>
+      <c r="E225" s="90"/>
+      <c r="F225" s="90"/>
+      <c r="G225" s="90"/>
+      <c r="H225" s="90"/>
+      <c r="I225" s="90">
+        <v>1</v>
+      </c>
+      <c r="J225" s="90"/>
+      <c r="K225" s="90"/>
+      <c r="L225" s="90"/>
+      <c r="M225" s="90"/>
+      <c r="N225" s="90"/>
       <c r="O225" s="72"/>
     </row>
     <row r="226" spans="1:17" x14ac:dyDescent="0.3">
@@ -5771,22 +5798,22 @@
       <c r="A230" s="43" t="s">
         <v>71</v>
       </c>
-      <c r="C230" s="90">
+      <c r="C230" s="88">
         <v>0.5</v>
       </c>
-      <c r="D230" s="90"/>
-      <c r="E230" s="90"/>
-      <c r="F230" s="90"/>
-      <c r="G230" s="90"/>
-      <c r="H230" s="90"/>
-      <c r="I230" s="90">
+      <c r="D230" s="88"/>
+      <c r="E230" s="88"/>
+      <c r="F230" s="88"/>
+      <c r="G230" s="88"/>
+      <c r="H230" s="88"/>
+      <c r="I230" s="88">
         <v>0.5</v>
       </c>
-      <c r="J230" s="90"/>
-      <c r="K230" s="90"/>
-      <c r="L230" s="90"/>
-      <c r="M230" s="90"/>
-      <c r="N230" s="90"/>
+      <c r="J230" s="88"/>
+      <c r="K230" s="88"/>
+      <c r="L230" s="88"/>
+      <c r="M230" s="88"/>
+      <c r="N230" s="88"/>
       <c r="O230" s="74"/>
       <c r="Q230" s="6"/>
     </row>
@@ -5970,66 +5997,66 @@
       <c r="A239" s="43" t="s">
         <v>61</v>
       </c>
-      <c r="C239" s="88">
-        <v>1</v>
-      </c>
-      <c r="D239" s="88"/>
-      <c r="E239" s="88"/>
-      <c r="F239" s="88"/>
-      <c r="G239" s="88"/>
-      <c r="H239" s="88"/>
-      <c r="I239" s="88">
-        <v>1</v>
-      </c>
-      <c r="J239" s="88"/>
-      <c r="K239" s="88"/>
-      <c r="L239" s="88"/>
-      <c r="M239" s="88"/>
-      <c r="N239" s="89"/>
+      <c r="C239" s="90">
+        <v>1</v>
+      </c>
+      <c r="D239" s="90"/>
+      <c r="E239" s="90"/>
+      <c r="F239" s="90"/>
+      <c r="G239" s="90"/>
+      <c r="H239" s="90"/>
+      <c r="I239" s="90">
+        <v>1</v>
+      </c>
+      <c r="J239" s="90"/>
+      <c r="K239" s="90"/>
+      <c r="L239" s="90"/>
+      <c r="M239" s="90"/>
+      <c r="N239" s="87"/>
       <c r="O239" s="72"/>
     </row>
     <row r="240" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A240" s="43" t="s">
         <v>62</v>
       </c>
-      <c r="C240" s="88" t="s">
+      <c r="C240" s="90" t="s">
         <v>146</v>
       </c>
-      <c r="D240" s="88"/>
-      <c r="E240" s="88"/>
-      <c r="F240" s="88"/>
-      <c r="G240" s="88"/>
-      <c r="H240" s="88"/>
-      <c r="I240" s="88" t="s">
+      <c r="D240" s="90"/>
+      <c r="E240" s="90"/>
+      <c r="F240" s="90"/>
+      <c r="G240" s="90"/>
+      <c r="H240" s="90"/>
+      <c r="I240" s="90" t="s">
         <v>147</v>
       </c>
-      <c r="J240" s="88"/>
-      <c r="K240" s="88"/>
-      <c r="L240" s="88"/>
-      <c r="M240" s="88"/>
-      <c r="N240" s="89"/>
+      <c r="J240" s="90"/>
+      <c r="K240" s="90"/>
+      <c r="L240" s="90"/>
+      <c r="M240" s="90"/>
+      <c r="N240" s="87"/>
       <c r="O240" s="73"/>
     </row>
     <row r="241" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A241" s="43" t="s">
         <v>63</v>
       </c>
-      <c r="C241" s="88">
-        <v>1</v>
-      </c>
-      <c r="D241" s="88"/>
-      <c r="E241" s="88"/>
-      <c r="F241" s="88"/>
-      <c r="G241" s="88"/>
-      <c r="H241" s="88"/>
-      <c r="I241" s="88">
-        <v>1</v>
-      </c>
-      <c r="J241" s="88"/>
-      <c r="K241" s="88"/>
-      <c r="L241" s="88"/>
-      <c r="M241" s="88"/>
-      <c r="N241" s="88"/>
+      <c r="C241" s="90">
+        <v>1</v>
+      </c>
+      <c r="D241" s="90"/>
+      <c r="E241" s="90"/>
+      <c r="F241" s="90"/>
+      <c r="G241" s="90"/>
+      <c r="H241" s="90"/>
+      <c r="I241" s="90">
+        <v>1</v>
+      </c>
+      <c r="J241" s="90"/>
+      <c r="K241" s="90"/>
+      <c r="L241" s="90"/>
+      <c r="M241" s="90"/>
+      <c r="N241" s="90"/>
       <c r="O241" s="72"/>
     </row>
     <row r="242" spans="1:17" x14ac:dyDescent="0.3">
@@ -6133,22 +6160,22 @@
       <c r="A246" s="43" t="s">
         <v>71</v>
       </c>
-      <c r="C246" s="90">
+      <c r="C246" s="88">
         <v>0.5</v>
       </c>
-      <c r="D246" s="90"/>
-      <c r="E246" s="90"/>
-      <c r="F246" s="90"/>
-      <c r="G246" s="90"/>
-      <c r="H246" s="90"/>
-      <c r="I246" s="90">
+      <c r="D246" s="88"/>
+      <c r="E246" s="88"/>
+      <c r="F246" s="88"/>
+      <c r="G246" s="88"/>
+      <c r="H246" s="88"/>
+      <c r="I246" s="88">
         <v>0.5</v>
       </c>
-      <c r="J246" s="90"/>
-      <c r="K246" s="90"/>
-      <c r="L246" s="90"/>
-      <c r="M246" s="90"/>
-      <c r="N246" s="90"/>
+      <c r="J246" s="88"/>
+      <c r="K246" s="88"/>
+      <c r="L246" s="88"/>
+      <c r="M246" s="88"/>
+      <c r="N246" s="88"/>
       <c r="O246" s="74"/>
       <c r="Q246" s="6"/>
     </row>
@@ -7164,25 +7191,25 @@
       <c r="A305" s="43" t="s">
         <v>61</v>
       </c>
-      <c r="C305" s="88">
-        <v>1</v>
-      </c>
-      <c r="D305" s="88"/>
+      <c r="C305" s="90">
+        <v>1</v>
+      </c>
+      <c r="D305" s="90"/>
       <c r="E305" s="86"/>
-      <c r="F305" s="88">
-        <v>1</v>
-      </c>
-      <c r="G305" s="88"/>
+      <c r="F305" s="90">
+        <v>1</v>
+      </c>
+      <c r="G305" s="90"/>
       <c r="H305" s="86"/>
-      <c r="I305" s="88">
-        <v>1</v>
-      </c>
-      <c r="J305" s="88"/>
+      <c r="I305" s="90">
+        <v>1</v>
+      </c>
+      <c r="J305" s="90"/>
       <c r="K305" s="86"/>
-      <c r="L305" s="88">
-        <v>1</v>
-      </c>
-      <c r="M305" s="88"/>
+      <c r="L305" s="90">
+        <v>1</v>
+      </c>
+      <c r="M305" s="90"/>
       <c r="N305" s="86"/>
       <c r="O305" s="72"/>
     </row>
@@ -7190,25 +7217,25 @@
       <c r="A306" s="43" t="s">
         <v>62</v>
       </c>
-      <c r="C306" s="88" t="s">
+      <c r="C306" s="90" t="s">
         <v>139</v>
       </c>
-      <c r="D306" s="88"/>
+      <c r="D306" s="90"/>
       <c r="E306" s="86"/>
-      <c r="F306" s="88" t="s">
+      <c r="F306" s="90" t="s">
         <v>140</v>
       </c>
-      <c r="G306" s="88"/>
+      <c r="G306" s="90"/>
       <c r="H306" s="86"/>
-      <c r="I306" s="88" t="s">
+      <c r="I306" s="90" t="s">
         <v>141</v>
       </c>
-      <c r="J306" s="88"/>
+      <c r="J306" s="90"/>
       <c r="K306" s="86"/>
-      <c r="L306" s="88" t="s">
+      <c r="L306" s="90" t="s">
         <v>142</v>
       </c>
-      <c r="M306" s="88"/>
+      <c r="M306" s="90"/>
       <c r="N306" s="86"/>
       <c r="O306" s="73"/>
     </row>
@@ -7216,25 +7243,25 @@
       <c r="A307" s="43" t="s">
         <v>63</v>
       </c>
-      <c r="C307" s="88">
-        <v>1</v>
-      </c>
-      <c r="D307" s="88"/>
+      <c r="C307" s="90">
+        <v>1</v>
+      </c>
+      <c r="D307" s="90"/>
       <c r="E307" s="86"/>
-      <c r="F307" s="88">
-        <v>1</v>
-      </c>
-      <c r="G307" s="88"/>
+      <c r="F307" s="90">
+        <v>1</v>
+      </c>
+      <c r="G307" s="90"/>
       <c r="H307" s="86"/>
-      <c r="I307" s="88">
-        <v>1</v>
-      </c>
-      <c r="J307" s="88"/>
+      <c r="I307" s="90">
+        <v>1</v>
+      </c>
+      <c r="J307" s="90"/>
       <c r="K307" s="86"/>
-      <c r="L307" s="88">
-        <v>1</v>
-      </c>
-      <c r="M307" s="88"/>
+      <c r="L307" s="90">
+        <v>1</v>
+      </c>
+      <c r="M307" s="90"/>
       <c r="N307" s="86"/>
       <c r="O307" s="72"/>
     </row>
@@ -7359,26 +7386,26 @@
       <c r="A312" s="43" t="s">
         <v>71</v>
       </c>
-      <c r="C312" s="90">
+      <c r="C312" s="88">
         <v>0.1</v>
       </c>
-      <c r="D312" s="90"/>
-      <c r="E312" s="90"/>
-      <c r="F312" s="90">
+      <c r="D312" s="88"/>
+      <c r="E312" s="88"/>
+      <c r="F312" s="88">
         <v>0.1</v>
       </c>
-      <c r="G312" s="90"/>
-      <c r="H312" s="90"/>
-      <c r="I312" s="90">
+      <c r="G312" s="88"/>
+      <c r="H312" s="88"/>
+      <c r="I312" s="88">
         <v>0.1</v>
       </c>
-      <c r="J312" s="90"/>
-      <c r="K312" s="90"/>
-      <c r="L312" s="90">
+      <c r="J312" s="88"/>
+      <c r="K312" s="88"/>
+      <c r="L312" s="88">
         <v>0.1</v>
       </c>
-      <c r="M312" s="90"/>
-      <c r="N312" s="91"/>
+      <c r="M312" s="88"/>
+      <c r="N312" s="89"/>
       <c r="O312" s="74"/>
       <c r="Q312" s="6"/>
     </row>
@@ -7409,7 +7436,7 @@
         <v>10</v>
       </c>
       <c r="M313" s="86"/>
-      <c r="N313" s="89"/>
+      <c r="N313" s="87"/>
       <c r="O313" s="72"/>
     </row>
     <row r="314" spans="1:17" x14ac:dyDescent="0.3">
@@ -7568,66 +7595,66 @@
       <c r="A321" s="43" t="s">
         <v>61</v>
       </c>
-      <c r="C321" s="88">
-        <v>1</v>
-      </c>
-      <c r="D321" s="88"/>
-      <c r="E321" s="88"/>
-      <c r="F321" s="88"/>
-      <c r="G321" s="88"/>
-      <c r="H321" s="88"/>
-      <c r="I321" s="88">
-        <v>1</v>
-      </c>
-      <c r="J321" s="88"/>
-      <c r="K321" s="88"/>
-      <c r="L321" s="88"/>
-      <c r="M321" s="88"/>
-      <c r="N321" s="89"/>
+      <c r="C321" s="90">
+        <v>1</v>
+      </c>
+      <c r="D321" s="90"/>
+      <c r="E321" s="90"/>
+      <c r="F321" s="90"/>
+      <c r="G321" s="90"/>
+      <c r="H321" s="90"/>
+      <c r="I321" s="90">
+        <v>1</v>
+      </c>
+      <c r="J321" s="90"/>
+      <c r="K321" s="90"/>
+      <c r="L321" s="90"/>
+      <c r="M321" s="90"/>
+      <c r="N321" s="87"/>
       <c r="O321" s="72"/>
     </row>
     <row r="322" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A322" s="43" t="s">
         <v>62</v>
       </c>
-      <c r="C322" s="88" t="s">
+      <c r="C322" s="90" t="s">
         <v>138</v>
       </c>
-      <c r="D322" s="88"/>
-      <c r="E322" s="88"/>
-      <c r="F322" s="88"/>
-      <c r="G322" s="88"/>
-      <c r="H322" s="88"/>
-      <c r="I322" s="88" t="s">
+      <c r="D322" s="90"/>
+      <c r="E322" s="90"/>
+      <c r="F322" s="90"/>
+      <c r="G322" s="90"/>
+      <c r="H322" s="90"/>
+      <c r="I322" s="90" t="s">
         <v>143</v>
       </c>
-      <c r="J322" s="88"/>
-      <c r="K322" s="88"/>
-      <c r="L322" s="88"/>
-      <c r="M322" s="88"/>
-      <c r="N322" s="89"/>
+      <c r="J322" s="90"/>
+      <c r="K322" s="90"/>
+      <c r="L322" s="90"/>
+      <c r="M322" s="90"/>
+      <c r="N322" s="87"/>
       <c r="O322" s="73"/>
     </row>
     <row r="323" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A323" s="43" t="s">
         <v>63</v>
       </c>
-      <c r="C323" s="88">
-        <v>1</v>
-      </c>
-      <c r="D323" s="88"/>
-      <c r="E323" s="88"/>
-      <c r="F323" s="88"/>
-      <c r="G323" s="88"/>
-      <c r="H323" s="88"/>
-      <c r="I323" s="88">
-        <v>1</v>
-      </c>
-      <c r="J323" s="88"/>
-      <c r="K323" s="88"/>
-      <c r="L323" s="88"/>
-      <c r="M323" s="88"/>
-      <c r="N323" s="88"/>
+      <c r="C323" s="90">
+        <v>1</v>
+      </c>
+      <c r="D323" s="90"/>
+      <c r="E323" s="90"/>
+      <c r="F323" s="90"/>
+      <c r="G323" s="90"/>
+      <c r="H323" s="90"/>
+      <c r="I323" s="90">
+        <v>1</v>
+      </c>
+      <c r="J323" s="90"/>
+      <c r="K323" s="90"/>
+      <c r="L323" s="90"/>
+      <c r="M323" s="90"/>
+      <c r="N323" s="90"/>
       <c r="O323" s="72"/>
     </row>
     <row r="324" spans="1:17" x14ac:dyDescent="0.3">
@@ -7731,22 +7758,22 @@
       <c r="A328" s="43" t="s">
         <v>71</v>
       </c>
-      <c r="C328" s="90">
+      <c r="C328" s="88">
         <v>0.1</v>
       </c>
-      <c r="D328" s="90"/>
-      <c r="E328" s="90"/>
-      <c r="F328" s="90"/>
-      <c r="G328" s="90"/>
-      <c r="H328" s="90"/>
-      <c r="I328" s="90">
+      <c r="D328" s="88"/>
+      <c r="E328" s="88"/>
+      <c r="F328" s="88"/>
+      <c r="G328" s="88"/>
+      <c r="H328" s="88"/>
+      <c r="I328" s="88">
         <v>0.1</v>
       </c>
-      <c r="J328" s="90"/>
-      <c r="K328" s="90"/>
-      <c r="L328" s="90"/>
-      <c r="M328" s="90"/>
-      <c r="N328" s="90"/>
+      <c r="J328" s="88"/>
+      <c r="K328" s="88"/>
+      <c r="L328" s="88"/>
+      <c r="M328" s="88"/>
+      <c r="N328" s="88"/>
       <c r="O328" s="74"/>
       <c r="Q328" s="6"/>
     </row>
@@ -7930,66 +7957,66 @@
       <c r="A337" s="43" t="s">
         <v>61</v>
       </c>
-      <c r="C337" s="88">
-        <v>1</v>
-      </c>
-      <c r="D337" s="88"/>
-      <c r="E337" s="88"/>
-      <c r="F337" s="88"/>
-      <c r="G337" s="88"/>
-      <c r="H337" s="88"/>
-      <c r="I337" s="88">
-        <v>1</v>
-      </c>
-      <c r="J337" s="88"/>
-      <c r="K337" s="88"/>
-      <c r="L337" s="88"/>
-      <c r="M337" s="88"/>
-      <c r="N337" s="89"/>
+      <c r="C337" s="90">
+        <v>1</v>
+      </c>
+      <c r="D337" s="90"/>
+      <c r="E337" s="90"/>
+      <c r="F337" s="90"/>
+      <c r="G337" s="90"/>
+      <c r="H337" s="90"/>
+      <c r="I337" s="90">
+        <v>1</v>
+      </c>
+      <c r="J337" s="90"/>
+      <c r="K337" s="90"/>
+      <c r="L337" s="90"/>
+      <c r="M337" s="90"/>
+      <c r="N337" s="87"/>
       <c r="O337" s="72"/>
     </row>
     <row r="338" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A338" s="43" t="s">
         <v>62</v>
       </c>
-      <c r="C338" s="88" t="s">
+      <c r="C338" s="90" t="s">
         <v>146</v>
       </c>
-      <c r="D338" s="88"/>
-      <c r="E338" s="88"/>
-      <c r="F338" s="88"/>
-      <c r="G338" s="88"/>
-      <c r="H338" s="88"/>
-      <c r="I338" s="88" t="s">
+      <c r="D338" s="90"/>
+      <c r="E338" s="90"/>
+      <c r="F338" s="90"/>
+      <c r="G338" s="90"/>
+      <c r="H338" s="90"/>
+      <c r="I338" s="90" t="s">
         <v>147</v>
       </c>
-      <c r="J338" s="88"/>
-      <c r="K338" s="88"/>
-      <c r="L338" s="88"/>
-      <c r="M338" s="88"/>
-      <c r="N338" s="89"/>
+      <c r="J338" s="90"/>
+      <c r="K338" s="90"/>
+      <c r="L338" s="90"/>
+      <c r="M338" s="90"/>
+      <c r="N338" s="87"/>
       <c r="O338" s="73"/>
     </row>
     <row r="339" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A339" s="43" t="s">
         <v>63</v>
       </c>
-      <c r="C339" s="88">
-        <v>1</v>
-      </c>
-      <c r="D339" s="88"/>
-      <c r="E339" s="88"/>
-      <c r="F339" s="88"/>
-      <c r="G339" s="88"/>
-      <c r="H339" s="88"/>
-      <c r="I339" s="88">
-        <v>1</v>
-      </c>
-      <c r="J339" s="88"/>
-      <c r="K339" s="88"/>
-      <c r="L339" s="88"/>
-      <c r="M339" s="88"/>
-      <c r="N339" s="88"/>
+      <c r="C339" s="90">
+        <v>1</v>
+      </c>
+      <c r="D339" s="90"/>
+      <c r="E339" s="90"/>
+      <c r="F339" s="90"/>
+      <c r="G339" s="90"/>
+      <c r="H339" s="90"/>
+      <c r="I339" s="90">
+        <v>1</v>
+      </c>
+      <c r="J339" s="90"/>
+      <c r="K339" s="90"/>
+      <c r="L339" s="90"/>
+      <c r="M339" s="90"/>
+      <c r="N339" s="90"/>
       <c r="O339" s="72"/>
     </row>
     <row r="340" spans="1:17" x14ac:dyDescent="0.3">
@@ -8093,22 +8120,22 @@
       <c r="A344" s="43" t="s">
         <v>71</v>
       </c>
-      <c r="C344" s="90">
+      <c r="C344" s="88">
         <v>0.1</v>
       </c>
-      <c r="D344" s="90"/>
-      <c r="E344" s="90"/>
-      <c r="F344" s="90"/>
-      <c r="G344" s="90"/>
-      <c r="H344" s="90"/>
-      <c r="I344" s="90">
+      <c r="D344" s="88"/>
+      <c r="E344" s="88"/>
+      <c r="F344" s="88"/>
+      <c r="G344" s="88"/>
+      <c r="H344" s="88"/>
+      <c r="I344" s="88">
         <v>0.1</v>
       </c>
-      <c r="J344" s="90"/>
-      <c r="K344" s="90"/>
-      <c r="L344" s="90"/>
-      <c r="M344" s="90"/>
-      <c r="N344" s="90"/>
+      <c r="J344" s="88"/>
+      <c r="K344" s="88"/>
+      <c r="L344" s="88"/>
+      <c r="M344" s="88"/>
+      <c r="N344" s="88"/>
       <c r="O344" s="74"/>
       <c r="Q344" s="6"/>
     </row>
@@ -8643,18 +8670,18 @@
       <c r="A364" s="45" t="s">
         <v>74</v>
       </c>
-      <c r="C364" s="88"/>
-      <c r="D364" s="88"/>
-      <c r="E364" s="88"/>
-      <c r="F364" s="88"/>
-      <c r="G364" s="88"/>
-      <c r="H364" s="88"/>
-      <c r="I364" s="88"/>
-      <c r="J364" s="88"/>
-      <c r="K364" s="88"/>
-      <c r="L364" s="88"/>
-      <c r="M364" s="88"/>
-      <c r="N364" s="88"/>
+      <c r="C364" s="90"/>
+      <c r="D364" s="90"/>
+      <c r="E364" s="90"/>
+      <c r="F364" s="90"/>
+      <c r="G364" s="90"/>
+      <c r="H364" s="90"/>
+      <c r="I364" s="90"/>
+      <c r="J364" s="90"/>
+      <c r="K364" s="90"/>
+      <c r="L364" s="90"/>
+      <c r="M364" s="90"/>
+      <c r="N364" s="90"/>
       <c r="O364" s="72">
         <f>SUM(C361:M361)</f>
         <v>120</v>
@@ -8869,88 +8896,88 @@
       <c r="A371" s="43" t="s">
         <v>61</v>
       </c>
-      <c r="C371" s="88">
-        <v>1</v>
-      </c>
-      <c r="D371" s="88"/>
-      <c r="E371" s="88"/>
-      <c r="F371" s="88"/>
-      <c r="G371" s="88"/>
-      <c r="H371" s="88"/>
-      <c r="I371" s="88">
-        <v>1</v>
-      </c>
-      <c r="J371" s="88"/>
-      <c r="K371" s="88"/>
-      <c r="L371" s="88"/>
-      <c r="M371" s="88"/>
-      <c r="N371" s="89"/>
+      <c r="C371" s="90">
+        <v>1</v>
+      </c>
+      <c r="D371" s="90"/>
+      <c r="E371" s="90"/>
+      <c r="F371" s="90"/>
+      <c r="G371" s="90"/>
+      <c r="H371" s="90"/>
+      <c r="I371" s="90">
+        <v>1</v>
+      </c>
+      <c r="J371" s="90"/>
+      <c r="K371" s="90"/>
+      <c r="L371" s="90"/>
+      <c r="M371" s="90"/>
+      <c r="N371" s="87"/>
       <c r="O371" s="72"/>
     </row>
     <row r="372" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A372" s="43" t="s">
         <v>62</v>
       </c>
-      <c r="C372" s="88" t="s">
+      <c r="C372" s="90" t="s">
         <v>146</v>
       </c>
-      <c r="D372" s="88"/>
-      <c r="E372" s="88"/>
-      <c r="F372" s="88"/>
-      <c r="G372" s="88"/>
-      <c r="H372" s="88"/>
-      <c r="I372" s="88" t="s">
+      <c r="D372" s="90"/>
+      <c r="E372" s="90"/>
+      <c r="F372" s="90"/>
+      <c r="G372" s="90"/>
+      <c r="H372" s="90"/>
+      <c r="I372" s="90" t="s">
         <v>147</v>
       </c>
-      <c r="J372" s="88"/>
-      <c r="K372" s="88"/>
-      <c r="L372" s="88"/>
-      <c r="M372" s="88"/>
-      <c r="N372" s="89"/>
+      <c r="J372" s="90"/>
+      <c r="K372" s="90"/>
+      <c r="L372" s="90"/>
+      <c r="M372" s="90"/>
+      <c r="N372" s="87"/>
       <c r="O372" s="73"/>
     </row>
     <row r="373" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A373" s="43" t="s">
         <v>63</v>
       </c>
-      <c r="C373" s="88">
-        <v>1</v>
-      </c>
-      <c r="D373" s="88"/>
-      <c r="E373" s="88"/>
-      <c r="F373" s="88"/>
-      <c r="G373" s="88"/>
-      <c r="H373" s="88"/>
-      <c r="I373" s="88">
-        <v>1</v>
-      </c>
-      <c r="J373" s="88"/>
-      <c r="K373" s="88"/>
-      <c r="L373" s="88"/>
-      <c r="M373" s="88"/>
-      <c r="N373" s="88"/>
+      <c r="C373" s="90">
+        <v>1</v>
+      </c>
+      <c r="D373" s="90"/>
+      <c r="E373" s="90"/>
+      <c r="F373" s="90"/>
+      <c r="G373" s="90"/>
+      <c r="H373" s="90"/>
+      <c r="I373" s="90">
+        <v>1</v>
+      </c>
+      <c r="J373" s="90"/>
+      <c r="K373" s="90"/>
+      <c r="L373" s="90"/>
+      <c r="M373" s="90"/>
+      <c r="N373" s="90"/>
       <c r="O373" s="72"/>
     </row>
     <row r="374" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A374" s="43" t="s">
         <v>71</v>
       </c>
-      <c r="C374" s="90">
+      <c r="C374" s="88">
         <v>0.5</v>
       </c>
-      <c r="D374" s="90"/>
-      <c r="E374" s="90"/>
-      <c r="F374" s="90"/>
-      <c r="G374" s="90"/>
-      <c r="H374" s="90"/>
-      <c r="I374" s="90">
+      <c r="D374" s="88"/>
+      <c r="E374" s="88"/>
+      <c r="F374" s="88"/>
+      <c r="G374" s="88"/>
+      <c r="H374" s="88"/>
+      <c r="I374" s="88">
         <v>0.5</v>
       </c>
-      <c r="J374" s="90"/>
-      <c r="K374" s="90"/>
-      <c r="L374" s="90"/>
-      <c r="M374" s="90"/>
-      <c r="N374" s="90"/>
+      <c r="J374" s="88"/>
+      <c r="K374" s="88"/>
+      <c r="L374" s="88"/>
+      <c r="M374" s="88"/>
+      <c r="N374" s="88"/>
       <c r="O374" s="72"/>
     </row>
     <row r="375" spans="1:17" x14ac:dyDescent="0.3">
@@ -9002,24 +9029,24 @@
       <c r="A378" s="45" t="s">
         <v>164</v>
       </c>
-      <c r="C378" s="88">
+      <c r="C378" s="90">
         <f>O$378*C375/$O375</f>
         <v>80</v>
       </c>
-      <c r="D378" s="88"/>
-      <c r="E378" s="88"/>
-      <c r="F378" s="88"/>
-      <c r="G378" s="88"/>
-      <c r="H378" s="88"/>
-      <c r="I378" s="88">
+      <c r="D378" s="90"/>
+      <c r="E378" s="90"/>
+      <c r="F378" s="90"/>
+      <c r="G378" s="90"/>
+      <c r="H378" s="90"/>
+      <c r="I378" s="90">
         <f>O$378*I375/$O375</f>
         <v>80</v>
       </c>
-      <c r="J378" s="88"/>
-      <c r="K378" s="88"/>
-      <c r="L378" s="88"/>
-      <c r="M378" s="88"/>
-      <c r="N378" s="88"/>
+      <c r="J378" s="90"/>
+      <c r="K378" s="90"/>
+      <c r="L378" s="90"/>
+      <c r="M378" s="90"/>
+      <c r="N378" s="90"/>
       <c r="O378" s="72">
         <f>O377*O375</f>
         <v>160</v>
@@ -9157,82 +9184,82 @@
       <c r="A383" s="43" t="s">
         <v>61</v>
       </c>
-      <c r="C383" s="88">
-        <v>1</v>
-      </c>
-      <c r="D383" s="88"/>
-      <c r="E383" s="88"/>
-      <c r="F383" s="88"/>
-      <c r="G383" s="88"/>
-      <c r="H383" s="88"/>
-      <c r="I383" s="88"/>
-      <c r="J383" s="88"/>
-      <c r="K383" s="88"/>
-      <c r="L383" s="88"/>
-      <c r="M383" s="88"/>
-      <c r="N383" s="89"/>
+      <c r="C383" s="90">
+        <v>1</v>
+      </c>
+      <c r="D383" s="90"/>
+      <c r="E383" s="90"/>
+      <c r="F383" s="90"/>
+      <c r="G383" s="90"/>
+      <c r="H383" s="90"/>
+      <c r="I383" s="90"/>
+      <c r="J383" s="90"/>
+      <c r="K383" s="90"/>
+      <c r="L383" s="90"/>
+      <c r="M383" s="90"/>
+      <c r="N383" s="87"/>
       <c r="O383" s="72"/>
     </row>
     <row r="384" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A384" s="43" t="s">
         <v>62</v>
       </c>
-      <c r="C384" s="88" t="s">
+      <c r="C384" s="90" t="s">
         <v>146</v>
       </c>
-      <c r="D384" s="88"/>
-      <c r="E384" s="88"/>
-      <c r="F384" s="88"/>
-      <c r="G384" s="88"/>
-      <c r="H384" s="88"/>
-      <c r="I384" s="88" t="s">
+      <c r="D384" s="90"/>
+      <c r="E384" s="90"/>
+      <c r="F384" s="90"/>
+      <c r="G384" s="90"/>
+      <c r="H384" s="90"/>
+      <c r="I384" s="90" t="s">
         <v>147</v>
       </c>
-      <c r="J384" s="88"/>
-      <c r="K384" s="88"/>
-      <c r="L384" s="88"/>
-      <c r="M384" s="88"/>
-      <c r="N384" s="89"/>
+      <c r="J384" s="90"/>
+      <c r="K384" s="90"/>
+      <c r="L384" s="90"/>
+      <c r="M384" s="90"/>
+      <c r="N384" s="87"/>
       <c r="O384" s="73"/>
     </row>
     <row r="385" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A385" s="43" t="s">
         <v>63</v>
       </c>
-      <c r="C385" s="88">
-        <v>1</v>
-      </c>
-      <c r="D385" s="88"/>
-      <c r="E385" s="88"/>
-      <c r="F385" s="88"/>
-      <c r="G385" s="88"/>
-      <c r="H385" s="88"/>
-      <c r="I385" s="88"/>
-      <c r="J385" s="88"/>
-      <c r="K385" s="88"/>
-      <c r="L385" s="88"/>
-      <c r="M385" s="88"/>
-      <c r="N385" s="88"/>
+      <c r="C385" s="90">
+        <v>1</v>
+      </c>
+      <c r="D385" s="90"/>
+      <c r="E385" s="90"/>
+      <c r="F385" s="90"/>
+      <c r="G385" s="90"/>
+      <c r="H385" s="90"/>
+      <c r="I385" s="90"/>
+      <c r="J385" s="90"/>
+      <c r="K385" s="90"/>
+      <c r="L385" s="90"/>
+      <c r="M385" s="90"/>
+      <c r="N385" s="90"/>
       <c r="O385" s="72"/>
     </row>
     <row r="386" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A386" s="43" t="s">
         <v>71</v>
       </c>
-      <c r="C386" s="90">
+      <c r="C386" s="88">
         <v>0.5</v>
       </c>
-      <c r="D386" s="90"/>
-      <c r="E386" s="90"/>
-      <c r="F386" s="90"/>
-      <c r="G386" s="90"/>
-      <c r="H386" s="90"/>
-      <c r="I386" s="90"/>
-      <c r="J386" s="90"/>
-      <c r="K386" s="90"/>
-      <c r="L386" s="90"/>
-      <c r="M386" s="90"/>
-      <c r="N386" s="90"/>
+      <c r="D386" s="88"/>
+      <c r="E386" s="88"/>
+      <c r="F386" s="88"/>
+      <c r="G386" s="88"/>
+      <c r="H386" s="88"/>
+      <c r="I386" s="88"/>
+      <c r="J386" s="88"/>
+      <c r="K386" s="88"/>
+      <c r="L386" s="88"/>
+      <c r="M386" s="88"/>
+      <c r="N386" s="88"/>
       <c r="O386" s="72"/>
     </row>
     <row r="387" spans="1:17" x14ac:dyDescent="0.3">
@@ -9272,14 +9299,14 @@
       <c r="A389" s="43" t="s">
         <v>161</v>
       </c>
-      <c r="C389" s="87">
+      <c r="C389" s="91">
         <v>0.8</v>
       </c>
-      <c r="D389" s="88"/>
-      <c r="E389" s="88"/>
-      <c r="F389" s="88"/>
-      <c r="G389" s="88"/>
-      <c r="H389" s="88"/>
+      <c r="D389" s="90"/>
+      <c r="E389" s="90"/>
+      <c r="F389" s="90"/>
+      <c r="G389" s="90"/>
+      <c r="H389" s="90"/>
       <c r="N389" s="13"/>
       <c r="O389" s="83">
         <v>0.8</v>
@@ -9289,21 +9316,21 @@
       <c r="A390" s="45" t="s">
         <v>164</v>
       </c>
-      <c r="C390" s="88">
+      <c r="C390" s="90">
         <f>C389*C387</f>
         <v>80</v>
       </c>
-      <c r="D390" s="88"/>
-      <c r="E390" s="88"/>
-      <c r="F390" s="88"/>
-      <c r="G390" s="88"/>
-      <c r="H390" s="88"/>
-      <c r="I390" s="88"/>
-      <c r="J390" s="88"/>
-      <c r="K390" s="88"/>
-      <c r="L390" s="88"/>
-      <c r="M390" s="88"/>
-      <c r="N390" s="88"/>
+      <c r="D390" s="90"/>
+      <c r="E390" s="90"/>
+      <c r="F390" s="90"/>
+      <c r="G390" s="90"/>
+      <c r="H390" s="90"/>
+      <c r="I390" s="90"/>
+      <c r="J390" s="90"/>
+      <c r="K390" s="90"/>
+      <c r="L390" s="90"/>
+      <c r="M390" s="90"/>
+      <c r="N390" s="90"/>
       <c r="O390" s="72">
         <f>SUM(C390:N390)</f>
         <v>80</v>
@@ -9441,88 +9468,88 @@
       <c r="A395" s="43" t="s">
         <v>61</v>
       </c>
-      <c r="C395" s="88">
-        <v>1</v>
-      </c>
-      <c r="D395" s="88"/>
-      <c r="E395" s="88"/>
-      <c r="F395" s="88"/>
-      <c r="G395" s="88"/>
-      <c r="H395" s="88"/>
-      <c r="I395" s="88">
-        <v>1</v>
-      </c>
-      <c r="J395" s="88"/>
-      <c r="K395" s="88"/>
-      <c r="L395" s="88"/>
-      <c r="M395" s="88"/>
-      <c r="N395" s="89"/>
+      <c r="C395" s="90">
+        <v>1</v>
+      </c>
+      <c r="D395" s="90"/>
+      <c r="E395" s="90"/>
+      <c r="F395" s="90"/>
+      <c r="G395" s="90"/>
+      <c r="H395" s="90"/>
+      <c r="I395" s="90">
+        <v>1</v>
+      </c>
+      <c r="J395" s="90"/>
+      <c r="K395" s="90"/>
+      <c r="L395" s="90"/>
+      <c r="M395" s="90"/>
+      <c r="N395" s="87"/>
       <c r="O395" s="72"/>
     </row>
     <row r="396" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A396" s="43" t="s">
         <v>62</v>
       </c>
-      <c r="C396" s="88" t="s">
+      <c r="C396" s="90" t="s">
         <v>146</v>
       </c>
-      <c r="D396" s="88"/>
-      <c r="E396" s="88"/>
-      <c r="F396" s="88"/>
-      <c r="G396" s="88"/>
-      <c r="H396" s="88"/>
-      <c r="I396" s="88" t="s">
+      <c r="D396" s="90"/>
+      <c r="E396" s="90"/>
+      <c r="F396" s="90"/>
+      <c r="G396" s="90"/>
+      <c r="H396" s="90"/>
+      <c r="I396" s="90" t="s">
         <v>147</v>
       </c>
-      <c r="J396" s="88"/>
-      <c r="K396" s="88"/>
-      <c r="L396" s="88"/>
-      <c r="M396" s="88"/>
-      <c r="N396" s="89"/>
+      <c r="J396" s="90"/>
+      <c r="K396" s="90"/>
+      <c r="L396" s="90"/>
+      <c r="M396" s="90"/>
+      <c r="N396" s="87"/>
       <c r="O396" s="73"/>
     </row>
     <row r="397" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A397" s="43" t="s">
         <v>63</v>
       </c>
-      <c r="C397" s="88">
-        <v>1</v>
-      </c>
-      <c r="D397" s="88"/>
-      <c r="E397" s="88"/>
-      <c r="F397" s="88"/>
-      <c r="G397" s="88"/>
-      <c r="H397" s="88"/>
-      <c r="I397" s="88">
-        <v>1</v>
-      </c>
-      <c r="J397" s="88"/>
-      <c r="K397" s="88"/>
-      <c r="L397" s="88"/>
-      <c r="M397" s="88"/>
-      <c r="N397" s="88"/>
+      <c r="C397" s="90">
+        <v>1</v>
+      </c>
+      <c r="D397" s="90"/>
+      <c r="E397" s="90"/>
+      <c r="F397" s="90"/>
+      <c r="G397" s="90"/>
+      <c r="H397" s="90"/>
+      <c r="I397" s="90">
+        <v>1</v>
+      </c>
+      <c r="J397" s="90"/>
+      <c r="K397" s="90"/>
+      <c r="L397" s="90"/>
+      <c r="M397" s="90"/>
+      <c r="N397" s="90"/>
       <c r="O397" s="72"/>
     </row>
     <row r="398" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A398" s="43" t="s">
         <v>71</v>
       </c>
-      <c r="C398" s="90">
+      <c r="C398" s="88">
         <v>0.5</v>
       </c>
-      <c r="D398" s="90"/>
-      <c r="E398" s="90"/>
-      <c r="F398" s="90"/>
-      <c r="G398" s="90"/>
-      <c r="H398" s="90"/>
-      <c r="I398" s="90">
+      <c r="D398" s="88"/>
+      <c r="E398" s="88"/>
+      <c r="F398" s="88"/>
+      <c r="G398" s="88"/>
+      <c r="H398" s="88"/>
+      <c r="I398" s="88">
         <v>0.5</v>
       </c>
-      <c r="J398" s="90"/>
-      <c r="K398" s="90"/>
-      <c r="L398" s="90"/>
-      <c r="M398" s="90"/>
-      <c r="N398" s="90"/>
+      <c r="J398" s="88"/>
+      <c r="K398" s="88"/>
+      <c r="L398" s="88"/>
+      <c r="M398" s="88"/>
+      <c r="N398" s="88"/>
       <c r="O398" s="72"/>
     </row>
     <row r="399" spans="1:17" x14ac:dyDescent="0.3">
@@ -9625,24 +9652,24 @@
       <c r="A404" s="45" t="s">
         <v>164</v>
       </c>
-      <c r="C404" s="88">
+      <c r="C404" s="90">
         <f>O$404*C401/$O401</f>
         <v>36</v>
       </c>
-      <c r="D404" s="88"/>
-      <c r="E404" s="88"/>
-      <c r="F404" s="88"/>
-      <c r="G404" s="88"/>
-      <c r="H404" s="88"/>
-      <c r="I404" s="88">
+      <c r="D404" s="90"/>
+      <c r="E404" s="90"/>
+      <c r="F404" s="90"/>
+      <c r="G404" s="90"/>
+      <c r="H404" s="90"/>
+      <c r="I404" s="90">
         <f>O$404*I401/$O401</f>
         <v>36</v>
       </c>
-      <c r="J404" s="88"/>
-      <c r="K404" s="88"/>
-      <c r="L404" s="88"/>
-      <c r="M404" s="88"/>
-      <c r="N404" s="88"/>
+      <c r="J404" s="90"/>
+      <c r="K404" s="90"/>
+      <c r="L404" s="90"/>
+      <c r="M404" s="90"/>
+      <c r="N404" s="90"/>
       <c r="O404" s="72">
         <f>O403*MIN(O401,O402)</f>
         <v>72</v>
@@ -9780,82 +9807,82 @@
       <c r="A409" s="43" t="s">
         <v>61</v>
       </c>
-      <c r="C409" s="88">
-        <v>1</v>
-      </c>
-      <c r="D409" s="88"/>
-      <c r="E409" s="88"/>
-      <c r="F409" s="88"/>
-      <c r="G409" s="88"/>
-      <c r="H409" s="88"/>
-      <c r="I409" s="88"/>
-      <c r="J409" s="88"/>
-      <c r="K409" s="88"/>
-      <c r="L409" s="88"/>
-      <c r="M409" s="88"/>
-      <c r="N409" s="89"/>
+      <c r="C409" s="90">
+        <v>1</v>
+      </c>
+      <c r="D409" s="90"/>
+      <c r="E409" s="90"/>
+      <c r="F409" s="90"/>
+      <c r="G409" s="90"/>
+      <c r="H409" s="90"/>
+      <c r="I409" s="90"/>
+      <c r="J409" s="90"/>
+      <c r="K409" s="90"/>
+      <c r="L409" s="90"/>
+      <c r="M409" s="90"/>
+      <c r="N409" s="87"/>
       <c r="O409" s="72"/>
     </row>
     <row r="410" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A410" s="43" t="s">
         <v>62</v>
       </c>
-      <c r="C410" s="88" t="s">
+      <c r="C410" s="90" t="s">
         <v>146</v>
       </c>
-      <c r="D410" s="88"/>
-      <c r="E410" s="88"/>
-      <c r="F410" s="88"/>
-      <c r="G410" s="88"/>
-      <c r="H410" s="88"/>
-      <c r="I410" s="88" t="s">
+      <c r="D410" s="90"/>
+      <c r="E410" s="90"/>
+      <c r="F410" s="90"/>
+      <c r="G410" s="90"/>
+      <c r="H410" s="90"/>
+      <c r="I410" s="90" t="s">
         <v>147</v>
       </c>
-      <c r="J410" s="88"/>
-      <c r="K410" s="88"/>
-      <c r="L410" s="88"/>
-      <c r="M410" s="88"/>
-      <c r="N410" s="89"/>
+      <c r="J410" s="90"/>
+      <c r="K410" s="90"/>
+      <c r="L410" s="90"/>
+      <c r="M410" s="90"/>
+      <c r="N410" s="87"/>
       <c r="O410" s="73"/>
     </row>
     <row r="411" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A411" s="43" t="s">
         <v>63</v>
       </c>
-      <c r="C411" s="88">
-        <v>1</v>
-      </c>
-      <c r="D411" s="88"/>
-      <c r="E411" s="88"/>
-      <c r="F411" s="88"/>
-      <c r="G411" s="88"/>
-      <c r="H411" s="88"/>
-      <c r="I411" s="88"/>
-      <c r="J411" s="88"/>
-      <c r="K411" s="88"/>
-      <c r="L411" s="88"/>
-      <c r="M411" s="88"/>
-      <c r="N411" s="88"/>
+      <c r="C411" s="90">
+        <v>1</v>
+      </c>
+      <c r="D411" s="90"/>
+      <c r="E411" s="90"/>
+      <c r="F411" s="90"/>
+      <c r="G411" s="90"/>
+      <c r="H411" s="90"/>
+      <c r="I411" s="90"/>
+      <c r="J411" s="90"/>
+      <c r="K411" s="90"/>
+      <c r="L411" s="90"/>
+      <c r="M411" s="90"/>
+      <c r="N411" s="90"/>
       <c r="O411" s="72"/>
     </row>
     <row r="412" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A412" s="43" t="s">
         <v>71</v>
       </c>
-      <c r="C412" s="90">
+      <c r="C412" s="88">
         <v>0.5</v>
       </c>
-      <c r="D412" s="90"/>
-      <c r="E412" s="90"/>
-      <c r="F412" s="90"/>
-      <c r="G412" s="90"/>
-      <c r="H412" s="90"/>
-      <c r="I412" s="90"/>
-      <c r="J412" s="90"/>
-      <c r="K412" s="90"/>
-      <c r="L412" s="90"/>
-      <c r="M412" s="90"/>
-      <c r="N412" s="90"/>
+      <c r="D412" s="88"/>
+      <c r="E412" s="88"/>
+      <c r="F412" s="88"/>
+      <c r="G412" s="88"/>
+      <c r="H412" s="88"/>
+      <c r="I412" s="88"/>
+      <c r="J412" s="88"/>
+      <c r="K412" s="88"/>
+      <c r="L412" s="88"/>
+      <c r="M412" s="88"/>
+      <c r="N412" s="88"/>
       <c r="O412" s="72"/>
     </row>
     <row r="413" spans="1:17" x14ac:dyDescent="0.3">
@@ -9947,14 +9974,14 @@
       <c r="A417" s="43" t="s">
         <v>161</v>
       </c>
-      <c r="C417" s="87">
+      <c r="C417" s="91">
         <v>0.8</v>
       </c>
-      <c r="D417" s="88"/>
-      <c r="E417" s="88"/>
-      <c r="F417" s="88"/>
-      <c r="G417" s="88"/>
-      <c r="H417" s="88"/>
+      <c r="D417" s="90"/>
+      <c r="E417" s="90"/>
+      <c r="F417" s="90"/>
+      <c r="G417" s="90"/>
+      <c r="H417" s="90"/>
       <c r="N417" s="13"/>
       <c r="O417" s="83">
         <v>0.8</v>
@@ -9964,21 +9991,21 @@
       <c r="A418" s="45" t="s">
         <v>164</v>
       </c>
-      <c r="C418" s="88">
+      <c r="C418" s="90">
         <f>C417*C416</f>
         <v>32</v>
       </c>
-      <c r="D418" s="88"/>
-      <c r="E418" s="88"/>
-      <c r="F418" s="88"/>
-      <c r="G418" s="88"/>
-      <c r="H418" s="88"/>
-      <c r="I418" s="88"/>
-      <c r="J418" s="88"/>
-      <c r="K418" s="88"/>
-      <c r="L418" s="88"/>
-      <c r="M418" s="88"/>
-      <c r="N418" s="88"/>
+      <c r="D418" s="90"/>
+      <c r="E418" s="90"/>
+      <c r="F418" s="90"/>
+      <c r="G418" s="90"/>
+      <c r="H418" s="90"/>
+      <c r="I418" s="90"/>
+      <c r="J418" s="90"/>
+      <c r="K418" s="90"/>
+      <c r="L418" s="90"/>
+      <c r="M418" s="90"/>
+      <c r="N418" s="90"/>
       <c r="O418" s="72">
         <f>SUM(C418:N418)</f>
         <v>32</v>
@@ -10116,25 +10143,25 @@
       <c r="A423" s="43" t="s">
         <v>61</v>
       </c>
-      <c r="C423" s="88">
-        <v>1</v>
-      </c>
-      <c r="D423" s="88"/>
+      <c r="C423" s="90">
+        <v>1</v>
+      </c>
+      <c r="D423" s="90"/>
       <c r="E423" s="86"/>
-      <c r="F423" s="88">
-        <v>1</v>
-      </c>
-      <c r="G423" s="88"/>
+      <c r="F423" s="90">
+        <v>1</v>
+      </c>
+      <c r="G423" s="90"/>
       <c r="H423" s="86"/>
-      <c r="I423" s="88">
-        <v>1</v>
-      </c>
-      <c r="J423" s="88"/>
+      <c r="I423" s="90">
+        <v>1</v>
+      </c>
+      <c r="J423" s="90"/>
       <c r="K423" s="86"/>
-      <c r="L423" s="88">
-        <v>1</v>
-      </c>
-      <c r="M423" s="88"/>
+      <c r="L423" s="90">
+        <v>1</v>
+      </c>
+      <c r="M423" s="90"/>
       <c r="N423" s="86"/>
       <c r="O423" s="72"/>
     </row>
@@ -10142,25 +10169,25 @@
       <c r="A424" s="43" t="s">
         <v>62</v>
       </c>
-      <c r="C424" s="88" t="s">
+      <c r="C424" s="90" t="s">
         <v>139</v>
       </c>
-      <c r="D424" s="88"/>
+      <c r="D424" s="90"/>
       <c r="E424" s="86"/>
-      <c r="F424" s="88" t="s">
+      <c r="F424" s="90" t="s">
         <v>140</v>
       </c>
-      <c r="G424" s="88"/>
+      <c r="G424" s="90"/>
       <c r="H424" s="86"/>
-      <c r="I424" s="88" t="s">
+      <c r="I424" s="90" t="s">
         <v>141</v>
       </c>
-      <c r="J424" s="88"/>
+      <c r="J424" s="90"/>
       <c r="K424" s="86"/>
-      <c r="L424" s="88" t="s">
+      <c r="L424" s="90" t="s">
         <v>142</v>
       </c>
-      <c r="M424" s="88"/>
+      <c r="M424" s="90"/>
       <c r="N424" s="86"/>
       <c r="O424" s="73"/>
     </row>
@@ -10168,25 +10195,25 @@
       <c r="A425" s="43" t="s">
         <v>63</v>
       </c>
-      <c r="C425" s="88">
-        <v>1</v>
-      </c>
-      <c r="D425" s="88"/>
+      <c r="C425" s="90">
+        <v>1</v>
+      </c>
+      <c r="D425" s="90"/>
       <c r="E425" s="86"/>
-      <c r="F425" s="88">
-        <v>1</v>
-      </c>
-      <c r="G425" s="88"/>
+      <c r="F425" s="90">
+        <v>1</v>
+      </c>
+      <c r="G425" s="90"/>
       <c r="H425" s="86"/>
-      <c r="I425" s="88">
-        <v>1</v>
-      </c>
-      <c r="J425" s="88"/>
+      <c r="I425" s="90">
+        <v>1</v>
+      </c>
+      <c r="J425" s="90"/>
       <c r="K425" s="86"/>
-      <c r="L425" s="88">
-        <v>1</v>
-      </c>
-      <c r="M425" s="88"/>
+      <c r="L425" s="90">
+        <v>1</v>
+      </c>
+      <c r="M425" s="90"/>
       <c r="N425" s="86"/>
       <c r="O425" s="72"/>
     </row>
@@ -10311,26 +10338,26 @@
       <c r="A430" s="43" t="s">
         <v>71</v>
       </c>
-      <c r="C430" s="90">
+      <c r="C430" s="88">
         <v>0.1</v>
       </c>
-      <c r="D430" s="90"/>
-      <c r="E430" s="90"/>
-      <c r="F430" s="90">
+      <c r="D430" s="88"/>
+      <c r="E430" s="88"/>
+      <c r="F430" s="88">
         <v>0.1</v>
       </c>
-      <c r="G430" s="90"/>
-      <c r="H430" s="90"/>
-      <c r="I430" s="90">
+      <c r="G430" s="88"/>
+      <c r="H430" s="88"/>
+      <c r="I430" s="88">
         <v>0.1</v>
       </c>
-      <c r="J430" s="90"/>
-      <c r="K430" s="90"/>
-      <c r="L430" s="90">
+      <c r="J430" s="88"/>
+      <c r="K430" s="88"/>
+      <c r="L430" s="88">
         <v>0.1</v>
       </c>
-      <c r="M430" s="90"/>
-      <c r="N430" s="91"/>
+      <c r="M430" s="88"/>
+      <c r="N430" s="89"/>
       <c r="O430" s="74"/>
       <c r="Q430" s="6"/>
     </row>
@@ -10361,7 +10388,7 @@
         <v>10</v>
       </c>
       <c r="M431" s="86"/>
-      <c r="N431" s="89"/>
+      <c r="N431" s="87"/>
       <c r="O431" s="72"/>
     </row>
     <row r="432" spans="1:17" x14ac:dyDescent="0.3">
@@ -10552,25 +10579,25 @@
       <c r="A440" s="43" t="s">
         <v>61</v>
       </c>
-      <c r="C440" s="88">
-        <v>1</v>
-      </c>
-      <c r="D440" s="88"/>
+      <c r="C440" s="90">
+        <v>1</v>
+      </c>
+      <c r="D440" s="90"/>
       <c r="E440" s="86"/>
-      <c r="F440" s="88">
-        <v>1</v>
-      </c>
-      <c r="G440" s="88"/>
+      <c r="F440" s="90">
+        <v>1</v>
+      </c>
+      <c r="G440" s="90"/>
       <c r="H440" s="86"/>
-      <c r="I440" s="88">
-        <v>1</v>
-      </c>
-      <c r="J440" s="88"/>
+      <c r="I440" s="90">
+        <v>1</v>
+      </c>
+      <c r="J440" s="90"/>
       <c r="K440" s="86"/>
-      <c r="L440" s="88">
-        <v>1</v>
-      </c>
-      <c r="M440" s="88"/>
+      <c r="L440" s="90">
+        <v>1</v>
+      </c>
+      <c r="M440" s="90"/>
       <c r="N440" s="86"/>
       <c r="O440" s="72"/>
     </row>
@@ -10578,25 +10605,25 @@
       <c r="A441" s="43" t="s">
         <v>62</v>
       </c>
-      <c r="C441" s="88" t="s">
+      <c r="C441" s="90" t="s">
         <v>139</v>
       </c>
-      <c r="D441" s="88"/>
+      <c r="D441" s="90"/>
       <c r="E441" s="86"/>
-      <c r="F441" s="88" t="s">
+      <c r="F441" s="90" t="s">
         <v>140</v>
       </c>
-      <c r="G441" s="88"/>
+      <c r="G441" s="90"/>
       <c r="H441" s="86"/>
-      <c r="I441" s="88" t="s">
+      <c r="I441" s="90" t="s">
         <v>141</v>
       </c>
-      <c r="J441" s="88"/>
+      <c r="J441" s="90"/>
       <c r="K441" s="86"/>
-      <c r="L441" s="88" t="s">
+      <c r="L441" s="90" t="s">
         <v>142</v>
       </c>
-      <c r="M441" s="88"/>
+      <c r="M441" s="90"/>
       <c r="N441" s="86"/>
       <c r="O441" s="73"/>
     </row>
@@ -10604,25 +10631,25 @@
       <c r="A442" s="43" t="s">
         <v>63</v>
       </c>
-      <c r="C442" s="88">
-        <v>1</v>
-      </c>
-      <c r="D442" s="88"/>
+      <c r="C442" s="90">
+        <v>1</v>
+      </c>
+      <c r="D442" s="90"/>
       <c r="E442" s="86"/>
-      <c r="F442" s="88">
-        <v>1</v>
-      </c>
-      <c r="G442" s="88"/>
+      <c r="F442" s="90">
+        <v>1</v>
+      </c>
+      <c r="G442" s="90"/>
       <c r="H442" s="86"/>
-      <c r="I442" s="88">
-        <v>1</v>
-      </c>
-      <c r="J442" s="88"/>
+      <c r="I442" s="90">
+        <v>1</v>
+      </c>
+      <c r="J442" s="90"/>
       <c r="K442" s="86"/>
-      <c r="L442" s="88">
-        <v>1</v>
-      </c>
-      <c r="M442" s="88"/>
+      <c r="L442" s="90">
+        <v>1</v>
+      </c>
+      <c r="M442" s="90"/>
       <c r="N442" s="86"/>
       <c r="O442" s="72"/>
     </row>
@@ -10747,26 +10774,26 @@
       <c r="A447" s="43" t="s">
         <v>71</v>
       </c>
-      <c r="C447" s="90">
+      <c r="C447" s="88">
         <v>0.1</v>
       </c>
-      <c r="D447" s="90"/>
-      <c r="E447" s="90"/>
-      <c r="F447" s="90">
+      <c r="D447" s="88"/>
+      <c r="E447" s="88"/>
+      <c r="F447" s="88">
         <v>0.1</v>
       </c>
-      <c r="G447" s="90"/>
-      <c r="H447" s="90"/>
-      <c r="I447" s="90">
+      <c r="G447" s="88"/>
+      <c r="H447" s="88"/>
+      <c r="I447" s="88">
         <v>0.1</v>
       </c>
-      <c r="J447" s="90"/>
-      <c r="K447" s="90"/>
-      <c r="L447" s="90">
+      <c r="J447" s="88"/>
+      <c r="K447" s="88"/>
+      <c r="L447" s="88">
         <v>0.1</v>
       </c>
-      <c r="M447" s="90"/>
-      <c r="N447" s="91"/>
+      <c r="M447" s="88"/>
+      <c r="N447" s="89"/>
       <c r="O447" s="74"/>
       <c r="Q447" s="6"/>
     </row>
@@ -10797,7 +10824,7 @@
         <v>10</v>
       </c>
       <c r="M448" s="86"/>
-      <c r="N448" s="89"/>
+      <c r="N448" s="87"/>
       <c r="O448" s="72"/>
     </row>
     <row r="449" spans="1:17" x14ac:dyDescent="0.3">
@@ -10836,23 +10863,23 @@
       <c r="D452" s="86"/>
       <c r="E452" s="86"/>
       <c r="F452" s="86">
-        <f t="shared" ref="F452:N452" si="103">$O452*F448/SUM($C$448:$N$448)</f>
+        <f t="shared" ref="F452" si="103">$O452*F448/SUM($C$448:$N$448)</f>
         <v>6</v>
       </c>
       <c r="G452" s="86"/>
       <c r="H452" s="86"/>
       <c r="I452" s="86">
-        <f t="shared" ref="I452:N452" si="104">$O452*I448/SUM($C$448:$N$448)</f>
+        <f t="shared" ref="I452" si="104">$O452*I448/SUM($C$448:$N$448)</f>
         <v>6</v>
       </c>
       <c r="J452" s="86"/>
       <c r="K452" s="86"/>
       <c r="L452" s="86">
-        <f t="shared" ref="L452:N452" si="105">$O452*L448/SUM($C$448:$N$448)</f>
+        <f t="shared" ref="L452" si="105">$O452*L448/SUM($C$448:$N$448)</f>
         <v>6</v>
       </c>
       <c r="M452" s="86"/>
-      <c r="N452" s="89"/>
+      <c r="N452" s="87"/>
       <c r="O452" s="72">
         <f>MIN(O450,SUM(C448:N448))*O451</f>
         <v>24</v>
@@ -10974,8 +11001,726 @@
         <v>376</v>
       </c>
     </row>
+    <row r="456" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A456" s="65" t="s">
+        <v>189</v>
+      </c>
+      <c r="B456" s="4" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="457" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A457" s="43" t="s">
+        <v>61</v>
+      </c>
+      <c r="C457" s="90">
+        <v>1</v>
+      </c>
+      <c r="D457" s="90"/>
+      <c r="E457" s="90"/>
+      <c r="F457" s="90"/>
+      <c r="G457" s="90"/>
+      <c r="H457" s="90"/>
+      <c r="N457" s="40"/>
+    </row>
+    <row r="458" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A458" s="43" t="s">
+        <v>62</v>
+      </c>
+      <c r="C458" s="90" t="s">
+        <v>77</v>
+      </c>
+      <c r="D458" s="90"/>
+      <c r="E458" s="90"/>
+      <c r="F458" s="90"/>
+      <c r="G458" s="90"/>
+      <c r="H458" s="90"/>
+      <c r="N458" s="40"/>
+      <c r="O458" s="50"/>
+    </row>
+    <row r="459" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A459" s="43" t="s">
+        <v>63</v>
+      </c>
+      <c r="C459" s="90">
+        <v>1</v>
+      </c>
+      <c r="D459" s="90"/>
+      <c r="E459" s="90"/>
+      <c r="F459" s="90"/>
+      <c r="G459" s="90"/>
+      <c r="H459" s="90"/>
+      <c r="N459" s="40"/>
+    </row>
+    <row r="460" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A460" s="43" t="s">
+        <v>64</v>
+      </c>
+      <c r="C460" s="103">
+        <v>50</v>
+      </c>
+      <c r="D460" s="103"/>
+      <c r="E460" s="103"/>
+      <c r="F460" s="103"/>
+      <c r="G460" s="103"/>
+      <c r="H460" s="103"/>
+      <c r="N460" s="40"/>
+    </row>
+    <row r="461" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A461" s="44" t="s">
+        <v>65</v>
+      </c>
+      <c r="C461" s="104">
+        <f>MAX(SUM($C$50:$H$50)-C460,0)</f>
+        <v>150</v>
+      </c>
+      <c r="D461" s="86"/>
+      <c r="E461" s="86"/>
+      <c r="F461" s="86"/>
+      <c r="G461" s="86"/>
+      <c r="H461" s="86"/>
+      <c r="N461" s="40"/>
+      <c r="O461" s="6"/>
+      <c r="P461" s="6"/>
+      <c r="Q461" s="6"/>
+    </row>
+    <row r="462" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A462" s="43" t="s">
+        <v>0</v>
+      </c>
+      <c r="C462" s="86">
+        <v>1000</v>
+      </c>
+      <c r="D462" s="86"/>
+      <c r="E462" s="86"/>
+      <c r="F462" s="86"/>
+      <c r="G462" s="86"/>
+      <c r="H462" s="86"/>
+      <c r="N462" s="40"/>
+      <c r="Q462" s="6"/>
+    </row>
+    <row r="463" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A463" s="44" t="s">
+        <v>66</v>
+      </c>
+      <c r="C463" s="86">
+        <f>IF(C462=0, C461, MIN(C461, C462))</f>
+        <v>150</v>
+      </c>
+      <c r="D463" s="86"/>
+      <c r="E463" s="86"/>
+      <c r="F463" s="86"/>
+      <c r="G463" s="86"/>
+      <c r="H463" s="86"/>
+      <c r="N463" s="40"/>
+      <c r="O463" s="6"/>
+      <c r="P463" s="6"/>
+      <c r="Q463" s="6"/>
+    </row>
+    <row r="464" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A464" s="43" t="s">
+        <v>161</v>
+      </c>
+      <c r="C464" s="105">
+        <v>1</v>
+      </c>
+      <c r="D464" s="86"/>
+      <c r="E464" s="86"/>
+      <c r="F464" s="86"/>
+      <c r="G464" s="86"/>
+      <c r="H464" s="86"/>
+      <c r="N464" s="40"/>
+      <c r="O464" s="48"/>
+      <c r="Q464" s="6"/>
+    </row>
+    <row r="465" spans="1:17" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A465" s="44" t="s">
+        <v>72</v>
+      </c>
+      <c r="C465" s="106">
+        <f>C463*C464</f>
+        <v>150</v>
+      </c>
+      <c r="D465" s="106"/>
+      <c r="E465" s="106"/>
+      <c r="F465" s="106"/>
+      <c r="G465" s="106"/>
+      <c r="H465" s="106"/>
+      <c r="N465" s="40"/>
+    </row>
+    <row r="466" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A466" s="43" t="s">
+        <v>3</v>
+      </c>
+      <c r="C466" s="90"/>
+      <c r="D466" s="90"/>
+      <c r="E466" s="90"/>
+      <c r="F466" s="90"/>
+      <c r="G466" s="90"/>
+      <c r="H466" s="90"/>
+      <c r="N466" s="40"/>
+    </row>
+    <row r="467" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A467" s="43"/>
+      <c r="N467" s="40"/>
+    </row>
+    <row r="468" spans="1:17" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A468" s="45" t="s">
+        <v>74</v>
+      </c>
+      <c r="C468" s="106">
+        <f>C465</f>
+        <v>150</v>
+      </c>
+      <c r="D468" s="106"/>
+      <c r="E468" s="106"/>
+      <c r="F468" s="106"/>
+      <c r="G468" s="106"/>
+      <c r="H468" s="106"/>
+      <c r="I468" s="90">
+        <v>0</v>
+      </c>
+      <c r="J468" s="90"/>
+      <c r="K468" s="90"/>
+      <c r="L468" s="90"/>
+      <c r="M468" s="90"/>
+      <c r="N468" s="87"/>
+      <c r="O468" s="107">
+        <f>SUM(C468:N468)</f>
+        <v>150</v>
+      </c>
+      <c r="P468" s="6"/>
+      <c r="Q468" s="6"/>
+    </row>
+    <row r="469" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A469" s="44" t="s">
+        <v>75</v>
+      </c>
+      <c r="C469" s="52">
+        <f>$C468*C$50/SUM($C$50:$H$50)</f>
+        <v>37.5</v>
+      </c>
+      <c r="D469" s="52">
+        <f t="shared" ref="D469:H469" si="111">$C468*D$50/SUM($C$50:$H$50)</f>
+        <v>18.75</v>
+      </c>
+      <c r="E469" s="52">
+        <f t="shared" si="111"/>
+        <v>18.75</v>
+      </c>
+      <c r="F469" s="52">
+        <f t="shared" si="111"/>
+        <v>37.5</v>
+      </c>
+      <c r="G469" s="52">
+        <f t="shared" si="111"/>
+        <v>18.75</v>
+      </c>
+      <c r="H469" s="52">
+        <f t="shared" si="111"/>
+        <v>18.75</v>
+      </c>
+      <c r="I469" s="52">
+        <v>0</v>
+      </c>
+      <c r="J469" s="52">
+        <v>0</v>
+      </c>
+      <c r="K469" s="52">
+        <v>0</v>
+      </c>
+      <c r="L469" s="52">
+        <v>0</v>
+      </c>
+      <c r="M469" s="52">
+        <v>0</v>
+      </c>
+      <c r="N469" s="52">
+        <v>0</v>
+      </c>
+      <c r="O469" s="49">
+        <f>SUM(C469:N469)</f>
+        <v>150</v>
+      </c>
+    </row>
+    <row r="470" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="A470" s="46" t="s">
+        <v>69</v>
+      </c>
+      <c r="C470" s="67">
+        <f>(SUM($C$36:$H$36)-$C$468)*C50/SUM($C$36:$H$36)</f>
+        <v>12.5</v>
+      </c>
+      <c r="D470" s="67">
+        <f t="shared" ref="D470:H470" si="112">(SUM($C$36:$H$36)-$C$468)*D50/SUM($C$36:$H$36)</f>
+        <v>6.25</v>
+      </c>
+      <c r="E470" s="67">
+        <f t="shared" si="112"/>
+        <v>6.25</v>
+      </c>
+      <c r="F470" s="67">
+        <f t="shared" si="112"/>
+        <v>12.5</v>
+      </c>
+      <c r="G470" s="67">
+        <f t="shared" si="112"/>
+        <v>6.25</v>
+      </c>
+      <c r="H470" s="67">
+        <f t="shared" si="112"/>
+        <v>6.25</v>
+      </c>
+      <c r="I470" s="67">
+        <f>I$50</f>
+        <v>50</v>
+      </c>
+      <c r="J470" s="67">
+        <f t="shared" ref="J469:N470" si="113">J$50</f>
+        <v>25</v>
+      </c>
+      <c r="K470" s="67">
+        <f t="shared" si="113"/>
+        <v>25</v>
+      </c>
+      <c r="L470" s="67">
+        <f t="shared" si="113"/>
+        <v>50</v>
+      </c>
+      <c r="M470" s="67">
+        <f t="shared" si="113"/>
+        <v>25</v>
+      </c>
+      <c r="N470" s="67">
+        <f t="shared" si="113"/>
+        <v>25</v>
+      </c>
+      <c r="O470" s="108">
+        <f>O50-O468</f>
+        <v>250</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="431">
+  <mergeCells count="443">
+    <mergeCell ref="C468:H468"/>
+    <mergeCell ref="I468:N468"/>
+    <mergeCell ref="C457:H457"/>
+    <mergeCell ref="C458:H458"/>
+    <mergeCell ref="C459:H459"/>
+    <mergeCell ref="C460:H460"/>
+    <mergeCell ref="C461:H461"/>
+    <mergeCell ref="C462:H462"/>
+    <mergeCell ref="C463:H463"/>
+    <mergeCell ref="C464:H464"/>
+    <mergeCell ref="C465:H465"/>
+    <mergeCell ref="C466:H466"/>
+    <mergeCell ref="C400:H400"/>
+    <mergeCell ref="I400:N400"/>
+    <mergeCell ref="C401:H401"/>
+    <mergeCell ref="I401:N401"/>
+    <mergeCell ref="C416:H416"/>
+    <mergeCell ref="C413:H413"/>
+    <mergeCell ref="I413:N413"/>
+    <mergeCell ref="C417:H417"/>
+    <mergeCell ref="C418:H418"/>
+    <mergeCell ref="I418:N418"/>
+    <mergeCell ref="C414:H414"/>
+    <mergeCell ref="I414:N414"/>
+    <mergeCell ref="C415:H415"/>
+    <mergeCell ref="I415:N415"/>
+    <mergeCell ref="C404:H404"/>
+    <mergeCell ref="I404:N404"/>
+    <mergeCell ref="C409:H409"/>
+    <mergeCell ref="I409:N409"/>
+    <mergeCell ref="C410:H410"/>
+    <mergeCell ref="I410:N410"/>
+    <mergeCell ref="C411:H411"/>
+    <mergeCell ref="I411:N411"/>
+    <mergeCell ref="C412:H412"/>
+    <mergeCell ref="I412:N412"/>
+    <mergeCell ref="C395:H395"/>
+    <mergeCell ref="I395:N395"/>
+    <mergeCell ref="C396:H396"/>
+    <mergeCell ref="I396:N396"/>
+    <mergeCell ref="C397:H397"/>
+    <mergeCell ref="I397:N397"/>
+    <mergeCell ref="C398:H398"/>
+    <mergeCell ref="I398:N398"/>
+    <mergeCell ref="C399:H399"/>
+    <mergeCell ref="I399:N399"/>
+    <mergeCell ref="C364:E364"/>
+    <mergeCell ref="F364:H364"/>
+    <mergeCell ref="I364:K364"/>
+    <mergeCell ref="L364:N364"/>
+    <mergeCell ref="C338:H338"/>
+    <mergeCell ref="I338:N338"/>
+    <mergeCell ref="C344:H344"/>
+    <mergeCell ref="I344:N344"/>
+    <mergeCell ref="C345:H345"/>
+    <mergeCell ref="I345:N345"/>
+    <mergeCell ref="C339:H339"/>
+    <mergeCell ref="I339:N339"/>
+    <mergeCell ref="C340:H340"/>
+    <mergeCell ref="I340:N340"/>
+    <mergeCell ref="C341:H341"/>
+    <mergeCell ref="I341:N341"/>
+    <mergeCell ref="C342:H342"/>
+    <mergeCell ref="I342:N342"/>
+    <mergeCell ref="C343:H343"/>
+    <mergeCell ref="I343:N343"/>
+    <mergeCell ref="C326:H326"/>
+    <mergeCell ref="I326:N326"/>
+    <mergeCell ref="C327:H327"/>
+    <mergeCell ref="I327:N327"/>
+    <mergeCell ref="C328:H328"/>
+    <mergeCell ref="I328:N328"/>
+    <mergeCell ref="C329:H329"/>
+    <mergeCell ref="I329:N329"/>
+    <mergeCell ref="C337:H337"/>
+    <mergeCell ref="I337:N337"/>
+    <mergeCell ref="C321:H321"/>
+    <mergeCell ref="I321:N321"/>
+    <mergeCell ref="C322:H322"/>
+    <mergeCell ref="I322:N322"/>
+    <mergeCell ref="C323:H323"/>
+    <mergeCell ref="I323:N323"/>
+    <mergeCell ref="C324:H324"/>
+    <mergeCell ref="I324:N324"/>
+    <mergeCell ref="C325:H325"/>
+    <mergeCell ref="I325:N325"/>
+    <mergeCell ref="C311:E311"/>
+    <mergeCell ref="F311:H311"/>
+    <mergeCell ref="I311:K311"/>
+    <mergeCell ref="L311:N311"/>
+    <mergeCell ref="C312:E312"/>
+    <mergeCell ref="F312:H312"/>
+    <mergeCell ref="I312:K312"/>
+    <mergeCell ref="L312:N312"/>
+    <mergeCell ref="C313:E313"/>
+    <mergeCell ref="F313:H313"/>
+    <mergeCell ref="I313:K313"/>
+    <mergeCell ref="L313:N313"/>
+    <mergeCell ref="L308:N308"/>
+    <mergeCell ref="C309:E309"/>
+    <mergeCell ref="F309:H309"/>
+    <mergeCell ref="I309:K309"/>
+    <mergeCell ref="L309:N309"/>
+    <mergeCell ref="C310:E310"/>
+    <mergeCell ref="F310:H310"/>
+    <mergeCell ref="I310:K310"/>
+    <mergeCell ref="L310:N310"/>
+    <mergeCell ref="C308:E308"/>
+    <mergeCell ref="F308:H308"/>
+    <mergeCell ref="I308:K308"/>
+    <mergeCell ref="C207:E207"/>
+    <mergeCell ref="C208:E208"/>
+    <mergeCell ref="C209:E209"/>
+    <mergeCell ref="C210:E210"/>
+    <mergeCell ref="C211:E211"/>
+    <mergeCell ref="C212:E212"/>
+    <mergeCell ref="C306:E306"/>
+    <mergeCell ref="F306:H306"/>
+    <mergeCell ref="I306:K306"/>
+    <mergeCell ref="F207:H207"/>
+    <mergeCell ref="I210:K210"/>
+    <mergeCell ref="I211:K211"/>
+    <mergeCell ref="I212:K212"/>
+    <mergeCell ref="I213:K213"/>
+    <mergeCell ref="I214:K214"/>
+    <mergeCell ref="I215:K215"/>
+    <mergeCell ref="F210:H210"/>
+    <mergeCell ref="C226:H226"/>
+    <mergeCell ref="C227:H227"/>
+    <mergeCell ref="C228:H228"/>
+    <mergeCell ref="I226:N226"/>
+    <mergeCell ref="I227:N227"/>
+    <mergeCell ref="I228:N228"/>
+    <mergeCell ref="C224:H224"/>
+    <mergeCell ref="I122:K122"/>
+    <mergeCell ref="I123:K123"/>
+    <mergeCell ref="I117:K117"/>
+    <mergeCell ref="I118:K118"/>
+    <mergeCell ref="I119:K119"/>
+    <mergeCell ref="I120:K120"/>
+    <mergeCell ref="I121:K121"/>
+    <mergeCell ref="C123:E123"/>
+    <mergeCell ref="F123:H123"/>
+    <mergeCell ref="I112:K112"/>
+    <mergeCell ref="I113:K113"/>
+    <mergeCell ref="I114:K114"/>
+    <mergeCell ref="I115:K115"/>
+    <mergeCell ref="I116:K116"/>
+    <mergeCell ref="C121:E121"/>
+    <mergeCell ref="F121:H121"/>
+    <mergeCell ref="C122:E122"/>
+    <mergeCell ref="F122:H122"/>
+    <mergeCell ref="C118:E118"/>
+    <mergeCell ref="F118:H118"/>
+    <mergeCell ref="C119:E119"/>
+    <mergeCell ref="F119:H119"/>
+    <mergeCell ref="C120:E120"/>
+    <mergeCell ref="F120:H120"/>
+    <mergeCell ref="C115:E115"/>
+    <mergeCell ref="F115:H115"/>
+    <mergeCell ref="C116:E116"/>
+    <mergeCell ref="F116:H116"/>
+    <mergeCell ref="C117:E117"/>
+    <mergeCell ref="F117:H117"/>
+    <mergeCell ref="C112:E112"/>
+    <mergeCell ref="F112:H112"/>
+    <mergeCell ref="C113:E113"/>
+    <mergeCell ref="F113:H113"/>
+    <mergeCell ref="C114:E114"/>
+    <mergeCell ref="F114:H114"/>
+    <mergeCell ref="C109:E109"/>
+    <mergeCell ref="F98:H98"/>
+    <mergeCell ref="F99:H99"/>
+    <mergeCell ref="F100:H100"/>
+    <mergeCell ref="F101:H101"/>
+    <mergeCell ref="F102:H102"/>
+    <mergeCell ref="F103:H103"/>
+    <mergeCell ref="F104:H104"/>
+    <mergeCell ref="F105:H105"/>
+    <mergeCell ref="F106:H106"/>
+    <mergeCell ref="F107:H107"/>
+    <mergeCell ref="F108:H108"/>
+    <mergeCell ref="F109:H109"/>
+    <mergeCell ref="C104:E104"/>
+    <mergeCell ref="C105:E105"/>
+    <mergeCell ref="C106:E106"/>
+    <mergeCell ref="C107:E107"/>
+    <mergeCell ref="C108:E108"/>
+    <mergeCell ref="C99:E99"/>
+    <mergeCell ref="C100:E100"/>
+    <mergeCell ref="C101:E101"/>
+    <mergeCell ref="C84:E84"/>
+    <mergeCell ref="C85:E85"/>
+    <mergeCell ref="C73:E73"/>
+    <mergeCell ref="C74:E74"/>
+    <mergeCell ref="C75:E75"/>
+    <mergeCell ref="C76:E76"/>
+    <mergeCell ref="C77:E77"/>
+    <mergeCell ref="C102:E102"/>
+    <mergeCell ref="C103:E103"/>
+    <mergeCell ref="C91:E91"/>
+    <mergeCell ref="C92:E92"/>
+    <mergeCell ref="C93:E93"/>
+    <mergeCell ref="C94:E94"/>
+    <mergeCell ref="C98:E98"/>
+    <mergeCell ref="C86:E86"/>
+    <mergeCell ref="C87:E87"/>
+    <mergeCell ref="C88:E88"/>
+    <mergeCell ref="C89:E89"/>
+    <mergeCell ref="C90:E90"/>
+    <mergeCell ref="C55:E55"/>
+    <mergeCell ref="C56:E56"/>
+    <mergeCell ref="C58:E58"/>
+    <mergeCell ref="C57:E57"/>
+    <mergeCell ref="C59:E59"/>
+    <mergeCell ref="C60:E60"/>
+    <mergeCell ref="C78:E78"/>
+    <mergeCell ref="C79:E79"/>
+    <mergeCell ref="C83:E83"/>
+    <mergeCell ref="C68:E68"/>
+    <mergeCell ref="C69:E69"/>
+    <mergeCell ref="C70:E70"/>
+    <mergeCell ref="C71:E71"/>
+    <mergeCell ref="C72:E72"/>
+    <mergeCell ref="C35:E35"/>
+    <mergeCell ref="F35:H35"/>
+    <mergeCell ref="I35:K35"/>
+    <mergeCell ref="L35:N35"/>
+    <mergeCell ref="C25:E25"/>
+    <mergeCell ref="F25:H25"/>
+    <mergeCell ref="I25:K25"/>
+    <mergeCell ref="L25:N25"/>
+    <mergeCell ref="C34:E34"/>
+    <mergeCell ref="F34:H34"/>
+    <mergeCell ref="I34:K34"/>
+    <mergeCell ref="L34:N34"/>
+    <mergeCell ref="C54:E54"/>
+    <mergeCell ref="C53:E53"/>
+    <mergeCell ref="C63:E63"/>
+    <mergeCell ref="C62:E62"/>
+    <mergeCell ref="C64:E64"/>
+    <mergeCell ref="C61:E61"/>
+    <mergeCell ref="I207:K207"/>
+    <mergeCell ref="I208:K208"/>
+    <mergeCell ref="I209:K209"/>
+    <mergeCell ref="F208:H208"/>
+    <mergeCell ref="F209:H209"/>
+    <mergeCell ref="C127:E127"/>
+    <mergeCell ref="F127:H127"/>
+    <mergeCell ref="I127:K127"/>
+    <mergeCell ref="C128:E128"/>
+    <mergeCell ref="F128:H128"/>
+    <mergeCell ref="I128:K128"/>
+    <mergeCell ref="C129:E129"/>
+    <mergeCell ref="F129:H129"/>
+    <mergeCell ref="I129:K129"/>
+    <mergeCell ref="C130:E130"/>
+    <mergeCell ref="F130:H130"/>
+    <mergeCell ref="I130:K130"/>
+    <mergeCell ref="C131:E131"/>
+    <mergeCell ref="L207:N207"/>
+    <mergeCell ref="L208:N208"/>
+    <mergeCell ref="L209:N209"/>
+    <mergeCell ref="L210:N210"/>
+    <mergeCell ref="L211:N211"/>
+    <mergeCell ref="L212:N212"/>
+    <mergeCell ref="L213:N213"/>
+    <mergeCell ref="L214:N214"/>
+    <mergeCell ref="L215:N215"/>
+    <mergeCell ref="I224:N224"/>
+    <mergeCell ref="C225:H225"/>
+    <mergeCell ref="I225:N225"/>
+    <mergeCell ref="C213:E213"/>
+    <mergeCell ref="C214:E214"/>
+    <mergeCell ref="C215:E215"/>
+    <mergeCell ref="C223:H223"/>
+    <mergeCell ref="I223:N223"/>
+    <mergeCell ref="F211:H211"/>
+    <mergeCell ref="F212:H212"/>
+    <mergeCell ref="F213:H213"/>
+    <mergeCell ref="F214:H214"/>
+    <mergeCell ref="F215:H215"/>
+    <mergeCell ref="C240:H240"/>
+    <mergeCell ref="I240:N240"/>
+    <mergeCell ref="C241:H241"/>
+    <mergeCell ref="I241:N241"/>
+    <mergeCell ref="C242:H242"/>
+    <mergeCell ref="I242:N242"/>
+    <mergeCell ref="C239:H239"/>
+    <mergeCell ref="I239:N239"/>
+    <mergeCell ref="C229:H229"/>
+    <mergeCell ref="C230:H230"/>
+    <mergeCell ref="C231:H231"/>
+    <mergeCell ref="I229:N229"/>
+    <mergeCell ref="I230:N230"/>
+    <mergeCell ref="I231:N231"/>
+    <mergeCell ref="C243:H243"/>
+    <mergeCell ref="I243:N243"/>
+    <mergeCell ref="C244:H244"/>
+    <mergeCell ref="I244:N244"/>
+    <mergeCell ref="C245:H245"/>
+    <mergeCell ref="I245:N245"/>
+    <mergeCell ref="C246:H246"/>
+    <mergeCell ref="I246:N246"/>
+    <mergeCell ref="C247:H247"/>
+    <mergeCell ref="I247:N247"/>
+    <mergeCell ref="C305:E305"/>
+    <mergeCell ref="F305:H305"/>
+    <mergeCell ref="I305:K305"/>
+    <mergeCell ref="L305:N305"/>
+    <mergeCell ref="L306:N306"/>
+    <mergeCell ref="C307:E307"/>
+    <mergeCell ref="F307:H307"/>
+    <mergeCell ref="I307:K307"/>
+    <mergeCell ref="L307:N307"/>
+    <mergeCell ref="F131:H131"/>
+    <mergeCell ref="I131:K131"/>
+    <mergeCell ref="C132:E132"/>
+    <mergeCell ref="F132:H132"/>
+    <mergeCell ref="I132:K132"/>
+    <mergeCell ref="C133:E133"/>
+    <mergeCell ref="F133:H133"/>
+    <mergeCell ref="I133:K133"/>
+    <mergeCell ref="C134:E134"/>
+    <mergeCell ref="F134:H134"/>
+    <mergeCell ref="I134:K134"/>
+    <mergeCell ref="C138:E138"/>
+    <mergeCell ref="F138:H138"/>
+    <mergeCell ref="I138:K138"/>
+    <mergeCell ref="C135:E135"/>
+    <mergeCell ref="F135:H135"/>
+    <mergeCell ref="I135:K135"/>
+    <mergeCell ref="C136:E136"/>
+    <mergeCell ref="F136:H136"/>
+    <mergeCell ref="I136:K136"/>
+    <mergeCell ref="C137:E137"/>
+    <mergeCell ref="F137:H137"/>
+    <mergeCell ref="I137:K137"/>
+    <mergeCell ref="C378:H378"/>
+    <mergeCell ref="I378:N378"/>
+    <mergeCell ref="C383:H383"/>
+    <mergeCell ref="I383:N383"/>
+    <mergeCell ref="C371:H371"/>
+    <mergeCell ref="I371:N371"/>
+    <mergeCell ref="C372:H372"/>
+    <mergeCell ref="I372:N372"/>
+    <mergeCell ref="C373:H373"/>
+    <mergeCell ref="I373:N373"/>
+    <mergeCell ref="C374:H374"/>
+    <mergeCell ref="I374:N374"/>
+    <mergeCell ref="C375:H375"/>
+    <mergeCell ref="I375:N375"/>
+    <mergeCell ref="C384:H384"/>
+    <mergeCell ref="I384:N384"/>
+    <mergeCell ref="C385:H385"/>
+    <mergeCell ref="I385:N385"/>
+    <mergeCell ref="C386:H386"/>
+    <mergeCell ref="I386:N386"/>
+    <mergeCell ref="C387:H387"/>
+    <mergeCell ref="I387:N387"/>
+    <mergeCell ref="C390:H390"/>
+    <mergeCell ref="I390:N390"/>
+    <mergeCell ref="C389:H389"/>
+    <mergeCell ref="C423:E423"/>
+    <mergeCell ref="F423:H423"/>
+    <mergeCell ref="I423:K423"/>
+    <mergeCell ref="L423:N423"/>
+    <mergeCell ref="C424:E424"/>
+    <mergeCell ref="F424:H424"/>
+    <mergeCell ref="I424:K424"/>
+    <mergeCell ref="L424:N424"/>
+    <mergeCell ref="C425:E425"/>
+    <mergeCell ref="F425:H425"/>
+    <mergeCell ref="I425:K425"/>
+    <mergeCell ref="L425:N425"/>
+    <mergeCell ref="C426:E426"/>
+    <mergeCell ref="F426:H426"/>
+    <mergeCell ref="I426:K426"/>
+    <mergeCell ref="L426:N426"/>
+    <mergeCell ref="C427:E427"/>
+    <mergeCell ref="F427:H427"/>
+    <mergeCell ref="I427:K427"/>
+    <mergeCell ref="L427:N427"/>
+    <mergeCell ref="C428:E428"/>
+    <mergeCell ref="F428:H428"/>
+    <mergeCell ref="I428:K428"/>
+    <mergeCell ref="L428:N428"/>
+    <mergeCell ref="C429:E429"/>
+    <mergeCell ref="F429:H429"/>
+    <mergeCell ref="I429:K429"/>
+    <mergeCell ref="L429:N429"/>
+    <mergeCell ref="C430:E430"/>
+    <mergeCell ref="F430:H430"/>
+    <mergeCell ref="I430:K430"/>
+    <mergeCell ref="L430:N430"/>
+    <mergeCell ref="C431:E431"/>
+    <mergeCell ref="F431:H431"/>
+    <mergeCell ref="I431:K431"/>
+    <mergeCell ref="L431:N431"/>
+    <mergeCell ref="C444:E444"/>
+    <mergeCell ref="F444:H444"/>
+    <mergeCell ref="I444:K444"/>
+    <mergeCell ref="L444:N444"/>
+    <mergeCell ref="C445:E445"/>
+    <mergeCell ref="F445:H445"/>
+    <mergeCell ref="I445:K445"/>
+    <mergeCell ref="L445:N445"/>
+    <mergeCell ref="C440:E440"/>
+    <mergeCell ref="F440:H440"/>
+    <mergeCell ref="I440:K440"/>
+    <mergeCell ref="L440:N440"/>
+    <mergeCell ref="C441:E441"/>
+    <mergeCell ref="F441:H441"/>
+    <mergeCell ref="I441:K441"/>
+    <mergeCell ref="L441:N441"/>
+    <mergeCell ref="C442:E442"/>
+    <mergeCell ref="F442:H442"/>
+    <mergeCell ref="I442:K442"/>
+    <mergeCell ref="L442:N442"/>
     <mergeCell ref="C435:E435"/>
     <mergeCell ref="F435:H435"/>
     <mergeCell ref="I435:K435"/>
@@ -11000,413 +11745,6 @@
     <mergeCell ref="F443:H443"/>
     <mergeCell ref="I443:K443"/>
     <mergeCell ref="L443:N443"/>
-    <mergeCell ref="C444:E444"/>
-    <mergeCell ref="F444:H444"/>
-    <mergeCell ref="I444:K444"/>
-    <mergeCell ref="L444:N444"/>
-    <mergeCell ref="C445:E445"/>
-    <mergeCell ref="F445:H445"/>
-    <mergeCell ref="I445:K445"/>
-    <mergeCell ref="L445:N445"/>
-    <mergeCell ref="C440:E440"/>
-    <mergeCell ref="F440:H440"/>
-    <mergeCell ref="I440:K440"/>
-    <mergeCell ref="L440:N440"/>
-    <mergeCell ref="C441:E441"/>
-    <mergeCell ref="F441:H441"/>
-    <mergeCell ref="I441:K441"/>
-    <mergeCell ref="L441:N441"/>
-    <mergeCell ref="C442:E442"/>
-    <mergeCell ref="F442:H442"/>
-    <mergeCell ref="I442:K442"/>
-    <mergeCell ref="L442:N442"/>
-    <mergeCell ref="C429:E429"/>
-    <mergeCell ref="F429:H429"/>
-    <mergeCell ref="I429:K429"/>
-    <mergeCell ref="L429:N429"/>
-    <mergeCell ref="C430:E430"/>
-    <mergeCell ref="F430:H430"/>
-    <mergeCell ref="I430:K430"/>
-    <mergeCell ref="L430:N430"/>
-    <mergeCell ref="C431:E431"/>
-    <mergeCell ref="F431:H431"/>
-    <mergeCell ref="I431:K431"/>
-    <mergeCell ref="L431:N431"/>
-    <mergeCell ref="C426:E426"/>
-    <mergeCell ref="F426:H426"/>
-    <mergeCell ref="I426:K426"/>
-    <mergeCell ref="L426:N426"/>
-    <mergeCell ref="C427:E427"/>
-    <mergeCell ref="F427:H427"/>
-    <mergeCell ref="I427:K427"/>
-    <mergeCell ref="L427:N427"/>
-    <mergeCell ref="C428:E428"/>
-    <mergeCell ref="F428:H428"/>
-    <mergeCell ref="I428:K428"/>
-    <mergeCell ref="L428:N428"/>
-    <mergeCell ref="C423:E423"/>
-    <mergeCell ref="F423:H423"/>
-    <mergeCell ref="I423:K423"/>
-    <mergeCell ref="L423:N423"/>
-    <mergeCell ref="C424:E424"/>
-    <mergeCell ref="F424:H424"/>
-    <mergeCell ref="I424:K424"/>
-    <mergeCell ref="L424:N424"/>
-    <mergeCell ref="C425:E425"/>
-    <mergeCell ref="F425:H425"/>
-    <mergeCell ref="I425:K425"/>
-    <mergeCell ref="L425:N425"/>
-    <mergeCell ref="C384:H384"/>
-    <mergeCell ref="I384:N384"/>
-    <mergeCell ref="C385:H385"/>
-    <mergeCell ref="I385:N385"/>
-    <mergeCell ref="C386:H386"/>
-    <mergeCell ref="I386:N386"/>
-    <mergeCell ref="C387:H387"/>
-    <mergeCell ref="I387:N387"/>
-    <mergeCell ref="C390:H390"/>
-    <mergeCell ref="I390:N390"/>
-    <mergeCell ref="C389:H389"/>
-    <mergeCell ref="C378:H378"/>
-    <mergeCell ref="I378:N378"/>
-    <mergeCell ref="C383:H383"/>
-    <mergeCell ref="I383:N383"/>
-    <mergeCell ref="C371:H371"/>
-    <mergeCell ref="I371:N371"/>
-    <mergeCell ref="C372:H372"/>
-    <mergeCell ref="I372:N372"/>
-    <mergeCell ref="C373:H373"/>
-    <mergeCell ref="I373:N373"/>
-    <mergeCell ref="C374:H374"/>
-    <mergeCell ref="I374:N374"/>
-    <mergeCell ref="C375:H375"/>
-    <mergeCell ref="I375:N375"/>
-    <mergeCell ref="C138:E138"/>
-    <mergeCell ref="F138:H138"/>
-    <mergeCell ref="I138:K138"/>
-    <mergeCell ref="C135:E135"/>
-    <mergeCell ref="F135:H135"/>
-    <mergeCell ref="I135:K135"/>
-    <mergeCell ref="C136:E136"/>
-    <mergeCell ref="F136:H136"/>
-    <mergeCell ref="I136:K136"/>
-    <mergeCell ref="C137:E137"/>
-    <mergeCell ref="F137:H137"/>
-    <mergeCell ref="I137:K137"/>
-    <mergeCell ref="F131:H131"/>
-    <mergeCell ref="I131:K131"/>
-    <mergeCell ref="C132:E132"/>
-    <mergeCell ref="F132:H132"/>
-    <mergeCell ref="I132:K132"/>
-    <mergeCell ref="C133:E133"/>
-    <mergeCell ref="F133:H133"/>
-    <mergeCell ref="I133:K133"/>
-    <mergeCell ref="C134:E134"/>
-    <mergeCell ref="F134:H134"/>
-    <mergeCell ref="I134:K134"/>
-    <mergeCell ref="C305:E305"/>
-    <mergeCell ref="F305:H305"/>
-    <mergeCell ref="I305:K305"/>
-    <mergeCell ref="L305:N305"/>
-    <mergeCell ref="L306:N306"/>
-    <mergeCell ref="C307:E307"/>
-    <mergeCell ref="F307:H307"/>
-    <mergeCell ref="I307:K307"/>
-    <mergeCell ref="L307:N307"/>
-    <mergeCell ref="C243:H243"/>
-    <mergeCell ref="I243:N243"/>
-    <mergeCell ref="C244:H244"/>
-    <mergeCell ref="I244:N244"/>
-    <mergeCell ref="C245:H245"/>
-    <mergeCell ref="I245:N245"/>
-    <mergeCell ref="C246:H246"/>
-    <mergeCell ref="I246:N246"/>
-    <mergeCell ref="C247:H247"/>
-    <mergeCell ref="I247:N247"/>
-    <mergeCell ref="C240:H240"/>
-    <mergeCell ref="I240:N240"/>
-    <mergeCell ref="C241:H241"/>
-    <mergeCell ref="I241:N241"/>
-    <mergeCell ref="C242:H242"/>
-    <mergeCell ref="I242:N242"/>
-    <mergeCell ref="C239:H239"/>
-    <mergeCell ref="I239:N239"/>
-    <mergeCell ref="C229:H229"/>
-    <mergeCell ref="C230:H230"/>
-    <mergeCell ref="C231:H231"/>
-    <mergeCell ref="I229:N229"/>
-    <mergeCell ref="I230:N230"/>
-    <mergeCell ref="I231:N231"/>
-    <mergeCell ref="I224:N224"/>
-    <mergeCell ref="C225:H225"/>
-    <mergeCell ref="I225:N225"/>
-    <mergeCell ref="C213:E213"/>
-    <mergeCell ref="C214:E214"/>
-    <mergeCell ref="C215:E215"/>
-    <mergeCell ref="C223:H223"/>
-    <mergeCell ref="I223:N223"/>
-    <mergeCell ref="F211:H211"/>
-    <mergeCell ref="F212:H212"/>
-    <mergeCell ref="F213:H213"/>
-    <mergeCell ref="F214:H214"/>
-    <mergeCell ref="F215:H215"/>
-    <mergeCell ref="L207:N207"/>
-    <mergeCell ref="L208:N208"/>
-    <mergeCell ref="L209:N209"/>
-    <mergeCell ref="L210:N210"/>
-    <mergeCell ref="L211:N211"/>
-    <mergeCell ref="L212:N212"/>
-    <mergeCell ref="L213:N213"/>
-    <mergeCell ref="L214:N214"/>
-    <mergeCell ref="L215:N215"/>
-    <mergeCell ref="C54:E54"/>
-    <mergeCell ref="C53:E53"/>
-    <mergeCell ref="C63:E63"/>
-    <mergeCell ref="C62:E62"/>
-    <mergeCell ref="C64:E64"/>
-    <mergeCell ref="C61:E61"/>
-    <mergeCell ref="I207:K207"/>
-    <mergeCell ref="I208:K208"/>
-    <mergeCell ref="I209:K209"/>
-    <mergeCell ref="F208:H208"/>
-    <mergeCell ref="F209:H209"/>
-    <mergeCell ref="C127:E127"/>
-    <mergeCell ref="F127:H127"/>
-    <mergeCell ref="I127:K127"/>
-    <mergeCell ref="C128:E128"/>
-    <mergeCell ref="F128:H128"/>
-    <mergeCell ref="I128:K128"/>
-    <mergeCell ref="C129:E129"/>
-    <mergeCell ref="F129:H129"/>
-    <mergeCell ref="I129:K129"/>
-    <mergeCell ref="C130:E130"/>
-    <mergeCell ref="F130:H130"/>
-    <mergeCell ref="I130:K130"/>
-    <mergeCell ref="C131:E131"/>
-    <mergeCell ref="C35:E35"/>
-    <mergeCell ref="F35:H35"/>
-    <mergeCell ref="I35:K35"/>
-    <mergeCell ref="L35:N35"/>
-    <mergeCell ref="C25:E25"/>
-    <mergeCell ref="F25:H25"/>
-    <mergeCell ref="I25:K25"/>
-    <mergeCell ref="L25:N25"/>
-    <mergeCell ref="C34:E34"/>
-    <mergeCell ref="F34:H34"/>
-    <mergeCell ref="I34:K34"/>
-    <mergeCell ref="L34:N34"/>
-    <mergeCell ref="C55:E55"/>
-    <mergeCell ref="C56:E56"/>
-    <mergeCell ref="C58:E58"/>
-    <mergeCell ref="C57:E57"/>
-    <mergeCell ref="C59:E59"/>
-    <mergeCell ref="C60:E60"/>
-    <mergeCell ref="C78:E78"/>
-    <mergeCell ref="C79:E79"/>
-    <mergeCell ref="C83:E83"/>
-    <mergeCell ref="C68:E68"/>
-    <mergeCell ref="C69:E69"/>
-    <mergeCell ref="C70:E70"/>
-    <mergeCell ref="C71:E71"/>
-    <mergeCell ref="C72:E72"/>
-    <mergeCell ref="C84:E84"/>
-    <mergeCell ref="C85:E85"/>
-    <mergeCell ref="C73:E73"/>
-    <mergeCell ref="C74:E74"/>
-    <mergeCell ref="C75:E75"/>
-    <mergeCell ref="C76:E76"/>
-    <mergeCell ref="C77:E77"/>
-    <mergeCell ref="C102:E102"/>
-    <mergeCell ref="C103:E103"/>
-    <mergeCell ref="C91:E91"/>
-    <mergeCell ref="C92:E92"/>
-    <mergeCell ref="C93:E93"/>
-    <mergeCell ref="C94:E94"/>
-    <mergeCell ref="C98:E98"/>
-    <mergeCell ref="C86:E86"/>
-    <mergeCell ref="C87:E87"/>
-    <mergeCell ref="C88:E88"/>
-    <mergeCell ref="C89:E89"/>
-    <mergeCell ref="C90:E90"/>
-    <mergeCell ref="F113:H113"/>
-    <mergeCell ref="C114:E114"/>
-    <mergeCell ref="F114:H114"/>
-    <mergeCell ref="C109:E109"/>
-    <mergeCell ref="F98:H98"/>
-    <mergeCell ref="F99:H99"/>
-    <mergeCell ref="F100:H100"/>
-    <mergeCell ref="F101:H101"/>
-    <mergeCell ref="F102:H102"/>
-    <mergeCell ref="F103:H103"/>
-    <mergeCell ref="F104:H104"/>
-    <mergeCell ref="F105:H105"/>
-    <mergeCell ref="F106:H106"/>
-    <mergeCell ref="F107:H107"/>
-    <mergeCell ref="F108:H108"/>
-    <mergeCell ref="F109:H109"/>
-    <mergeCell ref="C104:E104"/>
-    <mergeCell ref="C105:E105"/>
-    <mergeCell ref="C106:E106"/>
-    <mergeCell ref="C107:E107"/>
-    <mergeCell ref="C108:E108"/>
-    <mergeCell ref="C99:E99"/>
-    <mergeCell ref="C100:E100"/>
-    <mergeCell ref="C101:E101"/>
-    <mergeCell ref="I112:K112"/>
-    <mergeCell ref="I113:K113"/>
-    <mergeCell ref="I114:K114"/>
-    <mergeCell ref="I115:K115"/>
-    <mergeCell ref="I116:K116"/>
-    <mergeCell ref="C121:E121"/>
-    <mergeCell ref="F121:H121"/>
-    <mergeCell ref="C122:E122"/>
-    <mergeCell ref="F122:H122"/>
-    <mergeCell ref="C118:E118"/>
-    <mergeCell ref="F118:H118"/>
-    <mergeCell ref="C119:E119"/>
-    <mergeCell ref="F119:H119"/>
-    <mergeCell ref="C120:E120"/>
-    <mergeCell ref="F120:H120"/>
-    <mergeCell ref="C115:E115"/>
-    <mergeCell ref="F115:H115"/>
-    <mergeCell ref="C116:E116"/>
-    <mergeCell ref="F116:H116"/>
-    <mergeCell ref="C117:E117"/>
-    <mergeCell ref="F117:H117"/>
-    <mergeCell ref="C112:E112"/>
-    <mergeCell ref="F112:H112"/>
-    <mergeCell ref="C113:E113"/>
-    <mergeCell ref="I122:K122"/>
-    <mergeCell ref="I123:K123"/>
-    <mergeCell ref="I117:K117"/>
-    <mergeCell ref="I118:K118"/>
-    <mergeCell ref="I119:K119"/>
-    <mergeCell ref="I120:K120"/>
-    <mergeCell ref="I121:K121"/>
-    <mergeCell ref="C123:E123"/>
-    <mergeCell ref="F123:H123"/>
-    <mergeCell ref="C207:E207"/>
-    <mergeCell ref="C208:E208"/>
-    <mergeCell ref="C209:E209"/>
-    <mergeCell ref="C210:E210"/>
-    <mergeCell ref="C211:E211"/>
-    <mergeCell ref="C212:E212"/>
-    <mergeCell ref="C306:E306"/>
-    <mergeCell ref="F306:H306"/>
-    <mergeCell ref="I306:K306"/>
-    <mergeCell ref="F207:H207"/>
-    <mergeCell ref="I210:K210"/>
-    <mergeCell ref="I211:K211"/>
-    <mergeCell ref="I212:K212"/>
-    <mergeCell ref="I213:K213"/>
-    <mergeCell ref="I214:K214"/>
-    <mergeCell ref="I215:K215"/>
-    <mergeCell ref="F210:H210"/>
-    <mergeCell ref="C226:H226"/>
-    <mergeCell ref="C227:H227"/>
-    <mergeCell ref="C228:H228"/>
-    <mergeCell ref="I226:N226"/>
-    <mergeCell ref="I227:N227"/>
-    <mergeCell ref="I228:N228"/>
-    <mergeCell ref="C224:H224"/>
-    <mergeCell ref="L308:N308"/>
-    <mergeCell ref="C309:E309"/>
-    <mergeCell ref="F309:H309"/>
-    <mergeCell ref="I309:K309"/>
-    <mergeCell ref="L309:N309"/>
-    <mergeCell ref="C310:E310"/>
-    <mergeCell ref="F310:H310"/>
-    <mergeCell ref="I310:K310"/>
-    <mergeCell ref="L310:N310"/>
-    <mergeCell ref="C308:E308"/>
-    <mergeCell ref="F308:H308"/>
-    <mergeCell ref="I308:K308"/>
-    <mergeCell ref="C311:E311"/>
-    <mergeCell ref="F311:H311"/>
-    <mergeCell ref="I311:K311"/>
-    <mergeCell ref="L311:N311"/>
-    <mergeCell ref="C312:E312"/>
-    <mergeCell ref="F312:H312"/>
-    <mergeCell ref="I312:K312"/>
-    <mergeCell ref="L312:N312"/>
-    <mergeCell ref="C313:E313"/>
-    <mergeCell ref="F313:H313"/>
-    <mergeCell ref="I313:K313"/>
-    <mergeCell ref="L313:N313"/>
-    <mergeCell ref="C321:H321"/>
-    <mergeCell ref="I321:N321"/>
-    <mergeCell ref="C322:H322"/>
-    <mergeCell ref="I322:N322"/>
-    <mergeCell ref="C323:H323"/>
-    <mergeCell ref="I323:N323"/>
-    <mergeCell ref="C324:H324"/>
-    <mergeCell ref="I324:N324"/>
-    <mergeCell ref="C325:H325"/>
-    <mergeCell ref="I325:N325"/>
-    <mergeCell ref="C326:H326"/>
-    <mergeCell ref="I326:N326"/>
-    <mergeCell ref="C327:H327"/>
-    <mergeCell ref="I327:N327"/>
-    <mergeCell ref="C328:H328"/>
-    <mergeCell ref="I328:N328"/>
-    <mergeCell ref="C329:H329"/>
-    <mergeCell ref="I329:N329"/>
-    <mergeCell ref="C337:H337"/>
-    <mergeCell ref="I337:N337"/>
-    <mergeCell ref="C364:E364"/>
-    <mergeCell ref="F364:H364"/>
-    <mergeCell ref="I364:K364"/>
-    <mergeCell ref="L364:N364"/>
-    <mergeCell ref="C338:H338"/>
-    <mergeCell ref="I338:N338"/>
-    <mergeCell ref="C344:H344"/>
-    <mergeCell ref="I344:N344"/>
-    <mergeCell ref="C345:H345"/>
-    <mergeCell ref="I345:N345"/>
-    <mergeCell ref="C339:H339"/>
-    <mergeCell ref="I339:N339"/>
-    <mergeCell ref="C340:H340"/>
-    <mergeCell ref="I340:N340"/>
-    <mergeCell ref="C341:H341"/>
-    <mergeCell ref="I341:N341"/>
-    <mergeCell ref="C342:H342"/>
-    <mergeCell ref="I342:N342"/>
-    <mergeCell ref="C343:H343"/>
-    <mergeCell ref="I343:N343"/>
-    <mergeCell ref="C395:H395"/>
-    <mergeCell ref="I395:N395"/>
-    <mergeCell ref="C396:H396"/>
-    <mergeCell ref="I396:N396"/>
-    <mergeCell ref="C397:H397"/>
-    <mergeCell ref="I397:N397"/>
-    <mergeCell ref="C398:H398"/>
-    <mergeCell ref="I398:N398"/>
-    <mergeCell ref="C399:H399"/>
-    <mergeCell ref="I399:N399"/>
-    <mergeCell ref="C400:H400"/>
-    <mergeCell ref="I400:N400"/>
-    <mergeCell ref="C401:H401"/>
-    <mergeCell ref="I401:N401"/>
-    <mergeCell ref="C416:H416"/>
-    <mergeCell ref="C413:H413"/>
-    <mergeCell ref="I413:N413"/>
-    <mergeCell ref="C417:H417"/>
-    <mergeCell ref="C418:H418"/>
-    <mergeCell ref="I418:N418"/>
-    <mergeCell ref="C414:H414"/>
-    <mergeCell ref="I414:N414"/>
-    <mergeCell ref="C415:H415"/>
-    <mergeCell ref="I415:N415"/>
-    <mergeCell ref="C404:H404"/>
-    <mergeCell ref="I404:N404"/>
-    <mergeCell ref="C409:H409"/>
-    <mergeCell ref="I409:N409"/>
-    <mergeCell ref="C410:H410"/>
-    <mergeCell ref="I410:N410"/>
-    <mergeCell ref="C411:H411"/>
-    <mergeCell ref="I411:N411"/>
-    <mergeCell ref="C412:H412"/>
-    <mergeCell ref="I412:N412"/>
   </mergeCells>
   <pageMargins left="0.70866141732283472" right="0.70866141732283472" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup paperSize="9" scale="44" orientation="portrait" r:id="rId1"/>
@@ -11425,7 +11763,7 @@
   <dimension ref="A2:M25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B23" sqref="B23"/>
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -12003,9 +12341,15 @@
     </row>
     <row r="25" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A25" s="59"/>
-      <c r="B25" s="56"/>
-      <c r="C25" s="56"/>
-      <c r="D25" s="56"/>
+      <c r="B25" s="85" t="s">
+        <v>189</v>
+      </c>
+      <c r="C25" s="70" t="s">
+        <v>190</v>
+      </c>
+      <c r="D25" s="70" t="s">
+        <v>171</v>
+      </c>
       <c r="E25"/>
       <c r="F25" s="56"/>
       <c r="G25" s="56"/>
@@ -12040,6 +12384,7 @@
     <hyperlink ref="B22" location="Calculations!A408" display="placed_acc_1_limit_QS" xr:uid="{37046EE5-CB2C-4C4C-8B2D-470EF59821CE}"/>
     <hyperlink ref="B23" location="'OED examples list'!A422" display="placed_loc_SS" xr:uid="{D181DCC0-D0B6-4FA6-B490-3AD1A99B9A13}"/>
     <hyperlink ref="B24" location="'OED examples list'!A439" display="placed_loc_limit_SS" xr:uid="{69C2FBDD-3D0C-48CC-8702-700ECF34429D}"/>
+    <hyperlink ref="B25" location="'OED examples list'!A456" display="acc_1_CAT_XL" xr:uid="{3F240C2F-C227-444D-B0EF-55D6D8A6F5BC}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>